<commit_message>
Added test results for Signavio and vertical pool test case
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="14400" windowHeight="11640" tabRatio="631" firstSheet="1" activeTab="1"/>
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="81">
   <si>
     <t>Documentation</t>
   </si>
@@ -499,12 +499,21 @@
   <si>
     <t>A.4.0</t>
   </si>
+  <si>
+    <t>Vertical Pool/Lane</t>
+  </si>
+  <si>
+    <t>A.4.1</t>
+  </si>
+  <si>
+    <t>Same as A.4.0 but using a vertical modelling direction</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -596,7 +605,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -865,8 +874,78 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom style="dashed">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -877,41 +956,13 @@
       </left>
       <right/>
       <top/>
-      <bottom style="dashed">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="dashed">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -920,42 +971,7 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -966,13 +982,30 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -986,7 +1019,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1046,72 +1079,60 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1130,7 +1151,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1139,19 +1160,46 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1164,9 +1212,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1204,7 +1252,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1238,7 +1286,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1273,10 +1320,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1449,14 +1495,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:K67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="39.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
@@ -1465,8 +1511,8 @@
     <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" ht="125.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:11" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:11" ht="125.25" customHeight="1" thickBot="1">
       <c r="B2" s="5" t="s">
         <v>38</v>
       </c>
@@ -1498,17 +1544,17 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11">
       <c r="B3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11">
       <c r="B4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6">
       <c r="B17" t="s">
         <v>41</v>
       </c>
@@ -1520,7 +1566,7 @@
       </c>
       <c r="F17" s="11"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6">
       <c r="D18" s="10" t="s">
         <v>9</v>
       </c>
@@ -1531,7 +1577,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6">
       <c r="D19" s="10" t="s">
         <v>10</v>
       </c>
@@ -1542,7 +1588,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6">
       <c r="D20" s="10" t="s">
         <v>11</v>
       </c>
@@ -1553,7 +1599,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6">
       <c r="D21" s="10" t="s">
         <v>12</v>
       </c>
@@ -1562,7 +1608,7 @@
       </c>
       <c r="F21" s="11"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6">
       <c r="D22" s="10" t="s">
         <v>46</v>
       </c>
@@ -1573,7 +1619,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6">
       <c r="D23" s="10" t="s">
         <v>18</v>
       </c>
@@ -1584,7 +1630,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6">
       <c r="D24" s="10" t="s">
         <v>47</v>
       </c>
@@ -1595,7 +1641,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6">
       <c r="D25" s="18" t="s">
         <v>49</v>
       </c>
@@ -1606,7 +1652,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6">
       <c r="B37" t="s">
         <v>42</v>
       </c>
@@ -1618,7 +1664,7 @@
       </c>
       <c r="F37" s="11"/>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:6">
       <c r="D38" s="10" t="s">
         <v>9</v>
       </c>
@@ -1629,7 +1675,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6">
       <c r="D39" s="10" t="s">
         <v>10</v>
       </c>
@@ -1640,7 +1686,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:6">
       <c r="D40" s="10" t="s">
         <v>11</v>
       </c>
@@ -1651,7 +1697,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:6">
       <c r="D41" s="10" t="s">
         <v>12</v>
       </c>
@@ -1660,7 +1706,7 @@
       </c>
       <c r="F41" s="11"/>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:6">
       <c r="D42" s="10" t="s">
         <v>46</v>
       </c>
@@ -1671,7 +1717,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6">
       <c r="D43" s="10" t="s">
         <v>18</v>
       </c>
@@ -1682,7 +1728,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:6">
       <c r="D44" s="10" t="s">
         <v>47</v>
       </c>
@@ -1693,7 +1739,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:6">
       <c r="D45" s="13" t="s">
         <v>49</v>
       </c>
@@ -1704,7 +1750,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:6">
       <c r="D46" s="14" t="s">
         <v>1</v>
       </c>
@@ -1713,7 +1759,7 @@
       </c>
       <c r="F46" s="16"/>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:6">
       <c r="B51" t="s">
         <v>43</v>
       </c>
@@ -1725,7 +1771,7 @@
       </c>
       <c r="F51" s="11"/>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:6">
       <c r="D52" s="10" t="s">
         <v>9</v>
       </c>
@@ -1736,7 +1782,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:6">
       <c r="D53" s="10" t="s">
         <v>10</v>
       </c>
@@ -1747,7 +1793,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:6">
       <c r="D54" s="10" t="s">
         <v>11</v>
       </c>
@@ -1758,7 +1804,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:6">
       <c r="D55" s="10" t="s">
         <v>12</v>
       </c>
@@ -1767,7 +1813,7 @@
       </c>
       <c r="F55" s="11"/>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:6">
       <c r="D56" s="10" t="s">
         <v>46</v>
       </c>
@@ -1778,7 +1824,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:6">
       <c r="D57" s="10" t="s">
         <v>18</v>
       </c>
@@ -1789,7 +1835,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:6">
       <c r="D58" s="10" t="s">
         <v>47</v>
       </c>
@@ -1800,7 +1846,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:6">
       <c r="D59" s="13" t="s">
         <v>49</v>
       </c>
@@ -1811,7 +1857,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:6">
       <c r="D60" s="17" t="s">
         <v>21</v>
       </c>
@@ -1822,7 +1868,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:6">
       <c r="D61" s="15" t="s">
         <v>22</v>
       </c>
@@ -1833,12 +1879,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2">
       <c r="B66" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2">
       <c r="B67" t="s">
         <v>45</v>
       </c>
@@ -1870,40 +1916,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:H14"/>
+  <dimension ref="A2:H15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="44.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.85546875" customWidth="1"/>
-    <col min="4" max="4" width="40.140625" style="37" customWidth="1"/>
+    <col min="4" max="4" width="40.140625" style="33" customWidth="1"/>
     <col min="5" max="5" width="6.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="25.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" customWidth="1"/>
     <col min="8" max="8" width="54.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="56" t="s">
+    <row r="2" spans="1:8" ht="45.75" thickBot="1">
+      <c r="A2" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="56" t="s">
+      <c r="B2" s="53"/>
+      <c r="C2" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="56" t="s">
+      <c r="D2" s="53"/>
+      <c r="E2" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="57"/>
+      <c r="F2" s="53"/>
       <c r="G2" s="25" t="s">
         <v>36</v>
       </c>
@@ -1911,199 +1957,221 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
+    <row r="3" spans="1:8" ht="50.25" customHeight="1">
+      <c r="A3" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="35">
+      <c r="C3" s="31">
         <v>1</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="50">
+      <c r="E3" s="46">
         <v>0</v>
       </c>
       <c r="F3" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="51" t="s">
+      <c r="G3" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="48" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="59"/>
-      <c r="B4" s="43" t="s">
+    <row r="4" spans="1:8" ht="42.75" customHeight="1">
+      <c r="A4" s="55"/>
+      <c r="B4" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="34">
+      <c r="C4" s="30">
         <v>2</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="53">
+      <c r="E4" s="49">
         <v>0</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="48" t="s">
+      <c r="H4" s="44" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="59"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="34">
+    <row r="5" spans="1:8" ht="43.5" customHeight="1">
+      <c r="A5" s="55"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="30">
         <v>3</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="53">
+      <c r="E5" s="49">
         <v>0</v>
       </c>
       <c r="F5" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="32" t="s">
+      <c r="G5" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="48" t="s">
+      <c r="H5" s="44" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="60"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="34">
+    <row r="6" spans="1:8" ht="50.25" customHeight="1">
+      <c r="A6" s="55"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="30">
         <v>4</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E6" s="57">
         <v>0</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="G6" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="60" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="7" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="58" t="s">
+    <row r="7" spans="1:8" ht="50.25" customHeight="1" thickBot="1">
+      <c r="A7" s="56"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="64">
+        <v>41</v>
+      </c>
+      <c r="D7" s="62" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="61">
+        <v>0</v>
+      </c>
+      <c r="F7" s="62" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" s="65" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" s="63" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="7" customFormat="1" ht="58.5" customHeight="1">
+      <c r="A8" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="55" t="s">
+      <c r="B8" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C8" s="21">
         <v>1</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D8" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E8" s="21">
         <v>0</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F8" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G8" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="46" t="s">
+      <c r="H8" s="42" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="59"/>
-      <c r="B8" s="43" t="s">
+    <row r="9" spans="1:8" ht="58.5" customHeight="1">
+      <c r="A9" s="55"/>
+      <c r="B9" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C9" s="28">
         <v>2</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D9" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="8">
-        <v>0</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="47" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="59"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="40">
-        <v>3</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="38">
+      <c r="E9" s="8">
         <v>0</v>
       </c>
       <c r="F9" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="39" t="s">
+      <c r="G9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="63" customHeight="1">
+      <c r="A10" s="55"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="36">
+        <v>3</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="34">
+        <v>0</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="48" t="s">
+      <c r="H10" s="44" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="60"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="33">
+    <row r="11" spans="1:8" ht="45" customHeight="1" thickBot="1">
+      <c r="A11" s="56"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="29">
         <v>4</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D11" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="E10" s="31">
+      <c r="E11" s="27">
         <v>0</v>
       </c>
-      <c r="F10" s="36" t="s">
+      <c r="F11" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G11" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="49" t="s">
+      <c r="H11" s="45" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D14" s="54" t="s">
+    <row r="15" spans="1:8">
+      <c r="D15" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="H14" s="54" t="s">
+      <c r="H15" s="50" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2112,8 +2180,8 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A3:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="60" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Merge two spreadsheets into one as discussed on 2013-04-17
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="14400" windowHeight="11640" tabRatio="631" firstSheet="1" activeTab="1"/>
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="94">
   <si>
     <t>Documentation</t>
   </si>
@@ -508,12 +508,51 @@
   <si>
     <t>Same as A.4.0 but using a vertical modelling direction</t>
   </si>
+  <si>
+    <t>MID Innovator</t>
+  </si>
+  <si>
+    <t>Signavio Process Editor</t>
+  </si>
+  <si>
+    <t>11.5.1.30223</t>
+  </si>
+  <si>
+    <t>Import</t>
+  </si>
+  <si>
+    <t>Export</t>
+  </si>
+  <si>
+    <t>Roundtrip</t>
+  </si>
+  <si>
+    <t>Tool under Test -&gt;</t>
+  </si>
+  <si>
+    <t>Date of Test -&gt;</t>
+  </si>
+  <si>
+    <t>Tool Version -&gt;</t>
+  </si>
+  <si>
+    <t>Issues</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Tool used for Reference</t>
+  </si>
+  <si>
+    <t>Trisotech BPMN 2.0 Modeler for Visio 4.0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -605,7 +644,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -819,19 +858,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -848,69 +874,25 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -977,6 +959,65 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -985,28 +1026,220 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1019,7 +1252,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1044,9 +1277,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1058,9 +1288,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1079,13 +1306,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1094,7 +1321,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1103,9 +1330,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1115,27 +1339,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1151,55 +1357,258 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1212,9 +1621,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1252,7 +1661,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1286,6 +1695,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1320,9 +1730,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1495,14 +1906,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="39.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
@@ -1511,8 +1922,8 @@
     <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:11" ht="125.25" customHeight="1" thickBot="1">
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="125.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="5" t="s">
         <v>38</v>
       </c>
@@ -1544,347 +1955,347 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:11">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="2:11">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="11"/>
-    </row>
-    <row r="18" spans="2:6">
-      <c r="D18" s="10" t="s">
+      <c r="F17" s="10"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
-      <c r="D19" s="10" t="s">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D19" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
-      <c r="D20" s="10" t="s">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D20" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="2:6">
-      <c r="D21" s="10" t="s">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D21" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="11"/>
-    </row>
-    <row r="22" spans="2:6">
-      <c r="D22" s="10" t="s">
+      <c r="F21" s="10"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D22" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="2:6">
-      <c r="D23" s="10" t="s">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D23" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="2:6">
-      <c r="D24" s="10" t="s">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D24" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="2:6">
-      <c r="D25" s="18" t="s">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D25" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="F25" s="19" t="s">
+      <c r="F25" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="2:6">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>42</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D37" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F37" s="11"/>
-    </row>
-    <row r="38" spans="2:6">
-      <c r="D38" s="10" t="s">
+      <c r="F37" s="10"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D38" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E38" s="12" t="s">
+      <c r="E38" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F38" s="10" t="s">
+      <c r="F38" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="2:6">
-      <c r="D39" s="10" t="s">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D39" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="E39" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F39" s="10" t="s">
+      <c r="F39" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="2:6">
-      <c r="D40" s="10" t="s">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D40" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E40" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F40" s="10" t="s">
+      <c r="F40" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="2:6">
-      <c r="D41" s="10" t="s">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D41" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="E41" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F41" s="11"/>
-    </row>
-    <row r="42" spans="2:6">
-      <c r="D42" s="10" t="s">
+      <c r="F41" s="10"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D42" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E42" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F42" s="10" t="s">
+      <c r="F42" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="2:6">
-      <c r="D43" s="10" t="s">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D43" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="E43" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F43" s="10" t="s">
+      <c r="F43" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="2:6">
-      <c r="D44" s="10" t="s">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D44" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="E44" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F44" s="10" t="s">
+      <c r="F44" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="2:6">
-      <c r="D45" s="13" t="s">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D45" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="E45" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F45" s="10" t="s">
+      <c r="F45" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="2:6">
-      <c r="D46" s="14" t="s">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D46" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E46" s="15" t="s">
+      <c r="E46" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F46" s="16"/>
-    </row>
-    <row r="51" spans="2:6">
+      <c r="F46" s="15"/>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>43</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D51" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E51" s="10" t="s">
+      <c r="E51" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F51" s="11"/>
-    </row>
-    <row r="52" spans="2:6">
-      <c r="D52" s="10" t="s">
+      <c r="F51" s="10"/>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D52" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E52" s="12" t="s">
+      <c r="E52" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F52" s="10" t="s">
+      <c r="F52" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="2:6">
-      <c r="D53" s="10" t="s">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D53" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E53" s="12" t="s">
+      <c r="E53" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F53" s="10" t="s">
+      <c r="F53" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="2:6">
-      <c r="D54" s="10" t="s">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D54" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E54" s="12" t="s">
+      <c r="E54" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="10" t="s">
+      <c r="F54" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="2:6">
-      <c r="D55" s="10" t="s">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D55" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E55" s="10" t="s">
+      <c r="E55" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F55" s="11"/>
-    </row>
-    <row r="56" spans="2:6">
-      <c r="D56" s="10" t="s">
+      <c r="F55" s="10"/>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D56" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E56" s="12" t="s">
+      <c r="E56" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F56" s="10" t="s">
+      <c r="F56" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="2:6">
-      <c r="D57" s="10" t="s">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D57" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E57" s="12" t="s">
+      <c r="E57" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F57" s="10" t="s">
+      <c r="F57" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="2:6">
-      <c r="D58" s="10" t="s">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D58" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E58" s="12" t="s">
+      <c r="E58" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F58" s="10" t="s">
+      <c r="F58" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="2:6">
-      <c r="D59" s="13" t="s">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D59" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E59" s="10" t="s">
+      <c r="E59" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F59" s="10" t="s">
+      <c r="F59" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="2:6">
-      <c r="D60" s="17" t="s">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D60" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E60" s="17" t="s">
+      <c r="E60" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F60" s="17" t="s">
+      <c r="F60" s="16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="2:6">
-      <c r="D61" s="15" t="s">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D61" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E61" s="15" t="s">
+      <c r="E61" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F61" s="15" t="s">
+      <c r="F61" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="2:2">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="67" spans="2:2">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>45</v>
       </c>
@@ -1916,272 +2327,563 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:R18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="44.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.85546875" customWidth="1"/>
-    <col min="4" max="4" width="40.140625" style="33" customWidth="1"/>
+    <col min="4" max="4" width="40.140625" style="31" customWidth="1"/>
     <col min="5" max="5" width="6.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="25.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" customWidth="1"/>
     <col min="8" max="8" width="54.85546875" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="45.75" thickBot="1">
-      <c r="A2" s="52" t="s">
+    <row r="2" spans="1:18" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="129" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="52" t="s">
+      <c r="B2" s="130"/>
+      <c r="C2" s="129" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="52" t="s">
+      <c r="D2" s="130"/>
+      <c r="E2" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="53"/>
-      <c r="G2" s="25" t="s">
+      <c r="F2" s="130"/>
+      <c r="G2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="24" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="50.25" customHeight="1">
-      <c r="A3" s="54" t="s">
+      <c r="I2" s="101" t="s">
+        <v>92</v>
+      </c>
+      <c r="J2" s="49" t="s">
+        <v>84</v>
+      </c>
+      <c r="K2" s="49" t="s">
+        <v>85</v>
+      </c>
+      <c r="L2" s="49" t="s">
+        <v>86</v>
+      </c>
+      <c r="M2" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="N2" s="50" t="s">
+        <v>85</v>
+      </c>
+      <c r="O2" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="P2" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q2" s="50" t="s">
+        <v>85</v>
+      </c>
+      <c r="R2" s="50" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="85"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="89" t="s">
+        <v>87</v>
+      </c>
+      <c r="J3" s="114" t="s">
+        <v>81</v>
+      </c>
+      <c r="K3" s="115"/>
+      <c r="L3" s="116"/>
+      <c r="M3" s="117" t="s">
+        <v>82</v>
+      </c>
+      <c r="N3" s="118"/>
+      <c r="O3" s="119"/>
+      <c r="P3" s="102"/>
+      <c r="Q3" s="103"/>
+      <c r="R3" s="104"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="86"/>
+      <c r="B4" s="87"/>
+      <c r="C4" s="87"/>
+      <c r="D4" s="87"/>
+      <c r="E4" s="87"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="J4" s="120" t="s">
+        <v>83</v>
+      </c>
+      <c r="K4" s="121"/>
+      <c r="L4" s="122"/>
+      <c r="M4" s="126">
+        <v>38539</v>
+      </c>
+      <c r="N4" s="127"/>
+      <c r="O4" s="128"/>
+      <c r="P4" s="105"/>
+      <c r="Q4" s="106"/>
+      <c r="R4" s="107"/>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="88"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="J5" s="111">
+        <v>41380</v>
+      </c>
+      <c r="K5" s="112"/>
+      <c r="L5" s="113"/>
+      <c r="M5" s="123">
+        <v>41373</v>
+      </c>
+      <c r="N5" s="124"/>
+      <c r="O5" s="125"/>
+      <c r="P5" s="108"/>
+      <c r="Q5" s="109"/>
+      <c r="R5" s="110"/>
+    </row>
+    <row r="6" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="132" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B6" s="95" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C6" s="29">
         <v>1</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D6" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="46">
+      <c r="E6" s="37">
         <v>0</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F6" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="47" t="s">
+      <c r="G6" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="48" t="s">
+      <c r="H6" s="96" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="42.75" customHeight="1">
-      <c r="A4" s="55"/>
-      <c r="B4" s="39" t="s">
+      <c r="I6" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="J6" s="90" t="s">
+        <v>90</v>
+      </c>
+      <c r="K6" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="L6" s="69" t="s">
+        <v>90</v>
+      </c>
+      <c r="M6" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="N6" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="O6" s="63" t="s">
+        <v>91</v>
+      </c>
+      <c r="P6" s="74"/>
+      <c r="Q6" s="75"/>
+      <c r="R6" s="76"/>
+    </row>
+    <row r="7" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="132"/>
+      <c r="B7" s="97" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C7" s="28">
         <v>2</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D7" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="49">
+      <c r="E7" s="40">
         <v>0</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F7" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G7" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="44" t="s">
+      <c r="H7" s="56" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="43.5" customHeight="1">
-      <c r="A5" s="55"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="30">
+      <c r="I7" s="98" t="s">
+        <v>93</v>
+      </c>
+      <c r="J7" s="91" t="s">
+        <v>90</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="L7" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="M7" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="O7" s="64" t="s">
+        <v>91</v>
+      </c>
+      <c r="P7" s="66"/>
+      <c r="Q7" s="62"/>
+      <c r="R7" s="67"/>
+    </row>
+    <row r="8" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="132"/>
+      <c r="B8" s="97"/>
+      <c r="C8" s="28">
         <v>3</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D8" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="49">
+      <c r="E8" s="40">
         <v>0</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F8" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G8" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="44" t="s">
+      <c r="H8" s="56" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="50.25" customHeight="1">
-      <c r="A6" s="55"/>
-      <c r="B6" s="39"/>
-      <c r="C6" s="30">
+      <c r="I8" s="98" t="s">
+        <v>93</v>
+      </c>
+      <c r="J8" s="92" t="s">
+        <v>90</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="L8" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="M8" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="O8" s="64" t="s">
+        <v>91</v>
+      </c>
+      <c r="P8" s="66"/>
+      <c r="Q8" s="62"/>
+      <c r="R8" s="67"/>
+    </row>
+    <row r="9" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="132"/>
+      <c r="B9" s="97"/>
+      <c r="C9" s="28">
         <v>4</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D9" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="57">
+      <c r="E9" s="42">
         <v>0</v>
       </c>
-      <c r="F6" s="58" t="s">
+      <c r="F9" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="G6" s="59" t="s">
+      <c r="G9" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="H6" s="60" t="s">
+      <c r="H9" s="57" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="50.25" customHeight="1" thickBot="1">
-      <c r="A7" s="56"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="64">
+      <c r="I9" s="98" t="s">
+        <v>93</v>
+      </c>
+      <c r="J9" s="92" t="s">
+        <v>90</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="L9" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="M9" s="54" t="s">
+        <v>90</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="O9" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="P9" s="66"/>
+      <c r="Q9" s="62"/>
+      <c r="R9" s="67"/>
+    </row>
+    <row r="10" spans="1:18" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="133"/>
+      <c r="B10" s="99"/>
+      <c r="C10" s="47">
         <v>41</v>
       </c>
-      <c r="D7" s="62" t="s">
+      <c r="D10" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="61">
+      <c r="E10" s="45">
         <v>0</v>
       </c>
-      <c r="F7" s="62" t="s">
+      <c r="F10" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="G7" s="65" t="s">
+      <c r="G10" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="H7" s="63" t="s">
+      <c r="H10" s="58" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" s="7" customFormat="1" ht="58.5" customHeight="1">
-      <c r="A8" s="54" t="s">
+      <c r="I10" s="100" t="s">
+        <v>93</v>
+      </c>
+      <c r="J10" s="93"/>
+      <c r="K10" s="78"/>
+      <c r="L10" s="79"/>
+      <c r="M10" s="77"/>
+      <c r="N10" s="78"/>
+      <c r="O10" s="80"/>
+      <c r="P10" s="77"/>
+      <c r="Q10" s="78"/>
+      <c r="R10" s="80"/>
+    </row>
+    <row r="11" spans="1:18" s="7" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="131" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B11" s="95" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C11" s="19">
         <v>1</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D11" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E11" s="19">
         <v>0</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F11" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="42" t="s">
+      <c r="H11" s="59" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="58.5" customHeight="1">
-      <c r="A9" s="55"/>
-      <c r="B9" s="39" t="s">
+      <c r="I11" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="J11" s="90" t="s">
+        <v>90</v>
+      </c>
+      <c r="K11" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="L11" s="63"/>
+      <c r="M11" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="N11" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="O11" s="63" t="s">
+        <v>90</v>
+      </c>
+      <c r="P11" s="81"/>
+      <c r="Q11" s="82"/>
+      <c r="R11" s="83"/>
+    </row>
+    <row r="12" spans="1:18" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="132"/>
+      <c r="B12" s="97" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C12" s="26">
         <v>2</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D12" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E12" s="8">
         <v>0</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F12" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G12" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="43" t="s">
+      <c r="H12" s="60" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="63" customHeight="1">
-      <c r="A10" s="55"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="36">
+      <c r="I12" s="98" t="s">
+        <v>93</v>
+      </c>
+      <c r="J12" s="91"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="64"/>
+      <c r="M12" s="54" t="s">
+        <v>90</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="O12" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="P12" s="66"/>
+      <c r="Q12" s="62"/>
+      <c r="R12" s="67"/>
+    </row>
+    <row r="13" spans="1:18" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="132"/>
+      <c r="B13" s="97"/>
+      <c r="C13" s="33">
         <v>3</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D13" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E13" s="32">
         <v>0</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F13" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="35" t="s">
+      <c r="G13" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="44" t="s">
+      <c r="H13" s="56" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="45" customHeight="1" thickBot="1">
-      <c r="A11" s="56"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="29">
+      <c r="I13" s="98" t="s">
+        <v>93</v>
+      </c>
+      <c r="J13" s="91"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="64"/>
+      <c r="M13" s="66"/>
+      <c r="N13" s="62"/>
+      <c r="O13" s="67"/>
+      <c r="P13" s="66"/>
+      <c r="Q13" s="62"/>
+      <c r="R13" s="67"/>
+    </row>
+    <row r="14" spans="1:18" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="133"/>
+      <c r="B14" s="99"/>
+      <c r="C14" s="27">
         <v>4</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D14" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E14" s="25">
         <v>0</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F14" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G14" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="45" t="s">
+      <c r="H14" s="61" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="D15" s="50" t="s">
+      <c r="I14" s="100" t="s">
+        <v>93</v>
+      </c>
+      <c r="J14" s="94"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="68"/>
+      <c r="M14" s="71"/>
+      <c r="N14" s="72"/>
+      <c r="O14" s="73"/>
+      <c r="P14" s="71"/>
+      <c r="Q14" s="72"/>
+      <c r="R14" s="73"/>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D18" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="H15" s="50" t="s">
+      <c r="H18" s="41" t="s">
         <v>74</v>
       </c>
+      <c r="I18" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="14">
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="M4:O4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="60" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Add import & roundtrip results of camunda Modeler 2.0.11
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="96">
   <si>
     <t>Documentation</t>
   </si>
@@ -546,6 +546,12 @@
   </si>
   <si>
     <t>Trisotech BPMN 2.0 Modeler for Visio 4.0</t>
+  </si>
+  <si>
+    <t>camunda modeler</t>
+  </si>
+  <si>
+    <t>2.0.11</t>
   </si>
 </sst>
 </file>
@@ -1252,7 +1258,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1441,22 +1447,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1509,14 +1503,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1590,19 +1590,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2331,10 +2331,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:R18"/>
+  <dimension ref="A2:U18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2349,26 +2349,26 @@
     <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="129" t="s">
+    <row r="2" spans="1:21" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="96" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="130"/>
-      <c r="C2" s="129" t="s">
+      <c r="B2" s="97"/>
+      <c r="C2" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="130"/>
-      <c r="E2" s="129" t="s">
+      <c r="D2" s="97"/>
+      <c r="E2" s="96" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="130"/>
+      <c r="F2" s="97"/>
       <c r="G2" s="23" t="s">
         <v>36</v>
       </c>
       <c r="H2" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="101" t="s">
+      <c r="I2" s="95" t="s">
         <v>92</v>
       </c>
       <c r="J2" s="49" t="s">
@@ -2398,90 +2398,114 @@
       <c r="R2" s="50" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="85"/>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="89" t="s">
+      <c r="S2" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="T2" s="50" t="s">
+        <v>85</v>
+      </c>
+      <c r="U2" s="50" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="79"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="83" t="s">
         <v>87</v>
       </c>
-      <c r="J3" s="114" t="s">
+      <c r="J3" s="110" t="s">
         <v>81</v>
       </c>
-      <c r="K3" s="115"/>
-      <c r="L3" s="116"/>
-      <c r="M3" s="117" t="s">
+      <c r="K3" s="111"/>
+      <c r="L3" s="112"/>
+      <c r="M3" s="113" t="s">
         <v>82</v>
       </c>
-      <c r="N3" s="118"/>
-      <c r="O3" s="119"/>
-      <c r="P3" s="102"/>
-      <c r="Q3" s="103"/>
-      <c r="R3" s="104"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="86"/>
-      <c r="B4" s="87"/>
-      <c r="C4" s="87"/>
-      <c r="D4" s="87"/>
-      <c r="E4" s="87"/>
-      <c r="F4" s="87"/>
-      <c r="G4" s="87"/>
-      <c r="H4" s="87"/>
+      <c r="N3" s="114"/>
+      <c r="O3" s="115"/>
+      <c r="P3" s="110" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q3" s="111"/>
+      <c r="R3" s="125"/>
+      <c r="S3" s="110"/>
+      <c r="T3" s="111"/>
+      <c r="U3" s="125"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="80"/>
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
       <c r="I4" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="J4" s="120" t="s">
+      <c r="J4" s="116" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="121"/>
-      <c r="L4" s="122"/>
-      <c r="M4" s="126">
+      <c r="K4" s="117"/>
+      <c r="L4" s="118"/>
+      <c r="M4" s="122">
         <v>38539</v>
       </c>
-      <c r="N4" s="127"/>
-      <c r="O4" s="128"/>
-      <c r="P4" s="105"/>
-      <c r="Q4" s="106"/>
-      <c r="R4" s="107"/>
-    </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="88"/>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="87"/>
+      <c r="N4" s="123"/>
+      <c r="O4" s="124"/>
+      <c r="P4" s="101" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q4" s="102"/>
+      <c r="R4" s="103"/>
+      <c r="S4" s="101"/>
+      <c r="T4" s="102"/>
+      <c r="U4" s="103"/>
+    </row>
+    <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="82"/>
+      <c r="B5" s="81"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
       <c r="I5" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="J5" s="111">
+      <c r="J5" s="107">
         <v>41380</v>
       </c>
-      <c r="K5" s="112"/>
-      <c r="L5" s="113"/>
-      <c r="M5" s="123">
+      <c r="K5" s="108"/>
+      <c r="L5" s="109"/>
+      <c r="M5" s="119">
         <v>41373</v>
       </c>
-      <c r="N5" s="124"/>
-      <c r="O5" s="125"/>
-      <c r="P5" s="108"/>
-      <c r="Q5" s="109"/>
-      <c r="R5" s="110"/>
-    </row>
-    <row r="6" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="132" t="s">
+      <c r="N5" s="120"/>
+      <c r="O5" s="121"/>
+      <c r="P5" s="104">
+        <v>41367</v>
+      </c>
+      <c r="Q5" s="105"/>
+      <c r="R5" s="106"/>
+      <c r="S5" s="104"/>
+      <c r="T5" s="105"/>
+      <c r="U5" s="106"/>
+    </row>
+    <row r="6" spans="1:21" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="99" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="95" t="s">
+      <c r="B6" s="89" t="s">
         <v>76</v>
       </c>
       <c r="C6" s="29">
@@ -2499,13 +2523,13 @@
       <c r="G6" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="96" t="s">
+      <c r="H6" s="90" t="s">
         <v>59</v>
       </c>
       <c r="I6" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="J6" s="90" t="s">
+      <c r="J6" s="84" t="s">
         <v>90</v>
       </c>
       <c r="K6" s="21" t="s">
@@ -2523,13 +2547,20 @@
       <c r="O6" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="P6" s="74"/>
-      <c r="Q6" s="75"/>
-      <c r="R6" s="76"/>
-    </row>
-    <row r="7" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="132"/>
-      <c r="B7" s="97" t="s">
+      <c r="P6" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="63" t="s">
+        <v>91</v>
+      </c>
+      <c r="S6" s="53"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="63"/>
+    </row>
+    <row r="7" spans="1:21" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="99"/>
+      <c r="B7" s="91" t="s">
         <v>60</v>
       </c>
       <c r="C7" s="28">
@@ -2550,10 +2581,10 @@
       <c r="H7" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="I7" s="98" t="s">
+      <c r="I7" s="92" t="s">
         <v>93</v>
       </c>
-      <c r="J7" s="91" t="s">
+      <c r="J7" s="85" t="s">
         <v>90</v>
       </c>
       <c r="K7" s="22" t="s">
@@ -2571,13 +2602,20 @@
       <c r="O7" s="64" t="s">
         <v>91</v>
       </c>
-      <c r="P7" s="66"/>
-      <c r="Q7" s="62"/>
-      <c r="R7" s="67"/>
-    </row>
-    <row r="8" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="132"/>
-      <c r="B8" s="97"/>
+      <c r="P7" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="64" t="s">
+        <v>91</v>
+      </c>
+      <c r="S7" s="54"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="64"/>
+    </row>
+    <row r="8" spans="1:21" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="99"/>
+      <c r="B8" s="91"/>
       <c r="C8" s="28">
         <v>3</v>
       </c>
@@ -2596,10 +2634,10 @@
       <c r="H8" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="I8" s="98" t="s">
+      <c r="I8" s="92" t="s">
         <v>93</v>
       </c>
-      <c r="J8" s="92" t="s">
+      <c r="J8" s="86" t="s">
         <v>90</v>
       </c>
       <c r="K8" s="8" t="s">
@@ -2617,13 +2655,20 @@
       <c r="O8" s="64" t="s">
         <v>91</v>
       </c>
-      <c r="P8" s="66"/>
-      <c r="Q8" s="62"/>
-      <c r="R8" s="67"/>
-    </row>
-    <row r="9" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="132"/>
-      <c r="B9" s="97"/>
+      <c r="P8" s="54" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="64" t="s">
+        <v>91</v>
+      </c>
+      <c r="S8" s="54"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="64"/>
+    </row>
+    <row r="9" spans="1:21" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="99"/>
+      <c r="B9" s="91"/>
       <c r="C9" s="28">
         <v>4</v>
       </c>
@@ -2642,10 +2687,10 @@
       <c r="H9" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="I9" s="98" t="s">
+      <c r="I9" s="92" t="s">
         <v>93</v>
       </c>
-      <c r="J9" s="92" t="s">
+      <c r="J9" s="86" t="s">
         <v>90</v>
       </c>
       <c r="K9" s="8" t="s">
@@ -2663,13 +2708,16 @@
       <c r="O9" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="P9" s="66"/>
-      <c r="Q9" s="62"/>
-      <c r="R9" s="67"/>
-    </row>
-    <row r="10" spans="1:18" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="133"/>
-      <c r="B10" s="99"/>
+      <c r="P9" s="54"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="64"/>
+      <c r="S9" s="54"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="64"/>
+    </row>
+    <row r="10" spans="1:21" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="100"/>
+      <c r="B10" s="93"/>
       <c r="C10" s="47">
         <v>41</v>
       </c>
@@ -2688,24 +2736,27 @@
       <c r="H10" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="I10" s="100" t="s">
+      <c r="I10" s="94" t="s">
         <v>93</v>
       </c>
-      <c r="J10" s="93"/>
-      <c r="K10" s="78"/>
-      <c r="L10" s="79"/>
-      <c r="M10" s="77"/>
-      <c r="N10" s="78"/>
-      <c r="O10" s="80"/>
-      <c r="P10" s="77"/>
-      <c r="Q10" s="78"/>
-      <c r="R10" s="80"/>
-    </row>
-    <row r="11" spans="1:18" s="7" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="131" t="s">
+      <c r="J10" s="87"/>
+      <c r="K10" s="75"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="74"/>
+      <c r="N10" s="75"/>
+      <c r="O10" s="77"/>
+      <c r="P10" s="126"/>
+      <c r="Q10" s="127"/>
+      <c r="R10" s="128"/>
+      <c r="S10" s="126"/>
+      <c r="T10" s="127"/>
+      <c r="U10" s="128"/>
+    </row>
+    <row r="11" spans="1:21" s="7" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="98" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="95" t="s">
+      <c r="B11" s="89" t="s">
         <v>75</v>
       </c>
       <c r="C11" s="19">
@@ -2729,7 +2780,7 @@
       <c r="I11" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="J11" s="90" t="s">
+      <c r="J11" s="84" t="s">
         <v>90</v>
       </c>
       <c r="K11" s="19" t="s">
@@ -2745,13 +2796,20 @@
       <c r="O11" s="63" t="s">
         <v>90</v>
       </c>
-      <c r="P11" s="81"/>
-      <c r="Q11" s="82"/>
-      <c r="R11" s="83"/>
-    </row>
-    <row r="12" spans="1:18" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="132"/>
-      <c r="B12" s="97" t="s">
+      <c r="P11" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="63" t="s">
+        <v>90</v>
+      </c>
+      <c r="S11" s="53"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="63"/>
+    </row>
+    <row r="12" spans="1:21" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="99"/>
+      <c r="B12" s="91" t="s">
         <v>61</v>
       </c>
       <c r="C12" s="26">
@@ -2772,10 +2830,10 @@
       <c r="H12" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="I12" s="98" t="s">
+      <c r="I12" s="92" t="s">
         <v>93</v>
       </c>
-      <c r="J12" s="91"/>
+      <c r="J12" s="85"/>
       <c r="K12" s="8"/>
       <c r="L12" s="64"/>
       <c r="M12" s="54" t="s">
@@ -2787,13 +2845,20 @@
       <c r="O12" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="P12" s="66"/>
-      <c r="Q12" s="62"/>
-      <c r="R12" s="67"/>
-    </row>
-    <row r="13" spans="1:18" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="132"/>
-      <c r="B13" s="97"/>
+      <c r="P12" s="54" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="S12" s="54"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="64"/>
+    </row>
+    <row r="13" spans="1:21" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="99"/>
+      <c r="B13" s="91"/>
       <c r="C13" s="33">
         <v>3</v>
       </c>
@@ -2812,22 +2877,25 @@
       <c r="H13" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="I13" s="98" t="s">
+      <c r="I13" s="92" t="s">
         <v>93</v>
       </c>
-      <c r="J13" s="91"/>
+      <c r="J13" s="85"/>
       <c r="K13" s="8"/>
       <c r="L13" s="64"/>
       <c r="M13" s="66"/>
       <c r="N13" s="62"/>
       <c r="O13" s="67"/>
-      <c r="P13" s="66"/>
-      <c r="Q13" s="62"/>
-      <c r="R13" s="67"/>
-    </row>
-    <row r="14" spans="1:18" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="133"/>
-      <c r="B14" s="99"/>
+      <c r="P13" s="54"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="64"/>
+      <c r="S13" s="54"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="64"/>
+    </row>
+    <row r="14" spans="1:21" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="100"/>
+      <c r="B14" s="93"/>
       <c r="C14" s="27">
         <v>4</v>
       </c>
@@ -2846,18 +2914,21 @@
       <c r="H14" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="I14" s="100" t="s">
+      <c r="I14" s="94" t="s">
         <v>93</v>
       </c>
-      <c r="J14" s="94"/>
+      <c r="J14" s="88"/>
       <c r="K14" s="48"/>
       <c r="L14" s="68"/>
       <c r="M14" s="71"/>
       <c r="N14" s="72"/>
       <c r="O14" s="73"/>
-      <c r="P14" s="71"/>
-      <c r="Q14" s="72"/>
-      <c r="R14" s="73"/>
+      <c r="P14" s="129"/>
+      <c r="Q14" s="48"/>
+      <c r="R14" s="68"/>
+      <c r="S14" s="129"/>
+      <c r="T14" s="48"/>
+      <c r="U14" s="68"/>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D18" s="41" t="s">
@@ -2869,12 +2940,10 @@
       <c r="I18" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A6:A10"/>
+  <mergeCells count="17">
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="S5:U5"/>
     <mergeCell ref="P3:R3"/>
     <mergeCell ref="P4:R4"/>
     <mergeCell ref="P5:R5"/>
@@ -2884,6 +2953,11 @@
     <mergeCell ref="J4:L4"/>
     <mergeCell ref="M5:O5"/>
     <mergeCell ref="M4:O4"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A6:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="60" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Add test results for IBM Process Designer 8.0.1
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="99">
   <si>
     <t>Documentation</t>
   </si>
@@ -553,12 +553,21 @@
   <si>
     <t>2.0.11</t>
   </si>
+  <si>
+    <t>IBM Process Designer</t>
+  </si>
+  <si>
+    <t>8.0.1</t>
+  </si>
+  <si>
+    <t>Unsupported</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -629,6 +638,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -650,7 +666,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="49">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -1250,15 +1266,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1503,6 +1546,93 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1518,95 +1648,48 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Excel Built-in Normal" xfId="2"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2331,10 +2414,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:U18"/>
+  <dimension ref="A2:X18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2349,19 +2432,19 @@
     <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="96" t="s">
+    <row r="2" spans="1:24" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="125" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="96" t="s">
+      <c r="B2" s="126"/>
+      <c r="C2" s="125" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="97"/>
-      <c r="E2" s="96" t="s">
+      <c r="D2" s="126"/>
+      <c r="E2" s="125" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="97"/>
+      <c r="F2" s="126"/>
       <c r="G2" s="23" t="s">
         <v>36</v>
       </c>
@@ -2407,8 +2490,17 @@
       <c r="U2" s="50" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V2" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="W2" s="50" t="s">
+        <v>85</v>
+      </c>
+      <c r="X2" s="50" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="79"/>
       <c r="B3" s="78"/>
       <c r="C3" s="78"/>
@@ -2420,26 +2512,31 @@
       <c r="I3" s="83" t="s">
         <v>87</v>
       </c>
-      <c r="J3" s="110" t="s">
+      <c r="J3" s="100" t="s">
         <v>81</v>
       </c>
-      <c r="K3" s="111"/>
+      <c r="K3" s="101"/>
       <c r="L3" s="112"/>
       <c r="M3" s="113" t="s">
         <v>82</v>
       </c>
       <c r="N3" s="114"/>
       <c r="O3" s="115"/>
-      <c r="P3" s="110" t="s">
+      <c r="P3" s="100" t="s">
         <v>94</v>
       </c>
-      <c r="Q3" s="111"/>
-      <c r="R3" s="125"/>
-      <c r="S3" s="110"/>
-      <c r="T3" s="111"/>
-      <c r="U3" s="125"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q3" s="101"/>
+      <c r="R3" s="102"/>
+      <c r="S3" s="100" t="s">
+        <v>96</v>
+      </c>
+      <c r="T3" s="101"/>
+      <c r="U3" s="102"/>
+      <c r="V3" s="100"/>
+      <c r="W3" s="101"/>
+      <c r="X3" s="102"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="80"/>
       <c r="B4" s="81"/>
       <c r="C4" s="81"/>
@@ -2461,16 +2558,21 @@
       </c>
       <c r="N4" s="123"/>
       <c r="O4" s="124"/>
-      <c r="P4" s="101" t="s">
+      <c r="P4" s="103" t="s">
         <v>95</v>
       </c>
-      <c r="Q4" s="102"/>
-      <c r="R4" s="103"/>
-      <c r="S4" s="101"/>
-      <c r="T4" s="102"/>
-      <c r="U4" s="103"/>
-    </row>
-    <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q4" s="104"/>
+      <c r="R4" s="105"/>
+      <c r="S4" s="103" t="s">
+        <v>97</v>
+      </c>
+      <c r="T4" s="104"/>
+      <c r="U4" s="105"/>
+      <c r="V4" s="103"/>
+      <c r="W4" s="104"/>
+      <c r="X4" s="105"/>
+    </row>
+    <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="82"/>
       <c r="B5" s="81"/>
       <c r="C5" s="81"/>
@@ -2482,27 +2584,32 @@
       <c r="I5" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="J5" s="107">
+      <c r="J5" s="109">
         <v>41380</v>
       </c>
-      <c r="K5" s="108"/>
-      <c r="L5" s="109"/>
+      <c r="K5" s="110"/>
+      <c r="L5" s="111"/>
       <c r="M5" s="119">
         <v>41373</v>
       </c>
       <c r="N5" s="120"/>
       <c r="O5" s="121"/>
-      <c r="P5" s="104">
+      <c r="P5" s="106">
         <v>41367</v>
       </c>
-      <c r="Q5" s="105"/>
-      <c r="R5" s="106"/>
-      <c r="S5" s="104"/>
-      <c r="T5" s="105"/>
-      <c r="U5" s="106"/>
-    </row>
-    <row r="6" spans="1:21" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="99" t="s">
+      <c r="Q5" s="107"/>
+      <c r="R5" s="108"/>
+      <c r="S5" s="119">
+        <v>41383</v>
+      </c>
+      <c r="T5" s="120"/>
+      <c r="U5" s="132"/>
+      <c r="V5" s="106"/>
+      <c r="W5" s="107"/>
+      <c r="X5" s="108"/>
+    </row>
+    <row r="6" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="128" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="89" t="s">
@@ -2551,15 +2658,24 @@
         <v>91</v>
       </c>
       <c r="Q6" s="19"/>
-      <c r="R6" s="63" t="s">
+      <c r="R6" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="S6" s="53"/>
-      <c r="T6" s="19"/>
-      <c r="U6" s="63"/>
-    </row>
-    <row r="7" spans="1:21" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="99"/>
+      <c r="S6" s="137" t="s">
+        <v>91</v>
+      </c>
+      <c r="T6" s="138" t="s">
+        <v>90</v>
+      </c>
+      <c r="U6" s="139" t="s">
+        <v>90</v>
+      </c>
+      <c r="V6" s="84"/>
+      <c r="W6" s="19"/>
+      <c r="X6" s="63"/>
+    </row>
+    <row r="7" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="128"/>
       <c r="B7" s="91" t="s">
         <v>60</v>
       </c>
@@ -2606,15 +2722,24 @@
         <v>91</v>
       </c>
       <c r="Q7" s="8"/>
-      <c r="R7" s="64" t="s">
+      <c r="R7" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="S7" s="54"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="64"/>
-    </row>
-    <row r="8" spans="1:21" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="99"/>
+      <c r="S7" s="140" t="s">
+        <v>91</v>
+      </c>
+      <c r="T7" s="135" t="s">
+        <v>90</v>
+      </c>
+      <c r="U7" s="141" t="s">
+        <v>90</v>
+      </c>
+      <c r="V7" s="85"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="64"/>
+    </row>
+    <row r="8" spans="1:24" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="128"/>
       <c r="B8" s="91"/>
       <c r="C8" s="28">
         <v>3</v>
@@ -2659,15 +2784,24 @@
         <v>90</v>
       </c>
       <c r="Q8" s="8"/>
-      <c r="R8" s="64" t="s">
+      <c r="R8" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="S8" s="54"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="64"/>
-    </row>
-    <row r="9" spans="1:21" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="99"/>
+      <c r="S8" s="142" t="s">
+        <v>98</v>
+      </c>
+      <c r="T8" s="136" t="s">
+        <v>98</v>
+      </c>
+      <c r="U8" s="141" t="s">
+        <v>90</v>
+      </c>
+      <c r="V8" s="85"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="64"/>
+    </row>
+    <row r="9" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="128"/>
       <c r="B9" s="91"/>
       <c r="C9" s="28">
         <v>4</v>
@@ -2710,13 +2844,22 @@
       </c>
       <c r="P9" s="54"/>
       <c r="Q9" s="8"/>
-      <c r="R9" s="64"/>
-      <c r="S9" s="54"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="64"/>
-    </row>
-    <row r="10" spans="1:21" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="100"/>
+      <c r="R9" s="55"/>
+      <c r="S9" s="142" t="s">
+        <v>91</v>
+      </c>
+      <c r="T9" s="135" t="s">
+        <v>90</v>
+      </c>
+      <c r="U9" s="141" t="s">
+        <v>90</v>
+      </c>
+      <c r="V9" s="85"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="64"/>
+    </row>
+    <row r="10" spans="1:24" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="129"/>
       <c r="B10" s="93"/>
       <c r="C10" s="47">
         <v>41</v>
@@ -2745,15 +2888,18 @@
       <c r="M10" s="74"/>
       <c r="N10" s="75"/>
       <c r="O10" s="77"/>
-      <c r="P10" s="126"/>
-      <c r="Q10" s="127"/>
-      <c r="R10" s="128"/>
-      <c r="S10" s="126"/>
-      <c r="T10" s="127"/>
-      <c r="U10" s="128"/>
-    </row>
-    <row r="11" spans="1:21" s="7" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="98" t="s">
+      <c r="P10" s="96"/>
+      <c r="Q10" s="97"/>
+      <c r="R10" s="130"/>
+      <c r="S10" s="99"/>
+      <c r="T10" s="48"/>
+      <c r="U10" s="68"/>
+      <c r="V10" s="131"/>
+      <c r="W10" s="97"/>
+      <c r="X10" s="98"/>
+    </row>
+    <row r="11" spans="1:24" s="7" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="127" t="s">
         <v>35</v>
       </c>
       <c r="B11" s="89" t="s">
@@ -2803,12 +2949,15 @@
       <c r="R11" s="63" t="s">
         <v>90</v>
       </c>
-      <c r="S11" s="53"/>
-      <c r="T11" s="19"/>
-      <c r="U11" s="63"/>
-    </row>
-    <row r="12" spans="1:21" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="99"/>
+      <c r="S11" s="133"/>
+      <c r="T11" s="32"/>
+      <c r="U11" s="134"/>
+      <c r="V11" s="53"/>
+      <c r="W11" s="19"/>
+      <c r="X11" s="63"/>
+    </row>
+    <row r="12" spans="1:24" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="128"/>
       <c r="B12" s="91" t="s">
         <v>61</v>
       </c>
@@ -2855,9 +3004,12 @@
       <c r="S12" s="54"/>
       <c r="T12" s="8"/>
       <c r="U12" s="64"/>
-    </row>
-    <row r="13" spans="1:21" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="99"/>
+      <c r="V12" s="54"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="64"/>
+    </row>
+    <row r="13" spans="1:24" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="128"/>
       <c r="B13" s="91"/>
       <c r="C13" s="33">
         <v>3</v>
@@ -2892,9 +3044,12 @@
       <c r="S13" s="54"/>
       <c r="T13" s="8"/>
       <c r="U13" s="64"/>
-    </row>
-    <row r="14" spans="1:21" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="100"/>
+      <c r="V13" s="54"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="64"/>
+    </row>
+    <row r="14" spans="1:24" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="129"/>
       <c r="B14" s="93"/>
       <c r="C14" s="27">
         <v>4</v>
@@ -2923,12 +3078,15 @@
       <c r="M14" s="71"/>
       <c r="N14" s="72"/>
       <c r="O14" s="73"/>
-      <c r="P14" s="129"/>
+      <c r="P14" s="99"/>
       <c r="Q14" s="48"/>
       <c r="R14" s="68"/>
-      <c r="S14" s="129"/>
+      <c r="S14" s="99"/>
       <c r="T14" s="48"/>
       <c r="U14" s="68"/>
+      <c r="V14" s="99"/>
+      <c r="W14" s="48"/>
+      <c r="X14" s="68"/>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D18" s="41" t="s">
@@ -2940,24 +3098,27 @@
       <c r="I18" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="20">
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="M4:O4"/>
     <mergeCell ref="S3:U3"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="S5:U5"/>
     <mergeCell ref="P3:R3"/>
     <mergeCell ref="P4:R4"/>
     <mergeCell ref="P5:R5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A6:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="60" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Add test result for Yaoqiang 2.1.28
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="100">
   <si>
     <t>Documentation</t>
   </si>
@@ -560,7 +560,11 @@
     <t>8.0.1</t>
   </si>
   <si>
-    <t>Unsupported</t>
+    <t>Yaoqiang BPMN Editor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2.1.28  
+</t>
   </si>
 </sst>
 </file>
@@ -1301,7 +1305,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1466,7 +1470,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1476,8 +1479,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1487,13 +1488,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1521,7 +1515,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1558,6 +1551,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1585,6 +1632,21 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1597,6 +1659,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1606,21 +1689,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1632,60 +1700,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2414,10 +2428,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:X18"/>
+  <dimension ref="A2:AA18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2432,26 +2446,26 @@
     <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:24" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="125" t="s">
+    <row r="2" spans="1:27" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="116" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="126"/>
-      <c r="C2" s="125" t="s">
+      <c r="B2" s="117"/>
+      <c r="C2" s="116" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="126"/>
-      <c r="E2" s="125" t="s">
+      <c r="D2" s="117"/>
+      <c r="E2" s="116" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="126"/>
+      <c r="F2" s="117"/>
       <c r="G2" s="23" t="s">
         <v>36</v>
       </c>
       <c r="H2" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="95" t="s">
+      <c r="I2" s="84" t="s">
         <v>92</v>
       </c>
       <c r="J2" s="49" t="s">
@@ -2499,120 +2513,144 @@
       <c r="X2" s="50" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="79"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="83" t="s">
+      <c r="Y2" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z2" s="50" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA2" s="50" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" s="69"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="73" t="s">
         <v>87</v>
       </c>
-      <c r="J3" s="100" t="s">
+      <c r="J3" s="107" t="s">
         <v>81</v>
       </c>
-      <c r="K3" s="101"/>
-      <c r="L3" s="112"/>
-      <c r="M3" s="113" t="s">
+      <c r="K3" s="108"/>
+      <c r="L3" s="124"/>
+      <c r="M3" s="132" t="s">
         <v>82</v>
       </c>
-      <c r="N3" s="114"/>
-      <c r="O3" s="115"/>
-      <c r="P3" s="100" t="s">
+      <c r="N3" s="133"/>
+      <c r="O3" s="134"/>
+      <c r="P3" s="107" t="s">
         <v>94</v>
       </c>
-      <c r="Q3" s="101"/>
-      <c r="R3" s="102"/>
-      <c r="S3" s="100" t="s">
+      <c r="Q3" s="108"/>
+      <c r="R3" s="109"/>
+      <c r="S3" s="107" t="s">
         <v>96</v>
       </c>
-      <c r="T3" s="101"/>
-      <c r="U3" s="102"/>
-      <c r="V3" s="100"/>
-      <c r="W3" s="101"/>
-      <c r="X3" s="102"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="80"/>
-      <c r="B4" s="81"/>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
+      <c r="T3" s="108"/>
+      <c r="U3" s="109"/>
+      <c r="V3" s="107" t="s">
+        <v>98</v>
+      </c>
+      <c r="W3" s="108"/>
+      <c r="X3" s="109"/>
+      <c r="Y3" s="107"/>
+      <c r="Z3" s="108"/>
+      <c r="AA3" s="109"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="70"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
       <c r="I4" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="J4" s="116" t="s">
+      <c r="J4" s="125" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="117"/>
-      <c r="L4" s="118"/>
-      <c r="M4" s="122">
+      <c r="K4" s="126"/>
+      <c r="L4" s="127"/>
+      <c r="M4" s="136">
         <v>38539</v>
       </c>
-      <c r="N4" s="123"/>
-      <c r="O4" s="124"/>
-      <c r="P4" s="103" t="s">
+      <c r="N4" s="137"/>
+      <c r="O4" s="138"/>
+      <c r="P4" s="110" t="s">
         <v>95</v>
       </c>
-      <c r="Q4" s="104"/>
-      <c r="R4" s="105"/>
-      <c r="S4" s="103" t="s">
+      <c r="Q4" s="111"/>
+      <c r="R4" s="112"/>
+      <c r="S4" s="110" t="s">
         <v>97</v>
       </c>
-      <c r="T4" s="104"/>
-      <c r="U4" s="105"/>
-      <c r="V4" s="103"/>
-      <c r="W4" s="104"/>
-      <c r="X4" s="105"/>
-    </row>
-    <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="82"/>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
+      <c r="T4" s="111"/>
+      <c r="U4" s="112"/>
+      <c r="V4" s="128" t="s">
+        <v>99</v>
+      </c>
+      <c r="W4" s="111"/>
+      <c r="X4" s="112"/>
+      <c r="Y4" s="110"/>
+      <c r="Z4" s="111"/>
+      <c r="AA4" s="112"/>
+    </row>
+    <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="72"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
       <c r="I5" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="J5" s="109">
+      <c r="J5" s="121">
         <v>41380</v>
       </c>
-      <c r="K5" s="110"/>
-      <c r="L5" s="111"/>
-      <c r="M5" s="119">
+      <c r="K5" s="122"/>
+      <c r="L5" s="123"/>
+      <c r="M5" s="129">
         <v>41373</v>
       </c>
-      <c r="N5" s="120"/>
-      <c r="O5" s="121"/>
-      <c r="P5" s="106">
+      <c r="N5" s="130"/>
+      <c r="O5" s="135"/>
+      <c r="P5" s="113">
         <v>41367</v>
       </c>
-      <c r="Q5" s="107"/>
-      <c r="R5" s="108"/>
-      <c r="S5" s="119">
+      <c r="Q5" s="114"/>
+      <c r="R5" s="115"/>
+      <c r="S5" s="129">
         <v>41383</v>
       </c>
-      <c r="T5" s="120"/>
-      <c r="U5" s="132"/>
-      <c r="V5" s="106"/>
-      <c r="W5" s="107"/>
-      <c r="X5" s="108"/>
-    </row>
-    <row r="6" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="128" t="s">
+      <c r="T5" s="130"/>
+      <c r="U5" s="131"/>
+      <c r="V5" s="129">
+        <v>41386</v>
+      </c>
+      <c r="W5" s="130"/>
+      <c r="X5" s="131"/>
+      <c r="Y5" s="113"/>
+      <c r="Z5" s="114"/>
+      <c r="AA5" s="115"/>
+    </row>
+    <row r="6" spans="1:27" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="119" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="89" t="s">
+      <c r="B6" s="78" t="s">
         <v>76</v>
       </c>
       <c r="C6" s="29">
@@ -2630,19 +2668,19 @@
       <c r="G6" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="90" t="s">
+      <c r="H6" s="79" t="s">
         <v>59</v>
       </c>
       <c r="I6" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="J6" s="84" t="s">
+      <c r="J6" s="74" t="s">
         <v>90</v>
       </c>
       <c r="K6" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="L6" s="69" t="s">
+      <c r="L6" s="66" t="s">
         <v>90</v>
       </c>
       <c r="M6" s="53" t="s">
@@ -2651,32 +2689,41 @@
       <c r="N6" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="O6" s="63" t="s">
+      <c r="O6" s="62" t="s">
         <v>91</v>
       </c>
       <c r="P6" s="53" t="s">
         <v>91</v>
       </c>
       <c r="Q6" s="19"/>
-      <c r="R6" s="69" t="s">
+      <c r="R6" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="S6" s="137" t="s">
+      <c r="S6" s="99" t="s">
         <v>91</v>
       </c>
-      <c r="T6" s="138" t="s">
-        <v>90</v>
-      </c>
-      <c r="U6" s="139" t="s">
-        <v>90</v>
-      </c>
-      <c r="V6" s="84"/>
-      <c r="W6" s="19"/>
-      <c r="X6" s="63"/>
-    </row>
-    <row r="7" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="128"/>
-      <c r="B7" s="91" t="s">
+      <c r="T6" s="100" t="s">
+        <v>90</v>
+      </c>
+      <c r="U6" s="101" t="s">
+        <v>90</v>
+      </c>
+      <c r="V6" s="96" t="s">
+        <v>91</v>
+      </c>
+      <c r="W6" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="X6" s="98" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y6" s="74"/>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="62"/>
+    </row>
+    <row r="7" spans="1:27" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="119"/>
+      <c r="B7" s="80" t="s">
         <v>60</v>
       </c>
       <c r="C7" s="28">
@@ -2697,10 +2744,10 @@
       <c r="H7" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="I7" s="92" t="s">
+      <c r="I7" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="J7" s="85" t="s">
+      <c r="J7" s="75" t="s">
         <v>90</v>
       </c>
       <c r="K7" s="22" t="s">
@@ -2715,7 +2762,7 @@
       <c r="N7" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="O7" s="64" t="s">
+      <c r="O7" s="63" t="s">
         <v>91</v>
       </c>
       <c r="P7" s="54" t="s">
@@ -2725,22 +2772,31 @@
       <c r="R7" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="S7" s="140" t="s">
+      <c r="S7" s="102" t="s">
         <v>91</v>
       </c>
-      <c r="T7" s="135" t="s">
-        <v>90</v>
-      </c>
-      <c r="U7" s="141" t="s">
-        <v>90</v>
-      </c>
-      <c r="V7" s="85"/>
-      <c r="W7" s="8"/>
-      <c r="X7" s="64"/>
-    </row>
-    <row r="8" spans="1:24" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="128"/>
-      <c r="B8" s="91"/>
+      <c r="T7" s="103" t="s">
+        <v>90</v>
+      </c>
+      <c r="U7" s="104" t="s">
+        <v>90</v>
+      </c>
+      <c r="V7" s="97" t="s">
+        <v>91</v>
+      </c>
+      <c r="W7" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="X7" s="64" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y7" s="75"/>
+      <c r="Z7" s="8"/>
+      <c r="AA7" s="63"/>
+    </row>
+    <row r="8" spans="1:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="119"/>
+      <c r="B8" s="80"/>
       <c r="C8" s="28">
         <v>3</v>
       </c>
@@ -2759,16 +2815,16 @@
       <c r="H8" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="I8" s="92" t="s">
+      <c r="I8" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="J8" s="86" t="s">
+      <c r="J8" s="76" t="s">
         <v>90</v>
       </c>
       <c r="K8" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="L8" s="70" t="s">
+      <c r="L8" s="67" t="s">
         <v>90</v>
       </c>
       <c r="M8" s="54" t="s">
@@ -2777,7 +2833,7 @@
       <c r="N8" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="O8" s="64" t="s">
+      <c r="O8" s="63" t="s">
         <v>91</v>
       </c>
       <c r="P8" s="54" t="s">
@@ -2787,22 +2843,29 @@
       <c r="R8" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="S8" s="142" t="s">
-        <v>98</v>
-      </c>
-      <c r="T8" s="136" t="s">
-        <v>98</v>
-      </c>
-      <c r="U8" s="141" t="s">
-        <v>90</v>
-      </c>
-      <c r="V8" s="85"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="64"/>
-    </row>
-    <row r="9" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="128"/>
-      <c r="B9" s="91"/>
+      <c r="S8" s="105" t="s">
+        <v>90</v>
+      </c>
+      <c r="T8" s="106" t="s">
+        <v>90</v>
+      </c>
+      <c r="U8" s="104" t="s">
+        <v>90</v>
+      </c>
+      <c r="V8" s="97" t="s">
+        <v>90</v>
+      </c>
+      <c r="W8" s="22"/>
+      <c r="X8" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y8" s="75"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="63"/>
+    </row>
+    <row r="9" spans="1:27" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="119"/>
+      <c r="B9" s="80"/>
       <c r="C9" s="28">
         <v>4</v>
       </c>
@@ -2821,16 +2884,16 @@
       <c r="H9" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="I9" s="92" t="s">
+      <c r="I9" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="J9" s="86" t="s">
+      <c r="J9" s="76" t="s">
         <v>90</v>
       </c>
       <c r="K9" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="L9" s="70" t="s">
+      <c r="L9" s="67" t="s">
         <v>90</v>
       </c>
       <c r="M9" s="54" t="s">
@@ -2839,28 +2902,35 @@
       <c r="N9" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="O9" s="65" t="s">
+      <c r="O9" s="64" t="s">
         <v>90</v>
       </c>
       <c r="P9" s="54"/>
       <c r="Q9" s="8"/>
       <c r="R9" s="55"/>
-      <c r="S9" s="142" t="s">
+      <c r="S9" s="105" t="s">
         <v>91</v>
       </c>
-      <c r="T9" s="135" t="s">
-        <v>90</v>
-      </c>
-      <c r="U9" s="141" t="s">
-        <v>90</v>
-      </c>
-      <c r="V9" s="85"/>
-      <c r="W9" s="8"/>
-      <c r="X9" s="64"/>
-    </row>
-    <row r="10" spans="1:24" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="129"/>
-      <c r="B10" s="93"/>
+      <c r="T9" s="103" t="s">
+        <v>90</v>
+      </c>
+      <c r="U9" s="104" t="s">
+        <v>90</v>
+      </c>
+      <c r="V9" s="97" t="s">
+        <v>91</v>
+      </c>
+      <c r="W9" s="22"/>
+      <c r="X9" s="64" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y9" s="75"/>
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="63"/>
+    </row>
+    <row r="10" spans="1:27" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="120"/>
+      <c r="B10" s="82"/>
       <c r="C10" s="47">
         <v>41</v>
       </c>
@@ -2879,30 +2949,33 @@
       <c r="H10" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="I10" s="94" t="s">
-        <v>93</v>
-      </c>
-      <c r="J10" s="87"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="76"/>
-      <c r="M10" s="74"/>
-      <c r="N10" s="75"/>
-      <c r="O10" s="77"/>
-      <c r="P10" s="96"/>
-      <c r="Q10" s="97"/>
-      <c r="R10" s="130"/>
-      <c r="S10" s="99"/>
+      <c r="I10" s="83" t="s">
+        <v>82</v>
+      </c>
+      <c r="J10" s="90"/>
+      <c r="K10" s="86"/>
+      <c r="L10" s="89"/>
+      <c r="M10" s="85"/>
+      <c r="N10" s="86"/>
+      <c r="O10" s="87"/>
+      <c r="P10" s="85"/>
+      <c r="Q10" s="86"/>
+      <c r="R10" s="89"/>
+      <c r="S10" s="88"/>
       <c r="T10" s="48"/>
-      <c r="U10" s="68"/>
-      <c r="V10" s="131"/>
-      <c r="W10" s="97"/>
-      <c r="X10" s="98"/>
-    </row>
-    <row r="11" spans="1:24" s="7" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="127" t="s">
+      <c r="U10" s="95"/>
+      <c r="V10" s="88"/>
+      <c r="W10" s="48"/>
+      <c r="X10" s="65"/>
+      <c r="Y10" s="90"/>
+      <c r="Z10" s="86"/>
+      <c r="AA10" s="87"/>
+    </row>
+    <row r="11" spans="1:27" s="7" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="118" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="89" t="s">
+      <c r="B11" s="78" t="s">
         <v>75</v>
       </c>
       <c r="C11" s="19">
@@ -2926,39 +2999,48 @@
       <c r="I11" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="J11" s="84" t="s">
+      <c r="J11" s="74" t="s">
         <v>90</v>
       </c>
       <c r="K11" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="L11" s="63"/>
+      <c r="L11" s="62"/>
       <c r="M11" s="53" t="s">
         <v>90</v>
       </c>
       <c r="N11" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="O11" s="63" t="s">
+      <c r="O11" s="62" t="s">
         <v>90</v>
       </c>
       <c r="P11" s="53" t="s">
         <v>90</v>
       </c>
       <c r="Q11" s="19"/>
-      <c r="R11" s="63" t="s">
-        <v>90</v>
-      </c>
-      <c r="S11" s="133"/>
+      <c r="R11" s="62" t="s">
+        <v>90</v>
+      </c>
+      <c r="S11" s="91"/>
       <c r="T11" s="32"/>
-      <c r="U11" s="134"/>
-      <c r="V11" s="53"/>
-      <c r="W11" s="19"/>
-      <c r="X11" s="63"/>
-    </row>
-    <row r="12" spans="1:24" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="128"/>
-      <c r="B12" s="91" t="s">
+      <c r="U11" s="92"/>
+      <c r="V11" s="93" t="s">
+        <v>90</v>
+      </c>
+      <c r="W11" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="X11" s="94" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y11" s="53"/>
+      <c r="Z11" s="19"/>
+      <c r="AA11" s="62"/>
+    </row>
+    <row r="12" spans="1:27" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="119"/>
+      <c r="B12" s="80" t="s">
         <v>61</v>
       </c>
       <c r="C12" s="26">
@@ -2979,38 +3061,47 @@
       <c r="H12" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="I12" s="92" t="s">
+      <c r="I12" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="J12" s="85"/>
+      <c r="J12" s="75"/>
       <c r="K12" s="8"/>
-      <c r="L12" s="64"/>
+      <c r="L12" s="63"/>
       <c r="M12" s="54" t="s">
         <v>90</v>
       </c>
       <c r="N12" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="O12" s="64" t="s">
+      <c r="O12" s="63" t="s">
         <v>90</v>
       </c>
       <c r="P12" s="54" t="s">
         <v>90</v>
       </c>
       <c r="Q12" s="8"/>
-      <c r="R12" s="64" t="s">
+      <c r="R12" s="63" t="s">
         <v>90</v>
       </c>
       <c r="S12" s="54"/>
       <c r="T12" s="8"/>
-      <c r="U12" s="64"/>
-      <c r="V12" s="54"/>
-      <c r="W12" s="8"/>
-      <c r="X12" s="64"/>
-    </row>
-    <row r="13" spans="1:24" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="128"/>
-      <c r="B13" s="91"/>
+      <c r="U12" s="63"/>
+      <c r="V12" s="97" t="s">
+        <v>90</v>
+      </c>
+      <c r="W12" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="X12" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y12" s="54"/>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="63"/>
+    </row>
+    <row r="13" spans="1:27" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="119"/>
+      <c r="B13" s="80"/>
       <c r="C13" s="33">
         <v>3</v>
       </c>
@@ -3029,28 +3120,31 @@
       <c r="H13" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="I13" s="92" t="s">
+      <c r="I13" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="J13" s="85"/>
+      <c r="J13" s="75"/>
       <c r="K13" s="8"/>
-      <c r="L13" s="64"/>
-      <c r="M13" s="66"/>
-      <c r="N13" s="62"/>
-      <c r="O13" s="67"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="54"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="63"/>
       <c r="P13" s="54"/>
       <c r="Q13" s="8"/>
-      <c r="R13" s="64"/>
+      <c r="R13" s="63"/>
       <c r="S13" s="54"/>
       <c r="T13" s="8"/>
-      <c r="U13" s="64"/>
+      <c r="U13" s="63"/>
       <c r="V13" s="54"/>
       <c r="W13" s="8"/>
-      <c r="X13" s="64"/>
-    </row>
-    <row r="14" spans="1:24" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="129"/>
-      <c r="B14" s="93"/>
+      <c r="X13" s="63"/>
+      <c r="Y13" s="54"/>
+      <c r="Z13" s="8"/>
+      <c r="AA13" s="63"/>
+    </row>
+    <row r="14" spans="1:27" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="120"/>
+      <c r="B14" s="82"/>
       <c r="C14" s="27">
         <v>4</v>
       </c>
@@ -3069,24 +3163,27 @@
       <c r="H14" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="I14" s="94" t="s">
+      <c r="I14" s="83" t="s">
         <v>93</v>
       </c>
-      <c r="J14" s="88"/>
+      <c r="J14" s="77"/>
       <c r="K14" s="48"/>
-      <c r="L14" s="68"/>
-      <c r="M14" s="71"/>
-      <c r="N14" s="72"/>
-      <c r="O14" s="73"/>
-      <c r="P14" s="99"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="88"/>
+      <c r="N14" s="48"/>
+      <c r="O14" s="65"/>
+      <c r="P14" s="88"/>
       <c r="Q14" s="48"/>
-      <c r="R14" s="68"/>
-      <c r="S14" s="99"/>
+      <c r="R14" s="65"/>
+      <c r="S14" s="88"/>
       <c r="T14" s="48"/>
-      <c r="U14" s="68"/>
-      <c r="V14" s="99"/>
+      <c r="U14" s="65"/>
+      <c r="V14" s="88"/>
       <c r="W14" s="48"/>
-      <c r="X14" s="68"/>
+      <c r="X14" s="65"/>
+      <c r="Y14" s="88"/>
+      <c r="Z14" s="48"/>
+      <c r="AA14" s="65"/>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D18" s="41" t="s">
@@ -3098,20 +3195,7 @@
       <c r="I18" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="V4:X4"/>
-    <mergeCell ref="V5:X5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="M5:O5"/>
+  <mergeCells count="23">
     <mergeCell ref="M4:O4"/>
     <mergeCell ref="S3:U3"/>
     <mergeCell ref="S4:U4"/>
@@ -3119,6 +3203,22 @@
     <mergeCell ref="P3:R3"/>
     <mergeCell ref="P4:R4"/>
     <mergeCell ref="P5:R5"/>
+    <mergeCell ref="Y3:AA3"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="Y5:AA5"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="M5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="60" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Add note regarding untested tools
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="101">
   <si>
     <t>Documentation</t>
   </si>
@@ -565,6 +565,9 @@
   <si>
     <t xml:space="preserve"> 2.1.28  
 </t>
+  </si>
+  <si>
+    <t>Note: Tools that are not listed here have either not been tested or may not support both BPMN import and export.</t>
   </si>
 </sst>
 </file>
@@ -1305,7 +1308,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1605,6 +1608,15 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1623,6 +1635,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1671,15 +1692,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1692,15 +1704,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Normal" xfId="2"/>
@@ -2428,10 +2432,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:AA18"/>
+  <dimension ref="A1:AA18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2446,19 +2450,24 @@
     <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="K1" s="139" t="s">
+        <v>100</v>
+      </c>
+    </row>
     <row r="2" spans="1:27" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="116" t="s">
+      <c r="A2" s="122" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="117"/>
-      <c r="C2" s="116" t="s">
+      <c r="B2" s="123"/>
+      <c r="C2" s="122" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="117"/>
-      <c r="E2" s="116" t="s">
+      <c r="D2" s="123"/>
+      <c r="E2" s="122" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="117"/>
+      <c r="F2" s="123"/>
       <c r="G2" s="23" t="s">
         <v>36</v>
       </c>
@@ -2535,34 +2544,34 @@
       <c r="I3" s="73" t="s">
         <v>87</v>
       </c>
-      <c r="J3" s="107" t="s">
+      <c r="J3" s="110" t="s">
         <v>81</v>
       </c>
-      <c r="K3" s="108"/>
-      <c r="L3" s="124"/>
-      <c r="M3" s="132" t="s">
+      <c r="K3" s="111"/>
+      <c r="L3" s="130"/>
+      <c r="M3" s="135" t="s">
         <v>82</v>
       </c>
-      <c r="N3" s="133"/>
-      <c r="O3" s="134"/>
-      <c r="P3" s="107" t="s">
+      <c r="N3" s="136"/>
+      <c r="O3" s="137"/>
+      <c r="P3" s="110" t="s">
         <v>94</v>
       </c>
-      <c r="Q3" s="108"/>
-      <c r="R3" s="109"/>
-      <c r="S3" s="107" t="s">
+      <c r="Q3" s="111"/>
+      <c r="R3" s="112"/>
+      <c r="S3" s="110" t="s">
         <v>96</v>
       </c>
-      <c r="T3" s="108"/>
-      <c r="U3" s="109"/>
-      <c r="V3" s="107" t="s">
+      <c r="T3" s="111"/>
+      <c r="U3" s="112"/>
+      <c r="V3" s="110" t="s">
         <v>98</v>
       </c>
-      <c r="W3" s="108"/>
-      <c r="X3" s="109"/>
-      <c r="Y3" s="107"/>
-      <c r="Z3" s="108"/>
-      <c r="AA3" s="109"/>
+      <c r="W3" s="111"/>
+      <c r="X3" s="112"/>
+      <c r="Y3" s="110"/>
+      <c r="Z3" s="111"/>
+      <c r="AA3" s="112"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="70"/>
@@ -2576,34 +2585,34 @@
       <c r="I4" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="J4" s="125" t="s">
+      <c r="J4" s="131" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="126"/>
-      <c r="L4" s="127"/>
-      <c r="M4" s="136">
+      <c r="K4" s="132"/>
+      <c r="L4" s="133"/>
+      <c r="M4" s="107">
         <v>38539</v>
       </c>
-      <c r="N4" s="137"/>
-      <c r="O4" s="138"/>
-      <c r="P4" s="110" t="s">
+      <c r="N4" s="108"/>
+      <c r="O4" s="109"/>
+      <c r="P4" s="113" t="s">
         <v>95</v>
       </c>
-      <c r="Q4" s="111"/>
-      <c r="R4" s="112"/>
-      <c r="S4" s="110" t="s">
+      <c r="Q4" s="114"/>
+      <c r="R4" s="115"/>
+      <c r="S4" s="113" t="s">
         <v>97</v>
       </c>
-      <c r="T4" s="111"/>
-      <c r="U4" s="112"/>
-      <c r="V4" s="128" t="s">
+      <c r="T4" s="114"/>
+      <c r="U4" s="115"/>
+      <c r="V4" s="134" t="s">
         <v>99</v>
       </c>
-      <c r="W4" s="111"/>
-      <c r="X4" s="112"/>
-      <c r="Y4" s="110"/>
-      <c r="Z4" s="111"/>
-      <c r="AA4" s="112"/>
+      <c r="W4" s="114"/>
+      <c r="X4" s="115"/>
+      <c r="Y4" s="113"/>
+      <c r="Z4" s="114"/>
+      <c r="AA4" s="115"/>
     </row>
     <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="72"/>
@@ -2617,37 +2626,37 @@
       <c r="I5" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="J5" s="121">
+      <c r="J5" s="127">
         <v>41380</v>
       </c>
-      <c r="K5" s="122"/>
-      <c r="L5" s="123"/>
-      <c r="M5" s="129">
+      <c r="K5" s="128"/>
+      <c r="L5" s="129"/>
+      <c r="M5" s="116">
         <v>41373</v>
       </c>
-      <c r="N5" s="130"/>
-      <c r="O5" s="135"/>
-      <c r="P5" s="113">
+      <c r="N5" s="117"/>
+      <c r="O5" s="138"/>
+      <c r="P5" s="119">
         <v>41367</v>
       </c>
-      <c r="Q5" s="114"/>
-      <c r="R5" s="115"/>
-      <c r="S5" s="129">
+      <c r="Q5" s="120"/>
+      <c r="R5" s="121"/>
+      <c r="S5" s="116">
         <v>41383</v>
       </c>
-      <c r="T5" s="130"/>
-      <c r="U5" s="131"/>
-      <c r="V5" s="129">
+      <c r="T5" s="117"/>
+      <c r="U5" s="118"/>
+      <c r="V5" s="116">
         <v>41386</v>
       </c>
-      <c r="W5" s="130"/>
-      <c r="X5" s="131"/>
-      <c r="Y5" s="113"/>
-      <c r="Z5" s="114"/>
-      <c r="AA5" s="115"/>
+      <c r="W5" s="117"/>
+      <c r="X5" s="118"/>
+      <c r="Y5" s="119"/>
+      <c r="Z5" s="120"/>
+      <c r="AA5" s="121"/>
     </row>
     <row r="6" spans="1:27" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="119" t="s">
+      <c r="A6" s="125" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="78" t="s">
@@ -2722,7 +2731,7 @@
       <c r="AA6" s="62"/>
     </row>
     <row r="7" spans="1:27" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="119"/>
+      <c r="A7" s="125"/>
       <c r="B7" s="80" t="s">
         <v>60</v>
       </c>
@@ -2795,7 +2804,7 @@
       <c r="AA7" s="63"/>
     </row>
     <row r="8" spans="1:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="119"/>
+      <c r="A8" s="125"/>
       <c r="B8" s="80"/>
       <c r="C8" s="28">
         <v>3</v>
@@ -2864,7 +2873,7 @@
       <c r="AA8" s="63"/>
     </row>
     <row r="9" spans="1:27" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="119"/>
+      <c r="A9" s="125"/>
       <c r="B9" s="80"/>
       <c r="C9" s="28">
         <v>4</v>
@@ -2929,7 +2938,7 @@
       <c r="AA9" s="63"/>
     </row>
     <row r="10" spans="1:27" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="120"/>
+      <c r="A10" s="126"/>
       <c r="B10" s="82"/>
       <c r="C10" s="47">
         <v>41</v>
@@ -2972,7 +2981,7 @@
       <c r="AA10" s="87"/>
     </row>
     <row r="11" spans="1:27" s="7" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="118" t="s">
+      <c r="A11" s="124" t="s">
         <v>35</v>
       </c>
       <c r="B11" s="78" t="s">
@@ -3039,7 +3048,7 @@
       <c r="AA11" s="62"/>
     </row>
     <row r="12" spans="1:27" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="119"/>
+      <c r="A12" s="125"/>
       <c r="B12" s="80" t="s">
         <v>61</v>
       </c>
@@ -3100,7 +3109,7 @@
       <c r="AA12" s="63"/>
     </row>
     <row r="13" spans="1:27" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="119"/>
+      <c r="A13" s="125"/>
       <c r="B13" s="80"/>
       <c r="C13" s="33">
         <v>3</v>
@@ -3143,7 +3152,7 @@
       <c r="AA13" s="63"/>
     </row>
     <row r="14" spans="1:27" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="120"/>
+      <c r="A14" s="126"/>
       <c r="B14" s="82"/>
       <c r="C14" s="27">
         <v>4</v>
@@ -3196,13 +3205,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="P5:R5"/>
     <mergeCell ref="Y3:AA3"/>
     <mergeCell ref="Y4:AA4"/>
     <mergeCell ref="Y5:AA5"/>
@@ -3219,6 +3221,13 @@
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="M3:O3"/>
     <mergeCell ref="M5:O5"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="P5:R5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="60" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Remove test case A.4.1 until coverage map available
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="98">
   <si>
     <t>Documentation</t>
   </si>
@@ -498,15 +498,6 @@
   </si>
   <si>
     <t>A.4.0</t>
-  </si>
-  <si>
-    <t>Vertical Pool/Lane</t>
-  </si>
-  <si>
-    <t>A.4.1</t>
-  </si>
-  <si>
-    <t>Same as A.4.0 but using a vertical modelling direction</t>
   </si>
   <si>
     <t>MID Innovator</t>
@@ -673,7 +664,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="51">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -1268,32 +1259,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1308,7 +1273,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1422,15 +1387,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1461,9 +1417,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1518,9 +1471,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1560,21 +1510,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1705,6 +1640,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Normal" xfId="2"/>
@@ -2432,10 +2388,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA18"/>
+  <dimension ref="A1:AA17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2451,215 +2407,215 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="K1" s="139" t="s">
-        <v>100</v>
+      <c r="K1" s="129" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="123"/>
-      <c r="C2" s="122" t="s">
+      <c r="B2" s="113"/>
+      <c r="C2" s="112" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="123"/>
-      <c r="E2" s="122" t="s">
+      <c r="D2" s="113"/>
+      <c r="E2" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="123"/>
+      <c r="F2" s="113"/>
       <c r="G2" s="23" t="s">
         <v>36</v>
       </c>
       <c r="H2" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="84" t="s">
+      <c r="I2" s="79" t="s">
+        <v>89</v>
+      </c>
+      <c r="J2" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="K2" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="L2" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="M2" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="N2" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="O2" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="P2" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q2" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="R2" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="S2" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="T2" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="U2" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="V2" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="W2" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="X2" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y2" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z2" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA2" s="47" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" s="65"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="69" t="s">
+        <v>84</v>
+      </c>
+      <c r="J3" s="100" t="s">
+        <v>78</v>
+      </c>
+      <c r="K3" s="101"/>
+      <c r="L3" s="120"/>
+      <c r="M3" s="125" t="s">
+        <v>79</v>
+      </c>
+      <c r="N3" s="126"/>
+      <c r="O3" s="127"/>
+      <c r="P3" s="100" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q3" s="101"/>
+      <c r="R3" s="102"/>
+      <c r="S3" s="100" t="s">
+        <v>93</v>
+      </c>
+      <c r="T3" s="101"/>
+      <c r="U3" s="102"/>
+      <c r="V3" s="100" t="s">
+        <v>95</v>
+      </c>
+      <c r="W3" s="101"/>
+      <c r="X3" s="102"/>
+      <c r="Y3" s="100"/>
+      <c r="Z3" s="101"/>
+      <c r="AA3" s="102"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="66"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4" s="121" t="s">
+        <v>80</v>
+      </c>
+      <c r="K4" s="122"/>
+      <c r="L4" s="123"/>
+      <c r="M4" s="97">
+        <v>38539</v>
+      </c>
+      <c r="N4" s="98"/>
+      <c r="O4" s="99"/>
+      <c r="P4" s="103" t="s">
         <v>92</v>
       </c>
-      <c r="J2" s="49" t="s">
-        <v>84</v>
-      </c>
-      <c r="K2" s="49" t="s">
+      <c r="Q4" s="104"/>
+      <c r="R4" s="105"/>
+      <c r="S4" s="103" t="s">
+        <v>94</v>
+      </c>
+      <c r="T4" s="104"/>
+      <c r="U4" s="105"/>
+      <c r="V4" s="124" t="s">
+        <v>96</v>
+      </c>
+      <c r="W4" s="104"/>
+      <c r="X4" s="105"/>
+      <c r="Y4" s="103"/>
+      <c r="Z4" s="104"/>
+      <c r="AA4" s="105"/>
+    </row>
+    <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="68"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="L2" s="49" t="s">
-        <v>86</v>
-      </c>
-      <c r="M2" s="50" t="s">
-        <v>84</v>
-      </c>
-      <c r="N2" s="50" t="s">
-        <v>85</v>
-      </c>
-      <c r="O2" s="50" t="s">
-        <v>86</v>
-      </c>
-      <c r="P2" s="50" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q2" s="50" t="s">
-        <v>85</v>
-      </c>
-      <c r="R2" s="50" t="s">
-        <v>86</v>
-      </c>
-      <c r="S2" s="50" t="s">
-        <v>84</v>
-      </c>
-      <c r="T2" s="50" t="s">
-        <v>85</v>
-      </c>
-      <c r="U2" s="50" t="s">
-        <v>86</v>
-      </c>
-      <c r="V2" s="50" t="s">
-        <v>84</v>
-      </c>
-      <c r="W2" s="50" t="s">
-        <v>85</v>
-      </c>
-      <c r="X2" s="50" t="s">
-        <v>86</v>
-      </c>
-      <c r="Y2" s="50" t="s">
-        <v>84</v>
-      </c>
-      <c r="Z2" s="50" t="s">
-        <v>85</v>
-      </c>
-      <c r="AA2" s="50" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" s="69"/>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="73" t="s">
-        <v>87</v>
-      </c>
-      <c r="J3" s="110" t="s">
-        <v>81</v>
-      </c>
-      <c r="K3" s="111"/>
-      <c r="L3" s="130"/>
-      <c r="M3" s="135" t="s">
-        <v>82</v>
-      </c>
-      <c r="N3" s="136"/>
-      <c r="O3" s="137"/>
-      <c r="P3" s="110" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q3" s="111"/>
-      <c r="R3" s="112"/>
-      <c r="S3" s="110" t="s">
-        <v>96</v>
-      </c>
-      <c r="T3" s="111"/>
-      <c r="U3" s="112"/>
-      <c r="V3" s="110" t="s">
-        <v>98</v>
-      </c>
-      <c r="W3" s="111"/>
-      <c r="X3" s="112"/>
-      <c r="Y3" s="110"/>
-      <c r="Z3" s="111"/>
-      <c r="AA3" s="112"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="70"/>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="51" t="s">
-        <v>89</v>
-      </c>
-      <c r="J4" s="131" t="s">
-        <v>83</v>
-      </c>
-      <c r="K4" s="132"/>
-      <c r="L4" s="133"/>
-      <c r="M4" s="107">
-        <v>38539</v>
-      </c>
-      <c r="N4" s="108"/>
-      <c r="O4" s="109"/>
-      <c r="P4" s="113" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q4" s="114"/>
-      <c r="R4" s="115"/>
-      <c r="S4" s="113" t="s">
-        <v>97</v>
-      </c>
-      <c r="T4" s="114"/>
-      <c r="U4" s="115"/>
-      <c r="V4" s="134" t="s">
-        <v>99</v>
-      </c>
-      <c r="W4" s="114"/>
-      <c r="X4" s="115"/>
-      <c r="Y4" s="113"/>
-      <c r="Z4" s="114"/>
-      <c r="AA4" s="115"/>
-    </row>
-    <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="72"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="51" t="s">
-        <v>88</v>
-      </c>
-      <c r="J5" s="127">
+      <c r="J5" s="117">
         <v>41380</v>
       </c>
-      <c r="K5" s="128"/>
-      <c r="L5" s="129"/>
-      <c r="M5" s="116">
+      <c r="K5" s="118"/>
+      <c r="L5" s="119"/>
+      <c r="M5" s="106">
         <v>41373</v>
       </c>
-      <c r="N5" s="117"/>
-      <c r="O5" s="138"/>
-      <c r="P5" s="119">
+      <c r="N5" s="107"/>
+      <c r="O5" s="128"/>
+      <c r="P5" s="109">
         <v>41367</v>
       </c>
-      <c r="Q5" s="120"/>
-      <c r="R5" s="121"/>
-      <c r="S5" s="116">
+      <c r="Q5" s="110"/>
+      <c r="R5" s="111"/>
+      <c r="S5" s="106">
         <v>41383</v>
       </c>
-      <c r="T5" s="117"/>
-      <c r="U5" s="118"/>
-      <c r="V5" s="116">
+      <c r="T5" s="107"/>
+      <c r="U5" s="108"/>
+      <c r="V5" s="106">
         <v>41386</v>
       </c>
-      <c r="W5" s="117"/>
-      <c r="X5" s="118"/>
-      <c r="Y5" s="119"/>
-      <c r="Z5" s="120"/>
-      <c r="AA5" s="121"/>
+      <c r="W5" s="107"/>
+      <c r="X5" s="108"/>
+      <c r="Y5" s="109"/>
+      <c r="Z5" s="110"/>
+      <c r="AA5" s="111"/>
     </row>
     <row r="6" spans="1:27" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="125" t="s">
+      <c r="A6" s="115" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="78" t="s">
+      <c r="B6" s="73" t="s">
         <v>76</v>
       </c>
       <c r="C6" s="29">
@@ -2677,62 +2633,62 @@
       <c r="G6" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="79" t="s">
+      <c r="H6" s="74" t="s">
         <v>59</v>
       </c>
       <c r="I6" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="J6" s="74" t="s">
         <v>90</v>
       </c>
+      <c r="J6" s="70" t="s">
+        <v>87</v>
+      </c>
       <c r="K6" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="L6" s="66" t="s">
-        <v>90</v>
-      </c>
-      <c r="M6" s="53" t="s">
-        <v>91</v>
+        <v>88</v>
+      </c>
+      <c r="L6" s="62" t="s">
+        <v>87</v>
+      </c>
+      <c r="M6" s="50" t="s">
+        <v>88</v>
       </c>
       <c r="N6" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="O6" s="62" t="s">
-        <v>91</v>
-      </c>
-      <c r="P6" s="53" t="s">
-        <v>91</v>
+        <v>88</v>
+      </c>
+      <c r="O6" s="58" t="s">
+        <v>88</v>
+      </c>
+      <c r="P6" s="50" t="s">
+        <v>88</v>
       </c>
       <c r="Q6" s="19"/>
-      <c r="R6" s="66" t="s">
-        <v>91</v>
-      </c>
-      <c r="S6" s="99" t="s">
-        <v>91</v>
-      </c>
-      <c r="T6" s="100" t="s">
-        <v>90</v>
-      </c>
-      <c r="U6" s="101" t="s">
-        <v>90</v>
-      </c>
-      <c r="V6" s="96" t="s">
-        <v>91</v>
+      <c r="R6" s="62" t="s">
+        <v>88</v>
+      </c>
+      <c r="S6" s="89" t="s">
+        <v>88</v>
+      </c>
+      <c r="T6" s="90" t="s">
+        <v>87</v>
+      </c>
+      <c r="U6" s="91" t="s">
+        <v>87</v>
+      </c>
+      <c r="V6" s="86" t="s">
+        <v>88</v>
       </c>
       <c r="W6" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="X6" s="98" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y6" s="74"/>
+        <v>88</v>
+      </c>
+      <c r="X6" s="88" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y6" s="70"/>
       <c r="Z6" s="19"/>
-      <c r="AA6" s="62"/>
+      <c r="AA6" s="58"/>
     </row>
     <row r="7" spans="1:27" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="125"/>
-      <c r="B7" s="80" t="s">
+      <c r="A7" s="115"/>
+      <c r="B7" s="75" t="s">
         <v>60</v>
       </c>
       <c r="C7" s="28">
@@ -2750,62 +2706,62 @@
       <c r="G7" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="56" t="s">
+      <c r="H7" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="I7" s="81" t="s">
-        <v>93</v>
-      </c>
-      <c r="J7" s="75" t="s">
+      <c r="I7" s="76" t="s">
         <v>90</v>
       </c>
+      <c r="J7" s="71" t="s">
+        <v>87</v>
+      </c>
       <c r="K7" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="L7" s="55" t="s">
-        <v>90</v>
-      </c>
-      <c r="M7" s="54" t="s">
-        <v>91</v>
+        <v>88</v>
+      </c>
+      <c r="L7" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="M7" s="51" t="s">
+        <v>88</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="O7" s="63" t="s">
-        <v>91</v>
-      </c>
-      <c r="P7" s="54" t="s">
-        <v>91</v>
+        <v>88</v>
+      </c>
+      <c r="O7" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="P7" s="51" t="s">
+        <v>88</v>
       </c>
       <c r="Q7" s="8"/>
-      <c r="R7" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="S7" s="102" t="s">
-        <v>91</v>
-      </c>
-      <c r="T7" s="103" t="s">
-        <v>90</v>
-      </c>
-      <c r="U7" s="104" t="s">
-        <v>90</v>
-      </c>
-      <c r="V7" s="97" t="s">
-        <v>91</v>
+      <c r="R7" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="S7" s="92" t="s">
+        <v>88</v>
+      </c>
+      <c r="T7" s="93" t="s">
+        <v>87</v>
+      </c>
+      <c r="U7" s="94" t="s">
+        <v>87</v>
+      </c>
+      <c r="V7" s="87" t="s">
+        <v>88</v>
       </c>
       <c r="W7" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="X7" s="64" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y7" s="75"/>
+        <v>88</v>
+      </c>
+      <c r="X7" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y7" s="71"/>
       <c r="Z7" s="8"/>
-      <c r="AA7" s="63"/>
+      <c r="AA7" s="59"/>
     </row>
     <row r="8" spans="1:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="125"/>
-      <c r="B8" s="80"/>
+      <c r="A8" s="115"/>
+      <c r="B8" s="75"/>
       <c r="C8" s="28">
         <v>3</v>
       </c>
@@ -2821,60 +2777,60 @@
       <c r="G8" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="56" t="s">
+      <c r="H8" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="I8" s="81" t="s">
-        <v>93</v>
-      </c>
-      <c r="J8" s="76" t="s">
+      <c r="I8" s="76" t="s">
         <v>90</v>
       </c>
+      <c r="J8" s="72" t="s">
+        <v>87</v>
+      </c>
       <c r="K8" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="L8" s="67" t="s">
-        <v>90</v>
-      </c>
-      <c r="M8" s="54" t="s">
-        <v>91</v>
+        <v>88</v>
+      </c>
+      <c r="L8" s="63" t="s">
+        <v>87</v>
+      </c>
+      <c r="M8" s="51" t="s">
+        <v>88</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="O8" s="63" t="s">
-        <v>91</v>
-      </c>
-      <c r="P8" s="54" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="O8" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="P8" s="51" t="s">
+        <v>87</v>
       </c>
       <c r="Q8" s="8"/>
-      <c r="R8" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="S8" s="105" t="s">
-        <v>90</v>
-      </c>
-      <c r="T8" s="106" t="s">
-        <v>90</v>
-      </c>
-      <c r="U8" s="104" t="s">
-        <v>90</v>
-      </c>
-      <c r="V8" s="97" t="s">
-        <v>90</v>
+      <c r="R8" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="S8" s="95" t="s">
+        <v>87</v>
+      </c>
+      <c r="T8" s="96" t="s">
+        <v>87</v>
+      </c>
+      <c r="U8" s="94" t="s">
+        <v>87</v>
+      </c>
+      <c r="V8" s="87" t="s">
+        <v>87</v>
       </c>
       <c r="W8" s="22"/>
-      <c r="X8" s="64" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y8" s="75"/>
+      <c r="X8" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y8" s="71"/>
       <c r="Z8" s="8"/>
-      <c r="AA8" s="63"/>
-    </row>
-    <row r="9" spans="1:27" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="125"/>
-      <c r="B9" s="80"/>
+      <c r="AA8" s="59"/>
+    </row>
+    <row r="9" spans="1:27" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="115"/>
+      <c r="B9" s="75"/>
       <c r="C9" s="28">
         <v>4</v>
       </c>
@@ -2890,318 +2846,275 @@
       <c r="G9" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="H9" s="57" t="s">
+      <c r="H9" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="I9" s="81" t="s">
-        <v>93</v>
-      </c>
-      <c r="J9" s="76" t="s">
+      <c r="I9" s="76" t="s">
         <v>90</v>
       </c>
-      <c r="K9" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="L9" s="67" t="s">
+      <c r="J9" s="130" t="s">
+        <v>87</v>
+      </c>
+      <c r="K9" s="81" t="s">
+        <v>88</v>
+      </c>
+      <c r="L9" s="131" t="s">
+        <v>87</v>
+      </c>
+      <c r="M9" s="80" t="s">
+        <v>87</v>
+      </c>
+      <c r="N9" s="81" t="s">
+        <v>87</v>
+      </c>
+      <c r="O9" s="132" t="s">
+        <v>87</v>
+      </c>
+      <c r="P9" s="80"/>
+      <c r="Q9" s="81"/>
+      <c r="R9" s="84"/>
+      <c r="S9" s="133" t="s">
+        <v>88</v>
+      </c>
+      <c r="T9" s="134" t="s">
+        <v>87</v>
+      </c>
+      <c r="U9" s="135" t="s">
+        <v>87</v>
+      </c>
+      <c r="V9" s="136" t="s">
+        <v>88</v>
+      </c>
+      <c r="W9" s="36"/>
+      <c r="X9" s="132" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y9" s="85"/>
+      <c r="Z9" s="81"/>
+      <c r="AA9" s="82"/>
+    </row>
+    <row r="10" spans="1:27" s="7" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="114" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="73" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="19">
+        <v>1</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="19">
+        <v>0</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="M9" s="54" t="s">
+      <c r="J10" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="K10" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="L10" s="58"/>
+      <c r="M10" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="N10" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="O10" s="58" t="s">
+        <v>87</v>
+      </c>
+      <c r="P10" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="58" t="s">
+        <v>87</v>
+      </c>
+      <c r="S10" s="50"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="58"/>
+      <c r="V10" s="86" t="s">
+        <v>87</v>
+      </c>
+      <c r="W10" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="X10" s="88" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y10" s="50"/>
+      <c r="Z10" s="19"/>
+      <c r="AA10" s="58"/>
+    </row>
+    <row r="11" spans="1:27" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="115"/>
+      <c r="B11" s="75" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="26">
+        <v>2</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" s="76" t="s">
         <v>90</v>
       </c>
-      <c r="N9" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="O9" s="64" t="s">
-        <v>90</v>
-      </c>
-      <c r="P9" s="54"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="55"/>
-      <c r="S9" s="105" t="s">
-        <v>91</v>
-      </c>
-      <c r="T9" s="103" t="s">
-        <v>90</v>
-      </c>
-      <c r="U9" s="104" t="s">
-        <v>90</v>
-      </c>
-      <c r="V9" s="97" t="s">
-        <v>91</v>
-      </c>
-      <c r="W9" s="22"/>
-      <c r="X9" s="64" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y9" s="75"/>
-      <c r="Z9" s="8"/>
-      <c r="AA9" s="63"/>
-    </row>
-    <row r="10" spans="1:27" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="126"/>
-      <c r="B10" s="82"/>
-      <c r="C10" s="47">
-        <v>41</v>
-      </c>
-      <c r="D10" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="45">
-        <v>0</v>
-      </c>
-      <c r="F10" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="G10" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="H10" s="58" t="s">
-        <v>80</v>
-      </c>
-      <c r="I10" s="83" t="s">
-        <v>82</v>
-      </c>
-      <c r="J10" s="90"/>
-      <c r="K10" s="86"/>
-      <c r="L10" s="89"/>
-      <c r="M10" s="85"/>
-      <c r="N10" s="86"/>
-      <c r="O10" s="87"/>
-      <c r="P10" s="85"/>
-      <c r="Q10" s="86"/>
-      <c r="R10" s="89"/>
-      <c r="S10" s="88"/>
-      <c r="T10" s="48"/>
-      <c r="U10" s="95"/>
-      <c r="V10" s="88"/>
-      <c r="W10" s="48"/>
-      <c r="X10" s="65"/>
-      <c r="Y10" s="90"/>
-      <c r="Z10" s="86"/>
-      <c r="AA10" s="87"/>
-    </row>
-    <row r="11" spans="1:27" s="7" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="124" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="78" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="19">
-        <v>1</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" s="19">
-        <v>0</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="59" t="s">
-        <v>68</v>
-      </c>
-      <c r="I11" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="J11" s="74" t="s">
-        <v>90</v>
-      </c>
-      <c r="K11" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="L11" s="62"/>
-      <c r="M11" s="53" t="s">
-        <v>90</v>
-      </c>
-      <c r="N11" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="O11" s="62" t="s">
-        <v>90</v>
-      </c>
-      <c r="P11" s="53" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="62" t="s">
-        <v>90</v>
-      </c>
-      <c r="S11" s="91"/>
-      <c r="T11" s="32"/>
-      <c r="U11" s="92"/>
-      <c r="V11" s="93" t="s">
-        <v>90</v>
-      </c>
-      <c r="W11" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="X11" s="94" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y11" s="53"/>
-      <c r="Z11" s="19"/>
-      <c r="AA11" s="62"/>
-    </row>
-    <row r="12" spans="1:27" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="125"/>
-      <c r="B12" s="80" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="26">
-        <v>2</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="8">
+      <c r="J11" s="51"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="59"/>
+      <c r="M11" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="O11" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="P11" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="S11" s="51"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="59"/>
+      <c r="V11" s="87" t="s">
+        <v>87</v>
+      </c>
+      <c r="W11" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="X11" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y11" s="51"/>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="59"/>
+    </row>
+    <row r="12" spans="1:27" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="115"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="33">
+        <v>3</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="32">
         <v>0</v>
       </c>
       <c r="F12" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="G12" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="60" t="s">
-        <v>69</v>
-      </c>
-      <c r="I12" s="81" t="s">
-        <v>93</v>
-      </c>
-      <c r="J12" s="75"/>
+      <c r="G12" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="I12" s="76" t="s">
+        <v>90</v>
+      </c>
+      <c r="J12" s="51"/>
       <c r="K12" s="8"/>
-      <c r="L12" s="63"/>
-      <c r="M12" s="54" t="s">
+      <c r="L12" s="59"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="59"/>
+      <c r="P12" s="51"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="59"/>
+      <c r="S12" s="51"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="59"/>
+      <c r="V12" s="51"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="59"/>
+      <c r="Y12" s="51"/>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="59"/>
+    </row>
+    <row r="13" spans="1:27" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="116"/>
+      <c r="B13" s="77"/>
+      <c r="C13" s="27">
+        <v>4</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="25">
+        <v>0</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="I13" s="78" t="s">
         <v>90</v>
       </c>
-      <c r="N12" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="O12" s="63" t="s">
-        <v>90</v>
-      </c>
-      <c r="P12" s="54" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="63" t="s">
-        <v>90</v>
-      </c>
-      <c r="S12" s="54"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="63"/>
-      <c r="V12" s="97" t="s">
-        <v>90</v>
-      </c>
-      <c r="W12" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="X12" s="64" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y12" s="54"/>
-      <c r="Z12" s="8"/>
-      <c r="AA12" s="63"/>
-    </row>
-    <row r="13" spans="1:27" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="125"/>
-      <c r="B13" s="80"/>
-      <c r="C13" s="33">
-        <v>3</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="32">
-        <v>0</v>
-      </c>
-      <c r="F13" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" s="52" t="s">
-        <v>57</v>
-      </c>
-      <c r="H13" s="56" t="s">
-        <v>70</v>
-      </c>
-      <c r="I13" s="81" t="s">
-        <v>93</v>
-      </c>
-      <c r="J13" s="75"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="63"/>
-      <c r="M13" s="54"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="63"/>
-      <c r="P13" s="54"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="63"/>
-      <c r="S13" s="54"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="63"/>
-      <c r="V13" s="54"/>
-      <c r="W13" s="8"/>
-      <c r="X13" s="63"/>
-      <c r="Y13" s="54"/>
-      <c r="Z13" s="8"/>
-      <c r="AA13" s="63"/>
-    </row>
-    <row r="14" spans="1:27" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="126"/>
-      <c r="B14" s="82"/>
-      <c r="C14" s="27">
-        <v>4</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" s="25">
-        <v>0</v>
-      </c>
-      <c r="F14" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="G14" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="H14" s="61" t="s">
-        <v>71</v>
-      </c>
-      <c r="I14" s="83" t="s">
-        <v>93</v>
-      </c>
-      <c r="J14" s="77"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="65"/>
-      <c r="M14" s="88"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="65"/>
-      <c r="P14" s="88"/>
-      <c r="Q14" s="48"/>
-      <c r="R14" s="65"/>
-      <c r="S14" s="88"/>
-      <c r="T14" s="48"/>
-      <c r="U14" s="65"/>
-      <c r="V14" s="88"/>
-      <c r="W14" s="48"/>
-      <c r="X14" s="65"/>
-      <c r="Y14" s="88"/>
-      <c r="Z14" s="48"/>
-      <c r="AA14" s="65"/>
-    </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D18" s="41" t="s">
+      <c r="J13" s="83"/>
+      <c r="K13" s="45"/>
+      <c r="L13" s="61"/>
+      <c r="M13" s="83"/>
+      <c r="N13" s="45"/>
+      <c r="O13" s="61"/>
+      <c r="P13" s="83"/>
+      <c r="Q13" s="45"/>
+      <c r="R13" s="61"/>
+      <c r="S13" s="83"/>
+      <c r="T13" s="45"/>
+      <c r="U13" s="61"/>
+      <c r="V13" s="83"/>
+      <c r="W13" s="45"/>
+      <c r="X13" s="61"/>
+      <c r="Y13" s="83"/>
+      <c r="Z13" s="45"/>
+      <c r="AA13" s="61"/>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="H18" s="41" t="s">
+      <c r="H17" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="I18" s="41"/>
+      <c r="I17" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="23">
@@ -3209,8 +3122,8 @@
     <mergeCell ref="Y4:AA4"/>
     <mergeCell ref="Y5:AA5"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A6:A9"/>
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="J3:L3"/>
     <mergeCell ref="J4:L4"/>

</xml_diff>

<commit_message>
Annotated Spreadsheet for Cameo Business Modeler
No direct support for the *.BPMN file format.
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="14400" windowHeight="11640" tabRatio="631" firstSheet="1" activeTab="1"/>
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="101">
   <si>
     <t>Documentation</t>
   </si>
@@ -559,6 +559,15 @@
   </si>
   <si>
     <t>Note: Tools that are not listed here have either not been tested or may not support both BPMN import and export.</t>
+  </si>
+  <si>
+    <t>Cameo Business Modeler</t>
+  </si>
+  <si>
+    <t>17.0.3 sp1</t>
+  </si>
+  <si>
+    <t>The BPMN XML format is not supported. Model Interchange is only possible in the XPDL format. However, this has not been tested by the BPMN MIWG.</t>
   </si>
 </sst>
 </file>
@@ -664,7 +673,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="49">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -1260,6 +1269,26 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1273,7 +1302,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1543,102 +1572,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1659,6 +1592,129 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2388,10 +2444,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA17"/>
+  <dimension ref="A1:AD17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+      <selection activeCell="Y6" sqref="Y6:AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2406,24 +2462,24 @@
     <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="K1" s="129" t="s">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="K1" s="97" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="112" t="s">
+    <row r="2" spans="1:30" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="114" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="113"/>
-      <c r="C2" s="112" t="s">
+      <c r="B2" s="115"/>
+      <c r="C2" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="113"/>
-      <c r="E2" s="112" t="s">
+      <c r="D2" s="115"/>
+      <c r="E2" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="113"/>
+      <c r="F2" s="115"/>
       <c r="G2" s="23" t="s">
         <v>36</v>
       </c>
@@ -2487,8 +2543,17 @@
       <c r="AA2" s="47" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB2" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC2" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD2" s="47" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="65"/>
       <c r="B3" s="64"/>
       <c r="C3" s="64"/>
@@ -2500,36 +2565,41 @@
       <c r="I3" s="69" t="s">
         <v>84</v>
       </c>
-      <c r="J3" s="100" t="s">
+      <c r="J3" s="105" t="s">
         <v>78</v>
       </c>
-      <c r="K3" s="101"/>
-      <c r="L3" s="120"/>
-      <c r="M3" s="125" t="s">
+      <c r="K3" s="106"/>
+      <c r="L3" s="122"/>
+      <c r="M3" s="130" t="s">
         <v>79</v>
       </c>
-      <c r="N3" s="126"/>
-      <c r="O3" s="127"/>
-      <c r="P3" s="100" t="s">
+      <c r="N3" s="131"/>
+      <c r="O3" s="132"/>
+      <c r="P3" s="105" t="s">
         <v>91</v>
       </c>
-      <c r="Q3" s="101"/>
-      <c r="R3" s="102"/>
-      <c r="S3" s="100" t="s">
+      <c r="Q3" s="106"/>
+      <c r="R3" s="107"/>
+      <c r="S3" s="105" t="s">
         <v>93</v>
       </c>
-      <c r="T3" s="101"/>
-      <c r="U3" s="102"/>
-      <c r="V3" s="100" t="s">
+      <c r="T3" s="106"/>
+      <c r="U3" s="107"/>
+      <c r="V3" s="105" t="s">
         <v>95</v>
       </c>
-      <c r="W3" s="101"/>
-      <c r="X3" s="102"/>
-      <c r="Y3" s="100"/>
-      <c r="Z3" s="101"/>
-      <c r="AA3" s="102"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="W3" s="106"/>
+      <c r="X3" s="107"/>
+      <c r="Y3" s="105" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z3" s="106"/>
+      <c r="AA3" s="107"/>
+      <c r="AB3" s="105"/>
+      <c r="AC3" s="106"/>
+      <c r="AD3" s="107"/>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="66"/>
       <c r="B4" s="67"/>
       <c r="C4" s="67"/>
@@ -2541,36 +2611,41 @@
       <c r="I4" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="J4" s="121" t="s">
+      <c r="J4" s="123" t="s">
         <v>80</v>
       </c>
-      <c r="K4" s="122"/>
-      <c r="L4" s="123"/>
-      <c r="M4" s="97">
+      <c r="K4" s="124"/>
+      <c r="L4" s="125"/>
+      <c r="M4" s="134">
         <v>38539</v>
       </c>
-      <c r="N4" s="98"/>
-      <c r="O4" s="99"/>
-      <c r="P4" s="103" t="s">
+      <c r="N4" s="135"/>
+      <c r="O4" s="136"/>
+      <c r="P4" s="108" t="s">
         <v>92</v>
       </c>
-      <c r="Q4" s="104"/>
-      <c r="R4" s="105"/>
-      <c r="S4" s="103" t="s">
+      <c r="Q4" s="109"/>
+      <c r="R4" s="110"/>
+      <c r="S4" s="108" t="s">
         <v>94</v>
       </c>
-      <c r="T4" s="104"/>
-      <c r="U4" s="105"/>
-      <c r="V4" s="124" t="s">
+      <c r="T4" s="109"/>
+      <c r="U4" s="110"/>
+      <c r="V4" s="126" t="s">
         <v>96</v>
       </c>
-      <c r="W4" s="104"/>
-      <c r="X4" s="105"/>
-      <c r="Y4" s="103"/>
-      <c r="Z4" s="104"/>
-      <c r="AA4" s="105"/>
-    </row>
-    <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W4" s="109"/>
+      <c r="X4" s="110"/>
+      <c r="Y4" s="108" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z4" s="109"/>
+      <c r="AA4" s="110"/>
+      <c r="AB4" s="108"/>
+      <c r="AC4" s="109"/>
+      <c r="AD4" s="110"/>
+    </row>
+    <row r="5" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="68"/>
       <c r="B5" s="67"/>
       <c r="C5" s="67"/>
@@ -2582,37 +2657,42 @@
       <c r="I5" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="J5" s="117">
+      <c r="J5" s="119">
         <v>41380</v>
       </c>
-      <c r="K5" s="118"/>
-      <c r="L5" s="119"/>
-      <c r="M5" s="106">
+      <c r="K5" s="120"/>
+      <c r="L5" s="121"/>
+      <c r="M5" s="127">
         <v>41373</v>
       </c>
-      <c r="N5" s="107"/>
-      <c r="O5" s="128"/>
-      <c r="P5" s="109">
+      <c r="N5" s="128"/>
+      <c r="O5" s="133"/>
+      <c r="P5" s="111">
         <v>41367</v>
       </c>
-      <c r="Q5" s="110"/>
-      <c r="R5" s="111"/>
-      <c r="S5" s="106">
+      <c r="Q5" s="112"/>
+      <c r="R5" s="113"/>
+      <c r="S5" s="127">
         <v>41383</v>
       </c>
-      <c r="T5" s="107"/>
-      <c r="U5" s="108"/>
-      <c r="V5" s="106">
+      <c r="T5" s="128"/>
+      <c r="U5" s="129"/>
+      <c r="V5" s="127">
         <v>41386</v>
       </c>
-      <c r="W5" s="107"/>
-      <c r="X5" s="108"/>
-      <c r="Y5" s="109"/>
-      <c r="Z5" s="110"/>
-      <c r="AA5" s="111"/>
-    </row>
-    <row r="6" spans="1:27" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="115" t="s">
+      <c r="W5" s="128"/>
+      <c r="X5" s="129"/>
+      <c r="Y5" s="111">
+        <v>41394</v>
+      </c>
+      <c r="Z5" s="112"/>
+      <c r="AA5" s="113"/>
+      <c r="AB5" s="111"/>
+      <c r="AC5" s="112"/>
+      <c r="AD5" s="113"/>
+    </row>
+    <row r="6" spans="1:30" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="117" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="73" t="s">
@@ -2682,12 +2762,17 @@
       <c r="X6" s="88" t="s">
         <v>88</v>
       </c>
-      <c r="Y6" s="70"/>
-      <c r="Z6" s="19"/>
-      <c r="AA6" s="58"/>
-    </row>
-    <row r="7" spans="1:27" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="115"/>
+      <c r="Y6" s="137" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z6" s="138"/>
+      <c r="AA6" s="139"/>
+      <c r="AB6" s="70"/>
+      <c r="AC6" s="19"/>
+      <c r="AD6" s="58"/>
+    </row>
+    <row r="7" spans="1:30" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="117"/>
       <c r="B7" s="75" t="s">
         <v>60</v>
       </c>
@@ -2755,12 +2840,15 @@
       <c r="X7" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="Y7" s="71"/>
-      <c r="Z7" s="8"/>
-      <c r="AA7" s="59"/>
-    </row>
-    <row r="8" spans="1:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="115"/>
+      <c r="Y7" s="140"/>
+      <c r="Z7" s="141"/>
+      <c r="AA7" s="142"/>
+      <c r="AB7" s="71"/>
+      <c r="AC7" s="8"/>
+      <c r="AD7" s="59"/>
+    </row>
+    <row r="8" spans="1:30" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="117"/>
       <c r="B8" s="75"/>
       <c r="C8" s="28">
         <v>3</v>
@@ -2824,12 +2912,15 @@
       <c r="X8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="Y8" s="71"/>
-      <c r="Z8" s="8"/>
-      <c r="AA8" s="59"/>
-    </row>
-    <row r="9" spans="1:27" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="115"/>
+      <c r="Y8" s="140"/>
+      <c r="Z8" s="141"/>
+      <c r="AA8" s="142"/>
+      <c r="AB8" s="71"/>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="59"/>
+    </row>
+    <row r="9" spans="1:30" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="117"/>
       <c r="B9" s="75"/>
       <c r="C9" s="28">
         <v>4</v>
@@ -2852,13 +2943,13 @@
       <c r="I9" s="76" t="s">
         <v>90</v>
       </c>
-      <c r="J9" s="130" t="s">
+      <c r="J9" s="98" t="s">
         <v>87</v>
       </c>
       <c r="K9" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="L9" s="131" t="s">
+      <c r="L9" s="99" t="s">
         <v>87</v>
       </c>
       <c r="M9" s="80" t="s">
@@ -2867,34 +2958,37 @@
       <c r="N9" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="O9" s="132" t="s">
+      <c r="O9" s="100" t="s">
         <v>87</v>
       </c>
       <c r="P9" s="80"/>
       <c r="Q9" s="81"/>
       <c r="R9" s="84"/>
-      <c r="S9" s="133" t="s">
+      <c r="S9" s="101" t="s">
         <v>88</v>
       </c>
-      <c r="T9" s="134" t="s">
-        <v>87</v>
-      </c>
-      <c r="U9" s="135" t="s">
-        <v>87</v>
-      </c>
-      <c r="V9" s="136" t="s">
+      <c r="T9" s="102" t="s">
+        <v>87</v>
+      </c>
+      <c r="U9" s="103" t="s">
+        <v>87</v>
+      </c>
+      <c r="V9" s="104" t="s">
         <v>88</v>
       </c>
       <c r="W9" s="36"/>
-      <c r="X9" s="132" t="s">
+      <c r="X9" s="100" t="s">
         <v>88</v>
       </c>
-      <c r="Y9" s="85"/>
-      <c r="Z9" s="81"/>
-      <c r="AA9" s="82"/>
-    </row>
-    <row r="10" spans="1:27" s="7" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="114" t="s">
+      <c r="Y9" s="140"/>
+      <c r="Z9" s="141"/>
+      <c r="AA9" s="142"/>
+      <c r="AB9" s="85"/>
+      <c r="AC9" s="81"/>
+      <c r="AD9" s="82"/>
+    </row>
+    <row r="10" spans="1:30" s="7" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="116" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="73" t="s">
@@ -2956,12 +3050,15 @@
       <c r="X10" s="88" t="s">
         <v>87</v>
       </c>
-      <c r="Y10" s="50"/>
-      <c r="Z10" s="19"/>
-      <c r="AA10" s="58"/>
-    </row>
-    <row r="11" spans="1:27" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="115"/>
+      <c r="Y10" s="140"/>
+      <c r="Z10" s="141"/>
+      <c r="AA10" s="142"/>
+      <c r="AB10" s="50"/>
+      <c r="AC10" s="19"/>
+      <c r="AD10" s="58"/>
+    </row>
+    <row r="11" spans="1:30" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="117"/>
       <c r="B11" s="75" t="s">
         <v>61</v>
       </c>
@@ -3017,12 +3114,15 @@
       <c r="X11" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="Y11" s="51"/>
-      <c r="Z11" s="8"/>
-      <c r="AA11" s="59"/>
-    </row>
-    <row r="12" spans="1:27" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="115"/>
+      <c r="Y11" s="140"/>
+      <c r="Z11" s="141"/>
+      <c r="AA11" s="142"/>
+      <c r="AB11" s="51"/>
+      <c r="AC11" s="8"/>
+      <c r="AD11" s="59"/>
+    </row>
+    <row r="12" spans="1:30" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="117"/>
       <c r="B12" s="75"/>
       <c r="C12" s="33">
         <v>3</v>
@@ -3060,12 +3160,15 @@
       <c r="V12" s="51"/>
       <c r="W12" s="8"/>
       <c r="X12" s="59"/>
-      <c r="Y12" s="51"/>
-      <c r="Z12" s="8"/>
-      <c r="AA12" s="59"/>
-    </row>
-    <row r="13" spans="1:27" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="116"/>
+      <c r="Y12" s="140"/>
+      <c r="Z12" s="141"/>
+      <c r="AA12" s="142"/>
+      <c r="AB12" s="51"/>
+      <c r="AC12" s="8"/>
+      <c r="AD12" s="59"/>
+    </row>
+    <row r="13" spans="1:30" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="118"/>
       <c r="B13" s="77"/>
       <c r="C13" s="27">
         <v>4</v>
@@ -3103,9 +3206,12 @@
       <c r="V13" s="83"/>
       <c r="W13" s="45"/>
       <c r="X13" s="61"/>
-      <c r="Y13" s="83"/>
-      <c r="Z13" s="45"/>
-      <c r="AA13" s="61"/>
+      <c r="Y13" s="143"/>
+      <c r="Z13" s="144"/>
+      <c r="AA13" s="145"/>
+      <c r="AB13" s="83"/>
+      <c r="AC13" s="45"/>
+      <c r="AD13" s="61"/>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D17" s="41" t="s">
@@ -3117,7 +3223,18 @@
       <c r="I17" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="27">
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="AB4:AD4"/>
+    <mergeCell ref="AB5:AD5"/>
+    <mergeCell ref="Y6:AA13"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="P5:R5"/>
     <mergeCell ref="Y3:AA3"/>
     <mergeCell ref="Y4:AA4"/>
     <mergeCell ref="Y5:AA5"/>
@@ -3134,13 +3251,6 @@
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="M3:O3"/>
     <mergeCell ref="M5:O5"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="P5:R5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="60" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Add test results for camunda modeler 2.0.12
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="14400" windowHeight="11640" tabRatio="631" firstSheet="1" activeTab="1"/>
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="98">
   <si>
     <t>Documentation</t>
   </si>
@@ -542,9 +542,6 @@
     <t>camunda modeler</t>
   </si>
   <si>
-    <t>2.0.11</t>
-  </si>
-  <si>
     <t>IBM Process Designer</t>
   </si>
   <si>
@@ -559,6 +556,9 @@
   </si>
   <si>
     <t>Note: Tools that are not listed here have either not been tested or may not support both BPMN import and export.</t>
+  </si>
+  <si>
+    <t>2.0.12</t>
   </si>
 </sst>
 </file>
@@ -1543,102 +1543,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1660,12 +1564,108 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Normal" xfId="2"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1678,9 +1678,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1718,7 +1718,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1790,7 +1790,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1970,7 +1970,7 @@
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="39.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
@@ -2391,10 +2391,10 @@
   <dimension ref="A1:AA17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="44.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.85546875" customWidth="1"/>
@@ -2407,23 +2407,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="K1" s="129" t="s">
-        <v>97</v>
+      <c r="K1" s="97" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="114" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="113"/>
-      <c r="C2" s="112" t="s">
+      <c r="B2" s="115"/>
+      <c r="C2" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="113"/>
-      <c r="E2" s="112" t="s">
+      <c r="D2" s="115"/>
+      <c r="E2" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="113"/>
+      <c r="F2" s="115"/>
       <c r="G2" s="23" t="s">
         <v>36</v>
       </c>
@@ -2500,34 +2500,34 @@
       <c r="I3" s="69" t="s">
         <v>84</v>
       </c>
-      <c r="J3" s="100" t="s">
+      <c r="J3" s="105" t="s">
         <v>78</v>
       </c>
-      <c r="K3" s="101"/>
-      <c r="L3" s="120"/>
-      <c r="M3" s="125" t="s">
+      <c r="K3" s="106"/>
+      <c r="L3" s="122"/>
+      <c r="M3" s="130" t="s">
         <v>79</v>
       </c>
-      <c r="N3" s="126"/>
-      <c r="O3" s="127"/>
-      <c r="P3" s="100" t="s">
+      <c r="N3" s="131"/>
+      <c r="O3" s="132"/>
+      <c r="P3" s="105" t="s">
         <v>91</v>
       </c>
-      <c r="Q3" s="101"/>
-      <c r="R3" s="102"/>
-      <c r="S3" s="100" t="s">
-        <v>93</v>
-      </c>
-      <c r="T3" s="101"/>
-      <c r="U3" s="102"/>
-      <c r="V3" s="100" t="s">
-        <v>95</v>
-      </c>
-      <c r="W3" s="101"/>
-      <c r="X3" s="102"/>
-      <c r="Y3" s="100"/>
-      <c r="Z3" s="101"/>
-      <c r="AA3" s="102"/>
+      <c r="Q3" s="106"/>
+      <c r="R3" s="107"/>
+      <c r="S3" s="105" t="s">
+        <v>92</v>
+      </c>
+      <c r="T3" s="106"/>
+      <c r="U3" s="107"/>
+      <c r="V3" s="105" t="s">
+        <v>94</v>
+      </c>
+      <c r="W3" s="106"/>
+      <c r="X3" s="107"/>
+      <c r="Y3" s="105"/>
+      <c r="Z3" s="106"/>
+      <c r="AA3" s="107"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="66"/>
@@ -2541,34 +2541,34 @@
       <c r="I4" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="J4" s="121" t="s">
+      <c r="J4" s="123" t="s">
         <v>80</v>
       </c>
-      <c r="K4" s="122"/>
-      <c r="L4" s="123"/>
-      <c r="M4" s="97">
+      <c r="K4" s="124"/>
+      <c r="L4" s="125"/>
+      <c r="M4" s="134">
         <v>38539</v>
       </c>
-      <c r="N4" s="98"/>
-      <c r="O4" s="99"/>
-      <c r="P4" s="103" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q4" s="104"/>
-      <c r="R4" s="105"/>
-      <c r="S4" s="103" t="s">
-        <v>94</v>
-      </c>
-      <c r="T4" s="104"/>
-      <c r="U4" s="105"/>
-      <c r="V4" s="124" t="s">
-        <v>96</v>
-      </c>
-      <c r="W4" s="104"/>
-      <c r="X4" s="105"/>
-      <c r="Y4" s="103"/>
-      <c r="Z4" s="104"/>
-      <c r="AA4" s="105"/>
+      <c r="N4" s="135"/>
+      <c r="O4" s="136"/>
+      <c r="P4" s="108" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q4" s="109"/>
+      <c r="R4" s="110"/>
+      <c r="S4" s="108" t="s">
+        <v>93</v>
+      </c>
+      <c r="T4" s="109"/>
+      <c r="U4" s="110"/>
+      <c r="V4" s="126" t="s">
+        <v>95</v>
+      </c>
+      <c r="W4" s="109"/>
+      <c r="X4" s="110"/>
+      <c r="Y4" s="108"/>
+      <c r="Z4" s="109"/>
+      <c r="AA4" s="110"/>
     </row>
     <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="68"/>
@@ -2582,37 +2582,37 @@
       <c r="I5" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="J5" s="117">
+      <c r="J5" s="119">
         <v>41380</v>
       </c>
-      <c r="K5" s="118"/>
-      <c r="L5" s="119"/>
-      <c r="M5" s="106">
+      <c r="K5" s="120"/>
+      <c r="L5" s="121"/>
+      <c r="M5" s="127">
         <v>41373</v>
       </c>
-      <c r="N5" s="107"/>
-      <c r="O5" s="128"/>
-      <c r="P5" s="109">
-        <v>41367</v>
-      </c>
-      <c r="Q5" s="110"/>
-      <c r="R5" s="111"/>
-      <c r="S5" s="106">
+      <c r="N5" s="128"/>
+      <c r="O5" s="133"/>
+      <c r="P5" s="111">
+        <v>41396</v>
+      </c>
+      <c r="Q5" s="112"/>
+      <c r="R5" s="113"/>
+      <c r="S5" s="127">
         <v>41383</v>
       </c>
-      <c r="T5" s="107"/>
-      <c r="U5" s="108"/>
-      <c r="V5" s="106">
+      <c r="T5" s="128"/>
+      <c r="U5" s="129"/>
+      <c r="V5" s="127">
         <v>41386</v>
       </c>
-      <c r="W5" s="107"/>
-      <c r="X5" s="108"/>
-      <c r="Y5" s="109"/>
-      <c r="Z5" s="110"/>
-      <c r="AA5" s="111"/>
+      <c r="W5" s="128"/>
+      <c r="X5" s="129"/>
+      <c r="Y5" s="111"/>
+      <c r="Z5" s="112"/>
+      <c r="AA5" s="113"/>
     </row>
     <row r="6" spans="1:27" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="115" t="s">
+      <c r="A6" s="117" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="73" t="s">
@@ -2687,7 +2687,7 @@
       <c r="AA6" s="58"/>
     </row>
     <row r="7" spans="1:27" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="115"/>
+      <c r="A7" s="117"/>
       <c r="B7" s="75" t="s">
         <v>60</v>
       </c>
@@ -2760,7 +2760,7 @@
       <c r="AA7" s="59"/>
     </row>
     <row r="8" spans="1:27" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="115"/>
+      <c r="A8" s="117"/>
       <c r="B8" s="75"/>
       <c r="C8" s="28">
         <v>3</v>
@@ -2829,7 +2829,7 @@
       <c r="AA8" s="59"/>
     </row>
     <row r="9" spans="1:27" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="115"/>
+      <c r="A9" s="117"/>
       <c r="B9" s="75"/>
       <c r="C9" s="28">
         <v>4</v>
@@ -2852,13 +2852,13 @@
       <c r="I9" s="76" t="s">
         <v>90</v>
       </c>
-      <c r="J9" s="130" t="s">
+      <c r="J9" s="98" t="s">
         <v>87</v>
       </c>
       <c r="K9" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="L9" s="131" t="s">
+      <c r="L9" s="99" t="s">
         <v>87</v>
       </c>
       <c r="M9" s="80" t="s">
@@ -2867,26 +2867,30 @@
       <c r="N9" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="O9" s="132" t="s">
-        <v>87</v>
-      </c>
-      <c r="P9" s="80"/>
+      <c r="O9" s="100" t="s">
+        <v>87</v>
+      </c>
+      <c r="P9" s="80" t="s">
+        <v>87</v>
+      </c>
       <c r="Q9" s="81"/>
-      <c r="R9" s="84"/>
-      <c r="S9" s="133" t="s">
+      <c r="R9" s="84" t="s">
+        <v>87</v>
+      </c>
+      <c r="S9" s="101" t="s">
         <v>88</v>
       </c>
-      <c r="T9" s="134" t="s">
-        <v>87</v>
-      </c>
-      <c r="U9" s="135" t="s">
-        <v>87</v>
-      </c>
-      <c r="V9" s="136" t="s">
+      <c r="T9" s="102" t="s">
+        <v>87</v>
+      </c>
+      <c r="U9" s="103" t="s">
+        <v>87</v>
+      </c>
+      <c r="V9" s="104" t="s">
         <v>88</v>
       </c>
       <c r="W9" s="36"/>
-      <c r="X9" s="132" t="s">
+      <c r="X9" s="100" t="s">
         <v>88</v>
       </c>
       <c r="Y9" s="85"/>
@@ -2894,7 +2898,7 @@
       <c r="AA9" s="82"/>
     </row>
     <row r="10" spans="1:27" s="7" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="114" t="s">
+      <c r="A10" s="116" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="73" t="s">
@@ -2961,7 +2965,7 @@
       <c r="AA10" s="58"/>
     </row>
     <row r="11" spans="1:27" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="115"/>
+      <c r="A11" s="117"/>
       <c r="B11" s="75" t="s">
         <v>61</v>
       </c>
@@ -3022,7 +3026,7 @@
       <c r="AA11" s="59"/>
     </row>
     <row r="12" spans="1:27" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="115"/>
+      <c r="A12" s="117"/>
       <c r="B12" s="75"/>
       <c r="C12" s="33">
         <v>3</v>
@@ -3065,7 +3069,7 @@
       <c r="AA12" s="59"/>
     </row>
     <row r="13" spans="1:27" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="116"/>
+      <c r="A13" s="118"/>
       <c r="B13" s="77"/>
       <c r="C13" s="27">
         <v>4</v>
@@ -3118,6 +3122,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="P5:R5"/>
     <mergeCell ref="Y3:AA3"/>
     <mergeCell ref="Y4:AA4"/>
     <mergeCell ref="Y5:AA5"/>
@@ -3134,13 +3145,6 @@
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="M3:O3"/>
     <mergeCell ref="M5:O5"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="P5:R5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="60" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Add note about ARIS Express and Bizagi not supporting BPMN XML
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="106">
   <si>
     <t>Documentation</t>
   </si>
@@ -571,6 +571,18 @@
   </si>
   <si>
     <t>6.7.5</t>
+  </si>
+  <si>
+    <t>Bizagi Process Modeler</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>ARIS Express</t>
+  </si>
+  <si>
+    <t>The BPMN XML format is not supported. Model Interchange is only possible in the Visio VDX format. However, this has not been tested by the BPMN MIWG.</t>
   </si>
 </sst>
 </file>
@@ -676,7 +688,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="51">
+  <borders count="57">
     <border>
       <left/>
       <right/>
@@ -1291,6 +1303,80 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -1305,7 +1391,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1482,9 +1568,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1597,24 +1680,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1651,66 +1773,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1720,6 +1782,55 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Normal" xfId="2"/>
@@ -2447,10 +2558,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AD17"/>
+  <dimension ref="A1:AJ17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB6" sqref="AB6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2465,31 +2576,31 @@
     <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="K1" s="97" t="s">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="K1" s="96" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="126" t="s">
+    <row r="2" spans="1:36" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="107" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="127"/>
-      <c r="C2" s="126" t="s">
+      <c r="B2" s="108"/>
+      <c r="C2" s="107" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="127"/>
-      <c r="E2" s="126" t="s">
+      <c r="D2" s="108"/>
+      <c r="E2" s="107" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="127"/>
+      <c r="F2" s="108"/>
       <c r="G2" s="23" t="s">
         <v>36</v>
       </c>
       <c r="H2" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="79" t="s">
+      <c r="I2" s="78" t="s">
         <v>89</v>
       </c>
       <c r="J2" s="46" t="s">
@@ -2555,8 +2666,26 @@
       <c r="AD2" s="47" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE2" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF2" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG2" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH2" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="AI2" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ2" s="47" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="65"/>
       <c r="B3" s="64"/>
       <c r="C3" s="64"/>
@@ -2565,140 +2694,170 @@
       <c r="F3" s="64"/>
       <c r="G3" s="64"/>
       <c r="H3" s="64"/>
-      <c r="I3" s="69" t="s">
+      <c r="I3" s="68" t="s">
         <v>84</v>
       </c>
-      <c r="J3" s="105" t="s">
+      <c r="J3" s="119" t="s">
         <v>78</v>
       </c>
-      <c r="K3" s="106"/>
-      <c r="L3" s="134"/>
-      <c r="M3" s="139" t="s">
+      <c r="K3" s="120"/>
+      <c r="L3" s="121"/>
+      <c r="M3" s="109" t="s">
         <v>79</v>
       </c>
-      <c r="N3" s="140"/>
-      <c r="O3" s="141"/>
-      <c r="P3" s="105" t="s">
+      <c r="N3" s="110"/>
+      <c r="O3" s="111"/>
+      <c r="P3" s="119" t="s">
         <v>91</v>
       </c>
-      <c r="Q3" s="106"/>
-      <c r="R3" s="107"/>
-      <c r="S3" s="105" t="s">
+      <c r="Q3" s="120"/>
+      <c r="R3" s="122"/>
+      <c r="S3" s="119" t="s">
         <v>92</v>
       </c>
-      <c r="T3" s="106"/>
-      <c r="U3" s="107"/>
-      <c r="V3" s="105" t="s">
+      <c r="T3" s="120"/>
+      <c r="U3" s="122"/>
+      <c r="V3" s="119" t="s">
         <v>94</v>
       </c>
-      <c r="W3" s="106"/>
-      <c r="X3" s="107"/>
-      <c r="Y3" s="105" t="s">
+      <c r="W3" s="120"/>
+      <c r="X3" s="122"/>
+      <c r="Y3" s="119" t="s">
         <v>97</v>
       </c>
-      <c r="Z3" s="106"/>
-      <c r="AA3" s="107"/>
-      <c r="AB3" s="105"/>
-      <c r="AC3" s="106"/>
-      <c r="AD3" s="107"/>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A4" s="66"/>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="48" t="s">
+      <c r="Z3" s="120"/>
+      <c r="AA3" s="122"/>
+      <c r="AB3" s="119" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC3" s="120"/>
+      <c r="AD3" s="122"/>
+      <c r="AE3" s="119" t="s">
+        <v>104</v>
+      </c>
+      <c r="AF3" s="120"/>
+      <c r="AG3" s="122"/>
+      <c r="AH3" s="138"/>
+      <c r="AI3" s="139"/>
+      <c r="AJ3" s="140"/>
+    </row>
+    <row r="4" spans="1:36" s="154" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="144"/>
+      <c r="B4" s="145"/>
+      <c r="C4" s="145"/>
+      <c r="D4" s="145"/>
+      <c r="E4" s="145"/>
+      <c r="F4" s="145"/>
+      <c r="G4" s="145"/>
+      <c r="H4" s="145"/>
+      <c r="I4" s="146" t="s">
         <v>86</v>
       </c>
-      <c r="J4" s="135" t="s">
+      <c r="J4" s="147" t="s">
         <v>80</v>
       </c>
-      <c r="K4" s="136"/>
-      <c r="L4" s="137"/>
-      <c r="M4" s="143" t="s">
+      <c r="K4" s="148"/>
+      <c r="L4" s="149"/>
+      <c r="M4" s="135" t="s">
         <v>101</v>
       </c>
-      <c r="N4" s="144"/>
-      <c r="O4" s="145"/>
-      <c r="P4" s="108" t="s">
+      <c r="N4" s="136"/>
+      <c r="O4" s="137"/>
+      <c r="P4" s="150" t="s">
         <v>100</v>
       </c>
-      <c r="Q4" s="109"/>
-      <c r="R4" s="110"/>
-      <c r="S4" s="108" t="s">
+      <c r="Q4" s="151"/>
+      <c r="R4" s="152"/>
+      <c r="S4" s="150" t="s">
         <v>93</v>
       </c>
-      <c r="T4" s="109"/>
-      <c r="U4" s="110"/>
-      <c r="V4" s="138" t="s">
+      <c r="T4" s="151"/>
+      <c r="U4" s="152"/>
+      <c r="V4" s="153" t="s">
         <v>95</v>
       </c>
-      <c r="W4" s="109"/>
-      <c r="X4" s="110"/>
-      <c r="Y4" s="108" t="s">
+      <c r="W4" s="151"/>
+      <c r="X4" s="152"/>
+      <c r="Y4" s="150" t="s">
         <v>98</v>
       </c>
-      <c r="Z4" s="109"/>
-      <c r="AA4" s="110"/>
-      <c r="AB4" s="108"/>
-      <c r="AC4" s="109"/>
-      <c r="AD4" s="110"/>
-    </row>
-    <row r="5" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="68"/>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
+      <c r="Z4" s="151"/>
+      <c r="AA4" s="152"/>
+      <c r="AB4" s="150">
+        <v>2.4</v>
+      </c>
+      <c r="AC4" s="151"/>
+      <c r="AD4" s="152"/>
+      <c r="AE4" s="150" t="s">
+        <v>103</v>
+      </c>
+      <c r="AF4" s="151"/>
+      <c r="AG4" s="152"/>
+      <c r="AH4" s="135"/>
+      <c r="AI4" s="136"/>
+      <c r="AJ4" s="137"/>
+    </row>
+    <row r="5" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="67"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
       <c r="I5" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="J5" s="131">
+      <c r="J5" s="116">
         <v>41380</v>
       </c>
-      <c r="K5" s="132"/>
-      <c r="L5" s="133"/>
-      <c r="M5" s="123">
+      <c r="K5" s="117"/>
+      <c r="L5" s="118"/>
+      <c r="M5" s="104">
         <v>41373</v>
       </c>
-      <c r="N5" s="124"/>
-      <c r="O5" s="142"/>
-      <c r="P5" s="111">
+      <c r="N5" s="105"/>
+      <c r="O5" s="112"/>
+      <c r="P5" s="123">
         <v>41396</v>
       </c>
-      <c r="Q5" s="112"/>
-      <c r="R5" s="113"/>
-      <c r="S5" s="123">
+      <c r="Q5" s="124"/>
+      <c r="R5" s="125"/>
+      <c r="S5" s="104">
         <v>41383</v>
       </c>
-      <c r="T5" s="124"/>
-      <c r="U5" s="125"/>
-      <c r="V5" s="123">
+      <c r="T5" s="105"/>
+      <c r="U5" s="106"/>
+      <c r="V5" s="104">
         <v>41386</v>
       </c>
-      <c r="W5" s="124"/>
-      <c r="X5" s="125"/>
-      <c r="Y5" s="111">
+      <c r="W5" s="105"/>
+      <c r="X5" s="106"/>
+      <c r="Y5" s="123">
         <v>41394</v>
       </c>
-      <c r="Z5" s="112"/>
-      <c r="AA5" s="113"/>
-      <c r="AB5" s="111"/>
-      <c r="AC5" s="112"/>
-      <c r="AD5" s="113"/>
-    </row>
-    <row r="6" spans="1:30" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="129" t="s">
+      <c r="Z5" s="124"/>
+      <c r="AA5" s="125"/>
+      <c r="AB5" s="123">
+        <v>41388</v>
+      </c>
+      <c r="AC5" s="124"/>
+      <c r="AD5" s="125"/>
+      <c r="AE5" s="123">
+        <v>41388</v>
+      </c>
+      <c r="AF5" s="124"/>
+      <c r="AG5" s="125"/>
+      <c r="AH5" s="141"/>
+      <c r="AI5" s="142"/>
+      <c r="AJ5" s="143"/>
+    </row>
+    <row r="6" spans="1:36" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="114" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="73" t="s">
+      <c r="B6" s="72" t="s">
         <v>76</v>
       </c>
       <c r="C6" s="29">
@@ -2716,13 +2875,13 @@
       <c r="G6" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="74" t="s">
+      <c r="H6" s="73" t="s">
         <v>59</v>
       </c>
       <c r="I6" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="J6" s="70" t="s">
+      <c r="J6" s="69" t="s">
         <v>87</v>
       </c>
       <c r="K6" s="21" t="s">
@@ -2747,36 +2906,46 @@
       <c r="R6" s="62" t="s">
         <v>88</v>
       </c>
-      <c r="S6" s="89" t="s">
+      <c r="S6" s="88" t="s">
         <v>88</v>
       </c>
-      <c r="T6" s="90" t="s">
-        <v>87</v>
-      </c>
-      <c r="U6" s="91" t="s">
-        <v>87</v>
-      </c>
-      <c r="V6" s="86" t="s">
+      <c r="T6" s="89" t="s">
+        <v>87</v>
+      </c>
+      <c r="U6" s="90" t="s">
+        <v>87</v>
+      </c>
+      <c r="V6" s="85" t="s">
         <v>88</v>
       </c>
       <c r="W6" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="X6" s="88" t="s">
+      <c r="X6" s="87" t="s">
         <v>88</v>
       </c>
-      <c r="Y6" s="114" t="s">
+      <c r="Y6" s="126" t="s">
         <v>99</v>
       </c>
-      <c r="Z6" s="115"/>
-      <c r="AA6" s="116"/>
-      <c r="AB6" s="70"/>
-      <c r="AC6" s="19"/>
-      <c r="AD6" s="58"/>
-    </row>
-    <row r="7" spans="1:30" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="129"/>
-      <c r="B7" s="75" t="s">
+      <c r="Z6" s="127"/>
+      <c r="AA6" s="128"/>
+      <c r="AB6" s="126" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC6" s="127"/>
+      <c r="AD6" s="128"/>
+      <c r="AE6" s="126" t="s">
+        <v>105</v>
+      </c>
+      <c r="AF6" s="127"/>
+      <c r="AG6" s="128"/>
+      <c r="AH6" s="69"/>
+      <c r="AI6" s="19"/>
+      <c r="AJ6" s="58"/>
+    </row>
+    <row r="7" spans="1:36" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="114"/>
+      <c r="B7" s="74" t="s">
         <v>60</v>
       </c>
       <c r="C7" s="28">
@@ -2797,10 +2966,10 @@
       <c r="H7" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="I7" s="76" t="s">
+      <c r="I7" s="75" t="s">
         <v>90</v>
       </c>
-      <c r="J7" s="71" t="s">
+      <c r="J7" s="70" t="s">
         <v>87</v>
       </c>
       <c r="K7" s="22" t="s">
@@ -2825,16 +2994,16 @@
       <c r="R7" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="S7" s="92" t="s">
+      <c r="S7" s="91" t="s">
         <v>88</v>
       </c>
-      <c r="T7" s="93" t="s">
-        <v>87</v>
-      </c>
-      <c r="U7" s="94" t="s">
-        <v>87</v>
-      </c>
-      <c r="V7" s="87" t="s">
+      <c r="T7" s="92" t="s">
+        <v>87</v>
+      </c>
+      <c r="U7" s="93" t="s">
+        <v>87</v>
+      </c>
+      <c r="V7" s="86" t="s">
         <v>88</v>
       </c>
       <c r="W7" s="22" t="s">
@@ -2843,16 +3012,22 @@
       <c r="X7" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="Y7" s="117"/>
-      <c r="Z7" s="118"/>
-      <c r="AA7" s="119"/>
-      <c r="AB7" s="71"/>
-      <c r="AC7" s="8"/>
-      <c r="AD7" s="59"/>
-    </row>
-    <row r="8" spans="1:30" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="129"/>
-      <c r="B8" s="75"/>
+      <c r="Y7" s="129"/>
+      <c r="Z7" s="130"/>
+      <c r="AA7" s="131"/>
+      <c r="AB7" s="129"/>
+      <c r="AC7" s="130"/>
+      <c r="AD7" s="131"/>
+      <c r="AE7" s="129"/>
+      <c r="AF7" s="130"/>
+      <c r="AG7" s="131"/>
+      <c r="AH7" s="70"/>
+      <c r="AI7" s="8"/>
+      <c r="AJ7" s="59"/>
+    </row>
+    <row r="8" spans="1:36" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="114"/>
+      <c r="B8" s="74"/>
       <c r="C8" s="28">
         <v>3</v>
       </c>
@@ -2871,10 +3046,10 @@
       <c r="H8" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="I8" s="76" t="s">
+      <c r="I8" s="75" t="s">
         <v>90</v>
       </c>
-      <c r="J8" s="72" t="s">
+      <c r="J8" s="71" t="s">
         <v>87</v>
       </c>
       <c r="K8" s="8" t="s">
@@ -2899,32 +3074,38 @@
       <c r="R8" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="S8" s="95" t="s">
-        <v>87</v>
-      </c>
-      <c r="T8" s="96" t="s">
-        <v>87</v>
-      </c>
-      <c r="U8" s="94" t="s">
-        <v>87</v>
-      </c>
-      <c r="V8" s="87" t="s">
+      <c r="S8" s="94" t="s">
+        <v>87</v>
+      </c>
+      <c r="T8" s="95" t="s">
+        <v>87</v>
+      </c>
+      <c r="U8" s="93" t="s">
+        <v>87</v>
+      </c>
+      <c r="V8" s="86" t="s">
         <v>87</v>
       </c>
       <c r="W8" s="22"/>
       <c r="X8" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="Y8" s="117"/>
-      <c r="Z8" s="118"/>
-      <c r="AA8" s="119"/>
-      <c r="AB8" s="71"/>
-      <c r="AC8" s="8"/>
-      <c r="AD8" s="59"/>
-    </row>
-    <row r="9" spans="1:30" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="129"/>
-      <c r="B9" s="75"/>
+      <c r="Y8" s="129"/>
+      <c r="Z8" s="130"/>
+      <c r="AA8" s="131"/>
+      <c r="AB8" s="129"/>
+      <c r="AC8" s="130"/>
+      <c r="AD8" s="131"/>
+      <c r="AE8" s="129"/>
+      <c r="AF8" s="130"/>
+      <c r="AG8" s="131"/>
+      <c r="AH8" s="70"/>
+      <c r="AI8" s="8"/>
+      <c r="AJ8" s="59"/>
+    </row>
+    <row r="9" spans="1:36" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="114"/>
+      <c r="B9" s="74"/>
       <c r="C9" s="28">
         <v>4</v>
       </c>
@@ -2943,62 +3124,68 @@
       <c r="H9" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="I9" s="76" t="s">
+      <c r="I9" s="75" t="s">
         <v>90</v>
       </c>
-      <c r="J9" s="98" t="s">
-        <v>87</v>
-      </c>
-      <c r="K9" s="81" t="s">
+      <c r="J9" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="K9" s="80" t="s">
         <v>88</v>
       </c>
-      <c r="L9" s="99" t="s">
-        <v>87</v>
-      </c>
-      <c r="M9" s="80" t="s">
-        <v>87</v>
-      </c>
-      <c r="N9" s="81" t="s">
-        <v>87</v>
-      </c>
-      <c r="O9" s="100" t="s">
-        <v>87</v>
-      </c>
-      <c r="P9" s="80" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q9" s="81"/>
-      <c r="R9" s="84" t="s">
-        <v>87</v>
-      </c>
-      <c r="S9" s="101" t="s">
+      <c r="L9" s="98" t="s">
+        <v>87</v>
+      </c>
+      <c r="M9" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="N9" s="80" t="s">
+        <v>87</v>
+      </c>
+      <c r="O9" s="99" t="s">
+        <v>87</v>
+      </c>
+      <c r="P9" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q9" s="80"/>
+      <c r="R9" s="83" t="s">
+        <v>87</v>
+      </c>
+      <c r="S9" s="100" t="s">
         <v>88</v>
       </c>
-      <c r="T9" s="102" t="s">
-        <v>87</v>
-      </c>
-      <c r="U9" s="103" t="s">
-        <v>87</v>
-      </c>
-      <c r="V9" s="104" t="s">
+      <c r="T9" s="101" t="s">
+        <v>87</v>
+      </c>
+      <c r="U9" s="102" t="s">
+        <v>87</v>
+      </c>
+      <c r="V9" s="103" t="s">
         <v>88</v>
       </c>
       <c r="W9" s="36"/>
-      <c r="X9" s="100" t="s">
+      <c r="X9" s="99" t="s">
         <v>88</v>
       </c>
-      <c r="Y9" s="117"/>
-      <c r="Z9" s="118"/>
-      <c r="AA9" s="119"/>
-      <c r="AB9" s="85"/>
-      <c r="AC9" s="81"/>
-      <c r="AD9" s="82"/>
-    </row>
-    <row r="10" spans="1:30" s="7" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="128" t="s">
+      <c r="Y9" s="129"/>
+      <c r="Z9" s="130"/>
+      <c r="AA9" s="131"/>
+      <c r="AB9" s="129"/>
+      <c r="AC9" s="130"/>
+      <c r="AD9" s="131"/>
+      <c r="AE9" s="129"/>
+      <c r="AF9" s="130"/>
+      <c r="AG9" s="131"/>
+      <c r="AH9" s="84"/>
+      <c r="AI9" s="80"/>
+      <c r="AJ9" s="81"/>
+    </row>
+    <row r="10" spans="1:36" s="7" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="113" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="72" t="s">
         <v>75</v>
       </c>
       <c r="C10" s="19">
@@ -3048,25 +3235,31 @@
       <c r="S10" s="50"/>
       <c r="T10" s="19"/>
       <c r="U10" s="58"/>
-      <c r="V10" s="86" t="s">
+      <c r="V10" s="85" t="s">
         <v>87</v>
       </c>
       <c r="W10" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="X10" s="88" t="s">
-        <v>87</v>
-      </c>
-      <c r="Y10" s="117"/>
-      <c r="Z10" s="118"/>
-      <c r="AA10" s="119"/>
-      <c r="AB10" s="50"/>
-      <c r="AC10" s="19"/>
-      <c r="AD10" s="58"/>
-    </row>
-    <row r="11" spans="1:30" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="129"/>
-      <c r="B11" s="75" t="s">
+      <c r="X10" s="87" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y10" s="129"/>
+      <c r="Z10" s="130"/>
+      <c r="AA10" s="131"/>
+      <c r="AB10" s="129"/>
+      <c r="AC10" s="130"/>
+      <c r="AD10" s="131"/>
+      <c r="AE10" s="129"/>
+      <c r="AF10" s="130"/>
+      <c r="AG10" s="131"/>
+      <c r="AH10" s="50"/>
+      <c r="AI10" s="19"/>
+      <c r="AJ10" s="58"/>
+    </row>
+    <row r="11" spans="1:36" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="114"/>
+      <c r="B11" s="74" t="s">
         <v>61</v>
       </c>
       <c r="C11" s="26">
@@ -3087,7 +3280,7 @@
       <c r="H11" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="I11" s="76" t="s">
+      <c r="I11" s="75" t="s">
         <v>90</v>
       </c>
       <c r="J11" s="51"/>
@@ -3112,7 +3305,7 @@
       <c r="S11" s="51"/>
       <c r="T11" s="8"/>
       <c r="U11" s="59"/>
-      <c r="V11" s="87" t="s">
+      <c r="V11" s="86" t="s">
         <v>87</v>
       </c>
       <c r="W11" s="22" t="s">
@@ -3121,16 +3314,22 @@
       <c r="X11" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="Y11" s="117"/>
-      <c r="Z11" s="118"/>
-      <c r="AA11" s="119"/>
-      <c r="AB11" s="51"/>
-      <c r="AC11" s="8"/>
-      <c r="AD11" s="59"/>
-    </row>
-    <row r="12" spans="1:30" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="129"/>
-      <c r="B12" s="75"/>
+      <c r="Y11" s="129"/>
+      <c r="Z11" s="130"/>
+      <c r="AA11" s="131"/>
+      <c r="AB11" s="129"/>
+      <c r="AC11" s="130"/>
+      <c r="AD11" s="131"/>
+      <c r="AE11" s="129"/>
+      <c r="AF11" s="130"/>
+      <c r="AG11" s="131"/>
+      <c r="AH11" s="51"/>
+      <c r="AI11" s="8"/>
+      <c r="AJ11" s="59"/>
+    </row>
+    <row r="12" spans="1:36" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="114"/>
+      <c r="B12" s="74"/>
       <c r="C12" s="33">
         <v>3</v>
       </c>
@@ -3149,7 +3348,7 @@
       <c r="H12" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="I12" s="76" t="s">
+      <c r="I12" s="75" t="s">
         <v>90</v>
       </c>
       <c r="J12" s="51"/>
@@ -3167,16 +3366,22 @@
       <c r="V12" s="51"/>
       <c r="W12" s="8"/>
       <c r="X12" s="59"/>
-      <c r="Y12" s="117"/>
-      <c r="Z12" s="118"/>
-      <c r="AA12" s="119"/>
-      <c r="AB12" s="51"/>
-      <c r="AC12" s="8"/>
-      <c r="AD12" s="59"/>
-    </row>
-    <row r="13" spans="1:30" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="130"/>
-      <c r="B13" s="77"/>
+      <c r="Y12" s="129"/>
+      <c r="Z12" s="130"/>
+      <c r="AA12" s="131"/>
+      <c r="AB12" s="129"/>
+      <c r="AC12" s="130"/>
+      <c r="AD12" s="131"/>
+      <c r="AE12" s="129"/>
+      <c r="AF12" s="130"/>
+      <c r="AG12" s="131"/>
+      <c r="AH12" s="51"/>
+      <c r="AI12" s="8"/>
+      <c r="AJ12" s="59"/>
+    </row>
+    <row r="13" spans="1:36" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="115"/>
+      <c r="B13" s="76"/>
       <c r="C13" s="27">
         <v>4</v>
       </c>
@@ -3195,30 +3400,36 @@
       <c r="H13" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="I13" s="78" t="s">
+      <c r="I13" s="77" t="s">
         <v>90</v>
       </c>
-      <c r="J13" s="83"/>
+      <c r="J13" s="82"/>
       <c r="K13" s="45"/>
       <c r="L13" s="61"/>
-      <c r="M13" s="83"/>
+      <c r="M13" s="82"/>
       <c r="N13" s="45"/>
       <c r="O13" s="61"/>
-      <c r="P13" s="83"/>
+      <c r="P13" s="82"/>
       <c r="Q13" s="45"/>
       <c r="R13" s="61"/>
-      <c r="S13" s="83"/>
+      <c r="S13" s="82"/>
       <c r="T13" s="45"/>
       <c r="U13" s="61"/>
-      <c r="V13" s="83"/>
+      <c r="V13" s="82"/>
       <c r="W13" s="45"/>
       <c r="X13" s="61"/>
-      <c r="Y13" s="120"/>
-      <c r="Z13" s="121"/>
-      <c r="AA13" s="122"/>
-      <c r="AB13" s="83"/>
-      <c r="AC13" s="45"/>
-      <c r="AD13" s="61"/>
+      <c r="Y13" s="132"/>
+      <c r="Z13" s="133"/>
+      <c r="AA13" s="134"/>
+      <c r="AB13" s="132"/>
+      <c r="AC13" s="133"/>
+      <c r="AD13" s="134"/>
+      <c r="AE13" s="132"/>
+      <c r="AF13" s="133"/>
+      <c r="AG13" s="134"/>
+      <c r="AH13" s="82"/>
+      <c r="AI13" s="45"/>
+      <c r="AJ13" s="61"/>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D17" s="41" t="s">
@@ -3230,18 +3441,15 @@
       <c r="I17" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="V5:X5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="J4:L4"/>
+  <mergeCells count="35">
+    <mergeCell ref="AH3:AJ3"/>
+    <mergeCell ref="AH4:AJ4"/>
+    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AB6:AD13"/>
+    <mergeCell ref="AE6:AG13"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="AE4:AG4"/>
+    <mergeCell ref="AE3:AG3"/>
     <mergeCell ref="AB3:AD3"/>
     <mergeCell ref="AB4:AD4"/>
     <mergeCell ref="AB5:AD5"/>
@@ -3258,8 +3466,22 @@
     <mergeCell ref="Y5:AA5"/>
     <mergeCell ref="V3:X3"/>
     <mergeCell ref="V4:X4"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="M5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="60" orientation="landscape" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="AE4" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated version and date of Yaoqiang tested
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="105">
   <si>
     <t>Call Activities</t>
   </si>
@@ -379,8 +379,7 @@
     <t>8.0.1</t>
   </si>
   <si>
-    <t> 2.1.28  
-</t>
+    <t>2.1.33</t>
   </si>
   <si>
     <t>17.0.3 sp1</t>
@@ -396,8 +395,7 @@
   </si>
   <si>
     <t>Layout 
-Fixed Diagrams with Variations Attributes
-</t>
+Fixed Diagrams with Variations Attributes</t>
   </si>
   <si>
     <t>Connected elements depicted linearly on the canvas</t>
@@ -461,7 +459,7 @@
   </si>
   <si>
     <t>Conformance class coverage 
-Validate that tool covers conformance class set </t>
+Validate that tool covers conformance class set</t>
   </si>
   <si>
     <t>Descriptive Sub-Class</t>
@@ -593,9 +591,6 @@
       </rPr>
       <t xml:space="preserve"> in the BPMN 2.0 specification are present.</t>
     </r>
-  </si>
-  <si>
-    <t> </t>
   </si>
 </sst>
 </file>
@@ -866,7 +861,7 @@
       <protection hidden="false" locked="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="83">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -959,18 +954,10 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="0" fontId="10" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="0" fontId="10" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="45" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="0" fontId="10" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="45" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="0" fontId="10" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -1205,10 +1192,6 @@
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="5" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
@@ -1219,7 +1202,7 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Normal" xfId="21"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Normal" xfId="21"/>
     <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="20"/>
   </cellStyles>
   <colors>
@@ -1722,10 +1705,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AJ17"/>
+  <dimension ref="A1:AJ13"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="K1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100">
-      <selection activeCell="W9" activeCellId="0" pane="topLeft" sqref="W9"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="J2" view="normal" windowProtection="false" workbookViewId="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100">
+      <selection activeCell="V6" activeCellId="0" pane="topLeft" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1766,849 +1749,840 @@
       <c r="H2" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="K2" s="24" t="s">
+      <c r="K2" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="L2" s="24" t="s">
+      <c r="L2" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="M2" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="N2" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="O2" s="25" t="s">
+      <c r="O2" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="P2" s="25" t="s">
+      <c r="P2" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="Q2" s="25" t="s">
+      <c r="Q2" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="R2" s="25" t="s">
+      <c r="R2" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="S2" s="25" t="s">
+      <c r="S2" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="T2" s="25" t="s">
+      <c r="T2" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="U2" s="25" t="s">
+      <c r="U2" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="V2" s="25" t="s">
+      <c r="V2" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="W2" s="25" t="s">
+      <c r="W2" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="X2" s="25" t="s">
+      <c r="X2" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="Y2" s="25" t="s">
+      <c r="Y2" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="Z2" s="25" t="s">
+      <c r="Z2" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="AA2" s="25" t="s">
+      <c r="AA2" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="AB2" s="25" t="s">
+      <c r="AB2" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AC2" s="25" t="s">
+      <c r="AC2" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="AD2" s="25" t="s">
+      <c r="AD2" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="AE2" s="25" t="s">
+      <c r="AE2" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AF2" s="25" t="s">
+      <c r="AF2" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="AG2" s="25" t="s">
+      <c r="AG2" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="AH2" s="25" t="s">
+      <c r="AH2" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AI2" s="25" t="s">
+      <c r="AI2" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="AJ2" s="25" t="s">
+      <c r="AJ2" s="23" t="s">
         <v>50</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
-      <c r="A3" s="26"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="28" t="s">
+      <c r="A3" s="24"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="J3" s="29" t="s">
+      <c r="J3" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="30" t="s">
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="31" t="s">
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="31"/>
-      <c r="S3" s="31" t="s">
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="T3" s="31"/>
-      <c r="U3" s="31"/>
-      <c r="V3" s="31" t="s">
+      <c r="T3" s="29"/>
+      <c r="U3" s="29"/>
+      <c r="V3" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="W3" s="31"/>
-      <c r="X3" s="31"/>
-      <c r="Y3" s="31" t="s">
+      <c r="W3" s="29"/>
+      <c r="X3" s="29"/>
+      <c r="Y3" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="Z3" s="31"/>
-      <c r="AA3" s="31"/>
-      <c r="AB3" s="31" t="s">
+      <c r="Z3" s="29"/>
+      <c r="AA3" s="29"/>
+      <c r="AB3" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="AC3" s="31"/>
-      <c r="AD3" s="31"/>
-      <c r="AE3" s="31" t="s">
+      <c r="AC3" s="29"/>
+      <c r="AD3" s="29"/>
+      <c r="AE3" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="AF3" s="31"/>
-      <c r="AG3" s="31"/>
-      <c r="AH3" s="31"/>
-      <c r="AI3" s="31"/>
-      <c r="AJ3" s="31"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="4" s="38">
-      <c r="A4" s="32"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="34" t="s">
+      <c r="AF3" s="29"/>
+      <c r="AG3" s="29"/>
+      <c r="AH3" s="29"/>
+      <c r="AI3" s="29"/>
+      <c r="AJ3" s="29"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="4" s="36">
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="J4" s="35" t="s">
+      <c r="J4" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="36" t="s">
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36" t="s">
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="Q4" s="36"/>
-      <c r="R4" s="36"/>
-      <c r="S4" s="36" t="s">
+      <c r="Q4" s="34"/>
+      <c r="R4" s="34"/>
+      <c r="S4" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="T4" s="36"/>
-      <c r="U4" s="36"/>
-      <c r="V4" s="37" t="s">
+      <c r="T4" s="34"/>
+      <c r="U4" s="34"/>
+      <c r="V4" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="W4" s="37"/>
-      <c r="X4" s="37"/>
-      <c r="Y4" s="36" t="s">
+      <c r="W4" s="35"/>
+      <c r="X4" s="35"/>
+      <c r="Y4" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="Z4" s="36"/>
-      <c r="AA4" s="36"/>
-      <c r="AB4" s="36" t="n">
+      <c r="Z4" s="34"/>
+      <c r="AA4" s="34"/>
+      <c r="AB4" s="34" t="n">
         <v>2.4</v>
       </c>
-      <c r="AC4" s="36"/>
-      <c r="AD4" s="36"/>
-      <c r="AE4" s="36" t="s">
+      <c r="AC4" s="34"/>
+      <c r="AD4" s="34"/>
+      <c r="AE4" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="AF4" s="36"/>
-      <c r="AG4" s="36"/>
-      <c r="AH4" s="36"/>
-      <c r="AI4" s="36"/>
-      <c r="AJ4" s="36"/>
+      <c r="AF4" s="34"/>
+      <c r="AG4" s="34"/>
+      <c r="AH4" s="34"/>
+      <c r="AI4" s="34"/>
+      <c r="AJ4" s="34"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="5">
-      <c r="A5" s="39"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="41" t="s">
+      <c r="A5" s="37"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="J5" s="42" t="n">
+      <c r="J5" s="40" t="n">
         <v>41380</v>
       </c>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="43" t="n">
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="41" t="n">
         <v>41373</v>
       </c>
-      <c r="N5" s="43"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="44" t="n">
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="42" t="n">
         <v>41396</v>
       </c>
-      <c r="Q5" s="44"/>
-      <c r="R5" s="44"/>
-      <c r="S5" s="45" t="n">
+      <c r="Q5" s="42"/>
+      <c r="R5" s="42"/>
+      <c r="S5" s="43" t="n">
         <v>41383</v>
       </c>
-      <c r="T5" s="45"/>
-      <c r="U5" s="45"/>
-      <c r="V5" s="45" t="n">
-        <v>41386</v>
-      </c>
-      <c r="W5" s="45"/>
-      <c r="X5" s="45"/>
-      <c r="Y5" s="44" t="n">
+      <c r="T5" s="43"/>
+      <c r="U5" s="43"/>
+      <c r="V5" s="43" t="n">
+        <v>41410</v>
+      </c>
+      <c r="W5" s="43"/>
+      <c r="X5" s="43"/>
+      <c r="Y5" s="42" t="n">
         <v>41394</v>
       </c>
-      <c r="Z5" s="44"/>
-      <c r="AA5" s="44"/>
-      <c r="AB5" s="44" t="n">
+      <c r="Z5" s="42"/>
+      <c r="AA5" s="42"/>
+      <c r="AB5" s="42" t="n">
         <v>41388</v>
       </c>
-      <c r="AC5" s="44"/>
-      <c r="AD5" s="44"/>
-      <c r="AE5" s="44" t="n">
+      <c r="AC5" s="42"/>
+      <c r="AD5" s="42"/>
+      <c r="AE5" s="42" t="n">
         <v>41388</v>
       </c>
-      <c r="AF5" s="44"/>
-      <c r="AG5" s="44"/>
-      <c r="AH5" s="44"/>
-      <c r="AI5" s="44"/>
-      <c r="AJ5" s="44"/>
+      <c r="AF5" s="42"/>
+      <c r="AG5" s="42"/>
+      <c r="AH5" s="42"/>
+      <c r="AI5" s="42"/>
+      <c r="AJ5" s="42"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="50.25" outlineLevel="0" r="6">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="48" t="n">
+      <c r="C6" s="46" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="49" t="s">
+      <c r="D6" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="50" t="n">
+      <c r="E6" s="48" t="n">
         <v>0</v>
       </c>
-      <c r="F6" s="51" t="s">
+      <c r="F6" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="G6" s="52" t="s">
+      <c r="G6" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="H6" s="53" t="s">
+      <c r="H6" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="I6" s="54" t="s">
+      <c r="I6" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="J6" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="K6" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="L6" s="50" t="s">
-        <v>76</v>
-      </c>
-      <c r="M6" s="52" t="s">
-        <v>77</v>
-      </c>
-      <c r="N6" s="52" t="s">
-        <v>77</v>
-      </c>
-      <c r="O6" s="52" t="s">
-        <v>77</v>
-      </c>
-      <c r="P6" s="52" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q6" s="52"/>
-      <c r="R6" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="S6" s="56" t="s">
-        <v>77</v>
-      </c>
-      <c r="T6" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="U6" s="57" t="s">
-        <v>76</v>
-      </c>
-      <c r="V6" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="W6" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="X6" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="Y6" s="51" t="s">
+      <c r="J6" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="K6" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="L6" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="M6" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="N6" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="O6" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="P6" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q6" s="50"/>
+      <c r="R6" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="S6" s="54" t="s">
+        <v>77</v>
+      </c>
+      <c r="T6" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="U6" s="55" t="s">
+        <v>76</v>
+      </c>
+      <c r="V6" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="W6" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="X6" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y6" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="Z6" s="51"/>
-      <c r="AA6" s="51"/>
-      <c r="AB6" s="51" t="s">
+      <c r="Z6" s="49"/>
+      <c r="AA6" s="49"/>
+      <c r="AB6" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="AC6" s="51"/>
-      <c r="AD6" s="51"/>
-      <c r="AE6" s="51" t="s">
+      <c r="AC6" s="49"/>
+      <c r="AD6" s="49"/>
+      <c r="AE6" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="AF6" s="51"/>
-      <c r="AG6" s="51"/>
-      <c r="AH6" s="55"/>
-      <c r="AI6" s="52"/>
-      <c r="AJ6" s="52"/>
+      <c r="AF6" s="49"/>
+      <c r="AG6" s="49"/>
+      <c r="AH6" s="53"/>
+      <c r="AI6" s="50"/>
+      <c r="AJ6" s="50"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="42.75" outlineLevel="0" r="7">
-      <c r="A7" s="46"/>
-      <c r="B7" s="58" t="s">
+      <c r="A7" s="44"/>
+      <c r="B7" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="48" t="n">
+      <c r="C7" s="46" t="n">
         <v>2</v>
       </c>
-      <c r="D7" s="49" t="s">
+      <c r="D7" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="50" t="n">
+      <c r="E7" s="48" t="n">
         <v>0</v>
       </c>
-      <c r="F7" s="51" t="s">
+      <c r="F7" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="G7" s="52" t="s">
+      <c r="G7" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="H7" s="59" t="s">
+      <c r="H7" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="I7" s="54" t="s">
+      <c r="I7" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="J7" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="K7" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="L7" s="50" t="s">
-        <v>76</v>
-      </c>
-      <c r="M7" s="52" t="s">
-        <v>77</v>
-      </c>
-      <c r="N7" s="52" t="s">
-        <v>77</v>
-      </c>
-      <c r="O7" s="52" t="s">
-        <v>77</v>
-      </c>
-      <c r="P7" s="52" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q7" s="52"/>
-      <c r="R7" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="S7" s="56" t="s">
-        <v>77</v>
-      </c>
-      <c r="T7" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="U7" s="57" t="s">
-        <v>76</v>
-      </c>
-      <c r="V7" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="W7" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="X7" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="Y7" s="51"/>
-      <c r="Z7" s="51"/>
-      <c r="AA7" s="51"/>
-      <c r="AB7" s="51"/>
-      <c r="AC7" s="51"/>
-      <c r="AD7" s="51"/>
-      <c r="AE7" s="51"/>
-      <c r="AF7" s="51"/>
-      <c r="AG7" s="51"/>
-      <c r="AH7" s="55"/>
-      <c r="AI7" s="52"/>
-      <c r="AJ7" s="52"/>
+      <c r="J7" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="K7" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="L7" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="M7" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="N7" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="O7" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="P7" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q7" s="50"/>
+      <c r="R7" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="S7" s="54" t="s">
+        <v>77</v>
+      </c>
+      <c r="T7" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="U7" s="55" t="s">
+        <v>76</v>
+      </c>
+      <c r="V7" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="W7" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="X7" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y7" s="49"/>
+      <c r="Z7" s="49"/>
+      <c r="AA7" s="49"/>
+      <c r="AB7" s="49"/>
+      <c r="AC7" s="49"/>
+      <c r="AD7" s="49"/>
+      <c r="AE7" s="49"/>
+      <c r="AF7" s="49"/>
+      <c r="AG7" s="49"/>
+      <c r="AH7" s="53"/>
+      <c r="AI7" s="50"/>
+      <c r="AJ7" s="50"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="43.5" outlineLevel="0" r="8">
-      <c r="A8" s="46"/>
-      <c r="B8" s="58"/>
-      <c r="C8" s="48" t="n">
+      <c r="A8" s="44"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="46" t="n">
         <v>3</v>
       </c>
-      <c r="D8" s="49" t="s">
+      <c r="D8" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="E8" s="50" t="n">
+      <c r="E8" s="48" t="n">
         <v>0</v>
       </c>
-      <c r="F8" s="51" t="s">
+      <c r="F8" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="G8" s="52" t="s">
+      <c r="G8" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="H8" s="59" t="s">
+      <c r="H8" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="I8" s="54" t="s">
+      <c r="I8" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="J8" s="60" t="s">
-        <v>76</v>
-      </c>
-      <c r="K8" s="52" t="s">
-        <v>77</v>
-      </c>
-      <c r="L8" s="61" t="s">
-        <v>76</v>
-      </c>
-      <c r="M8" s="52" t="s">
-        <v>77</v>
-      </c>
-      <c r="N8" s="52" t="s">
-        <v>77</v>
-      </c>
-      <c r="O8" s="52" t="s">
-        <v>77</v>
-      </c>
-      <c r="P8" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q8" s="52"/>
-      <c r="R8" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="S8" s="62" t="s">
-        <v>76</v>
-      </c>
-      <c r="T8" s="62" t="s">
-        <v>76</v>
-      </c>
-      <c r="U8" s="57" t="s">
-        <v>76</v>
-      </c>
-      <c r="V8" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="W8" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="X8" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="Y8" s="51"/>
-      <c r="Z8" s="51"/>
-      <c r="AA8" s="51"/>
-      <c r="AB8" s="51"/>
-      <c r="AC8" s="51"/>
-      <c r="AD8" s="51"/>
-      <c r="AE8" s="51"/>
-      <c r="AF8" s="51"/>
-      <c r="AG8" s="51"/>
-      <c r="AH8" s="55"/>
-      <c r="AI8" s="52"/>
-      <c r="AJ8" s="52"/>
+      <c r="J8" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="K8" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="L8" s="59" t="s">
+        <v>76</v>
+      </c>
+      <c r="M8" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="N8" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="O8" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="P8" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q8" s="50"/>
+      <c r="R8" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="S8" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="T8" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="U8" s="55" t="s">
+        <v>76</v>
+      </c>
+      <c r="V8" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="W8" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="X8" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y8" s="49"/>
+      <c r="Z8" s="49"/>
+      <c r="AA8" s="49"/>
+      <c r="AB8" s="49"/>
+      <c r="AC8" s="49"/>
+      <c r="AD8" s="49"/>
+      <c r="AE8" s="49"/>
+      <c r="AF8" s="49"/>
+      <c r="AG8" s="49"/>
+      <c r="AH8" s="53"/>
+      <c r="AI8" s="50"/>
+      <c r="AJ8" s="50"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="50.25" outlineLevel="0" r="9">
-      <c r="A9" s="46"/>
-      <c r="B9" s="58"/>
-      <c r="C9" s="48" t="n">
+      <c r="A9" s="44"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="46" t="n">
         <v>4</v>
       </c>
-      <c r="D9" s="49" t="s">
+      <c r="D9" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="E9" s="63" t="n">
+      <c r="E9" s="61" t="n">
         <v>0</v>
       </c>
-      <c r="F9" s="64" t="s">
+      <c r="F9" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="G9" s="65" t="s">
+      <c r="G9" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="H9" s="66" t="s">
+      <c r="H9" s="64" t="s">
         <v>89</v>
       </c>
-      <c r="I9" s="54" t="s">
+      <c r="I9" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="67" t="s">
-        <v>76</v>
-      </c>
-      <c r="K9" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="L9" s="68" t="s">
-        <v>76</v>
-      </c>
-      <c r="M9" s="48" t="s">
-        <v>76</v>
-      </c>
-      <c r="N9" s="48" t="s">
-        <v>76</v>
-      </c>
-      <c r="O9" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="P9" s="48" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q9" s="48"/>
-      <c r="R9" s="69" t="s">
-        <v>76</v>
-      </c>
-      <c r="S9" s="70" t="s">
-        <v>77</v>
-      </c>
-      <c r="T9" s="71" t="s">
-        <v>76</v>
-      </c>
-      <c r="U9" s="72" t="s">
-        <v>76</v>
-      </c>
-      <c r="V9" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="W9" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="X9" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="Y9" s="51"/>
-      <c r="Z9" s="51"/>
-      <c r="AA9" s="51"/>
-      <c r="AB9" s="51"/>
-      <c r="AC9" s="51"/>
-      <c r="AD9" s="51"/>
-      <c r="AE9" s="51"/>
-      <c r="AF9" s="51"/>
-      <c r="AG9" s="51"/>
-      <c r="AH9" s="73"/>
-      <c r="AI9" s="48"/>
-      <c r="AJ9" s="74"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="58.5" outlineLevel="0" r="10" s="77">
-      <c r="A10" s="75" t="s">
+      <c r="J9" s="65" t="s">
+        <v>76</v>
+      </c>
+      <c r="K9" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="L9" s="66" t="s">
+        <v>76</v>
+      </c>
+      <c r="M9" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="N9" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="O9" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="P9" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q9" s="46"/>
+      <c r="R9" s="67" t="s">
+        <v>76</v>
+      </c>
+      <c r="S9" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="T9" s="69" t="s">
+        <v>76</v>
+      </c>
+      <c r="U9" s="70" t="s">
+        <v>76</v>
+      </c>
+      <c r="V9" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="W9" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="X9" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y9" s="49"/>
+      <c r="Z9" s="49"/>
+      <c r="AA9" s="49"/>
+      <c r="AB9" s="49"/>
+      <c r="AC9" s="49"/>
+      <c r="AD9" s="49"/>
+      <c r="AE9" s="49"/>
+      <c r="AF9" s="49"/>
+      <c r="AG9" s="49"/>
+      <c r="AH9" s="71"/>
+      <c r="AI9" s="46"/>
+      <c r="AJ9" s="72"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="58.5" outlineLevel="0" r="10" s="75">
+      <c r="A10" s="73" t="s">
         <v>90</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="52" t="n">
+      <c r="C10" s="50" t="n">
         <v>1</v>
       </c>
-      <c r="D10" s="51" t="s">
+      <c r="D10" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="E10" s="52" t="n">
+      <c r="E10" s="50" t="n">
         <v>0</v>
       </c>
-      <c r="F10" s="51" t="s">
+      <c r="F10" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="G10" s="52" t="s">
+      <c r="G10" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="H10" s="76" t="s">
+      <c r="H10" s="74" t="s">
         <v>94</v>
       </c>
-      <c r="I10" s="54" t="s">
+      <c r="I10" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="J10" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="K10" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="L10" s="52"/>
-      <c r="M10" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="N10" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="O10" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="P10" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q10" s="52"/>
-      <c r="R10" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="S10" s="52"/>
-      <c r="T10" s="52"/>
-      <c r="U10" s="52"/>
-      <c r="V10" s="51" t="s">
-        <v>76</v>
-      </c>
-      <c r="W10" s="51" t="s">
-        <v>76</v>
-      </c>
-      <c r="X10" s="51" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y10" s="51"/>
-      <c r="Z10" s="51"/>
-      <c r="AA10" s="51"/>
-      <c r="AB10" s="51"/>
-      <c r="AC10" s="51"/>
-      <c r="AD10" s="51"/>
-      <c r="AE10" s="51"/>
-      <c r="AF10" s="51"/>
-      <c r="AG10" s="51"/>
-      <c r="AH10" s="52"/>
-      <c r="AI10" s="52"/>
-      <c r="AJ10" s="52"/>
+      <c r="J10" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="K10" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="N10" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="O10" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="P10" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q10" s="50"/>
+      <c r="R10" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="S10" s="50"/>
+      <c r="T10" s="50"/>
+      <c r="U10" s="50"/>
+      <c r="V10" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="W10" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="X10" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y10" s="49"/>
+      <c r="Z10" s="49"/>
+      <c r="AA10" s="49"/>
+      <c r="AB10" s="49"/>
+      <c r="AC10" s="49"/>
+      <c r="AD10" s="49"/>
+      <c r="AE10" s="49"/>
+      <c r="AF10" s="49"/>
+      <c r="AG10" s="49"/>
+      <c r="AH10" s="50"/>
+      <c r="AI10" s="50"/>
+      <c r="AJ10" s="50"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="58.5" outlineLevel="0" r="11">
-      <c r="A11" s="75"/>
-      <c r="B11" s="58" t="s">
+      <c r="A11" s="73"/>
+      <c r="B11" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="52" t="n">
+      <c r="C11" s="50" t="n">
         <v>2</v>
       </c>
-      <c r="D11" s="51" t="s">
+      <c r="D11" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="52" t="n">
+      <c r="E11" s="50" t="n">
         <v>0</v>
       </c>
-      <c r="F11" s="51" t="s">
+      <c r="F11" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="G11" s="52" t="s">
+      <c r="G11" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="H11" s="76" t="s">
+      <c r="H11" s="74" t="s">
         <v>98</v>
       </c>
-      <c r="I11" s="54" t="s">
+      <c r="I11" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="N11" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="O11" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="P11" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q11" s="52"/>
-      <c r="R11" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="S11" s="52"/>
-      <c r="T11" s="52"/>
-      <c r="U11" s="52"/>
-      <c r="V11" s="51" t="s">
-        <v>76</v>
-      </c>
-      <c r="W11" s="51" t="s">
-        <v>76</v>
-      </c>
-      <c r="X11" s="51" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y11" s="51"/>
-      <c r="Z11" s="51"/>
-      <c r="AA11" s="51"/>
-      <c r="AB11" s="51"/>
-      <c r="AC11" s="51"/>
-      <c r="AD11" s="51"/>
-      <c r="AE11" s="51"/>
-      <c r="AF11" s="51"/>
-      <c r="AG11" s="51"/>
-      <c r="AH11" s="52"/>
-      <c r="AI11" s="52"/>
-      <c r="AJ11" s="52"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="N11" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="O11" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="P11" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q11" s="50"/>
+      <c r="R11" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="S11" s="50"/>
+      <c r="T11" s="50"/>
+      <c r="U11" s="50"/>
+      <c r="V11" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="W11" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="X11" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y11" s="49"/>
+      <c r="Z11" s="49"/>
+      <c r="AA11" s="49"/>
+      <c r="AB11" s="49"/>
+      <c r="AC11" s="49"/>
+      <c r="AD11" s="49"/>
+      <c r="AE11" s="49"/>
+      <c r="AF11" s="49"/>
+      <c r="AG11" s="49"/>
+      <c r="AH11" s="50"/>
+      <c r="AI11" s="50"/>
+      <c r="AJ11" s="50"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="63" outlineLevel="0" r="12">
-      <c r="A12" s="75"/>
-      <c r="B12" s="58"/>
-      <c r="C12" s="78" t="n">
+      <c r="A12" s="73"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="76" t="n">
         <v>3</v>
       </c>
-      <c r="D12" s="79" t="s">
+      <c r="D12" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="E12" s="80" t="n">
+      <c r="E12" s="78" t="n">
         <v>0</v>
       </c>
-      <c r="F12" s="51" t="s">
+      <c r="F12" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="G12" s="81" t="s">
+      <c r="G12" s="79" t="s">
         <v>100</v>
       </c>
-      <c r="H12" s="59" t="s">
+      <c r="H12" s="57" t="s">
         <v>101</v>
       </c>
-      <c r="I12" s="54" t="s">
+      <c r="I12" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="J12" s="52"/>
-      <c r="K12" s="52"/>
-      <c r="L12" s="52"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="52"/>
-      <c r="O12" s="52"/>
-      <c r="P12" s="52"/>
-      <c r="Q12" s="52"/>
-      <c r="R12" s="52"/>
-      <c r="S12" s="52"/>
-      <c r="T12" s="52"/>
-      <c r="U12" s="52"/>
-      <c r="V12" s="52"/>
-      <c r="W12" s="52"/>
-      <c r="X12" s="52"/>
-      <c r="Y12" s="51"/>
-      <c r="Z12" s="51"/>
-      <c r="AA12" s="51"/>
-      <c r="AB12" s="51"/>
-      <c r="AC12" s="51"/>
-      <c r="AD12" s="51"/>
-      <c r="AE12" s="51"/>
-      <c r="AF12" s="51"/>
-      <c r="AG12" s="51"/>
-      <c r="AH12" s="52"/>
-      <c r="AI12" s="52"/>
-      <c r="AJ12" s="52"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="50"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="50"/>
+      <c r="R12" s="50"/>
+      <c r="S12" s="50"/>
+      <c r="T12" s="50"/>
+      <c r="U12" s="50"/>
+      <c r="V12" s="50"/>
+      <c r="W12" s="50"/>
+      <c r="X12" s="50"/>
+      <c r="Y12" s="49"/>
+      <c r="Z12" s="49"/>
+      <c r="AA12" s="49"/>
+      <c r="AB12" s="49"/>
+      <c r="AC12" s="49"/>
+      <c r="AD12" s="49"/>
+      <c r="AE12" s="49"/>
+      <c r="AF12" s="49"/>
+      <c r="AG12" s="49"/>
+      <c r="AH12" s="50"/>
+      <c r="AI12" s="50"/>
+      <c r="AJ12" s="50"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="45" outlineLevel="0" r="13">
-      <c r="A13" s="75"/>
-      <c r="B13" s="82"/>
-      <c r="C13" s="81" t="n">
+      <c r="A13" s="73"/>
+      <c r="B13" s="80"/>
+      <c r="C13" s="79" t="n">
         <v>4</v>
       </c>
-      <c r="D13" s="79" t="s">
+      <c r="D13" s="77" t="s">
         <v>102</v>
       </c>
-      <c r="E13" s="80" t="n">
+      <c r="E13" s="78" t="n">
         <v>0</v>
       </c>
-      <c r="F13" s="79" t="s">
+      <c r="F13" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="G13" s="81" t="s">
+      <c r="G13" s="79" t="s">
         <v>103</v>
       </c>
-      <c r="H13" s="83" t="s">
+      <c r="H13" s="81" t="s">
         <v>104</v>
       </c>
-      <c r="I13" s="54" t="s">
+      <c r="I13" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="J13" s="84"/>
-      <c r="K13" s="84"/>
-      <c r="L13" s="84"/>
-      <c r="M13" s="84"/>
-      <c r="N13" s="84"/>
-      <c r="O13" s="84"/>
-      <c r="P13" s="84"/>
-      <c r="Q13" s="84"/>
-      <c r="R13" s="84"/>
-      <c r="S13" s="84"/>
-      <c r="T13" s="84"/>
-      <c r="U13" s="84"/>
-      <c r="V13" s="84"/>
-      <c r="W13" s="84"/>
-      <c r="X13" s="84"/>
-      <c r="Y13" s="51"/>
-      <c r="Z13" s="51"/>
-      <c r="AA13" s="51"/>
-      <c r="AB13" s="51"/>
-      <c r="AC13" s="51"/>
-      <c r="AD13" s="51"/>
-      <c r="AE13" s="51"/>
-      <c r="AF13" s="51"/>
-      <c r="AG13" s="51"/>
-      <c r="AH13" s="84"/>
-      <c r="AI13" s="84"/>
-      <c r="AJ13" s="84"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="17">
-      <c r="D17" s="85" t="s">
-        <v>105</v>
-      </c>
-      <c r="H17" s="85" t="s">
-        <v>105</v>
-      </c>
-      <c r="I17" s="85"/>
+      <c r="J13" s="82"/>
+      <c r="K13" s="82"/>
+      <c r="L13" s="82"/>
+      <c r="M13" s="82"/>
+      <c r="N13" s="82"/>
+      <c r="O13" s="82"/>
+      <c r="P13" s="82"/>
+      <c r="Q13" s="82"/>
+      <c r="R13" s="82"/>
+      <c r="S13" s="82"/>
+      <c r="T13" s="82"/>
+      <c r="U13" s="82"/>
+      <c r="V13" s="82"/>
+      <c r="W13" s="82"/>
+      <c r="X13" s="82"/>
+      <c r="Y13" s="49"/>
+      <c r="Z13" s="49"/>
+      <c r="AA13" s="49"/>
+      <c r="AB13" s="49"/>
+      <c r="AC13" s="49"/>
+      <c r="AD13" s="49"/>
+      <c r="AE13" s="49"/>
+      <c r="AF13" s="49"/>
+      <c r="AG13" s="49"/>
+      <c r="AH13" s="82"/>
+      <c r="AI13" s="82"/>
+      <c r="AJ13" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="35">

</xml_diff>

<commit_message>
Added Trisotech BPMN Web Modeler 4.1 results
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="631" activeTab="1"/>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="109">
   <si>
     <t>Call Activities</t>
   </si>
@@ -597,13 +597,19 @@
   <si>
     <t>6.3442.15675</t>
   </si>
+  <si>
+    <t>Business Process Incubator BPMN 2.0 Web Modeler</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -892,7 +898,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1072,6 +1078,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1081,43 +1126,37 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1980,6 +2019,264 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="shapetype_202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="shapetype_202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="shapetype_202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="shapetype_202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="shapetype_202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="shapetype_202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2699,8 +2996,8 @@
   </sheetPr>
   <dimension ref="A1:AMK14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5:AM5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AM11" sqref="AM11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2717,24 +3014,24 @@
     <col min="10" max="1025" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K1" s="19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="47.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="69" t="s">
+    <row r="2" spans="1:42" ht="47.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69" t="s">
+      <c r="B2" s="82"/>
+      <c r="C2" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69" t="s">
+      <c r="D2" s="82"/>
+      <c r="E2" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="69"/>
+      <c r="F2" s="82"/>
       <c r="G2" s="21" t="s">
         <v>45</v>
       </c>
@@ -2834,8 +3131,17 @@
       <c r="AM2" s="23" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:39" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AN2" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="AO2" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP2" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
@@ -2847,56 +3153,61 @@
       <c r="I3" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="J3" s="70" t="s">
+      <c r="J3" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="71" t="s">
+      <c r="K3" s="83"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="N3" s="71"/>
-      <c r="O3" s="71"/>
-      <c r="P3" s="72" t="s">
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="71" t="s">
         <v>54</v>
       </c>
-      <c r="Q3" s="72"/>
-      <c r="R3" s="72"/>
-      <c r="S3" s="72" t="s">
+      <c r="Q3" s="71"/>
+      <c r="R3" s="71"/>
+      <c r="S3" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="T3" s="72"/>
-      <c r="U3" s="72"/>
-      <c r="V3" s="72" t="s">
+      <c r="T3" s="71"/>
+      <c r="U3" s="71"/>
+      <c r="V3" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="W3" s="72"/>
-      <c r="X3" s="72"/>
-      <c r="Y3" s="72" t="s">
+      <c r="W3" s="71"/>
+      <c r="X3" s="71"/>
+      <c r="Y3" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="Z3" s="72"/>
-      <c r="AA3" s="72"/>
-      <c r="AB3" s="72" t="s">
+      <c r="Z3" s="71"/>
+      <c r="AA3" s="71"/>
+      <c r="AB3" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="AC3" s="72"/>
-      <c r="AD3" s="72"/>
-      <c r="AE3" s="72" t="s">
+      <c r="AC3" s="71"/>
+      <c r="AD3" s="71"/>
+      <c r="AE3" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="AF3" s="72"/>
-      <c r="AG3" s="72"/>
-      <c r="AH3" s="72" t="s">
+      <c r="AF3" s="71"/>
+      <c r="AG3" s="71"/>
+      <c r="AH3" s="71" t="s">
         <v>105</v>
       </c>
-      <c r="AI3" s="72"/>
-      <c r="AJ3" s="72"/>
-      <c r="AK3" s="72"/>
-      <c r="AL3" s="72"/>
-      <c r="AM3" s="72"/>
-    </row>
-    <row r="4" spans="1:39" s="30" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AI3" s="71"/>
+      <c r="AJ3" s="71"/>
+      <c r="AK3" s="92" t="s">
+        <v>107</v>
+      </c>
+      <c r="AL3" s="93"/>
+      <c r="AM3" s="94"/>
+      <c r="AN3" s="83"/>
+      <c r="AO3" s="85"/>
+      <c r="AP3" s="86"/>
+    </row>
+    <row r="4" spans="1:42" s="30" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27"/>
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
@@ -2908,56 +3219,61 @@
       <c r="I4" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="J4" s="73" t="s">
+      <c r="J4" s="80" t="s">
         <v>61</v>
       </c>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="74" t="s">
+      <c r="K4" s="80"/>
+      <c r="L4" s="80"/>
+      <c r="M4" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="N4" s="74"/>
-      <c r="O4" s="74"/>
-      <c r="P4" s="74" t="s">
+      <c r="N4" s="72"/>
+      <c r="O4" s="72"/>
+      <c r="P4" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="Q4" s="74"/>
-      <c r="R4" s="74"/>
-      <c r="S4" s="74" t="s">
+      <c r="Q4" s="72"/>
+      <c r="R4" s="72"/>
+      <c r="S4" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="T4" s="74"/>
-      <c r="U4" s="74"/>
-      <c r="V4" s="75" t="s">
+      <c r="T4" s="72"/>
+      <c r="U4" s="72"/>
+      <c r="V4" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="W4" s="75"/>
-      <c r="X4" s="75"/>
-      <c r="Y4" s="74" t="s">
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
+      <c r="Y4" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="Z4" s="74"/>
-      <c r="AA4" s="74"/>
-      <c r="AB4" s="74">
+      <c r="Z4" s="72"/>
+      <c r="AA4" s="72"/>
+      <c r="AB4" s="72">
         <v>2.4</v>
       </c>
-      <c r="AC4" s="74"/>
-      <c r="AD4" s="74"/>
-      <c r="AE4" s="74" t="s">
+      <c r="AC4" s="72"/>
+      <c r="AD4" s="72"/>
+      <c r="AE4" s="72" t="s">
         <v>67</v>
       </c>
-      <c r="AF4" s="74"/>
-      <c r="AG4" s="74"/>
-      <c r="AH4" s="74" t="s">
+      <c r="AF4" s="72"/>
+      <c r="AG4" s="72"/>
+      <c r="AH4" s="72" t="s">
         <v>106</v>
       </c>
-      <c r="AI4" s="74"/>
-      <c r="AJ4" s="74"/>
-      <c r="AK4" s="74"/>
-      <c r="AL4" s="74"/>
-      <c r="AM4" s="74"/>
-    </row>
-    <row r="5" spans="1:39" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AI4" s="72"/>
+      <c r="AJ4" s="72"/>
+      <c r="AK4" s="72" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL4" s="72"/>
+      <c r="AM4" s="72"/>
+      <c r="AN4" s="80"/>
+      <c r="AO4" s="87"/>
+      <c r="AP4" s="88"/>
+    </row>
+    <row r="5" spans="1:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="31"/>
       <c r="B5" s="32"/>
       <c r="C5" s="32"/>
@@ -2969,57 +3285,62 @@
       <c r="I5" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="J5" s="81">
+      <c r="J5" s="77">
         <v>41380</v>
       </c>
-      <c r="K5" s="81"/>
-      <c r="L5" s="81"/>
-      <c r="M5" s="82">
+      <c r="K5" s="77"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="78">
         <v>41373</v>
       </c>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="83">
+      <c r="N5" s="78"/>
+      <c r="O5" s="78"/>
+      <c r="P5" s="73">
         <v>41396</v>
       </c>
-      <c r="Q5" s="83"/>
-      <c r="R5" s="83"/>
-      <c r="S5" s="84">
+      <c r="Q5" s="73"/>
+      <c r="R5" s="73"/>
+      <c r="S5" s="79">
         <v>41383</v>
       </c>
-      <c r="T5" s="84"/>
-      <c r="U5" s="84"/>
-      <c r="V5" s="84">
+      <c r="T5" s="79"/>
+      <c r="U5" s="79"/>
+      <c r="V5" s="79">
         <v>41410</v>
       </c>
-      <c r="W5" s="84"/>
-      <c r="X5" s="84"/>
-      <c r="Y5" s="83">
+      <c r="W5" s="79"/>
+      <c r="X5" s="79"/>
+      <c r="Y5" s="73">
         <v>41394</v>
       </c>
-      <c r="Z5" s="83"/>
-      <c r="AA5" s="83"/>
-      <c r="AB5" s="83">
+      <c r="Z5" s="73"/>
+      <c r="AA5" s="73"/>
+      <c r="AB5" s="73">
         <v>41388</v>
       </c>
-      <c r="AC5" s="83"/>
-      <c r="AD5" s="83"/>
-      <c r="AE5" s="83">
+      <c r="AC5" s="73"/>
+      <c r="AD5" s="73"/>
+      <c r="AE5" s="73">
         <v>41388</v>
       </c>
-      <c r="AF5" s="83"/>
-      <c r="AG5" s="83"/>
-      <c r="AH5" s="83">
+      <c r="AF5" s="73"/>
+      <c r="AG5" s="73"/>
+      <c r="AH5" s="73">
         <v>41431</v>
       </c>
-      <c r="AI5" s="83"/>
-      <c r="AJ5" s="83"/>
-      <c r="AK5" s="83"/>
-      <c r="AL5" s="83"/>
-      <c r="AM5" s="83"/>
-    </row>
-    <row r="6" spans="1:39" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="76" t="s">
+      <c r="AI5" s="73"/>
+      <c r="AJ5" s="73"/>
+      <c r="AK5" s="95">
+        <v>41429</v>
+      </c>
+      <c r="AL5" s="95"/>
+      <c r="AM5" s="95"/>
+      <c r="AN5" s="89"/>
+      <c r="AO5" s="90"/>
+      <c r="AP5" s="91"/>
+    </row>
+    <row r="6" spans="1:42" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="74" t="s">
         <v>69</v>
       </c>
       <c r="B6" s="34" t="s">
@@ -3089,21 +3410,21 @@
       <c r="X6" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="Y6" s="77" t="s">
+      <c r="Y6" s="75" t="s">
         <v>78</v>
       </c>
-      <c r="Z6" s="77"/>
-      <c r="AA6" s="77"/>
-      <c r="AB6" s="77" t="s">
+      <c r="Z6" s="75"/>
+      <c r="AA6" s="75"/>
+      <c r="AB6" s="75" t="s">
         <v>78</v>
       </c>
-      <c r="AC6" s="77"/>
-      <c r="AD6" s="77"/>
-      <c r="AE6" s="77" t="s">
+      <c r="AC6" s="75"/>
+      <c r="AD6" s="75"/>
+      <c r="AE6" s="75" t="s">
         <v>79</v>
       </c>
-      <c r="AF6" s="77"/>
-      <c r="AG6" s="77"/>
+      <c r="AF6" s="75"/>
+      <c r="AG6" s="75"/>
       <c r="AH6" s="42" t="s">
         <v>77</v>
       </c>
@@ -3113,12 +3434,21 @@
       <c r="AJ6" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="AK6" s="42"/>
-      <c r="AL6" s="39"/>
-      <c r="AM6" s="39"/>
-    </row>
-    <row r="7" spans="1:39" ht="42.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="76"/>
+      <c r="AK6" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL6" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM6" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN6" s="42"/>
+      <c r="AO6" s="39"/>
+      <c r="AP6" s="39"/>
+    </row>
+    <row r="7" spans="1:42" ht="42.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="74"/>
       <c r="B7" s="45" t="s">
         <v>80</v>
       </c>
@@ -3186,15 +3516,15 @@
       <c r="X7" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="Y7" s="77"/>
-      <c r="Z7" s="77"/>
-      <c r="AA7" s="77"/>
-      <c r="AB7" s="77"/>
-      <c r="AC7" s="77"/>
-      <c r="AD7" s="77"/>
-      <c r="AE7" s="77"/>
-      <c r="AF7" s="77"/>
-      <c r="AG7" s="77"/>
+      <c r="Y7" s="75"/>
+      <c r="Z7" s="75"/>
+      <c r="AA7" s="75"/>
+      <c r="AB7" s="75"/>
+      <c r="AC7" s="75"/>
+      <c r="AD7" s="75"/>
+      <c r="AE7" s="75"/>
+      <c r="AF7" s="75"/>
+      <c r="AG7" s="75"/>
       <c r="AH7" s="42" t="s">
         <v>77</v>
       </c>
@@ -3204,12 +3534,21 @@
       <c r="AJ7" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="AK7" s="42"/>
-      <c r="AL7" s="39"/>
-      <c r="AM7" s="39"/>
-    </row>
-    <row r="8" spans="1:39" ht="43.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="76"/>
+      <c r="AK7" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL7" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM7" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN7" s="42"/>
+      <c r="AO7" s="39"/>
+      <c r="AP7" s="39"/>
+    </row>
+    <row r="8" spans="1:42" ht="43.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="74"/>
       <c r="B8" s="45"/>
       <c r="C8" s="35">
         <v>3</v>
@@ -3275,15 +3614,15 @@
       <c r="X8" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="Y8" s="77"/>
-      <c r="Z8" s="77"/>
-      <c r="AA8" s="77"/>
-      <c r="AB8" s="77"/>
-      <c r="AC8" s="77"/>
-      <c r="AD8" s="77"/>
-      <c r="AE8" s="77"/>
-      <c r="AF8" s="77"/>
-      <c r="AG8" s="77"/>
+      <c r="Y8" s="75"/>
+      <c r="Z8" s="75"/>
+      <c r="AA8" s="75"/>
+      <c r="AB8" s="75"/>
+      <c r="AC8" s="75"/>
+      <c r="AD8" s="75"/>
+      <c r="AE8" s="75"/>
+      <c r="AF8" s="75"/>
+      <c r="AG8" s="75"/>
       <c r="AH8" s="42" t="s">
         <v>76</v>
       </c>
@@ -3293,12 +3632,21 @@
       <c r="AJ8" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="AK8" s="42"/>
-      <c r="AL8" s="39"/>
-      <c r="AM8" s="39"/>
-    </row>
-    <row r="9" spans="1:39" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="76"/>
+      <c r="AK8" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL8" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM8" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN8" s="42"/>
+      <c r="AO8" s="39"/>
+      <c r="AP8" s="39"/>
+    </row>
+    <row r="9" spans="1:42" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="74"/>
       <c r="B9" s="45"/>
       <c r="C9" s="35">
         <v>4</v>
@@ -3364,15 +3712,15 @@
       <c r="X9" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="Y9" s="77"/>
-      <c r="Z9" s="77"/>
-      <c r="AA9" s="77"/>
-      <c r="AB9" s="77"/>
-      <c r="AC9" s="77"/>
-      <c r="AD9" s="77"/>
-      <c r="AE9" s="77"/>
-      <c r="AF9" s="77"/>
-      <c r="AG9" s="77"/>
+      <c r="Y9" s="75"/>
+      <c r="Z9" s="75"/>
+      <c r="AA9" s="75"/>
+      <c r="AB9" s="75"/>
+      <c r="AC9" s="75"/>
+      <c r="AD9" s="75"/>
+      <c r="AE9" s="75"/>
+      <c r="AF9" s="75"/>
+      <c r="AG9" s="75"/>
       <c r="AH9" s="39" t="s">
         <v>76</v>
       </c>
@@ -3382,12 +3730,21 @@
       <c r="AJ9" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="AK9" s="79"/>
-      <c r="AL9" s="35"/>
-      <c r="AM9" s="80"/>
-    </row>
-    <row r="10" spans="1:39" s="61" customFormat="1" ht="58.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="78" t="s">
+      <c r="AK9" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL9" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM9" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN9" s="69"/>
+      <c r="AO9" s="35"/>
+      <c r="AP9" s="70"/>
+    </row>
+    <row r="10" spans="1:42" s="61" customFormat="1" ht="58.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="76" t="s">
         <v>90</v>
       </c>
       <c r="B10" s="34" t="s">
@@ -3449,15 +3806,15 @@
       <c r="X10" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="Y10" s="77"/>
-      <c r="Z10" s="77"/>
-      <c r="AA10" s="77"/>
-      <c r="AB10" s="77"/>
-      <c r="AC10" s="77"/>
-      <c r="AD10" s="77"/>
-      <c r="AE10" s="77"/>
-      <c r="AF10" s="77"/>
-      <c r="AG10" s="77"/>
+      <c r="Y10" s="75"/>
+      <c r="Z10" s="75"/>
+      <c r="AA10" s="75"/>
+      <c r="AB10" s="75"/>
+      <c r="AC10" s="75"/>
+      <c r="AD10" s="75"/>
+      <c r="AE10" s="75"/>
+      <c r="AF10" s="75"/>
+      <c r="AG10" s="75"/>
       <c r="AH10" s="39" t="s">
         <v>76</v>
       </c>
@@ -3465,12 +3822,21 @@
       <c r="AJ10" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="AK10" s="39"/>
-      <c r="AL10" s="39"/>
-      <c r="AM10" s="39"/>
-    </row>
-    <row r="11" spans="1:39" ht="58.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="78"/>
+      <c r="AK10" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL10" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM10" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN10" s="39"/>
+      <c r="AO10" s="39"/>
+      <c r="AP10" s="39"/>
+    </row>
+    <row r="11" spans="1:42" ht="58.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="76"/>
       <c r="B11" s="45" t="s">
         <v>95</v>
       </c>
@@ -3526,15 +3892,15 @@
       <c r="X11" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="Y11" s="77"/>
-      <c r="Z11" s="77"/>
-      <c r="AA11" s="77"/>
-      <c r="AB11" s="77"/>
-      <c r="AC11" s="77"/>
-      <c r="AD11" s="77"/>
-      <c r="AE11" s="77"/>
-      <c r="AF11" s="77"/>
-      <c r="AG11" s="77"/>
+      <c r="Y11" s="75"/>
+      <c r="Z11" s="75"/>
+      <c r="AA11" s="75"/>
+      <c r="AB11" s="75"/>
+      <c r="AC11" s="75"/>
+      <c r="AD11" s="75"/>
+      <c r="AE11" s="75"/>
+      <c r="AF11" s="75"/>
+      <c r="AG11" s="75"/>
       <c r="AH11" s="39" t="s">
         <v>76</v>
       </c>
@@ -3542,12 +3908,21 @@
       <c r="AJ11" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="AK11" s="39"/>
-      <c r="AL11" s="39"/>
-      <c r="AM11" s="39"/>
-    </row>
-    <row r="12" spans="1:39" ht="63" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="78"/>
+      <c r="AK11" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL11" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM11" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="AN11" s="39"/>
+      <c r="AO11" s="39"/>
+      <c r="AP11" s="39"/>
+    </row>
+    <row r="12" spans="1:42" ht="63" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="76"/>
       <c r="B12" s="45"/>
       <c r="C12" s="62">
         <v>3</v>
@@ -3585,24 +3960,27 @@
       <c r="V12" s="39"/>
       <c r="W12" s="39"/>
       <c r="X12" s="39"/>
-      <c r="Y12" s="77"/>
-      <c r="Z12" s="77"/>
-      <c r="AA12" s="77"/>
-      <c r="AB12" s="77"/>
-      <c r="AC12" s="77"/>
-      <c r="AD12" s="77"/>
-      <c r="AE12" s="77"/>
-      <c r="AF12" s="77"/>
-      <c r="AG12" s="77"/>
+      <c r="Y12" s="75"/>
+      <c r="Z12" s="75"/>
+      <c r="AA12" s="75"/>
+      <c r="AB12" s="75"/>
+      <c r="AC12" s="75"/>
+      <c r="AD12" s="75"/>
+      <c r="AE12" s="75"/>
+      <c r="AF12" s="75"/>
+      <c r="AG12" s="75"/>
       <c r="AH12" s="39"/>
       <c r="AI12" s="39"/>
       <c r="AJ12" s="39"/>
       <c r="AK12" s="39"/>
       <c r="AL12" s="39"/>
       <c r="AM12" s="39"/>
-    </row>
-    <row r="13" spans="1:39" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="78"/>
+      <c r="AN12" s="39"/>
+      <c r="AO12" s="39"/>
+      <c r="AP12" s="39"/>
+    </row>
+    <row r="13" spans="1:42" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="76"/>
       <c r="B13" s="66"/>
       <c r="C13" s="65">
         <v>4</v>
@@ -3640,25 +4018,56 @@
       <c r="V13" s="68"/>
       <c r="W13" s="68"/>
       <c r="X13" s="68"/>
-      <c r="Y13" s="77"/>
-      <c r="Z13" s="77"/>
-      <c r="AA13" s="77"/>
-      <c r="AB13" s="77"/>
-      <c r="AC13" s="77"/>
-      <c r="AD13" s="77"/>
-      <c r="AE13" s="77"/>
-      <c r="AF13" s="77"/>
-      <c r="AG13" s="77"/>
+      <c r="Y13" s="75"/>
+      <c r="Z13" s="75"/>
+      <c r="AA13" s="75"/>
+      <c r="AB13" s="75"/>
+      <c r="AC13" s="75"/>
+      <c r="AD13" s="75"/>
+      <c r="AE13" s="75"/>
+      <c r="AF13" s="75"/>
+      <c r="AG13" s="75"/>
       <c r="AH13" s="68"/>
       <c r="AI13" s="68"/>
       <c r="AJ13" s="68"/>
       <c r="AK13" s="68"/>
       <c r="AL13" s="68"/>
       <c r="AM13" s="68"/>
-    </row>
-    <row r="14" spans="1:39" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="AN13" s="68"/>
+      <c r="AO13" s="68"/>
+      <c r="AP13" s="68"/>
+    </row>
+    <row r="14" spans="1:42" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="38">
+  <mergeCells count="41">
+    <mergeCell ref="AN3:AP3"/>
+    <mergeCell ref="AN4:AP4"/>
+    <mergeCell ref="AN5:AP5"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="Y3:AA3"/>
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="Y6:AA13"/>
+    <mergeCell ref="AB6:AD13"/>
+    <mergeCell ref="AE6:AG13"/>
+    <mergeCell ref="A10:A13"/>
     <mergeCell ref="AK3:AM3"/>
     <mergeCell ref="AK4:AM4"/>
     <mergeCell ref="AK5:AM5"/>
@@ -3666,37 +4075,12 @@
     <mergeCell ref="AB5:AD5"/>
     <mergeCell ref="AE5:AG5"/>
     <mergeCell ref="AH5:AJ5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="Y6:AA13"/>
-    <mergeCell ref="AB6:AD13"/>
-    <mergeCell ref="AE6:AG13"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="V5:X5"/>
     <mergeCell ref="AE3:AG3"/>
     <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="V4:X4"/>
     <mergeCell ref="Y4:AA4"/>
     <mergeCell ref="AB4:AD4"/>
     <mergeCell ref="AE4:AG4"/>
     <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="Y3:AA3"/>
-    <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixes #58. Tests were done on reference model commit d438e3d75719aabef468185fea1e63df635387cb on Trisotech BPMN Web Modeler 4.1.1.
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="631"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="80">
   <si>
     <t>Note: Tools that are not listed here have either not been tested or may not support both BPMN import and export.</t>
   </si>
@@ -115,9 +115,6 @@
     <t>6.3442.15675</t>
   </si>
   <si>
-    <t>4.1</t>
-  </si>
-  <si>
     <t>5.1 UL5 (mfb_bpmn_1.1)</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
   </si>
   <si>
     <t>Date of Test -&gt;</t>
-  </si>
-  <si>
-    <t>10-06-2013</t>
   </si>
   <si>
     <t>A</t>
@@ -351,6 +345,9 @@
   </si>
   <si>
     <t>Signavio Process Editor 7.1.0</t>
+  </si>
+  <si>
+    <t>4.1.1</t>
   </si>
 </sst>
 </file>
@@ -570,7 +567,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -734,12 +731,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -749,44 +773,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1163,8 +1154,8 @@
   </sheetPr>
   <dimension ref="A1:AMK15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AB1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AJ12" sqref="AJ12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1187,18 +1178,18 @@
       </c>
     </row>
     <row r="2" spans="1:54" ht="47.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71" t="s">
+      <c r="B2" s="61"/>
+      <c r="C2" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71" t="s">
+      <c r="D2" s="61"/>
+      <c r="E2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="71"/>
+      <c r="F2" s="61"/>
       <c r="G2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1356,79 +1347,79 @@
       <c r="I3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="72" t="s">
+      <c r="J3" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="73" t="s">
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
-      <c r="P3" s="66" t="s">
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="66"/>
-      <c r="R3" s="66"/>
-      <c r="S3" s="66" t="s">
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="T3" s="66"/>
-      <c r="U3" s="66"/>
-      <c r="V3" s="66" t="s">
+      <c r="T3" s="58"/>
+      <c r="U3" s="58"/>
+      <c r="V3" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="W3" s="66"/>
-      <c r="X3" s="66"/>
-      <c r="Y3" s="66" t="s">
+      <c r="W3" s="58"/>
+      <c r="X3" s="58"/>
+      <c r="Y3" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="Z3" s="66"/>
-      <c r="AA3" s="66"/>
-      <c r="AB3" s="66" t="s">
+      <c r="Z3" s="58"/>
+      <c r="AA3" s="58"/>
+      <c r="AB3" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="AC3" s="66"/>
-      <c r="AD3" s="66"/>
-      <c r="AE3" s="66" t="s">
+      <c r="AC3" s="58"/>
+      <c r="AD3" s="58"/>
+      <c r="AE3" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="AF3" s="66"/>
-      <c r="AG3" s="66"/>
-      <c r="AH3" s="66" t="s">
+      <c r="AF3" s="58"/>
+      <c r="AG3" s="58"/>
+      <c r="AH3" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="AI3" s="66"/>
-      <c r="AJ3" s="66"/>
-      <c r="AK3" s="70" t="s">
+      <c r="AI3" s="58"/>
+      <c r="AJ3" s="58"/>
+      <c r="AK3" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="AL3" s="70"/>
-      <c r="AM3" s="70"/>
-      <c r="AN3" s="66" t="s">
+      <c r="AL3" s="64"/>
+      <c r="AM3" s="64"/>
+      <c r="AN3" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="AO3" s="66"/>
-      <c r="AP3" s="66"/>
-      <c r="AQ3" s="66" t="s">
+      <c r="AO3" s="58"/>
+      <c r="AP3" s="58"/>
+      <c r="AQ3" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="AR3" s="66"/>
-      <c r="AS3" s="66"/>
-      <c r="AT3" s="66" t="s">
+      <c r="AR3" s="58"/>
+      <c r="AS3" s="58"/>
+      <c r="AT3" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="AU3" s="66"/>
-      <c r="AV3" s="66"/>
-      <c r="AW3" s="66" t="s">
-        <v>75</v>
-      </c>
-      <c r="AX3" s="66"/>
-      <c r="AY3" s="66"/>
-      <c r="AZ3" s="66"/>
-      <c r="BA3" s="66"/>
-      <c r="BB3" s="66"/>
+      <c r="AU3" s="58"/>
+      <c r="AV3" s="58"/>
+      <c r="AW3" s="58" t="s">
+        <v>73</v>
+      </c>
+      <c r="AX3" s="58"/>
+      <c r="AY3" s="58"/>
+      <c r="AZ3" s="58"/>
+      <c r="BA3" s="58"/>
+      <c r="BB3" s="58"/>
     </row>
     <row r="4" spans="1:54" s="15" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
@@ -1442,79 +1433,79 @@
       <c r="I4" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="67" t="s">
+      <c r="J4" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
-      <c r="M4" s="68" t="s">
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="68"/>
-      <c r="O4" s="68"/>
-      <c r="P4" s="68" t="s">
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="Q4" s="68"/>
-      <c r="R4" s="68"/>
-      <c r="S4" s="68" t="s">
+      <c r="Q4" s="59"/>
+      <c r="R4" s="59"/>
+      <c r="S4" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="T4" s="68"/>
-      <c r="U4" s="68"/>
-      <c r="V4" s="69" t="s">
+      <c r="T4" s="59"/>
+      <c r="U4" s="59"/>
+      <c r="V4" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="W4" s="69"/>
-      <c r="X4" s="69"/>
-      <c r="Y4" s="68" t="s">
+      <c r="W4" s="67"/>
+      <c r="X4" s="67"/>
+      <c r="Y4" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="Z4" s="68"/>
-      <c r="AA4" s="68"/>
-      <c r="AB4" s="68">
+      <c r="Z4" s="59"/>
+      <c r="AA4" s="59"/>
+      <c r="AB4" s="59">
         <v>2.4</v>
       </c>
-      <c r="AC4" s="68"/>
-      <c r="AD4" s="68"/>
-      <c r="AE4" s="68" t="s">
+      <c r="AC4" s="59"/>
+      <c r="AD4" s="59"/>
+      <c r="AE4" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="AF4" s="68"/>
-      <c r="AG4" s="68"/>
-      <c r="AH4" s="68" t="s">
+      <c r="AF4" s="59"/>
+      <c r="AG4" s="59"/>
+      <c r="AH4" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="AI4" s="68"/>
-      <c r="AJ4" s="68"/>
-      <c r="AK4" s="68" t="s">
+      <c r="AI4" s="59"/>
+      <c r="AJ4" s="59"/>
+      <c r="AK4" s="59" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL4" s="59"/>
+      <c r="AM4" s="59"/>
+      <c r="AN4" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="AL4" s="68"/>
-      <c r="AM4" s="68"/>
-      <c r="AN4" s="68" t="s">
+      <c r="AO4" s="59"/>
+      <c r="AP4" s="59"/>
+      <c r="AQ4" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="AO4" s="68"/>
-      <c r="AP4" s="68"/>
-      <c r="AQ4" s="68" t="s">
+      <c r="AR4" s="59"/>
+      <c r="AS4" s="59"/>
+      <c r="AT4" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="AR4" s="68"/>
-      <c r="AS4" s="68"/>
-      <c r="AT4" s="68" t="s">
-        <v>36</v>
-      </c>
-      <c r="AU4" s="68"/>
-      <c r="AV4" s="68"/>
-      <c r="AW4" s="68" t="s">
-        <v>76</v>
-      </c>
-      <c r="AX4" s="68"/>
-      <c r="AY4" s="68"/>
-      <c r="AZ4" s="68"/>
-      <c r="BA4" s="68"/>
-      <c r="BB4" s="68"/>
+      <c r="AU4" s="59"/>
+      <c r="AV4" s="59"/>
+      <c r="AW4" s="59" t="s">
+        <v>74</v>
+      </c>
+      <c r="AX4" s="59"/>
+      <c r="AY4" s="59"/>
+      <c r="AZ4" s="59"/>
+      <c r="BA4" s="59"/>
+      <c r="BB4" s="59"/>
     </row>
     <row r="5" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
@@ -1526,23 +1517,23 @@
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
       <c r="I5" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" s="63">
+        <v>36</v>
+      </c>
+      <c r="J5" s="71">
         <v>41380</v>
       </c>
-      <c r="K5" s="63"/>
-      <c r="L5" s="63"/>
-      <c r="M5" s="64">
+      <c r="K5" s="71"/>
+      <c r="L5" s="71"/>
+      <c r="M5" s="72">
         <v>41373</v>
       </c>
-      <c r="N5" s="64"/>
-      <c r="O5" s="64"/>
-      <c r="P5" s="58">
+      <c r="N5" s="72"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="60">
         <v>41396</v>
       </c>
-      <c r="Q5" s="58"/>
-      <c r="R5" s="58"/>
+      <c r="Q5" s="60"/>
+      <c r="R5" s="60"/>
       <c r="S5" s="65">
         <v>41383</v>
       </c>
@@ -1553,184 +1544,184 @@
       </c>
       <c r="W5" s="65"/>
       <c r="X5" s="65"/>
-      <c r="Y5" s="58">
+      <c r="Y5" s="60">
         <v>41394</v>
       </c>
-      <c r="Z5" s="58"/>
-      <c r="AA5" s="58"/>
-      <c r="AB5" s="58">
+      <c r="Z5" s="60"/>
+      <c r="AA5" s="60"/>
+      <c r="AB5" s="60">
         <v>41388</v>
       </c>
-      <c r="AC5" s="58"/>
-      <c r="AD5" s="58"/>
-      <c r="AE5" s="58">
+      <c r="AC5" s="60"/>
+      <c r="AD5" s="60"/>
+      <c r="AE5" s="60">
         <v>41388</v>
       </c>
-      <c r="AF5" s="58"/>
-      <c r="AG5" s="58"/>
-      <c r="AH5" s="58">
+      <c r="AF5" s="60"/>
+      <c r="AG5" s="60"/>
+      <c r="AH5" s="60">
         <v>41431</v>
       </c>
-      <c r="AI5" s="58"/>
-      <c r="AJ5" s="58"/>
-      <c r="AK5" s="62">
-        <v>41429</v>
-      </c>
-      <c r="AL5" s="62"/>
-      <c r="AM5" s="62"/>
-      <c r="AN5" s="57" t="s">
-        <v>38</v>
-      </c>
-      <c r="AO5" s="57"/>
-      <c r="AP5" s="57"/>
-      <c r="AQ5" s="58">
+      <c r="AI5" s="60"/>
+      <c r="AJ5" s="60"/>
+      <c r="AK5" s="60">
+        <v>41467</v>
+      </c>
+      <c r="AL5" s="60"/>
+      <c r="AM5" s="60"/>
+      <c r="AN5" s="60">
+        <v>41435</v>
+      </c>
+      <c r="AO5" s="60"/>
+      <c r="AP5" s="60"/>
+      <c r="AQ5" s="60">
         <v>41449</v>
       </c>
-      <c r="AR5" s="58"/>
-      <c r="AS5" s="58"/>
-      <c r="AT5" s="58">
+      <c r="AR5" s="60"/>
+      <c r="AS5" s="60"/>
+      <c r="AT5" s="60">
         <v>41444</v>
       </c>
-      <c r="AU5" s="58"/>
-      <c r="AV5" s="58"/>
-      <c r="AW5" s="58">
+      <c r="AU5" s="60"/>
+      <c r="AV5" s="60"/>
+      <c r="AW5" s="60">
         <v>41465</v>
       </c>
-      <c r="AX5" s="58"/>
-      <c r="AY5" s="58"/>
-      <c r="AZ5" s="58"/>
-      <c r="BA5" s="58"/>
-      <c r="BB5" s="58"/>
+      <c r="AX5" s="60"/>
+      <c r="AY5" s="60"/>
+      <c r="AZ5" s="60"/>
+      <c r="BA5" s="60"/>
+      <c r="BB5" s="60"/>
     </row>
     <row r="6" spans="1:54" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="59" t="s">
-        <v>39</v>
+      <c r="A6" s="68" t="s">
+        <v>37</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" s="20">
         <v>1</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E6" s="22">
         <v>0</v>
       </c>
       <c r="F6" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="I6" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6" s="26" t="s">
-        <v>45</v>
-      </c>
       <c r="J6" s="27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M6" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="N6" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O6" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P6" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q6" s="24"/>
       <c r="R6" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="S6" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="T6" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="U6" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="V6" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="W6" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="X6" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y6" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z6" s="69"/>
+      <c r="AA6" s="69"/>
+      <c r="AB6" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC6" s="69"/>
+      <c r="AD6" s="69"/>
+      <c r="AE6" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="S6" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="T6" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="U6" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="V6" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="W6" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="X6" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y6" s="60" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z6" s="60"/>
-      <c r="AA6" s="60"/>
-      <c r="AB6" s="60" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC6" s="60"/>
-      <c r="AD6" s="60"/>
-      <c r="AE6" s="60" t="s">
-        <v>49</v>
-      </c>
-      <c r="AF6" s="60"/>
-      <c r="AG6" s="60"/>
+      <c r="AF6" s="69"/>
+      <c r="AG6" s="69"/>
       <c r="AH6" s="27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AI6" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AJ6" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AK6" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AL6" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AM6" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AN6" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AO6" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AP6" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AQ6" s="27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AR6" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AS6" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AT6" s="27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AU6" s="24"/>
       <c r="AV6" s="24"/>
       <c r="AW6" s="27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AX6" s="24"/>
       <c r="AY6" s="24"/>
@@ -1739,126 +1730,126 @@
       <c r="BB6" s="24"/>
     </row>
     <row r="7" spans="1:54" ht="42.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="59"/>
+      <c r="A7" s="68"/>
       <c r="B7" s="30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C7" s="20">
         <v>2</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E7" s="22">
         <v>0</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H7" s="31" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I7" s="26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J7" s="27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K7" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M7" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="N7" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O7" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P7" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q7" s="24"/>
       <c r="R7" s="22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="S7" s="28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="T7" s="28" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="U7" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="V7" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="W7" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="X7" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y7" s="60"/>
-      <c r="Z7" s="60"/>
-      <c r="AA7" s="60"/>
-      <c r="AB7" s="60"/>
-      <c r="AC7" s="60"/>
-      <c r="AD7" s="60"/>
-      <c r="AE7" s="60"/>
-      <c r="AF7" s="60"/>
-      <c r="AG7" s="60"/>
+        <v>45</v>
+      </c>
+      <c r="Y7" s="69"/>
+      <c r="Z7" s="69"/>
+      <c r="AA7" s="69"/>
+      <c r="AB7" s="69"/>
+      <c r="AC7" s="69"/>
+      <c r="AD7" s="69"/>
+      <c r="AE7" s="69"/>
+      <c r="AF7" s="69"/>
+      <c r="AG7" s="69"/>
       <c r="AH7" s="27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AI7" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AJ7" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AK7" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AL7" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AM7" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AN7" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AO7" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AP7" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AQ7" s="27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AR7" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AS7" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AT7" s="27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AU7" s="24"/>
       <c r="AV7" s="24"/>
       <c r="AW7" s="27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AX7" s="24"/>
       <c r="AY7" s="24"/>
@@ -1867,124 +1858,124 @@
       <c r="BB7" s="24"/>
     </row>
     <row r="8" spans="1:54" ht="43.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="59"/>
+      <c r="A8" s="68"/>
       <c r="B8" s="30"/>
       <c r="C8" s="20">
         <v>3</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E8" s="22">
         <v>0</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I8" s="26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J8" s="32" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L8" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M8" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="N8" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O8" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P8" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="Q8" s="24"/>
       <c r="R8" s="22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="S8" s="34" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="T8" s="34" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="U8" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="V8" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="W8" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="X8" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y8" s="60"/>
-      <c r="Z8" s="60"/>
-      <c r="AA8" s="60"/>
-      <c r="AB8" s="60"/>
-      <c r="AC8" s="60"/>
-      <c r="AD8" s="60"/>
-      <c r="AE8" s="60"/>
-      <c r="AF8" s="60"/>
-      <c r="AG8" s="60"/>
+        <v>45</v>
+      </c>
+      <c r="Y8" s="69"/>
+      <c r="Z8" s="69"/>
+      <c r="AA8" s="69"/>
+      <c r="AB8" s="69"/>
+      <c r="AC8" s="69"/>
+      <c r="AD8" s="69"/>
+      <c r="AE8" s="69"/>
+      <c r="AF8" s="69"/>
+      <c r="AG8" s="69"/>
       <c r="AH8" s="27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AI8" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AJ8" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AK8" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AL8" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AM8" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AN8" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AO8" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AP8" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AQ8" s="27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AR8" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AS8" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AT8" s="27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AU8" s="24"/>
       <c r="AV8" s="24"/>
       <c r="AW8" s="27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AX8" s="24"/>
       <c r="AY8" s="24"/>
@@ -1993,124 +1984,124 @@
       <c r="BB8" s="24"/>
     </row>
     <row r="9" spans="1:54" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="59"/>
+      <c r="A9" s="68"/>
       <c r="B9" s="30"/>
       <c r="C9" s="20">
         <v>4</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E9" s="22">
         <v>0</v>
       </c>
       <c r="F9" s="56" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" s="74" t="s">
-        <v>59</v>
+        <v>56</v>
+      </c>
+      <c r="H9" s="57" t="s">
+        <v>57</v>
       </c>
       <c r="I9" s="26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J9" s="39" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L9" s="40" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M9" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N9" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O9" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P9" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="Q9" s="20"/>
       <c r="R9" s="41" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="S9" s="42" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="T9" s="43" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="U9" s="44" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="V9" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="W9" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="X9" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y9" s="60"/>
-      <c r="Z9" s="60"/>
-      <c r="AA9" s="60"/>
-      <c r="AB9" s="60"/>
-      <c r="AC9" s="60"/>
-      <c r="AD9" s="60"/>
-      <c r="AE9" s="60"/>
-      <c r="AF9" s="60"/>
-      <c r="AG9" s="60"/>
+        <v>45</v>
+      </c>
+      <c r="Y9" s="69"/>
+      <c r="Z9" s="69"/>
+      <c r="AA9" s="69"/>
+      <c r="AB9" s="69"/>
+      <c r="AC9" s="69"/>
+      <c r="AD9" s="69"/>
+      <c r="AE9" s="69"/>
+      <c r="AF9" s="69"/>
+      <c r="AG9" s="69"/>
       <c r="AH9" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AI9" s="20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AJ9" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AK9" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AL9" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AM9" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AN9" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AO9" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AP9" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AQ9" s="45" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AR9" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AS9" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AT9" s="27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AU9" s="20"/>
       <c r="AV9" s="24"/>
       <c r="AW9" s="27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AX9" s="20"/>
       <c r="AY9" s="24"/>
@@ -2125,22 +2116,22 @@
         <v>4</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E10" s="35">
         <v>1</v>
       </c>
       <c r="F10" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="37" t="s">
+      <c r="I10" s="26" t="s">
         <v>78</v>
-      </c>
-      <c r="H10" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="I10" s="26" t="s">
-        <v>80</v>
       </c>
       <c r="J10" s="39"/>
       <c r="K10" s="20"/>
@@ -2149,11 +2140,11 @@
       <c r="N10" s="20"/>
       <c r="O10" s="21"/>
       <c r="P10" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="Q10" s="20"/>
       <c r="R10" s="41" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="S10" s="42"/>
       <c r="T10" s="43"/>
@@ -2161,15 +2152,15 @@
       <c r="V10" s="21"/>
       <c r="W10" s="21"/>
       <c r="X10" s="21"/>
-      <c r="Y10" s="60"/>
-      <c r="Z10" s="60"/>
-      <c r="AA10" s="60"/>
-      <c r="AB10" s="60"/>
-      <c r="AC10" s="60"/>
-      <c r="AD10" s="60"/>
-      <c r="AE10" s="60"/>
-      <c r="AF10" s="60"/>
-      <c r="AG10" s="60"/>
+      <c r="Y10" s="69"/>
+      <c r="Z10" s="69"/>
+      <c r="AA10" s="69"/>
+      <c r="AB10" s="69"/>
+      <c r="AC10" s="69"/>
+      <c r="AD10" s="69"/>
+      <c r="AE10" s="69"/>
+      <c r="AF10" s="69"/>
+      <c r="AG10" s="69"/>
       <c r="AH10" s="24"/>
       <c r="AI10" s="20"/>
       <c r="AJ10" s="24"/>
@@ -2186,7 +2177,7 @@
       <c r="AU10" s="20"/>
       <c r="AV10" s="24"/>
       <c r="AW10" s="27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AX10" s="20"/>
       <c r="AY10" s="24"/>
@@ -2195,116 +2186,116 @@
       <c r="BB10" s="24"/>
     </row>
     <row r="11" spans="1:54" s="47" customFormat="1" ht="58.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="61" t="s">
-        <v>60</v>
+      <c r="A11" s="70" t="s">
+        <v>58</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C11" s="24">
         <v>1</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E11" s="24">
         <v>0</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H11" s="46" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I11" s="26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K11" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L11" s="24"/>
       <c r="M11" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N11" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O11" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P11" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="Q11" s="24"/>
       <c r="R11" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="S11" s="24"/>
       <c r="T11" s="24"/>
       <c r="U11" s="24"/>
       <c r="V11" s="23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="W11" s="23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="X11" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y11" s="60"/>
-      <c r="Z11" s="60"/>
-      <c r="AA11" s="60"/>
-      <c r="AB11" s="60"/>
-      <c r="AC11" s="60"/>
-      <c r="AD11" s="60"/>
-      <c r="AE11" s="60"/>
-      <c r="AF11" s="60"/>
-      <c r="AG11" s="60"/>
+        <v>44</v>
+      </c>
+      <c r="Y11" s="69"/>
+      <c r="Z11" s="69"/>
+      <c r="AA11" s="69"/>
+      <c r="AB11" s="69"/>
+      <c r="AC11" s="69"/>
+      <c r="AD11" s="69"/>
+      <c r="AE11" s="69"/>
+      <c r="AF11" s="69"/>
+      <c r="AG11" s="69"/>
       <c r="AH11" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AI11" s="24"/>
       <c r="AJ11" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AK11" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AL11" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AM11" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AN11" s="23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AO11" s="23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AP11" s="23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AQ11" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AR11" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AS11" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AT11" s="24"/>
       <c r="AU11" s="24"/>
       <c r="AV11" s="24"/>
       <c r="AW11" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AX11" s="24"/>
       <c r="AY11" s="24"/>
@@ -2313,110 +2304,110 @@
       <c r="BB11" s="24"/>
     </row>
     <row r="12" spans="1:54" ht="58.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="61"/>
+      <c r="A12" s="70"/>
       <c r="B12" s="30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C12" s="24">
         <v>2</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E12" s="24">
         <v>0</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H12" s="46" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I12" s="26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J12" s="24"/>
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N12" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O12" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P12" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="Q12" s="24"/>
       <c r="R12" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="S12" s="24"/>
       <c r="T12" s="24"/>
       <c r="U12" s="24"/>
       <c r="V12" s="23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="W12" s="23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="X12" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y12" s="60"/>
-      <c r="Z12" s="60"/>
-      <c r="AA12" s="60"/>
-      <c r="AB12" s="60"/>
-      <c r="AC12" s="60"/>
-      <c r="AD12" s="60"/>
-      <c r="AE12" s="60"/>
-      <c r="AF12" s="60"/>
-      <c r="AG12" s="60"/>
+        <v>44</v>
+      </c>
+      <c r="Y12" s="69"/>
+      <c r="Z12" s="69"/>
+      <c r="AA12" s="69"/>
+      <c r="AB12" s="69"/>
+      <c r="AC12" s="69"/>
+      <c r="AD12" s="69"/>
+      <c r="AE12" s="69"/>
+      <c r="AF12" s="69"/>
+      <c r="AG12" s="69"/>
       <c r="AH12" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AI12" s="24"/>
       <c r="AJ12" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AK12" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AL12" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AM12" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AN12" s="23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AO12" s="23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AP12" s="23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AQ12" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AR12" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AS12" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AT12" s="24"/>
       <c r="AU12" s="24"/>
       <c r="AV12" s="24"/>
       <c r="AW12" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AX12" s="24"/>
       <c r="AY12" s="24"/>
@@ -2425,28 +2416,28 @@
       <c r="BB12" s="24"/>
     </row>
     <row r="13" spans="1:54" ht="63" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="61"/>
+      <c r="A13" s="70"/>
       <c r="B13" s="30"/>
       <c r="C13" s="48">
         <v>3</v>
       </c>
       <c r="D13" s="49" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E13" s="50">
         <v>0</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G13" s="51" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H13" s="31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I13" s="26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J13" s="24"/>
       <c r="K13" s="24"/>
@@ -2463,15 +2454,15 @@
       <c r="V13" s="24"/>
       <c r="W13" s="24"/>
       <c r="X13" s="24"/>
-      <c r="Y13" s="60"/>
-      <c r="Z13" s="60"/>
-      <c r="AA13" s="60"/>
-      <c r="AB13" s="60"/>
-      <c r="AC13" s="60"/>
-      <c r="AD13" s="60"/>
-      <c r="AE13" s="60"/>
-      <c r="AF13" s="60"/>
-      <c r="AG13" s="60"/>
+      <c r="Y13" s="69"/>
+      <c r="Z13" s="69"/>
+      <c r="AA13" s="69"/>
+      <c r="AB13" s="69"/>
+      <c r="AC13" s="69"/>
+      <c r="AD13" s="69"/>
+      <c r="AE13" s="69"/>
+      <c r="AF13" s="69"/>
+      <c r="AG13" s="69"/>
       <c r="AH13" s="24"/>
       <c r="AI13" s="24"/>
       <c r="AJ13" s="24"/>
@@ -2495,28 +2486,28 @@
       <c r="BB13" s="24"/>
     </row>
     <row r="14" spans="1:54" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="61"/>
+      <c r="A14" s="70"/>
       <c r="B14" s="52"/>
       <c r="C14" s="51">
         <v>4</v>
       </c>
       <c r="D14" s="49" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E14" s="50">
         <v>0</v>
       </c>
       <c r="F14" s="49" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G14" s="51" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H14" s="53" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I14" s="26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J14" s="54"/>
       <c r="K14" s="54"/>
@@ -2533,15 +2524,15 @@
       <c r="V14" s="54"/>
       <c r="W14" s="54"/>
       <c r="X14" s="54"/>
-      <c r="Y14" s="60"/>
-      <c r="Z14" s="60"/>
-      <c r="AA14" s="60"/>
-      <c r="AB14" s="60"/>
-      <c r="AC14" s="60"/>
-      <c r="AD14" s="60"/>
-      <c r="AE14" s="60"/>
-      <c r="AF14" s="60"/>
-      <c r="AG14" s="60"/>
+      <c r="Y14" s="69"/>
+      <c r="Z14" s="69"/>
+      <c r="AA14" s="69"/>
+      <c r="AB14" s="69"/>
+      <c r="AC14" s="69"/>
+      <c r="AD14" s="69"/>
+      <c r="AE14" s="69"/>
+      <c r="AF14" s="69"/>
+      <c r="AG14" s="69"/>
       <c r="AH14" s="54"/>
       <c r="AI14" s="54"/>
       <c r="AJ14" s="54"/>
@@ -2567,27 +2558,22 @@
     <row r="15" spans="1:54" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="AW3:AY3"/>
-    <mergeCell ref="AW4:AY4"/>
-    <mergeCell ref="AW5:AY5"/>
-    <mergeCell ref="AZ3:BB3"/>
-    <mergeCell ref="AZ4:BB4"/>
-    <mergeCell ref="AZ5:BB5"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="Y3:AA3"/>
-    <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="AK3:AM3"/>
-    <mergeCell ref="AN3:AP3"/>
-    <mergeCell ref="AQ3:AS3"/>
+    <mergeCell ref="AN5:AP5"/>
+    <mergeCell ref="AQ5:AS5"/>
+    <mergeCell ref="AT5:AV5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="Y6:AA14"/>
+    <mergeCell ref="AB6:AD14"/>
+    <mergeCell ref="AE6:AG14"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="Y5:AA5"/>
+    <mergeCell ref="AB5:AD5"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AK5:AM5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="P5:R5"/>
     <mergeCell ref="S5:U5"/>
     <mergeCell ref="V5:X5"/>
     <mergeCell ref="AT3:AV3"/>
@@ -2604,24 +2590,29 @@
     <mergeCell ref="AN4:AP4"/>
     <mergeCell ref="AQ4:AS4"/>
     <mergeCell ref="AT4:AV4"/>
-    <mergeCell ref="AN5:AP5"/>
-    <mergeCell ref="AQ5:AS5"/>
-    <mergeCell ref="AT5:AV5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="Y6:AA14"/>
-    <mergeCell ref="AB6:AD14"/>
-    <mergeCell ref="AE6:AG14"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="Y5:AA5"/>
-    <mergeCell ref="AB5:AD5"/>
-    <mergeCell ref="AE5:AG5"/>
-    <mergeCell ref="AH5:AJ5"/>
-    <mergeCell ref="AK5:AM5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="AH3:AJ3"/>
+    <mergeCell ref="AK3:AM3"/>
+    <mergeCell ref="AN3:AP3"/>
+    <mergeCell ref="AQ3:AS3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="Y3:AA3"/>
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="AW3:AY3"/>
+    <mergeCell ref="AW4:AY4"/>
+    <mergeCell ref="AW5:AY5"/>
+    <mergeCell ref="AZ3:BB3"/>
+    <mergeCell ref="AZ4:BB4"/>
+    <mergeCell ref="AZ5:BB5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added export test results for YaoQiang 2.2.2 part 2, updated Excel sheet
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\MIWG\bpmn-miwg-test-suite-fork\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="631"/>
   </bookViews>
@@ -734,14 +739,41 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -750,33 +782,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -858,6 +863,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -905,7 +913,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -940,7 +948,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1154,8 +1162,8 @@
   </sheetPr>
   <dimension ref="A1:AMK15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AB1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AJ12" sqref="AJ12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,18 +1186,18 @@
       </c>
     </row>
     <row r="2" spans="1:54" ht="47.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61" t="s">
+      <c r="B2" s="70"/>
+      <c r="C2" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61" t="s">
+      <c r="D2" s="70"/>
+      <c r="E2" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="61"/>
+      <c r="F2" s="70"/>
       <c r="G2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1347,79 +1355,79 @@
       <c r="I3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="62" t="s">
+      <c r="J3" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="63" t="s">
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="58" t="s">
+      <c r="N3" s="72"/>
+      <c r="O3" s="72"/>
+      <c r="P3" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="58"/>
-      <c r="S3" s="58" t="s">
+      <c r="Q3" s="65"/>
+      <c r="R3" s="65"/>
+      <c r="S3" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="T3" s="58"/>
-      <c r="U3" s="58"/>
-      <c r="V3" s="58" t="s">
+      <c r="T3" s="65"/>
+      <c r="U3" s="65"/>
+      <c r="V3" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="W3" s="58"/>
-      <c r="X3" s="58"/>
-      <c r="Y3" s="58" t="s">
+      <c r="W3" s="65"/>
+      <c r="X3" s="65"/>
+      <c r="Y3" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="Z3" s="58"/>
-      <c r="AA3" s="58"/>
-      <c r="AB3" s="58" t="s">
+      <c r="Z3" s="65"/>
+      <c r="AA3" s="65"/>
+      <c r="AB3" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="AC3" s="58"/>
-      <c r="AD3" s="58"/>
-      <c r="AE3" s="58" t="s">
+      <c r="AC3" s="65"/>
+      <c r="AD3" s="65"/>
+      <c r="AE3" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="AF3" s="58"/>
-      <c r="AG3" s="58"/>
-      <c r="AH3" s="58" t="s">
+      <c r="AF3" s="65"/>
+      <c r="AG3" s="65"/>
+      <c r="AH3" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="AI3" s="58"/>
-      <c r="AJ3" s="58"/>
-      <c r="AK3" s="64" t="s">
+      <c r="AI3" s="65"/>
+      <c r="AJ3" s="65"/>
+      <c r="AK3" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="AL3" s="64"/>
-      <c r="AM3" s="64"/>
-      <c r="AN3" s="58" t="s">
+      <c r="AL3" s="69"/>
+      <c r="AM3" s="69"/>
+      <c r="AN3" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="AO3" s="58"/>
-      <c r="AP3" s="58"/>
-      <c r="AQ3" s="58" t="s">
+      <c r="AO3" s="65"/>
+      <c r="AP3" s="65"/>
+      <c r="AQ3" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="AR3" s="58"/>
-      <c r="AS3" s="58"/>
-      <c r="AT3" s="58" t="s">
+      <c r="AR3" s="65"/>
+      <c r="AS3" s="65"/>
+      <c r="AT3" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="AU3" s="58"/>
-      <c r="AV3" s="58"/>
-      <c r="AW3" s="58" t="s">
+      <c r="AU3" s="65"/>
+      <c r="AV3" s="65"/>
+      <c r="AW3" s="65" t="s">
         <v>73</v>
       </c>
-      <c r="AX3" s="58"/>
-      <c r="AY3" s="58"/>
-      <c r="AZ3" s="58"/>
-      <c r="BA3" s="58"/>
-      <c r="BB3" s="58"/>
+      <c r="AX3" s="65"/>
+      <c r="AY3" s="65"/>
+      <c r="AZ3" s="65"/>
+      <c r="BA3" s="65"/>
+      <c r="BB3" s="65"/>
     </row>
     <row r="4" spans="1:54" s="15" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
@@ -1438,74 +1446,74 @@
       </c>
       <c r="K4" s="66"/>
       <c r="L4" s="66"/>
-      <c r="M4" s="59" t="s">
+      <c r="M4" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="59"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="59" t="s">
+      <c r="N4" s="67"/>
+      <c r="O4" s="67"/>
+      <c r="P4" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="Q4" s="59"/>
-      <c r="R4" s="59"/>
-      <c r="S4" s="59" t="s">
+      <c r="Q4" s="67"/>
+      <c r="R4" s="67"/>
+      <c r="S4" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="T4" s="59"/>
-      <c r="U4" s="59"/>
-      <c r="V4" s="67" t="s">
+      <c r="T4" s="67"/>
+      <c r="U4" s="67"/>
+      <c r="V4" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="W4" s="67"/>
-      <c r="X4" s="67"/>
-      <c r="Y4" s="59" t="s">
+      <c r="W4" s="68"/>
+      <c r="X4" s="68"/>
+      <c r="Y4" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="Z4" s="59"/>
-      <c r="AA4" s="59"/>
-      <c r="AB4" s="59">
+      <c r="Z4" s="67"/>
+      <c r="AA4" s="67"/>
+      <c r="AB4" s="67">
         <v>2.4</v>
       </c>
-      <c r="AC4" s="59"/>
-      <c r="AD4" s="59"/>
-      <c r="AE4" s="59" t="s">
+      <c r="AC4" s="67"/>
+      <c r="AD4" s="67"/>
+      <c r="AE4" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="AF4" s="59"/>
-      <c r="AG4" s="59"/>
-      <c r="AH4" s="59" t="s">
+      <c r="AF4" s="67"/>
+      <c r="AG4" s="67"/>
+      <c r="AH4" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="AI4" s="59"/>
-      <c r="AJ4" s="59"/>
-      <c r="AK4" s="59" t="s">
+      <c r="AI4" s="67"/>
+      <c r="AJ4" s="67"/>
+      <c r="AK4" s="67" t="s">
         <v>79</v>
       </c>
-      <c r="AL4" s="59"/>
-      <c r="AM4" s="59"/>
-      <c r="AN4" s="59" t="s">
+      <c r="AL4" s="67"/>
+      <c r="AM4" s="67"/>
+      <c r="AN4" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="AO4" s="59"/>
-      <c r="AP4" s="59"/>
-      <c r="AQ4" s="59" t="s">
+      <c r="AO4" s="67"/>
+      <c r="AP4" s="67"/>
+      <c r="AQ4" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="AR4" s="59"/>
-      <c r="AS4" s="59"/>
-      <c r="AT4" s="59" t="s">
+      <c r="AR4" s="67"/>
+      <c r="AS4" s="67"/>
+      <c r="AT4" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="AU4" s="59"/>
-      <c r="AV4" s="59"/>
-      <c r="AW4" s="59" t="s">
+      <c r="AU4" s="67"/>
+      <c r="AV4" s="67"/>
+      <c r="AW4" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="AX4" s="59"/>
-      <c r="AY4" s="59"/>
-      <c r="AZ4" s="59"/>
-      <c r="BA4" s="59"/>
-      <c r="BB4" s="59"/>
+      <c r="AX4" s="67"/>
+      <c r="AY4" s="67"/>
+      <c r="AZ4" s="67"/>
+      <c r="BA4" s="67"/>
+      <c r="BB4" s="67"/>
     </row>
     <row r="5" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
@@ -1519,82 +1527,82 @@
       <c r="I5" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="71">
+      <c r="J5" s="62">
         <v>41380</v>
       </c>
-      <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="72">
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="63">
         <v>41373</v>
       </c>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
-      <c r="P5" s="60">
+      <c r="N5" s="63"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="58">
         <v>41396</v>
       </c>
-      <c r="Q5" s="60"/>
-      <c r="R5" s="60"/>
-      <c r="S5" s="65">
+      <c r="Q5" s="58"/>
+      <c r="R5" s="58"/>
+      <c r="S5" s="64">
         <v>41383</v>
       </c>
-      <c r="T5" s="65"/>
-      <c r="U5" s="65"/>
-      <c r="V5" s="65">
+      <c r="T5" s="64"/>
+      <c r="U5" s="64"/>
+      <c r="V5" s="64">
         <v>41410</v>
       </c>
-      <c r="W5" s="65"/>
-      <c r="X5" s="65"/>
-      <c r="Y5" s="60">
+      <c r="W5" s="64"/>
+      <c r="X5" s="64"/>
+      <c r="Y5" s="58">
         <v>41394</v>
       </c>
-      <c r="Z5" s="60"/>
-      <c r="AA5" s="60"/>
-      <c r="AB5" s="60">
+      <c r="Z5" s="58"/>
+      <c r="AA5" s="58"/>
+      <c r="AB5" s="58">
         <v>41388</v>
       </c>
-      <c r="AC5" s="60"/>
-      <c r="AD5" s="60"/>
-      <c r="AE5" s="60">
+      <c r="AC5" s="58"/>
+      <c r="AD5" s="58"/>
+      <c r="AE5" s="58">
         <v>41388</v>
       </c>
-      <c r="AF5" s="60"/>
-      <c r="AG5" s="60"/>
-      <c r="AH5" s="60">
+      <c r="AF5" s="58"/>
+      <c r="AG5" s="58"/>
+      <c r="AH5" s="58">
         <v>41431</v>
       </c>
-      <c r="AI5" s="60"/>
-      <c r="AJ5" s="60"/>
-      <c r="AK5" s="60">
+      <c r="AI5" s="58"/>
+      <c r="AJ5" s="58"/>
+      <c r="AK5" s="58">
         <v>41467</v>
       </c>
-      <c r="AL5" s="60"/>
-      <c r="AM5" s="60"/>
-      <c r="AN5" s="60">
+      <c r="AL5" s="58"/>
+      <c r="AM5" s="58"/>
+      <c r="AN5" s="58">
         <v>41435</v>
       </c>
-      <c r="AO5" s="60"/>
-      <c r="AP5" s="60"/>
-      <c r="AQ5" s="60">
+      <c r="AO5" s="58"/>
+      <c r="AP5" s="58"/>
+      <c r="AQ5" s="58">
         <v>41449</v>
       </c>
-      <c r="AR5" s="60"/>
-      <c r="AS5" s="60"/>
-      <c r="AT5" s="60">
+      <c r="AR5" s="58"/>
+      <c r="AS5" s="58"/>
+      <c r="AT5" s="58">
         <v>41444</v>
       </c>
-      <c r="AU5" s="60"/>
-      <c r="AV5" s="60"/>
-      <c r="AW5" s="60">
+      <c r="AU5" s="58"/>
+      <c r="AV5" s="58"/>
+      <c r="AW5" s="58">
         <v>41465</v>
       </c>
-      <c r="AX5" s="60"/>
-      <c r="AY5" s="60"/>
-      <c r="AZ5" s="60"/>
-      <c r="BA5" s="60"/>
-      <c r="BB5" s="60"/>
+      <c r="AX5" s="58"/>
+      <c r="AY5" s="58"/>
+      <c r="AZ5" s="58"/>
+      <c r="BA5" s="58"/>
+      <c r="BB5" s="58"/>
     </row>
     <row r="6" spans="1:54" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="59" t="s">
         <v>37</v>
       </c>
       <c r="B6" s="19" t="s">
@@ -1664,21 +1672,21 @@
       <c r="X6" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="Y6" s="69" t="s">
+      <c r="Y6" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="Z6" s="69"/>
-      <c r="AA6" s="69"/>
-      <c r="AB6" s="69" t="s">
+      <c r="Z6" s="60"/>
+      <c r="AA6" s="60"/>
+      <c r="AB6" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="AC6" s="69"/>
-      <c r="AD6" s="69"/>
-      <c r="AE6" s="69" t="s">
+      <c r="AC6" s="60"/>
+      <c r="AD6" s="60"/>
+      <c r="AE6" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="AF6" s="69"/>
-      <c r="AG6" s="69"/>
+      <c r="AF6" s="60"/>
+      <c r="AG6" s="60"/>
       <c r="AH6" s="27" t="s">
         <v>45</v>
       </c>
@@ -1730,7 +1738,7 @@
       <c r="BB6" s="24"/>
     </row>
     <row r="7" spans="1:54" ht="42.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="68"/>
+      <c r="A7" s="59"/>
       <c r="B7" s="30" t="s">
         <v>48</v>
       </c>
@@ -1798,15 +1806,15 @@
       <c r="X7" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="Y7" s="69"/>
-      <c r="Z7" s="69"/>
-      <c r="AA7" s="69"/>
-      <c r="AB7" s="69"/>
-      <c r="AC7" s="69"/>
-      <c r="AD7" s="69"/>
-      <c r="AE7" s="69"/>
-      <c r="AF7" s="69"/>
-      <c r="AG7" s="69"/>
+      <c r="Y7" s="60"/>
+      <c r="Z7" s="60"/>
+      <c r="AA7" s="60"/>
+      <c r="AB7" s="60"/>
+      <c r="AC7" s="60"/>
+      <c r="AD7" s="60"/>
+      <c r="AE7" s="60"/>
+      <c r="AF7" s="60"/>
+      <c r="AG7" s="60"/>
       <c r="AH7" s="27" t="s">
         <v>45</v>
       </c>
@@ -1858,7 +1866,7 @@
       <c r="BB7" s="24"/>
     </row>
     <row r="8" spans="1:54" ht="43.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="68"/>
+      <c r="A8" s="59"/>
       <c r="B8" s="30"/>
       <c r="C8" s="20">
         <v>3</v>
@@ -1924,15 +1932,15 @@
       <c r="X8" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="Y8" s="69"/>
-      <c r="Z8" s="69"/>
-      <c r="AA8" s="69"/>
-      <c r="AB8" s="69"/>
-      <c r="AC8" s="69"/>
-      <c r="AD8" s="69"/>
-      <c r="AE8" s="69"/>
-      <c r="AF8" s="69"/>
-      <c r="AG8" s="69"/>
+      <c r="Y8" s="60"/>
+      <c r="Z8" s="60"/>
+      <c r="AA8" s="60"/>
+      <c r="AB8" s="60"/>
+      <c r="AC8" s="60"/>
+      <c r="AD8" s="60"/>
+      <c r="AE8" s="60"/>
+      <c r="AF8" s="60"/>
+      <c r="AG8" s="60"/>
       <c r="AH8" s="27" t="s">
         <v>44</v>
       </c>
@@ -1984,7 +1992,7 @@
       <c r="BB8" s="24"/>
     </row>
     <row r="9" spans="1:54" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="68"/>
+      <c r="A9" s="59"/>
       <c r="B9" s="30"/>
       <c r="C9" s="20">
         <v>4</v>
@@ -2050,15 +2058,15 @@
       <c r="X9" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="Y9" s="69"/>
-      <c r="Z9" s="69"/>
-      <c r="AA9" s="69"/>
-      <c r="AB9" s="69"/>
-      <c r="AC9" s="69"/>
-      <c r="AD9" s="69"/>
-      <c r="AE9" s="69"/>
-      <c r="AF9" s="69"/>
-      <c r="AG9" s="69"/>
+      <c r="Y9" s="60"/>
+      <c r="Z9" s="60"/>
+      <c r="AA9" s="60"/>
+      <c r="AB9" s="60"/>
+      <c r="AC9" s="60"/>
+      <c r="AD9" s="60"/>
+      <c r="AE9" s="60"/>
+      <c r="AF9" s="60"/>
+      <c r="AG9" s="60"/>
       <c r="AH9" s="24" t="s">
         <v>44</v>
       </c>
@@ -2152,15 +2160,15 @@
       <c r="V10" s="21"/>
       <c r="W10" s="21"/>
       <c r="X10" s="21"/>
-      <c r="Y10" s="69"/>
-      <c r="Z10" s="69"/>
-      <c r="AA10" s="69"/>
-      <c r="AB10" s="69"/>
-      <c r="AC10" s="69"/>
-      <c r="AD10" s="69"/>
-      <c r="AE10" s="69"/>
-      <c r="AF10" s="69"/>
-      <c r="AG10" s="69"/>
+      <c r="Y10" s="60"/>
+      <c r="Z10" s="60"/>
+      <c r="AA10" s="60"/>
+      <c r="AB10" s="60"/>
+      <c r="AC10" s="60"/>
+      <c r="AD10" s="60"/>
+      <c r="AE10" s="60"/>
+      <c r="AF10" s="60"/>
+      <c r="AG10" s="60"/>
       <c r="AH10" s="24"/>
       <c r="AI10" s="20"/>
       <c r="AJ10" s="24"/>
@@ -2186,7 +2194,7 @@
       <c r="BB10" s="24"/>
     </row>
     <row r="11" spans="1:54" s="47" customFormat="1" ht="58.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="70" t="s">
+      <c r="A11" s="61" t="s">
         <v>58</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -2246,17 +2254,17 @@
         <v>44</v>
       </c>
       <c r="X11" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y11" s="69"/>
-      <c r="Z11" s="69"/>
-      <c r="AA11" s="69"/>
-      <c r="AB11" s="69"/>
-      <c r="AC11" s="69"/>
-      <c r="AD11" s="69"/>
-      <c r="AE11" s="69"/>
-      <c r="AF11" s="69"/>
-      <c r="AG11" s="69"/>
+        <v>45</v>
+      </c>
+      <c r="Y11" s="60"/>
+      <c r="Z11" s="60"/>
+      <c r="AA11" s="60"/>
+      <c r="AB11" s="60"/>
+      <c r="AC11" s="60"/>
+      <c r="AD11" s="60"/>
+      <c r="AE11" s="60"/>
+      <c r="AF11" s="60"/>
+      <c r="AG11" s="60"/>
       <c r="AH11" s="24" t="s">
         <v>44</v>
       </c>
@@ -2304,7 +2312,7 @@
       <c r="BB11" s="24"/>
     </row>
     <row r="12" spans="1:54" ht="58.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="70"/>
+      <c r="A12" s="61"/>
       <c r="B12" s="30" t="s">
         <v>63</v>
       </c>
@@ -2358,17 +2366,17 @@
         <v>44</v>
       </c>
       <c r="X12" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y12" s="69"/>
-      <c r="Z12" s="69"/>
-      <c r="AA12" s="69"/>
-      <c r="AB12" s="69"/>
-      <c r="AC12" s="69"/>
-      <c r="AD12" s="69"/>
-      <c r="AE12" s="69"/>
-      <c r="AF12" s="69"/>
-      <c r="AG12" s="69"/>
+        <v>45</v>
+      </c>
+      <c r="Y12" s="60"/>
+      <c r="Z12" s="60"/>
+      <c r="AA12" s="60"/>
+      <c r="AB12" s="60"/>
+      <c r="AC12" s="60"/>
+      <c r="AD12" s="60"/>
+      <c r="AE12" s="60"/>
+      <c r="AF12" s="60"/>
+      <c r="AG12" s="60"/>
       <c r="AH12" s="24" t="s">
         <v>44</v>
       </c>
@@ -2416,7 +2424,7 @@
       <c r="BB12" s="24"/>
     </row>
     <row r="13" spans="1:54" ht="63" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="70"/>
+      <c r="A13" s="61"/>
       <c r="B13" s="30"/>
       <c r="C13" s="48">
         <v>3</v>
@@ -2454,15 +2462,15 @@
       <c r="V13" s="24"/>
       <c r="W13" s="24"/>
       <c r="X13" s="24"/>
-      <c r="Y13" s="69"/>
-      <c r="Z13" s="69"/>
-      <c r="AA13" s="69"/>
-      <c r="AB13" s="69"/>
-      <c r="AC13" s="69"/>
-      <c r="AD13" s="69"/>
-      <c r="AE13" s="69"/>
-      <c r="AF13" s="69"/>
-      <c r="AG13" s="69"/>
+      <c r="Y13" s="60"/>
+      <c r="Z13" s="60"/>
+      <c r="AA13" s="60"/>
+      <c r="AB13" s="60"/>
+      <c r="AC13" s="60"/>
+      <c r="AD13" s="60"/>
+      <c r="AE13" s="60"/>
+      <c r="AF13" s="60"/>
+      <c r="AG13" s="60"/>
       <c r="AH13" s="24"/>
       <c r="AI13" s="24"/>
       <c r="AJ13" s="24"/>
@@ -2486,7 +2494,7 @@
       <c r="BB13" s="24"/>
     </row>
     <row r="14" spans="1:54" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="70"/>
+      <c r="A14" s="61"/>
       <c r="B14" s="52"/>
       <c r="C14" s="51">
         <v>4</v>
@@ -2524,15 +2532,15 @@
       <c r="V14" s="54"/>
       <c r="W14" s="54"/>
       <c r="X14" s="54"/>
-      <c r="Y14" s="69"/>
-      <c r="Z14" s="69"/>
-      <c r="AA14" s="69"/>
-      <c r="AB14" s="69"/>
-      <c r="AC14" s="69"/>
-      <c r="AD14" s="69"/>
-      <c r="AE14" s="69"/>
-      <c r="AF14" s="69"/>
-      <c r="AG14" s="69"/>
+      <c r="Y14" s="60"/>
+      <c r="Z14" s="60"/>
+      <c r="AA14" s="60"/>
+      <c r="AB14" s="60"/>
+      <c r="AC14" s="60"/>
+      <c r="AD14" s="60"/>
+      <c r="AE14" s="60"/>
+      <c r="AF14" s="60"/>
+      <c r="AG14" s="60"/>
       <c r="AH14" s="54"/>
       <c r="AI14" s="54"/>
       <c r="AJ14" s="54"/>
@@ -2558,6 +2566,43 @@
     <row r="15" spans="1:54" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="AW3:AY3"/>
+    <mergeCell ref="AW4:AY4"/>
+    <mergeCell ref="AW5:AY5"/>
+    <mergeCell ref="AZ3:BB3"/>
+    <mergeCell ref="AZ4:BB4"/>
+    <mergeCell ref="AZ5:BB5"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="Y3:AA3"/>
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="AH3:AJ3"/>
+    <mergeCell ref="AK3:AM3"/>
+    <mergeCell ref="AN3:AP3"/>
+    <mergeCell ref="AQ3:AS3"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="AT3:AV3"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="AB4:AD4"/>
+    <mergeCell ref="AE4:AG4"/>
+    <mergeCell ref="AH4:AJ4"/>
+    <mergeCell ref="AK4:AM4"/>
+    <mergeCell ref="AN4:AP4"/>
+    <mergeCell ref="AQ4:AS4"/>
+    <mergeCell ref="AT4:AV4"/>
     <mergeCell ref="AN5:AP5"/>
     <mergeCell ref="AQ5:AS5"/>
     <mergeCell ref="AT5:AV5"/>
@@ -2574,43 +2619,6 @@
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="M5:O5"/>
     <mergeCell ref="P5:R5"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="V5:X5"/>
-    <mergeCell ref="AT3:AV3"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="V4:X4"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="AB4:AD4"/>
-    <mergeCell ref="AE4:AG4"/>
-    <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="AK4:AM4"/>
-    <mergeCell ref="AN4:AP4"/>
-    <mergeCell ref="AQ4:AS4"/>
-    <mergeCell ref="AT4:AV4"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="AK3:AM3"/>
-    <mergeCell ref="AN3:AP3"/>
-    <mergeCell ref="AQ3:AS3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="Y3:AA3"/>
-    <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="AW3:AY3"/>
-    <mergeCell ref="AW4:AY4"/>
-    <mergeCell ref="AW5:AY5"/>
-    <mergeCell ref="AZ3:BB3"/>
-    <mergeCell ref="AZ4:BB4"/>
-    <mergeCell ref="AZ5:BB5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Yaoqiang 2.2.6 test results
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\MIWG\bpmn-miwg-test-suite-fork\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="631"/>
   </bookViews>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="81">
   <si>
     <t>Note: Tools that are not listed here have either not been tested or may not support both BPMN import and export.</t>
   </si>
@@ -106,9 +101,6 @@
   </si>
   <si>
     <t>8.0.1</t>
-  </si>
-  <si>
-    <t>2.1.33</t>
   </si>
   <si>
     <t>17.0.3 sp1</t>
@@ -354,15 +346,23 @@
   <si>
     <t>4.1.1</t>
   </si>
+  <si>
+    <t>2.2.6</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>OK</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -401,6 +401,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -739,8 +745,35 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -751,43 +784,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="TableStyleLight1" xfId="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -871,7 +877,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -913,7 +919,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -948,7 +954,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1162,8 +1168,8 @@
   </sheetPr>
   <dimension ref="A1:AMK15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="X13" sqref="X13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="V3" sqref="V3:X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1186,18 +1192,18 @@
       </c>
     </row>
     <row r="2" spans="1:54" ht="47.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70" t="s">
+      <c r="B2" s="61"/>
+      <c r="C2" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70" t="s">
+      <c r="D2" s="61"/>
+      <c r="E2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="70"/>
+      <c r="F2" s="61"/>
       <c r="G2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1355,79 +1361,79 @@
       <c r="I3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="71" t="s">
+      <c r="J3" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="72" t="s">
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="65" t="s">
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="65" t="s">
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="T3" s="65"/>
-      <c r="U3" s="65"/>
-      <c r="V3" s="65" t="s">
+      <c r="T3" s="58"/>
+      <c r="U3" s="58"/>
+      <c r="V3" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="W3" s="65"/>
-      <c r="X3" s="65"/>
-      <c r="Y3" s="65" t="s">
+      <c r="W3" s="58"/>
+      <c r="X3" s="58"/>
+      <c r="Y3" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="Z3" s="65"/>
-      <c r="AA3" s="65"/>
-      <c r="AB3" s="65" t="s">
+      <c r="Z3" s="58"/>
+      <c r="AA3" s="58"/>
+      <c r="AB3" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="AC3" s="65"/>
-      <c r="AD3" s="65"/>
-      <c r="AE3" s="65" t="s">
+      <c r="AC3" s="58"/>
+      <c r="AD3" s="58"/>
+      <c r="AE3" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="AF3" s="65"/>
-      <c r="AG3" s="65"/>
-      <c r="AH3" s="65" t="s">
+      <c r="AF3" s="58"/>
+      <c r="AG3" s="58"/>
+      <c r="AH3" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="AI3" s="65"/>
-      <c r="AJ3" s="65"/>
-      <c r="AK3" s="69" t="s">
+      <c r="AI3" s="58"/>
+      <c r="AJ3" s="58"/>
+      <c r="AK3" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="AL3" s="69"/>
-      <c r="AM3" s="69"/>
-      <c r="AN3" s="65" t="s">
+      <c r="AL3" s="64"/>
+      <c r="AM3" s="64"/>
+      <c r="AN3" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="AO3" s="65"/>
-      <c r="AP3" s="65"/>
-      <c r="AQ3" s="65" t="s">
+      <c r="AO3" s="58"/>
+      <c r="AP3" s="58"/>
+      <c r="AQ3" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="AR3" s="65"/>
-      <c r="AS3" s="65"/>
-      <c r="AT3" s="65" t="s">
+      <c r="AR3" s="58"/>
+      <c r="AS3" s="58"/>
+      <c r="AT3" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="AU3" s="65"/>
-      <c r="AV3" s="65"/>
-      <c r="AW3" s="65" t="s">
-        <v>73</v>
-      </c>
-      <c r="AX3" s="65"/>
-      <c r="AY3" s="65"/>
-      <c r="AZ3" s="65"/>
-      <c r="BA3" s="65"/>
-      <c r="BB3" s="65"/>
+      <c r="AU3" s="58"/>
+      <c r="AV3" s="58"/>
+      <c r="AW3" s="58" t="s">
+        <v>72</v>
+      </c>
+      <c r="AX3" s="58"/>
+      <c r="AY3" s="58"/>
+      <c r="AZ3" s="58"/>
+      <c r="BA3" s="58"/>
+      <c r="BB3" s="58"/>
     </row>
     <row r="4" spans="1:54" s="15" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
@@ -1446,74 +1452,74 @@
       </c>
       <c r="K4" s="66"/>
       <c r="L4" s="66"/>
-      <c r="M4" s="67" t="s">
+      <c r="M4" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="67"/>
-      <c r="O4" s="67"/>
-      <c r="P4" s="67" t="s">
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67" t="s">
+      <c r="Q4" s="59"/>
+      <c r="R4" s="59"/>
+      <c r="S4" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="T4" s="67"/>
-      <c r="U4" s="67"/>
-      <c r="V4" s="68" t="s">
+      <c r="T4" s="59"/>
+      <c r="U4" s="59"/>
+      <c r="V4" s="67" t="s">
+        <v>79</v>
+      </c>
+      <c r="W4" s="67"/>
+      <c r="X4" s="67"/>
+      <c r="Y4" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="W4" s="68"/>
-      <c r="X4" s="68"/>
-      <c r="Y4" s="67" t="s">
+      <c r="Z4" s="59"/>
+      <c r="AA4" s="59"/>
+      <c r="AB4" s="59">
+        <v>2.4</v>
+      </c>
+      <c r="AC4" s="59"/>
+      <c r="AD4" s="59"/>
+      <c r="AE4" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="Z4" s="67"/>
-      <c r="AA4" s="67"/>
-      <c r="AB4" s="67">
-        <v>2.4</v>
-      </c>
-      <c r="AC4" s="67"/>
-      <c r="AD4" s="67"/>
-      <c r="AE4" s="67" t="s">
+      <c r="AF4" s="59"/>
+      <c r="AG4" s="59"/>
+      <c r="AH4" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="AF4" s="67"/>
-      <c r="AG4" s="67"/>
-      <c r="AH4" s="67" t="s">
+      <c r="AI4" s="59"/>
+      <c r="AJ4" s="59"/>
+      <c r="AK4" s="59" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL4" s="59"/>
+      <c r="AM4" s="59"/>
+      <c r="AN4" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="AI4" s="67"/>
-      <c r="AJ4" s="67"/>
-      <c r="AK4" s="67" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL4" s="67"/>
-      <c r="AM4" s="67"/>
-      <c r="AN4" s="67" t="s">
+      <c r="AO4" s="59"/>
+      <c r="AP4" s="59"/>
+      <c r="AQ4" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="AO4" s="67"/>
-      <c r="AP4" s="67"/>
-      <c r="AQ4" s="67" t="s">
+      <c r="AR4" s="59"/>
+      <c r="AS4" s="59"/>
+      <c r="AT4" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="AR4" s="67"/>
-      <c r="AS4" s="67"/>
-      <c r="AT4" s="67" t="s">
-        <v>35</v>
-      </c>
-      <c r="AU4" s="67"/>
-      <c r="AV4" s="67"/>
-      <c r="AW4" s="67" t="s">
-        <v>74</v>
-      </c>
-      <c r="AX4" s="67"/>
-      <c r="AY4" s="67"/>
-      <c r="AZ4" s="67"/>
-      <c r="BA4" s="67"/>
-      <c r="BB4" s="67"/>
+      <c r="AU4" s="59"/>
+      <c r="AV4" s="59"/>
+      <c r="AW4" s="59" t="s">
+        <v>73</v>
+      </c>
+      <c r="AX4" s="59"/>
+      <c r="AY4" s="59"/>
+      <c r="AZ4" s="59"/>
+      <c r="BA4" s="59"/>
+      <c r="BB4" s="59"/>
     </row>
     <row r="5" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
@@ -1525,211 +1531,211 @@
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
       <c r="I5" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="62">
+        <v>35</v>
+      </c>
+      <c r="J5" s="71">
         <v>41380</v>
       </c>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="63">
+      <c r="K5" s="71"/>
+      <c r="L5" s="71"/>
+      <c r="M5" s="72">
         <v>41373</v>
       </c>
-      <c r="N5" s="63"/>
-      <c r="O5" s="63"/>
-      <c r="P5" s="58">
+      <c r="N5" s="72"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="60">
         <v>41396</v>
       </c>
-      <c r="Q5" s="58"/>
-      <c r="R5" s="58"/>
-      <c r="S5" s="64">
+      <c r="Q5" s="60"/>
+      <c r="R5" s="60"/>
+      <c r="S5" s="65">
         <v>41383</v>
       </c>
-      <c r="T5" s="64"/>
-      <c r="U5" s="64"/>
-      <c r="V5" s="64">
-        <v>41410</v>
-      </c>
-      <c r="W5" s="64"/>
-      <c r="X5" s="64"/>
-      <c r="Y5" s="58">
+      <c r="T5" s="65"/>
+      <c r="U5" s="65"/>
+      <c r="V5" s="65">
+        <v>41491</v>
+      </c>
+      <c r="W5" s="65"/>
+      <c r="X5" s="65"/>
+      <c r="Y5" s="60">
         <v>41394</v>
       </c>
-      <c r="Z5" s="58"/>
-      <c r="AA5" s="58"/>
-      <c r="AB5" s="58">
+      <c r="Z5" s="60"/>
+      <c r="AA5" s="60"/>
+      <c r="AB5" s="60">
         <v>41388</v>
       </c>
-      <c r="AC5" s="58"/>
-      <c r="AD5" s="58"/>
-      <c r="AE5" s="58">
+      <c r="AC5" s="60"/>
+      <c r="AD5" s="60"/>
+      <c r="AE5" s="60">
         <v>41388</v>
       </c>
-      <c r="AF5" s="58"/>
-      <c r="AG5" s="58"/>
-      <c r="AH5" s="58">
+      <c r="AF5" s="60"/>
+      <c r="AG5" s="60"/>
+      <c r="AH5" s="60">
         <v>41431</v>
       </c>
-      <c r="AI5" s="58"/>
-      <c r="AJ5" s="58"/>
-      <c r="AK5" s="58">
+      <c r="AI5" s="60"/>
+      <c r="AJ5" s="60"/>
+      <c r="AK5" s="60">
         <v>41467</v>
       </c>
-      <c r="AL5" s="58"/>
-      <c r="AM5" s="58"/>
-      <c r="AN5" s="58">
+      <c r="AL5" s="60"/>
+      <c r="AM5" s="60"/>
+      <c r="AN5" s="60">
         <v>41435</v>
       </c>
-      <c r="AO5" s="58"/>
-      <c r="AP5" s="58"/>
-      <c r="AQ5" s="58">
+      <c r="AO5" s="60"/>
+      <c r="AP5" s="60"/>
+      <c r="AQ5" s="60">
         <v>41449</v>
       </c>
-      <c r="AR5" s="58"/>
-      <c r="AS5" s="58"/>
-      <c r="AT5" s="58">
+      <c r="AR5" s="60"/>
+      <c r="AS5" s="60"/>
+      <c r="AT5" s="60">
         <v>41444</v>
       </c>
-      <c r="AU5" s="58"/>
-      <c r="AV5" s="58"/>
-      <c r="AW5" s="58">
+      <c r="AU5" s="60"/>
+      <c r="AV5" s="60"/>
+      <c r="AW5" s="60">
         <v>41465</v>
       </c>
-      <c r="AX5" s="58"/>
-      <c r="AY5" s="58"/>
-      <c r="AZ5" s="58"/>
-      <c r="BA5" s="58"/>
-      <c r="BB5" s="58"/>
+      <c r="AX5" s="60"/>
+      <c r="AY5" s="60"/>
+      <c r="AZ5" s="60"/>
+      <c r="BA5" s="60"/>
+      <c r="BB5" s="60"/>
     </row>
     <row r="6" spans="1:54" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="68" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="19" t="s">
         <v>37</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>38</v>
       </c>
       <c r="C6" s="20">
         <v>1</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6" s="22">
         <v>0</v>
       </c>
       <c r="F6" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="H6" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="I6" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="26" t="s">
-        <v>43</v>
-      </c>
       <c r="J6" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M6" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N6" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O6" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P6" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q6" s="24"/>
       <c r="R6" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="S6" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="T6" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="U6" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="V6" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="W6" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="X6" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y6" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="S6" s="28" t="s">
+      <c r="Z6" s="69"/>
+      <c r="AA6" s="69"/>
+      <c r="AB6" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="T6" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="U6" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="V6" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="W6" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="X6" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y6" s="60" t="s">
+      <c r="AC6" s="69"/>
+      <c r="AD6" s="69"/>
+      <c r="AE6" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="Z6" s="60"/>
-      <c r="AA6" s="60"/>
-      <c r="AB6" s="60" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC6" s="60"/>
-      <c r="AD6" s="60"/>
-      <c r="AE6" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="AF6" s="60"/>
-      <c r="AG6" s="60"/>
+      <c r="AF6" s="69"/>
+      <c r="AG6" s="69"/>
       <c r="AH6" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AI6" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AJ6" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AK6" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AL6" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AM6" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AN6" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AO6" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AP6" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AQ6" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AR6" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AS6" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AT6" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AU6" s="24"/>
       <c r="AV6" s="24"/>
       <c r="AW6" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AX6" s="24"/>
       <c r="AY6" s="24"/>
@@ -1738,126 +1744,126 @@
       <c r="BB6" s="24"/>
     </row>
     <row r="7" spans="1:54" ht="42.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="59"/>
+      <c r="A7" s="68"/>
       <c r="B7" s="30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="20">
         <v>2</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" s="22">
         <v>0</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G7" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="31" t="s">
-        <v>51</v>
-      </c>
       <c r="I7" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J7" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K7" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M7" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N7" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O7" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P7" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q7" s="24"/>
       <c r="R7" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S7" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T7" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="U7" s="29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="V7" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="W7" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="X7" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y7" s="60"/>
-      <c r="Z7" s="60"/>
-      <c r="AA7" s="60"/>
-      <c r="AB7" s="60"/>
-      <c r="AC7" s="60"/>
-      <c r="AD7" s="60"/>
-      <c r="AE7" s="60"/>
-      <c r="AF7" s="60"/>
-      <c r="AG7" s="60"/>
+        <v>44</v>
+      </c>
+      <c r="Y7" s="69"/>
+      <c r="Z7" s="69"/>
+      <c r="AA7" s="69"/>
+      <c r="AB7" s="69"/>
+      <c r="AC7" s="69"/>
+      <c r="AD7" s="69"/>
+      <c r="AE7" s="69"/>
+      <c r="AF7" s="69"/>
+      <c r="AG7" s="69"/>
       <c r="AH7" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AI7" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AJ7" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AK7" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AL7" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AM7" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AN7" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AO7" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AP7" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AQ7" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AR7" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AS7" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AT7" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AU7" s="24"/>
       <c r="AV7" s="24"/>
       <c r="AW7" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AX7" s="24"/>
       <c r="AY7" s="24"/>
@@ -1866,124 +1872,124 @@
       <c r="BB7" s="24"/>
     </row>
     <row r="8" spans="1:54" ht="43.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="59"/>
+      <c r="A8" s="68"/>
       <c r="B8" s="30"/>
       <c r="C8" s="20">
         <v>3</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E8" s="22">
         <v>0</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="31" t="s">
-        <v>54</v>
-      </c>
       <c r="I8" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J8" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L8" s="33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M8" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N8" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O8" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P8" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q8" s="24"/>
       <c r="R8" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S8" s="34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T8" s="34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="U8" s="29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="V8" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="W8" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="X8" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y8" s="60"/>
-      <c r="Z8" s="60"/>
-      <c r="AA8" s="60"/>
-      <c r="AB8" s="60"/>
-      <c r="AC8" s="60"/>
-      <c r="AD8" s="60"/>
-      <c r="AE8" s="60"/>
-      <c r="AF8" s="60"/>
-      <c r="AG8" s="60"/>
+        <v>44</v>
+      </c>
+      <c r="Y8" s="69"/>
+      <c r="Z8" s="69"/>
+      <c r="AA8" s="69"/>
+      <c r="AB8" s="69"/>
+      <c r="AC8" s="69"/>
+      <c r="AD8" s="69"/>
+      <c r="AE8" s="69"/>
+      <c r="AF8" s="69"/>
+      <c r="AG8" s="69"/>
       <c r="AH8" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AI8" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AJ8" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AK8" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AL8" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AM8" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AN8" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AO8" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AP8" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AQ8" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AR8" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AS8" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AT8" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AU8" s="24"/>
       <c r="AV8" s="24"/>
       <c r="AW8" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AX8" s="24"/>
       <c r="AY8" s="24"/>
@@ -1992,124 +1998,124 @@
       <c r="BB8" s="24"/>
     </row>
     <row r="9" spans="1:54" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="59"/>
+      <c r="A9" s="68"/>
       <c r="B9" s="30"/>
       <c r="C9" s="20">
         <v>4</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E9" s="22">
         <v>0</v>
       </c>
       <c r="F9" s="56" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G9" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="H9" s="57" t="s">
-        <v>57</v>
-      </c>
       <c r="I9" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J9" s="39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L9" s="40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M9" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N9" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O9" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P9" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q9" s="20"/>
       <c r="R9" s="41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="S9" s="42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T9" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="U9" s="44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="V9" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="W9" s="21" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="X9" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y9" s="60"/>
-      <c r="Z9" s="60"/>
-      <c r="AA9" s="60"/>
-      <c r="AB9" s="60"/>
-      <c r="AC9" s="60"/>
-      <c r="AD9" s="60"/>
-      <c r="AE9" s="60"/>
-      <c r="AF9" s="60"/>
-      <c r="AG9" s="60"/>
+        <v>44</v>
+      </c>
+      <c r="Y9" s="69"/>
+      <c r="Z9" s="69"/>
+      <c r="AA9" s="69"/>
+      <c r="AB9" s="69"/>
+      <c r="AC9" s="69"/>
+      <c r="AD9" s="69"/>
+      <c r="AE9" s="69"/>
+      <c r="AF9" s="69"/>
+      <c r="AG9" s="69"/>
       <c r="AH9" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AI9" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AJ9" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AK9" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AL9" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AM9" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AN9" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AO9" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AP9" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AQ9" s="45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AR9" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AS9" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AT9" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AU9" s="20"/>
       <c r="AV9" s="24"/>
       <c r="AW9" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AX9" s="20"/>
       <c r="AY9" s="24"/>
@@ -2124,22 +2130,22 @@
         <v>4</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E10" s="35">
         <v>1</v>
       </c>
       <c r="F10" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="G10" s="37" t="s">
+      <c r="H10" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="H10" s="38" t="s">
+      <c r="I10" s="26" t="s">
         <v>77</v>
-      </c>
-      <c r="I10" s="26" t="s">
-        <v>78</v>
       </c>
       <c r="J10" s="39"/>
       <c r="K10" s="20"/>
@@ -2148,11 +2154,11 @@
       <c r="N10" s="20"/>
       <c r="O10" s="21"/>
       <c r="P10" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q10" s="20"/>
       <c r="R10" s="41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="S10" s="42"/>
       <c r="T10" s="43"/>
@@ -2160,15 +2166,15 @@
       <c r="V10" s="21"/>
       <c r="W10" s="21"/>
       <c r="X10" s="21"/>
-      <c r="Y10" s="60"/>
-      <c r="Z10" s="60"/>
-      <c r="AA10" s="60"/>
-      <c r="AB10" s="60"/>
-      <c r="AC10" s="60"/>
-      <c r="AD10" s="60"/>
-      <c r="AE10" s="60"/>
-      <c r="AF10" s="60"/>
-      <c r="AG10" s="60"/>
+      <c r="Y10" s="69"/>
+      <c r="Z10" s="69"/>
+      <c r="AA10" s="69"/>
+      <c r="AB10" s="69"/>
+      <c r="AC10" s="69"/>
+      <c r="AD10" s="69"/>
+      <c r="AE10" s="69"/>
+      <c r="AF10" s="69"/>
+      <c r="AG10" s="69"/>
       <c r="AH10" s="24"/>
       <c r="AI10" s="20"/>
       <c r="AJ10" s="24"/>
@@ -2185,7 +2191,7 @@
       <c r="AU10" s="20"/>
       <c r="AV10" s="24"/>
       <c r="AW10" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AX10" s="20"/>
       <c r="AY10" s="24"/>
@@ -2194,116 +2200,116 @@
       <c r="BB10" s="24"/>
     </row>
     <row r="11" spans="1:54" s="47" customFormat="1" ht="58.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="61" t="s">
+      <c r="A11" s="70" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>58</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>59</v>
       </c>
       <c r="C11" s="24">
         <v>1</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" s="24">
         <v>0</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G11" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="46" t="s">
-        <v>62</v>
-      </c>
       <c r="I11" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K11" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L11" s="24"/>
       <c r="M11" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N11" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O11" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P11" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q11" s="24"/>
       <c r="R11" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="S11" s="24"/>
       <c r="T11" s="24"/>
       <c r="U11" s="24"/>
       <c r="V11" s="23" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="W11" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="X11" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y11" s="60"/>
-      <c r="Z11" s="60"/>
-      <c r="AA11" s="60"/>
-      <c r="AB11" s="60"/>
-      <c r="AC11" s="60"/>
-      <c r="AD11" s="60"/>
-      <c r="AE11" s="60"/>
-      <c r="AF11" s="60"/>
-      <c r="AG11" s="60"/>
+        <v>44</v>
+      </c>
+      <c r="Y11" s="69"/>
+      <c r="Z11" s="69"/>
+      <c r="AA11" s="69"/>
+      <c r="AB11" s="69"/>
+      <c r="AC11" s="69"/>
+      <c r="AD11" s="69"/>
+      <c r="AE11" s="69"/>
+      <c r="AF11" s="69"/>
+      <c r="AG11" s="69"/>
       <c r="AH11" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AI11" s="24"/>
       <c r="AJ11" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AK11" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AL11" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AM11" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AN11" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AO11" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AP11" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AQ11" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AR11" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AS11" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AT11" s="24"/>
       <c r="AU11" s="24"/>
       <c r="AV11" s="24"/>
       <c r="AW11" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AX11" s="24"/>
       <c r="AY11" s="24"/>
@@ -2312,110 +2318,110 @@
       <c r="BB11" s="24"/>
     </row>
     <row r="12" spans="1:54" ht="58.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="61"/>
+      <c r="A12" s="70"/>
       <c r="B12" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="24">
         <v>2</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E12" s="24">
         <v>0</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G12" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="46" t="s">
-        <v>66</v>
-      </c>
       <c r="I12" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J12" s="24"/>
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N12" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O12" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P12" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q12" s="24"/>
       <c r="R12" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="S12" s="24"/>
       <c r="T12" s="24"/>
       <c r="U12" s="24"/>
       <c r="V12" s="23" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="W12" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="X12" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y12" s="60"/>
-      <c r="Z12" s="60"/>
-      <c r="AA12" s="60"/>
-      <c r="AB12" s="60"/>
-      <c r="AC12" s="60"/>
-      <c r="AD12" s="60"/>
-      <c r="AE12" s="60"/>
-      <c r="AF12" s="60"/>
-      <c r="AG12" s="60"/>
+        <v>44</v>
+      </c>
+      <c r="Y12" s="69"/>
+      <c r="Z12" s="69"/>
+      <c r="AA12" s="69"/>
+      <c r="AB12" s="69"/>
+      <c r="AC12" s="69"/>
+      <c r="AD12" s="69"/>
+      <c r="AE12" s="69"/>
+      <c r="AF12" s="69"/>
+      <c r="AG12" s="69"/>
       <c r="AH12" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AI12" s="24"/>
       <c r="AJ12" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AK12" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AL12" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AM12" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AN12" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AO12" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AP12" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AQ12" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AR12" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AS12" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AT12" s="24"/>
       <c r="AU12" s="24"/>
       <c r="AV12" s="24"/>
       <c r="AW12" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AX12" s="24"/>
       <c r="AY12" s="24"/>
@@ -2424,28 +2430,28 @@
       <c r="BB12" s="24"/>
     </row>
     <row r="13" spans="1:54" ht="63" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="61"/>
+      <c r="A13" s="70"/>
       <c r="B13" s="30"/>
       <c r="C13" s="48">
         <v>3</v>
       </c>
       <c r="D13" s="49" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E13" s="50">
         <v>0</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G13" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="H13" s="31" t="s">
-        <v>69</v>
-      </c>
       <c r="I13" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J13" s="24"/>
       <c r="K13" s="24"/>
@@ -2462,15 +2468,15 @@
       <c r="V13" s="24"/>
       <c r="W13" s="24"/>
       <c r="X13" s="24"/>
-      <c r="Y13" s="60"/>
-      <c r="Z13" s="60"/>
-      <c r="AA13" s="60"/>
-      <c r="AB13" s="60"/>
-      <c r="AC13" s="60"/>
-      <c r="AD13" s="60"/>
-      <c r="AE13" s="60"/>
-      <c r="AF13" s="60"/>
-      <c r="AG13" s="60"/>
+      <c r="Y13" s="69"/>
+      <c r="Z13" s="69"/>
+      <c r="AA13" s="69"/>
+      <c r="AB13" s="69"/>
+      <c r="AC13" s="69"/>
+      <c r="AD13" s="69"/>
+      <c r="AE13" s="69"/>
+      <c r="AF13" s="69"/>
+      <c r="AG13" s="69"/>
       <c r="AH13" s="24"/>
       <c r="AI13" s="24"/>
       <c r="AJ13" s="24"/>
@@ -2494,28 +2500,28 @@
       <c r="BB13" s="24"/>
     </row>
     <row r="14" spans="1:54" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="61"/>
+      <c r="A14" s="70"/>
       <c r="B14" s="52"/>
       <c r="C14" s="51">
         <v>4</v>
       </c>
       <c r="D14" s="49" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E14" s="50">
         <v>0</v>
       </c>
       <c r="F14" s="49" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G14" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="H14" s="53" t="s">
-        <v>72</v>
-      </c>
       <c r="I14" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J14" s="54"/>
       <c r="K14" s="54"/>
@@ -2532,15 +2538,15 @@
       <c r="V14" s="54"/>
       <c r="W14" s="54"/>
       <c r="X14" s="54"/>
-      <c r="Y14" s="60"/>
-      <c r="Z14" s="60"/>
-      <c r="AA14" s="60"/>
-      <c r="AB14" s="60"/>
-      <c r="AC14" s="60"/>
-      <c r="AD14" s="60"/>
-      <c r="AE14" s="60"/>
-      <c r="AF14" s="60"/>
-      <c r="AG14" s="60"/>
+      <c r="Y14" s="69"/>
+      <c r="Z14" s="69"/>
+      <c r="AA14" s="69"/>
+      <c r="AB14" s="69"/>
+      <c r="AC14" s="69"/>
+      <c r="AD14" s="69"/>
+      <c r="AE14" s="69"/>
+      <c r="AF14" s="69"/>
+      <c r="AG14" s="69"/>
       <c r="AH14" s="54"/>
       <c r="AI14" s="54"/>
       <c r="AJ14" s="54"/>
@@ -2566,27 +2572,22 @@
     <row r="15" spans="1:54" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="AW3:AY3"/>
-    <mergeCell ref="AW4:AY4"/>
-    <mergeCell ref="AW5:AY5"/>
-    <mergeCell ref="AZ3:BB3"/>
-    <mergeCell ref="AZ4:BB4"/>
-    <mergeCell ref="AZ5:BB5"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="Y3:AA3"/>
-    <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="AK3:AM3"/>
-    <mergeCell ref="AN3:AP3"/>
-    <mergeCell ref="AQ3:AS3"/>
+    <mergeCell ref="AN5:AP5"/>
+    <mergeCell ref="AQ5:AS5"/>
+    <mergeCell ref="AT5:AV5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="Y6:AA14"/>
+    <mergeCell ref="AB6:AD14"/>
+    <mergeCell ref="AE6:AG14"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="Y5:AA5"/>
+    <mergeCell ref="AB5:AD5"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AK5:AM5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="P5:R5"/>
     <mergeCell ref="S5:U5"/>
     <mergeCell ref="V5:X5"/>
     <mergeCell ref="AT3:AV3"/>
@@ -2603,23 +2604,29 @@
     <mergeCell ref="AN4:AP4"/>
     <mergeCell ref="AQ4:AS4"/>
     <mergeCell ref="AT4:AV4"/>
-    <mergeCell ref="AN5:AP5"/>
-    <mergeCell ref="AQ5:AS5"/>
-    <mergeCell ref="AT5:AV5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="Y6:AA14"/>
-    <mergeCell ref="AB6:AD14"/>
-    <mergeCell ref="AE6:AG14"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="Y5:AA5"/>
-    <mergeCell ref="AB5:AD5"/>
-    <mergeCell ref="AE5:AG5"/>
-    <mergeCell ref="AH5:AJ5"/>
-    <mergeCell ref="AK5:AM5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="AH3:AJ3"/>
+    <mergeCell ref="AK3:AM3"/>
+    <mergeCell ref="AN3:AP3"/>
+    <mergeCell ref="AQ3:AS3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="Y3:AA3"/>
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="AW3:AY3"/>
+    <mergeCell ref="AW4:AY4"/>
+    <mergeCell ref="AW5:AY5"/>
+    <mergeCell ref="AZ3:BB3"/>
+    <mergeCell ref="AZ4:BB4"/>
+    <mergeCell ref="AZ5:BB5"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add ARIS to spreadsheet
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="631"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="83">
   <si>
     <t>Note: Tools that are not listed here have either not been tested or may not support both BPMN import and export.</t>
   </si>
@@ -354,15 +354,21 @@
     <t>OK</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
+  <si>
+    <t>ARIS Business Architect</t>
+  </si>
+  <si>
+    <t>7.2.4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -745,14 +751,41 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -763,37 +796,10 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="TableStyleLight1" xfId="1"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -877,7 +883,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1168,11 +1174,11 @@
   </sheetPr>
   <dimension ref="A1:AMK15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3:X3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AA1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BA10" sqref="BA10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="44.85546875" style="1"/>
@@ -1186,24 +1192,24 @@
     <col min="10" max="1025" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:57" ht="15.75" thickBot="1">
       <c r="K1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:54" ht="47.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="61" t="s">
+    <row r="2" spans="1:57" ht="47.25" thickTop="1" thickBot="1">
+      <c r="A2" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61" t="s">
+      <c r="B2" s="70"/>
+      <c r="C2" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61" t="s">
+      <c r="D2" s="70"/>
+      <c r="E2" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="61"/>
+      <c r="F2" s="70"/>
       <c r="G2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1348,8 +1354,17 @@
       <c r="BB2" s="8" t="s">
         <v>9</v>
       </c>
+      <c r="BC2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="BD2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="BE2" s="8" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:54" ht="25.35" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:57" ht="25.35" customHeight="1" thickTop="1" thickBot="1">
       <c r="A3" s="9"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -1361,81 +1376,86 @@
       <c r="I3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="62" t="s">
+      <c r="J3" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="63" t="s">
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="58" t="s">
+      <c r="N3" s="72"/>
+      <c r="O3" s="72"/>
+      <c r="P3" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="58"/>
-      <c r="S3" s="58" t="s">
+      <c r="Q3" s="65"/>
+      <c r="R3" s="65"/>
+      <c r="S3" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="T3" s="58"/>
-      <c r="U3" s="58"/>
-      <c r="V3" s="58" t="s">
+      <c r="T3" s="65"/>
+      <c r="U3" s="65"/>
+      <c r="V3" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="W3" s="58"/>
-      <c r="X3" s="58"/>
-      <c r="Y3" s="58" t="s">
+      <c r="W3" s="65"/>
+      <c r="X3" s="65"/>
+      <c r="Y3" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="Z3" s="58"/>
-      <c r="AA3" s="58"/>
-      <c r="AB3" s="58" t="s">
+      <c r="Z3" s="65"/>
+      <c r="AA3" s="65"/>
+      <c r="AB3" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="AC3" s="58"/>
-      <c r="AD3" s="58"/>
-      <c r="AE3" s="58" t="s">
+      <c r="AC3" s="65"/>
+      <c r="AD3" s="65"/>
+      <c r="AE3" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="AF3" s="58"/>
-      <c r="AG3" s="58"/>
-      <c r="AH3" s="58" t="s">
+      <c r="AF3" s="65"/>
+      <c r="AG3" s="65"/>
+      <c r="AH3" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="AI3" s="58"/>
-      <c r="AJ3" s="58"/>
-      <c r="AK3" s="64" t="s">
+      <c r="AI3" s="65"/>
+      <c r="AJ3" s="65"/>
+      <c r="AK3" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="AL3" s="64"/>
-      <c r="AM3" s="64"/>
-      <c r="AN3" s="58" t="s">
+      <c r="AL3" s="69"/>
+      <c r="AM3" s="69"/>
+      <c r="AN3" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="AO3" s="58"/>
-      <c r="AP3" s="58"/>
-      <c r="AQ3" s="58" t="s">
+      <c r="AO3" s="65"/>
+      <c r="AP3" s="65"/>
+      <c r="AQ3" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="AR3" s="58"/>
-      <c r="AS3" s="58"/>
-      <c r="AT3" s="58" t="s">
+      <c r="AR3" s="65"/>
+      <c r="AS3" s="65"/>
+      <c r="AT3" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="AU3" s="58"/>
-      <c r="AV3" s="58"/>
-      <c r="AW3" s="58" t="s">
+      <c r="AU3" s="65"/>
+      <c r="AV3" s="65"/>
+      <c r="AW3" s="65" t="s">
         <v>72</v>
       </c>
-      <c r="AX3" s="58"/>
-      <c r="AY3" s="58"/>
-      <c r="AZ3" s="58"/>
-      <c r="BA3" s="58"/>
-      <c r="BB3" s="58"/>
+      <c r="AX3" s="65"/>
+      <c r="AY3" s="65"/>
+      <c r="AZ3" s="65" t="s">
+        <v>81</v>
+      </c>
+      <c r="BA3" s="65"/>
+      <c r="BB3" s="65"/>
+      <c r="BC3" s="65"/>
+      <c r="BD3" s="65"/>
+      <c r="BE3" s="65"/>
     </row>
-    <row r="4" spans="1:54" s="15" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:57" s="15" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A4" s="12"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -1452,76 +1472,81 @@
       </c>
       <c r="K4" s="66"/>
       <c r="L4" s="66"/>
-      <c r="M4" s="59" t="s">
+      <c r="M4" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="59"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="59" t="s">
+      <c r="N4" s="67"/>
+      <c r="O4" s="67"/>
+      <c r="P4" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="Q4" s="59"/>
-      <c r="R4" s="59"/>
-      <c r="S4" s="59" t="s">
+      <c r="Q4" s="67"/>
+      <c r="R4" s="67"/>
+      <c r="S4" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="T4" s="59"/>
-      <c r="U4" s="59"/>
-      <c r="V4" s="67" t="s">
+      <c r="T4" s="67"/>
+      <c r="U4" s="67"/>
+      <c r="V4" s="68" t="s">
         <v>79</v>
       </c>
-      <c r="W4" s="67"/>
-      <c r="X4" s="67"/>
-      <c r="Y4" s="59" t="s">
+      <c r="W4" s="68"/>
+      <c r="X4" s="68"/>
+      <c r="Y4" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="Z4" s="59"/>
-      <c r="AA4" s="59"/>
-      <c r="AB4" s="59">
+      <c r="Z4" s="67"/>
+      <c r="AA4" s="67"/>
+      <c r="AB4" s="67">
         <v>2.4</v>
       </c>
-      <c r="AC4" s="59"/>
-      <c r="AD4" s="59"/>
-      <c r="AE4" s="59" t="s">
+      <c r="AC4" s="67"/>
+      <c r="AD4" s="67"/>
+      <c r="AE4" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="AF4" s="59"/>
-      <c r="AG4" s="59"/>
-      <c r="AH4" s="59" t="s">
+      <c r="AF4" s="67"/>
+      <c r="AG4" s="67"/>
+      <c r="AH4" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="AI4" s="59"/>
-      <c r="AJ4" s="59"/>
-      <c r="AK4" s="59" t="s">
+      <c r="AI4" s="67"/>
+      <c r="AJ4" s="67"/>
+      <c r="AK4" s="67" t="s">
         <v>78</v>
       </c>
-      <c r="AL4" s="59"/>
-      <c r="AM4" s="59"/>
-      <c r="AN4" s="59" t="s">
+      <c r="AL4" s="67"/>
+      <c r="AM4" s="67"/>
+      <c r="AN4" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="AO4" s="59"/>
-      <c r="AP4" s="59"/>
-      <c r="AQ4" s="59" t="s">
+      <c r="AO4" s="67"/>
+      <c r="AP4" s="67"/>
+      <c r="AQ4" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="AR4" s="59"/>
-      <c r="AS4" s="59"/>
-      <c r="AT4" s="59" t="s">
+      <c r="AR4" s="67"/>
+      <c r="AS4" s="67"/>
+      <c r="AT4" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="AU4" s="59"/>
-      <c r="AV4" s="59"/>
-      <c r="AW4" s="59" t="s">
+      <c r="AU4" s="67"/>
+      <c r="AV4" s="67"/>
+      <c r="AW4" s="67" t="s">
         <v>73</v>
       </c>
-      <c r="AX4" s="59"/>
-      <c r="AY4" s="59"/>
-      <c r="AZ4" s="59"/>
-      <c r="BA4" s="59"/>
-      <c r="BB4" s="59"/>
+      <c r="AX4" s="67"/>
+      <c r="AY4" s="67"/>
+      <c r="AZ4" s="67" t="s">
+        <v>82</v>
+      </c>
+      <c r="BA4" s="67"/>
+      <c r="BB4" s="67"/>
+      <c r="BC4" s="67"/>
+      <c r="BD4" s="67"/>
+      <c r="BE4" s="67"/>
     </row>
-    <row r="5" spans="1:54" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:57" ht="16.5" thickTop="1" thickBot="1">
       <c r="A5" s="16"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -1533,82 +1558,87 @@
       <c r="I5" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="71">
+      <c r="J5" s="62">
         <v>41380</v>
       </c>
-      <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="72">
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="63">
         <v>41373</v>
       </c>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
-      <c r="P5" s="60">
+      <c r="N5" s="63"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="58">
         <v>41396</v>
       </c>
-      <c r="Q5" s="60"/>
-      <c r="R5" s="60"/>
-      <c r="S5" s="65">
+      <c r="Q5" s="58"/>
+      <c r="R5" s="58"/>
+      <c r="S5" s="64">
         <v>41383</v>
       </c>
-      <c r="T5" s="65"/>
-      <c r="U5" s="65"/>
-      <c r="V5" s="65">
+      <c r="T5" s="64"/>
+      <c r="U5" s="64"/>
+      <c r="V5" s="64">
         <v>41491</v>
       </c>
-      <c r="W5" s="65"/>
-      <c r="X5" s="65"/>
-      <c r="Y5" s="60">
+      <c r="W5" s="64"/>
+      <c r="X5" s="64"/>
+      <c r="Y5" s="58">
         <v>41394</v>
       </c>
-      <c r="Z5" s="60"/>
-      <c r="AA5" s="60"/>
-      <c r="AB5" s="60">
+      <c r="Z5" s="58"/>
+      <c r="AA5" s="58"/>
+      <c r="AB5" s="58">
         <v>41388</v>
       </c>
-      <c r="AC5" s="60"/>
-      <c r="AD5" s="60"/>
-      <c r="AE5" s="60">
+      <c r="AC5" s="58"/>
+      <c r="AD5" s="58"/>
+      <c r="AE5" s="58">
         <v>41388</v>
       </c>
-      <c r="AF5" s="60"/>
-      <c r="AG5" s="60"/>
-      <c r="AH5" s="60">
+      <c r="AF5" s="58"/>
+      <c r="AG5" s="58"/>
+      <c r="AH5" s="58">
         <v>41431</v>
       </c>
-      <c r="AI5" s="60"/>
-      <c r="AJ5" s="60"/>
-      <c r="AK5" s="60">
+      <c r="AI5" s="58"/>
+      <c r="AJ5" s="58"/>
+      <c r="AK5" s="58">
         <v>41467</v>
       </c>
-      <c r="AL5" s="60"/>
-      <c r="AM5" s="60"/>
-      <c r="AN5" s="60">
+      <c r="AL5" s="58"/>
+      <c r="AM5" s="58"/>
+      <c r="AN5" s="58">
         <v>41435</v>
       </c>
-      <c r="AO5" s="60"/>
-      <c r="AP5" s="60"/>
-      <c r="AQ5" s="60">
+      <c r="AO5" s="58"/>
+      <c r="AP5" s="58"/>
+      <c r="AQ5" s="58">
         <v>41449</v>
       </c>
-      <c r="AR5" s="60"/>
-      <c r="AS5" s="60"/>
-      <c r="AT5" s="60">
+      <c r="AR5" s="58"/>
+      <c r="AS5" s="58"/>
+      <c r="AT5" s="58">
         <v>41444</v>
       </c>
-      <c r="AU5" s="60"/>
-      <c r="AV5" s="60"/>
-      <c r="AW5" s="60">
+      <c r="AU5" s="58"/>
+      <c r="AV5" s="58"/>
+      <c r="AW5" s="58">
         <v>41465</v>
       </c>
-      <c r="AX5" s="60"/>
-      <c r="AY5" s="60"/>
-      <c r="AZ5" s="60"/>
-      <c r="BA5" s="60"/>
-      <c r="BB5" s="60"/>
+      <c r="AX5" s="58"/>
+      <c r="AY5" s="58"/>
+      <c r="AZ5" s="58">
+        <v>41571</v>
+      </c>
+      <c r="BA5" s="58"/>
+      <c r="BB5" s="58"/>
+      <c r="BC5" s="58"/>
+      <c r="BD5" s="58"/>
+      <c r="BE5" s="58"/>
     </row>
-    <row r="6" spans="1:54" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="68" t="s">
+    <row r="6" spans="1:57" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A6" s="59" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="19" t="s">
@@ -1678,21 +1708,21 @@
       <c r="X6" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="Y6" s="69" t="s">
+      <c r="Y6" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="Z6" s="69"/>
-      <c r="AA6" s="69"/>
-      <c r="AB6" s="69" t="s">
+      <c r="Z6" s="60"/>
+      <c r="AA6" s="60"/>
+      <c r="AB6" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="AC6" s="69"/>
-      <c r="AD6" s="69"/>
-      <c r="AE6" s="69" t="s">
+      <c r="AC6" s="60"/>
+      <c r="AD6" s="60"/>
+      <c r="AE6" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="AF6" s="69"/>
-      <c r="AG6" s="69"/>
+      <c r="AF6" s="60"/>
+      <c r="AG6" s="60"/>
       <c r="AH6" s="27" t="s">
         <v>44</v>
       </c>
@@ -1740,11 +1770,16 @@
       <c r="AX6" s="24"/>
       <c r="AY6" s="24"/>
       <c r="AZ6" s="27"/>
-      <c r="BA6" s="24"/>
+      <c r="BA6" s="24" t="s">
+        <v>43</v>
+      </c>
       <c r="BB6" s="24"/>
+      <c r="BC6" s="27"/>
+      <c r="BD6" s="24"/>
+      <c r="BE6" s="24"/>
     </row>
-    <row r="7" spans="1:54" ht="42.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="68"/>
+    <row r="7" spans="1:57" ht="42.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A7" s="59"/>
       <c r="B7" s="30" t="s">
         <v>47</v>
       </c>
@@ -1812,15 +1847,15 @@
       <c r="X7" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="Y7" s="69"/>
-      <c r="Z7" s="69"/>
-      <c r="AA7" s="69"/>
-      <c r="AB7" s="69"/>
-      <c r="AC7" s="69"/>
-      <c r="AD7" s="69"/>
-      <c r="AE7" s="69"/>
-      <c r="AF7" s="69"/>
-      <c r="AG7" s="69"/>
+      <c r="Y7" s="60"/>
+      <c r="Z7" s="60"/>
+      <c r="AA7" s="60"/>
+      <c r="AB7" s="60"/>
+      <c r="AC7" s="60"/>
+      <c r="AD7" s="60"/>
+      <c r="AE7" s="60"/>
+      <c r="AF7" s="60"/>
+      <c r="AG7" s="60"/>
       <c r="AH7" s="27" t="s">
         <v>44</v>
       </c>
@@ -1868,11 +1903,16 @@
       <c r="AX7" s="24"/>
       <c r="AY7" s="24"/>
       <c r="AZ7" s="27"/>
-      <c r="BA7" s="24"/>
+      <c r="BA7" s="24" t="s">
+        <v>43</v>
+      </c>
       <c r="BB7" s="24"/>
+      <c r="BC7" s="27"/>
+      <c r="BD7" s="24"/>
+      <c r="BE7" s="24"/>
     </row>
-    <row r="8" spans="1:54" ht="43.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="68"/>
+    <row r="8" spans="1:57" ht="43.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A8" s="59"/>
       <c r="B8" s="30"/>
       <c r="C8" s="20">
         <v>3</v>
@@ -1938,15 +1978,15 @@
       <c r="X8" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="Y8" s="69"/>
-      <c r="Z8" s="69"/>
-      <c r="AA8" s="69"/>
-      <c r="AB8" s="69"/>
-      <c r="AC8" s="69"/>
-      <c r="AD8" s="69"/>
-      <c r="AE8" s="69"/>
-      <c r="AF8" s="69"/>
-      <c r="AG8" s="69"/>
+      <c r="Y8" s="60"/>
+      <c r="Z8" s="60"/>
+      <c r="AA8" s="60"/>
+      <c r="AB8" s="60"/>
+      <c r="AC8" s="60"/>
+      <c r="AD8" s="60"/>
+      <c r="AE8" s="60"/>
+      <c r="AF8" s="60"/>
+      <c r="AG8" s="60"/>
       <c r="AH8" s="27" t="s">
         <v>43</v>
       </c>
@@ -1994,11 +2034,16 @@
       <c r="AX8" s="24"/>
       <c r="AY8" s="24"/>
       <c r="AZ8" s="27"/>
-      <c r="BA8" s="24"/>
+      <c r="BA8" s="24" t="s">
+        <v>43</v>
+      </c>
       <c r="BB8" s="24"/>
+      <c r="BC8" s="27"/>
+      <c r="BD8" s="24"/>
+      <c r="BE8" s="24"/>
     </row>
-    <row r="9" spans="1:54" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="68"/>
+    <row r="9" spans="1:57" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A9" s="59"/>
       <c r="B9" s="30"/>
       <c r="C9" s="20">
         <v>4</v>
@@ -2064,15 +2109,15 @@
       <c r="X9" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="Y9" s="69"/>
-      <c r="Z9" s="69"/>
-      <c r="AA9" s="69"/>
-      <c r="AB9" s="69"/>
-      <c r="AC9" s="69"/>
-      <c r="AD9" s="69"/>
-      <c r="AE9" s="69"/>
-      <c r="AF9" s="69"/>
-      <c r="AG9" s="69"/>
+      <c r="Y9" s="60"/>
+      <c r="Z9" s="60"/>
+      <c r="AA9" s="60"/>
+      <c r="AB9" s="60"/>
+      <c r="AC9" s="60"/>
+      <c r="AD9" s="60"/>
+      <c r="AE9" s="60"/>
+      <c r="AF9" s="60"/>
+      <c r="AG9" s="60"/>
       <c r="AH9" s="24" t="s">
         <v>43</v>
       </c>
@@ -2120,10 +2165,15 @@
       <c r="AX9" s="20"/>
       <c r="AY9" s="24"/>
       <c r="AZ9" s="27"/>
-      <c r="BA9" s="20"/>
+      <c r="BA9" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="BB9" s="24"/>
+      <c r="BC9" s="27"/>
+      <c r="BD9" s="20"/>
+      <c r="BE9" s="24"/>
     </row>
-    <row r="10" spans="1:54" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:57" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A10" s="55"/>
       <c r="B10" s="30"/>
       <c r="C10" s="20">
@@ -2166,15 +2216,15 @@
       <c r="V10" s="21"/>
       <c r="W10" s="21"/>
       <c r="X10" s="21"/>
-      <c r="Y10" s="69"/>
-      <c r="Z10" s="69"/>
-      <c r="AA10" s="69"/>
-      <c r="AB10" s="69"/>
-      <c r="AC10" s="69"/>
-      <c r="AD10" s="69"/>
-      <c r="AE10" s="69"/>
-      <c r="AF10" s="69"/>
-      <c r="AG10" s="69"/>
+      <c r="Y10" s="60"/>
+      <c r="Z10" s="60"/>
+      <c r="AA10" s="60"/>
+      <c r="AB10" s="60"/>
+      <c r="AC10" s="60"/>
+      <c r="AD10" s="60"/>
+      <c r="AE10" s="60"/>
+      <c r="AF10" s="60"/>
+      <c r="AG10" s="60"/>
       <c r="AH10" s="24"/>
       <c r="AI10" s="20"/>
       <c r="AJ10" s="24"/>
@@ -2198,9 +2248,12 @@
       <c r="AZ10" s="27"/>
       <c r="BA10" s="20"/>
       <c r="BB10" s="24"/>
+      <c r="BC10" s="27"/>
+      <c r="BD10" s="20"/>
+      <c r="BE10" s="24"/>
     </row>
-    <row r="11" spans="1:54" s="47" customFormat="1" ht="58.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="70" t="s">
+    <row r="11" spans="1:57" s="47" customFormat="1" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A11" s="61" t="s">
         <v>57</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -2262,15 +2315,15 @@
       <c r="X11" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="Y11" s="69"/>
-      <c r="Z11" s="69"/>
-      <c r="AA11" s="69"/>
-      <c r="AB11" s="69"/>
-      <c r="AC11" s="69"/>
-      <c r="AD11" s="69"/>
-      <c r="AE11" s="69"/>
-      <c r="AF11" s="69"/>
-      <c r="AG11" s="69"/>
+      <c r="Y11" s="60"/>
+      <c r="Z11" s="60"/>
+      <c r="AA11" s="60"/>
+      <c r="AB11" s="60"/>
+      <c r="AC11" s="60"/>
+      <c r="AD11" s="60"/>
+      <c r="AE11" s="60"/>
+      <c r="AF11" s="60"/>
+      <c r="AG11" s="60"/>
       <c r="AH11" s="24" t="s">
         <v>43</v>
       </c>
@@ -2316,9 +2369,12 @@
       <c r="AZ11" s="24"/>
       <c r="BA11" s="24"/>
       <c r="BB11" s="24"/>
+      <c r="BC11" s="24"/>
+      <c r="BD11" s="24"/>
+      <c r="BE11" s="24"/>
     </row>
-    <row r="12" spans="1:54" ht="58.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="70"/>
+    <row r="12" spans="1:57" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A12" s="61"/>
       <c r="B12" s="30" t="s">
         <v>62</v>
       </c>
@@ -2374,15 +2430,15 @@
       <c r="X12" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="Y12" s="69"/>
-      <c r="Z12" s="69"/>
-      <c r="AA12" s="69"/>
-      <c r="AB12" s="69"/>
-      <c r="AC12" s="69"/>
-      <c r="AD12" s="69"/>
-      <c r="AE12" s="69"/>
-      <c r="AF12" s="69"/>
-      <c r="AG12" s="69"/>
+      <c r="Y12" s="60"/>
+      <c r="Z12" s="60"/>
+      <c r="AA12" s="60"/>
+      <c r="AB12" s="60"/>
+      <c r="AC12" s="60"/>
+      <c r="AD12" s="60"/>
+      <c r="AE12" s="60"/>
+      <c r="AF12" s="60"/>
+      <c r="AG12" s="60"/>
       <c r="AH12" s="24" t="s">
         <v>43</v>
       </c>
@@ -2428,9 +2484,12 @@
       <c r="AZ12" s="24"/>
       <c r="BA12" s="24"/>
       <c r="BB12" s="24"/>
+      <c r="BC12" s="24"/>
+      <c r="BD12" s="24"/>
+      <c r="BE12" s="24"/>
     </row>
-    <row r="13" spans="1:54" ht="63" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="70"/>
+    <row r="13" spans="1:57" ht="63" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A13" s="61"/>
       <c r="B13" s="30"/>
       <c r="C13" s="48">
         <v>3</v>
@@ -2468,15 +2527,15 @@
       <c r="V13" s="24"/>
       <c r="W13" s="24"/>
       <c r="X13" s="24"/>
-      <c r="Y13" s="69"/>
-      <c r="Z13" s="69"/>
-      <c r="AA13" s="69"/>
-      <c r="AB13" s="69"/>
-      <c r="AC13" s="69"/>
-      <c r="AD13" s="69"/>
-      <c r="AE13" s="69"/>
-      <c r="AF13" s="69"/>
-      <c r="AG13" s="69"/>
+      <c r="Y13" s="60"/>
+      <c r="Z13" s="60"/>
+      <c r="AA13" s="60"/>
+      <c r="AB13" s="60"/>
+      <c r="AC13" s="60"/>
+      <c r="AD13" s="60"/>
+      <c r="AE13" s="60"/>
+      <c r="AF13" s="60"/>
+      <c r="AG13" s="60"/>
       <c r="AH13" s="24"/>
       <c r="AI13" s="24"/>
       <c r="AJ13" s="24"/>
@@ -2498,9 +2557,12 @@
       <c r="AZ13" s="24"/>
       <c r="BA13" s="24"/>
       <c r="BB13" s="24"/>
+      <c r="BC13" s="24"/>
+      <c r="BD13" s="24"/>
+      <c r="BE13" s="24"/>
     </row>
-    <row r="14" spans="1:54" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="70"/>
+    <row r="14" spans="1:57" ht="45" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A14" s="61"/>
       <c r="B14" s="52"/>
       <c r="C14" s="51">
         <v>4</v>
@@ -2538,15 +2600,15 @@
       <c r="V14" s="54"/>
       <c r="W14" s="54"/>
       <c r="X14" s="54"/>
-      <c r="Y14" s="69"/>
-      <c r="Z14" s="69"/>
-      <c r="AA14" s="69"/>
-      <c r="AB14" s="69"/>
-      <c r="AC14" s="69"/>
-      <c r="AD14" s="69"/>
-      <c r="AE14" s="69"/>
-      <c r="AF14" s="69"/>
-      <c r="AG14" s="69"/>
+      <c r="Y14" s="60"/>
+      <c r="Z14" s="60"/>
+      <c r="AA14" s="60"/>
+      <c r="AB14" s="60"/>
+      <c r="AC14" s="60"/>
+      <c r="AD14" s="60"/>
+      <c r="AE14" s="60"/>
+      <c r="AF14" s="60"/>
+      <c r="AG14" s="60"/>
       <c r="AH14" s="54"/>
       <c r="AI14" s="54"/>
       <c r="AJ14" s="54"/>
@@ -2568,10 +2630,53 @@
       <c r="AZ14" s="54"/>
       <c r="BA14" s="54"/>
       <c r="BB14" s="54"/>
+      <c r="BC14" s="54"/>
+      <c r="BD14" s="54"/>
+      <c r="BE14" s="54"/>
     </row>
-    <row r="15" spans="1:54" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:57" ht="15.75" thickTop="1"/>
   </sheetData>
-  <mergeCells count="53">
+  <mergeCells count="56">
+    <mergeCell ref="BC3:BE3"/>
+    <mergeCell ref="BC4:BE4"/>
+    <mergeCell ref="BC5:BE5"/>
+    <mergeCell ref="AW3:AY3"/>
+    <mergeCell ref="AW4:AY4"/>
+    <mergeCell ref="AW5:AY5"/>
+    <mergeCell ref="AZ3:BB3"/>
+    <mergeCell ref="AZ4:BB4"/>
+    <mergeCell ref="AZ5:BB5"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="Y3:AA3"/>
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="AH3:AJ3"/>
+    <mergeCell ref="AK3:AM3"/>
+    <mergeCell ref="AN3:AP3"/>
+    <mergeCell ref="AQ3:AS3"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="AT3:AV3"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="AB4:AD4"/>
+    <mergeCell ref="AE4:AG4"/>
+    <mergeCell ref="AH4:AJ4"/>
+    <mergeCell ref="AK4:AM4"/>
+    <mergeCell ref="AN4:AP4"/>
+    <mergeCell ref="AQ4:AS4"/>
+    <mergeCell ref="AT4:AV4"/>
     <mergeCell ref="AN5:AP5"/>
     <mergeCell ref="AQ5:AS5"/>
     <mergeCell ref="AT5:AV5"/>
@@ -2588,43 +2693,6 @@
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="M5:O5"/>
     <mergeCell ref="P5:R5"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="V5:X5"/>
-    <mergeCell ref="AT3:AV3"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="V4:X4"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="AB4:AD4"/>
-    <mergeCell ref="AE4:AG4"/>
-    <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="AK4:AM4"/>
-    <mergeCell ref="AN4:AP4"/>
-    <mergeCell ref="AQ4:AS4"/>
-    <mergeCell ref="AT4:AV4"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="AK3:AM3"/>
-    <mergeCell ref="AN3:AP3"/>
-    <mergeCell ref="AQ3:AS3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="Y3:AA3"/>
-    <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="AW3:AY3"/>
-    <mergeCell ref="AW4:AY4"/>
-    <mergeCell ref="AW5:AY5"/>
-    <mergeCell ref="AZ3:BB3"/>
-    <mergeCell ref="AZ4:BB4"/>
-    <mergeCell ref="AZ5:BB5"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Update results for ARIS
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -751,9 +751,36 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -767,33 +794,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1174,8 +1174,8 @@
   </sheetPr>
   <dimension ref="A1:AMK15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AA1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BA10" sqref="BA10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AN1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BA8" sqref="BA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1198,18 +1198,18 @@
       </c>
     </row>
     <row r="2" spans="1:57" ht="47.25" thickTop="1" thickBot="1">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70" t="s">
+      <c r="B2" s="61"/>
+      <c r="C2" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70" t="s">
+      <c r="D2" s="61"/>
+      <c r="E2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="70"/>
+      <c r="F2" s="61"/>
       <c r="G2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1376,84 +1376,84 @@
       <c r="I3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="71" t="s">
+      <c r="J3" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="72" t="s">
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="65" t="s">
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="65" t="s">
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="T3" s="65"/>
-      <c r="U3" s="65"/>
-      <c r="V3" s="65" t="s">
+      <c r="T3" s="58"/>
+      <c r="U3" s="58"/>
+      <c r="V3" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="W3" s="65"/>
-      <c r="X3" s="65"/>
-      <c r="Y3" s="65" t="s">
+      <c r="W3" s="58"/>
+      <c r="X3" s="58"/>
+      <c r="Y3" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="Z3" s="65"/>
-      <c r="AA3" s="65"/>
-      <c r="AB3" s="65" t="s">
+      <c r="Z3" s="58"/>
+      <c r="AA3" s="58"/>
+      <c r="AB3" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="AC3" s="65"/>
-      <c r="AD3" s="65"/>
-      <c r="AE3" s="65" t="s">
+      <c r="AC3" s="58"/>
+      <c r="AD3" s="58"/>
+      <c r="AE3" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="AF3" s="65"/>
-      <c r="AG3" s="65"/>
-      <c r="AH3" s="65" t="s">
+      <c r="AF3" s="58"/>
+      <c r="AG3" s="58"/>
+      <c r="AH3" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="AI3" s="65"/>
-      <c r="AJ3" s="65"/>
-      <c r="AK3" s="69" t="s">
+      <c r="AI3" s="58"/>
+      <c r="AJ3" s="58"/>
+      <c r="AK3" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="AL3" s="69"/>
-      <c r="AM3" s="69"/>
-      <c r="AN3" s="65" t="s">
+      <c r="AL3" s="64"/>
+      <c r="AM3" s="64"/>
+      <c r="AN3" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="AO3" s="65"/>
-      <c r="AP3" s="65"/>
-      <c r="AQ3" s="65" t="s">
+      <c r="AO3" s="58"/>
+      <c r="AP3" s="58"/>
+      <c r="AQ3" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="AR3" s="65"/>
-      <c r="AS3" s="65"/>
-      <c r="AT3" s="65" t="s">
+      <c r="AR3" s="58"/>
+      <c r="AS3" s="58"/>
+      <c r="AT3" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="AU3" s="65"/>
-      <c r="AV3" s="65"/>
-      <c r="AW3" s="65" t="s">
+      <c r="AU3" s="58"/>
+      <c r="AV3" s="58"/>
+      <c r="AW3" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="AX3" s="65"/>
-      <c r="AY3" s="65"/>
-      <c r="AZ3" s="65" t="s">
+      <c r="AX3" s="58"/>
+      <c r="AY3" s="58"/>
+      <c r="AZ3" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="BA3" s="65"/>
-      <c r="BB3" s="65"/>
-      <c r="BC3" s="65"/>
-      <c r="BD3" s="65"/>
-      <c r="BE3" s="65"/>
+      <c r="BA3" s="58"/>
+      <c r="BB3" s="58"/>
+      <c r="BC3" s="58"/>
+      <c r="BD3" s="58"/>
+      <c r="BE3" s="58"/>
     </row>
     <row r="4" spans="1:57" s="15" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A4" s="12"/>
@@ -1472,79 +1472,79 @@
       </c>
       <c r="K4" s="66"/>
       <c r="L4" s="66"/>
-      <c r="M4" s="67" t="s">
+      <c r="M4" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="67"/>
-      <c r="O4" s="67"/>
-      <c r="P4" s="67" t="s">
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67" t="s">
+      <c r="Q4" s="59"/>
+      <c r="R4" s="59"/>
+      <c r="S4" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="T4" s="67"/>
-      <c r="U4" s="67"/>
-      <c r="V4" s="68" t="s">
+      <c r="T4" s="59"/>
+      <c r="U4" s="59"/>
+      <c r="V4" s="67" t="s">
         <v>79</v>
       </c>
-      <c r="W4" s="68"/>
-      <c r="X4" s="68"/>
-      <c r="Y4" s="67" t="s">
+      <c r="W4" s="67"/>
+      <c r="X4" s="67"/>
+      <c r="Y4" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="Z4" s="67"/>
-      <c r="AA4" s="67"/>
-      <c r="AB4" s="67">
+      <c r="Z4" s="59"/>
+      <c r="AA4" s="59"/>
+      <c r="AB4" s="59">
         <v>2.4</v>
       </c>
-      <c r="AC4" s="67"/>
-      <c r="AD4" s="67"/>
-      <c r="AE4" s="67" t="s">
+      <c r="AC4" s="59"/>
+      <c r="AD4" s="59"/>
+      <c r="AE4" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="AF4" s="67"/>
-      <c r="AG4" s="67"/>
-      <c r="AH4" s="67" t="s">
+      <c r="AF4" s="59"/>
+      <c r="AG4" s="59"/>
+      <c r="AH4" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="AI4" s="67"/>
-      <c r="AJ4" s="67"/>
-      <c r="AK4" s="67" t="s">
+      <c r="AI4" s="59"/>
+      <c r="AJ4" s="59"/>
+      <c r="AK4" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="AL4" s="67"/>
-      <c r="AM4" s="67"/>
-      <c r="AN4" s="67" t="s">
+      <c r="AL4" s="59"/>
+      <c r="AM4" s="59"/>
+      <c r="AN4" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="AO4" s="67"/>
-      <c r="AP4" s="67"/>
-      <c r="AQ4" s="67" t="s">
+      <c r="AO4" s="59"/>
+      <c r="AP4" s="59"/>
+      <c r="AQ4" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="AR4" s="67"/>
-      <c r="AS4" s="67"/>
-      <c r="AT4" s="67" t="s">
+      <c r="AR4" s="59"/>
+      <c r="AS4" s="59"/>
+      <c r="AT4" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="AU4" s="67"/>
-      <c r="AV4" s="67"/>
-      <c r="AW4" s="67" t="s">
+      <c r="AU4" s="59"/>
+      <c r="AV4" s="59"/>
+      <c r="AW4" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="AX4" s="67"/>
-      <c r="AY4" s="67"/>
-      <c r="AZ4" s="67" t="s">
+      <c r="AX4" s="59"/>
+      <c r="AY4" s="59"/>
+      <c r="AZ4" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="BA4" s="67"/>
-      <c r="BB4" s="67"/>
-      <c r="BC4" s="67"/>
-      <c r="BD4" s="67"/>
-      <c r="BE4" s="67"/>
+      <c r="BA4" s="59"/>
+      <c r="BB4" s="59"/>
+      <c r="BC4" s="59"/>
+      <c r="BD4" s="59"/>
+      <c r="BE4" s="59"/>
     </row>
     <row r="5" spans="1:57" ht="16.5" thickTop="1" thickBot="1">
       <c r="A5" s="16"/>
@@ -1558,87 +1558,87 @@
       <c r="I5" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="62">
+      <c r="J5" s="71">
         <v>41380</v>
       </c>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="63">
+      <c r="K5" s="71"/>
+      <c r="L5" s="71"/>
+      <c r="M5" s="72">
         <v>41373</v>
       </c>
-      <c r="N5" s="63"/>
-      <c r="O5" s="63"/>
-      <c r="P5" s="58">
+      <c r="N5" s="72"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="60">
         <v>41396</v>
       </c>
-      <c r="Q5" s="58"/>
-      <c r="R5" s="58"/>
-      <c r="S5" s="64">
+      <c r="Q5" s="60"/>
+      <c r="R5" s="60"/>
+      <c r="S5" s="65">
         <v>41383</v>
       </c>
-      <c r="T5" s="64"/>
-      <c r="U5" s="64"/>
-      <c r="V5" s="64">
+      <c r="T5" s="65"/>
+      <c r="U5" s="65"/>
+      <c r="V5" s="65">
         <v>41491</v>
       </c>
-      <c r="W5" s="64"/>
-      <c r="X5" s="64"/>
-      <c r="Y5" s="58">
+      <c r="W5" s="65"/>
+      <c r="X5" s="65"/>
+      <c r="Y5" s="60">
         <v>41394</v>
       </c>
-      <c r="Z5" s="58"/>
-      <c r="AA5" s="58"/>
-      <c r="AB5" s="58">
+      <c r="Z5" s="60"/>
+      <c r="AA5" s="60"/>
+      <c r="AB5" s="60">
         <v>41388</v>
       </c>
-      <c r="AC5" s="58"/>
-      <c r="AD5" s="58"/>
-      <c r="AE5" s="58">
+      <c r="AC5" s="60"/>
+      <c r="AD5" s="60"/>
+      <c r="AE5" s="60">
         <v>41388</v>
       </c>
-      <c r="AF5" s="58"/>
-      <c r="AG5" s="58"/>
-      <c r="AH5" s="58">
+      <c r="AF5" s="60"/>
+      <c r="AG5" s="60"/>
+      <c r="AH5" s="60">
         <v>41431</v>
       </c>
-      <c r="AI5" s="58"/>
-      <c r="AJ5" s="58"/>
-      <c r="AK5" s="58">
+      <c r="AI5" s="60"/>
+      <c r="AJ5" s="60"/>
+      <c r="AK5" s="60">
         <v>41467</v>
       </c>
-      <c r="AL5" s="58"/>
-      <c r="AM5" s="58"/>
-      <c r="AN5" s="58">
+      <c r="AL5" s="60"/>
+      <c r="AM5" s="60"/>
+      <c r="AN5" s="60">
         <v>41435</v>
       </c>
-      <c r="AO5" s="58"/>
-      <c r="AP5" s="58"/>
-      <c r="AQ5" s="58">
+      <c r="AO5" s="60"/>
+      <c r="AP5" s="60"/>
+      <c r="AQ5" s="60">
         <v>41449</v>
       </c>
-      <c r="AR5" s="58"/>
-      <c r="AS5" s="58"/>
-      <c r="AT5" s="58">
+      <c r="AR5" s="60"/>
+      <c r="AS5" s="60"/>
+      <c r="AT5" s="60">
         <v>41444</v>
       </c>
-      <c r="AU5" s="58"/>
-      <c r="AV5" s="58"/>
-      <c r="AW5" s="58">
+      <c r="AU5" s="60"/>
+      <c r="AV5" s="60"/>
+      <c r="AW5" s="60">
         <v>41465</v>
       </c>
-      <c r="AX5" s="58"/>
-      <c r="AY5" s="58"/>
-      <c r="AZ5" s="58">
+      <c r="AX5" s="60"/>
+      <c r="AY5" s="60"/>
+      <c r="AZ5" s="60">
         <v>41571</v>
       </c>
-      <c r="BA5" s="58"/>
-      <c r="BB5" s="58"/>
-      <c r="BC5" s="58"/>
-      <c r="BD5" s="58"/>
-      <c r="BE5" s="58"/>
+      <c r="BA5" s="60"/>
+      <c r="BB5" s="60"/>
+      <c r="BC5" s="60"/>
+      <c r="BD5" s="60"/>
+      <c r="BE5" s="60"/>
     </row>
     <row r="6" spans="1:57" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="68" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="19" t="s">
@@ -1708,21 +1708,21 @@
       <c r="X6" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="Y6" s="60" t="s">
+      <c r="Y6" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="Z6" s="60"/>
-      <c r="AA6" s="60"/>
-      <c r="AB6" s="60" t="s">
+      <c r="Z6" s="69"/>
+      <c r="AA6" s="69"/>
+      <c r="AB6" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="AC6" s="60"/>
-      <c r="AD6" s="60"/>
-      <c r="AE6" s="60" t="s">
+      <c r="AC6" s="69"/>
+      <c r="AD6" s="69"/>
+      <c r="AE6" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="AF6" s="60"/>
-      <c r="AG6" s="60"/>
+      <c r="AF6" s="69"/>
+      <c r="AG6" s="69"/>
       <c r="AH6" s="27" t="s">
         <v>44</v>
       </c>
@@ -1771,7 +1771,7 @@
       <c r="AY6" s="24"/>
       <c r="AZ6" s="27"/>
       <c r="BA6" s="24" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="BB6" s="24"/>
       <c r="BC6" s="27"/>
@@ -1779,7 +1779,7 @@
       <c r="BE6" s="24"/>
     </row>
     <row r="7" spans="1:57" ht="42.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="59"/>
+      <c r="A7" s="68"/>
       <c r="B7" s="30" t="s">
         <v>47</v>
       </c>
@@ -1847,15 +1847,15 @@
       <c r="X7" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="Y7" s="60"/>
-      <c r="Z7" s="60"/>
-      <c r="AA7" s="60"/>
-      <c r="AB7" s="60"/>
-      <c r="AC7" s="60"/>
-      <c r="AD7" s="60"/>
-      <c r="AE7" s="60"/>
-      <c r="AF7" s="60"/>
-      <c r="AG7" s="60"/>
+      <c r="Y7" s="69"/>
+      <c r="Z7" s="69"/>
+      <c r="AA7" s="69"/>
+      <c r="AB7" s="69"/>
+      <c r="AC7" s="69"/>
+      <c r="AD7" s="69"/>
+      <c r="AE7" s="69"/>
+      <c r="AF7" s="69"/>
+      <c r="AG7" s="69"/>
       <c r="AH7" s="27" t="s">
         <v>44</v>
       </c>
@@ -1904,7 +1904,7 @@
       <c r="AY7" s="24"/>
       <c r="AZ7" s="27"/>
       <c r="BA7" s="24" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="BB7" s="24"/>
       <c r="BC7" s="27"/>
@@ -1912,7 +1912,7 @@
       <c r="BE7" s="24"/>
     </row>
     <row r="8" spans="1:57" ht="43.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A8" s="59"/>
+      <c r="A8" s="68"/>
       <c r="B8" s="30"/>
       <c r="C8" s="20">
         <v>3</v>
@@ -1978,15 +1978,15 @@
       <c r="X8" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="Y8" s="60"/>
-      <c r="Z8" s="60"/>
-      <c r="AA8" s="60"/>
-      <c r="AB8" s="60"/>
-      <c r="AC8" s="60"/>
-      <c r="AD8" s="60"/>
-      <c r="AE8" s="60"/>
-      <c r="AF8" s="60"/>
-      <c r="AG8" s="60"/>
+      <c r="Y8" s="69"/>
+      <c r="Z8" s="69"/>
+      <c r="AA8" s="69"/>
+      <c r="AB8" s="69"/>
+      <c r="AC8" s="69"/>
+      <c r="AD8" s="69"/>
+      <c r="AE8" s="69"/>
+      <c r="AF8" s="69"/>
+      <c r="AG8" s="69"/>
       <c r="AH8" s="27" t="s">
         <v>43</v>
       </c>
@@ -2043,7 +2043,7 @@
       <c r="BE8" s="24"/>
     </row>
     <row r="9" spans="1:57" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A9" s="59"/>
+      <c r="A9" s="68"/>
       <c r="B9" s="30"/>
       <c r="C9" s="20">
         <v>4</v>
@@ -2109,15 +2109,15 @@
       <c r="X9" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="Y9" s="60"/>
-      <c r="Z9" s="60"/>
-      <c r="AA9" s="60"/>
-      <c r="AB9" s="60"/>
-      <c r="AC9" s="60"/>
-      <c r="AD9" s="60"/>
-      <c r="AE9" s="60"/>
-      <c r="AF9" s="60"/>
-      <c r="AG9" s="60"/>
+      <c r="Y9" s="69"/>
+      <c r="Z9" s="69"/>
+      <c r="AA9" s="69"/>
+      <c r="AB9" s="69"/>
+      <c r="AC9" s="69"/>
+      <c r="AD9" s="69"/>
+      <c r="AE9" s="69"/>
+      <c r="AF9" s="69"/>
+      <c r="AG9" s="69"/>
       <c r="AH9" s="24" t="s">
         <v>43</v>
       </c>
@@ -2216,15 +2216,15 @@
       <c r="V10" s="21"/>
       <c r="W10" s="21"/>
       <c r="X10" s="21"/>
-      <c r="Y10" s="60"/>
-      <c r="Z10" s="60"/>
-      <c r="AA10" s="60"/>
-      <c r="AB10" s="60"/>
-      <c r="AC10" s="60"/>
-      <c r="AD10" s="60"/>
-      <c r="AE10" s="60"/>
-      <c r="AF10" s="60"/>
-      <c r="AG10" s="60"/>
+      <c r="Y10" s="69"/>
+      <c r="Z10" s="69"/>
+      <c r="AA10" s="69"/>
+      <c r="AB10" s="69"/>
+      <c r="AC10" s="69"/>
+      <c r="AD10" s="69"/>
+      <c r="AE10" s="69"/>
+      <c r="AF10" s="69"/>
+      <c r="AG10" s="69"/>
       <c r="AH10" s="24"/>
       <c r="AI10" s="20"/>
       <c r="AJ10" s="24"/>
@@ -2253,7 +2253,7 @@
       <c r="BE10" s="24"/>
     </row>
     <row r="11" spans="1:57" s="47" customFormat="1" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A11" s="61" t="s">
+      <c r="A11" s="70" t="s">
         <v>57</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -2315,15 +2315,15 @@
       <c r="X11" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="Y11" s="60"/>
-      <c r="Z11" s="60"/>
-      <c r="AA11" s="60"/>
-      <c r="AB11" s="60"/>
-      <c r="AC11" s="60"/>
-      <c r="AD11" s="60"/>
-      <c r="AE11" s="60"/>
-      <c r="AF11" s="60"/>
-      <c r="AG11" s="60"/>
+      <c r="Y11" s="69"/>
+      <c r="Z11" s="69"/>
+      <c r="AA11" s="69"/>
+      <c r="AB11" s="69"/>
+      <c r="AC11" s="69"/>
+      <c r="AD11" s="69"/>
+      <c r="AE11" s="69"/>
+      <c r="AF11" s="69"/>
+      <c r="AG11" s="69"/>
       <c r="AH11" s="24" t="s">
         <v>43</v>
       </c>
@@ -2374,7 +2374,7 @@
       <c r="BE11" s="24"/>
     </row>
     <row r="12" spans="1:57" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A12" s="61"/>
+      <c r="A12" s="70"/>
       <c r="B12" s="30" t="s">
         <v>62</v>
       </c>
@@ -2430,15 +2430,15 @@
       <c r="X12" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="Y12" s="60"/>
-      <c r="Z12" s="60"/>
-      <c r="AA12" s="60"/>
-      <c r="AB12" s="60"/>
-      <c r="AC12" s="60"/>
-      <c r="AD12" s="60"/>
-      <c r="AE12" s="60"/>
-      <c r="AF12" s="60"/>
-      <c r="AG12" s="60"/>
+      <c r="Y12" s="69"/>
+      <c r="Z12" s="69"/>
+      <c r="AA12" s="69"/>
+      <c r="AB12" s="69"/>
+      <c r="AC12" s="69"/>
+      <c r="AD12" s="69"/>
+      <c r="AE12" s="69"/>
+      <c r="AF12" s="69"/>
+      <c r="AG12" s="69"/>
       <c r="AH12" s="24" t="s">
         <v>43</v>
       </c>
@@ -2489,7 +2489,7 @@
       <c r="BE12" s="24"/>
     </row>
     <row r="13" spans="1:57" ht="63" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A13" s="61"/>
+      <c r="A13" s="70"/>
       <c r="B13" s="30"/>
       <c r="C13" s="48">
         <v>3</v>
@@ -2527,15 +2527,15 @@
       <c r="V13" s="24"/>
       <c r="W13" s="24"/>
       <c r="X13" s="24"/>
-      <c r="Y13" s="60"/>
-      <c r="Z13" s="60"/>
-      <c r="AA13" s="60"/>
-      <c r="AB13" s="60"/>
-      <c r="AC13" s="60"/>
-      <c r="AD13" s="60"/>
-      <c r="AE13" s="60"/>
-      <c r="AF13" s="60"/>
-      <c r="AG13" s="60"/>
+      <c r="Y13" s="69"/>
+      <c r="Z13" s="69"/>
+      <c r="AA13" s="69"/>
+      <c r="AB13" s="69"/>
+      <c r="AC13" s="69"/>
+      <c r="AD13" s="69"/>
+      <c r="AE13" s="69"/>
+      <c r="AF13" s="69"/>
+      <c r="AG13" s="69"/>
       <c r="AH13" s="24"/>
       <c r="AI13" s="24"/>
       <c r="AJ13" s="24"/>
@@ -2562,7 +2562,7 @@
       <c r="BE13" s="24"/>
     </row>
     <row r="14" spans="1:57" ht="45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A14" s="61"/>
+      <c r="A14" s="70"/>
       <c r="B14" s="52"/>
       <c r="C14" s="51">
         <v>4</v>
@@ -2600,15 +2600,15 @@
       <c r="V14" s="54"/>
       <c r="W14" s="54"/>
       <c r="X14" s="54"/>
-      <c r="Y14" s="60"/>
-      <c r="Z14" s="60"/>
-      <c r="AA14" s="60"/>
-      <c r="AB14" s="60"/>
-      <c r="AC14" s="60"/>
-      <c r="AD14" s="60"/>
-      <c r="AE14" s="60"/>
-      <c r="AF14" s="60"/>
-      <c r="AG14" s="60"/>
+      <c r="Y14" s="69"/>
+      <c r="Z14" s="69"/>
+      <c r="AA14" s="69"/>
+      <c r="AB14" s="69"/>
+      <c r="AC14" s="69"/>
+      <c r="AD14" s="69"/>
+      <c r="AE14" s="69"/>
+      <c r="AF14" s="69"/>
+      <c r="AG14" s="69"/>
       <c r="AH14" s="54"/>
       <c r="AI14" s="54"/>
       <c r="AJ14" s="54"/>
@@ -2637,30 +2637,22 @@
     <row r="15" spans="1:57" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="BC3:BE3"/>
-    <mergeCell ref="BC4:BE4"/>
-    <mergeCell ref="BC5:BE5"/>
-    <mergeCell ref="AW3:AY3"/>
-    <mergeCell ref="AW4:AY4"/>
-    <mergeCell ref="AW5:AY5"/>
-    <mergeCell ref="AZ3:BB3"/>
-    <mergeCell ref="AZ4:BB4"/>
-    <mergeCell ref="AZ5:BB5"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="Y3:AA3"/>
-    <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="AK3:AM3"/>
-    <mergeCell ref="AN3:AP3"/>
-    <mergeCell ref="AQ3:AS3"/>
+    <mergeCell ref="AN5:AP5"/>
+    <mergeCell ref="AQ5:AS5"/>
+    <mergeCell ref="AT5:AV5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="Y6:AA14"/>
+    <mergeCell ref="AB6:AD14"/>
+    <mergeCell ref="AE6:AG14"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="Y5:AA5"/>
+    <mergeCell ref="AB5:AD5"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AK5:AM5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="P5:R5"/>
     <mergeCell ref="S5:U5"/>
     <mergeCell ref="V5:X5"/>
     <mergeCell ref="AT3:AV3"/>
@@ -2677,22 +2669,30 @@
     <mergeCell ref="AN4:AP4"/>
     <mergeCell ref="AQ4:AS4"/>
     <mergeCell ref="AT4:AV4"/>
-    <mergeCell ref="AN5:AP5"/>
-    <mergeCell ref="AQ5:AS5"/>
-    <mergeCell ref="AT5:AV5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="Y6:AA14"/>
-    <mergeCell ref="AB6:AD14"/>
-    <mergeCell ref="AE6:AG14"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="Y5:AA5"/>
-    <mergeCell ref="AB5:AD5"/>
-    <mergeCell ref="AE5:AG5"/>
-    <mergeCell ref="AH5:AJ5"/>
-    <mergeCell ref="AK5:AM5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="AH3:AJ3"/>
+    <mergeCell ref="AK3:AM3"/>
+    <mergeCell ref="AN3:AP3"/>
+    <mergeCell ref="AQ3:AS3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="Y3:AA3"/>
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="BC3:BE3"/>
+    <mergeCell ref="BC4:BE4"/>
+    <mergeCell ref="BC5:BE5"/>
+    <mergeCell ref="AW3:AY3"/>
+    <mergeCell ref="AW4:AY4"/>
+    <mergeCell ref="AW5:AY5"/>
+    <mergeCell ref="AZ3:BB3"/>
+    <mergeCell ref="AZ4:BB4"/>
+    <mergeCell ref="AZ5:BB5"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Add test results camunda Modeler 2.2.0 and bpmn.js
- add results for camunda Modeler 2.2.0 import and roundtrip test
- add results for camunda-bpmn.js import test
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="631"/>
@@ -13,6 +13,116 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>mschoe</author>
+  </authors>
+  <commentList>
+    <comment ref="P8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>mschoe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+sub process not collapsed. Wrong interpretaion of missing isExpanded attribute </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>mschoe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+modeler cannot display lanes without pools</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>mschoe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- collapsed Call Activities can be displayed only
+- Group is missing
+- collapsed sub process is displayed as expanded</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>mschoe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- collapsed Call Activities can be displayed only
+- collapsed sub process is displayed as expanded
+- group is missing</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="83">
   <si>
@@ -95,9 +205,6 @@
   </si>
   <si>
     <t>6.7.5</t>
-  </si>
-  <si>
-    <t>2.0.12</t>
   </si>
   <si>
     <t>8.0.1</t>
@@ -329,9 +436,6 @@
     <t>camunda-bpmn.js</t>
   </si>
   <si>
-    <t>c69eb6372f5d76135d83fd3a5d3a87d09470b37e</t>
-  </si>
-  <si>
     <t>Vertical</t>
   </si>
   <si>
@@ -359,6 +463,12 @@
   </si>
   <si>
     <t>7.2.4</t>
+  </si>
+  <si>
+    <t>2.0.2</t>
+  </si>
+  <si>
+    <t>c906a7c941b82dbb832ed9be62989c171c724199</t>
   </si>
 </sst>
 </file>
@@ -368,7 +478,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -412,6 +522,19 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -751,14 +874,41 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -769,36 +919,9 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="TableStyleLight1" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -883,9 +1006,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -923,7 +1046,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -995,7 +1118,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1168,17 +1291,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AMK15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AN1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BA8" sqref="BA8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AH4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AW11" sqref="AW11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="44.85546875" style="1"/>
@@ -1198,18 +1321,18 @@
       </c>
     </row>
     <row r="2" spans="1:57" ht="47.25" thickTop="1" thickBot="1">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61" t="s">
+      <c r="B2" s="70"/>
+      <c r="C2" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61" t="s">
+      <c r="D2" s="70"/>
+      <c r="E2" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="61"/>
+      <c r="F2" s="70"/>
       <c r="G2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1376,84 +1499,84 @@
       <c r="I3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="62" t="s">
+      <c r="J3" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="63" t="s">
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="58" t="s">
+      <c r="N3" s="72"/>
+      <c r="O3" s="72"/>
+      <c r="P3" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="58"/>
-      <c r="S3" s="58" t="s">
+      <c r="Q3" s="65"/>
+      <c r="R3" s="65"/>
+      <c r="S3" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="T3" s="58"/>
-      <c r="U3" s="58"/>
-      <c r="V3" s="58" t="s">
+      <c r="T3" s="65"/>
+      <c r="U3" s="65"/>
+      <c r="V3" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="W3" s="58"/>
-      <c r="X3" s="58"/>
-      <c r="Y3" s="58" t="s">
+      <c r="W3" s="65"/>
+      <c r="X3" s="65"/>
+      <c r="Y3" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="Z3" s="58"/>
-      <c r="AA3" s="58"/>
-      <c r="AB3" s="58" t="s">
+      <c r="Z3" s="65"/>
+      <c r="AA3" s="65"/>
+      <c r="AB3" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="AC3" s="58"/>
-      <c r="AD3" s="58"/>
-      <c r="AE3" s="58" t="s">
+      <c r="AC3" s="65"/>
+      <c r="AD3" s="65"/>
+      <c r="AE3" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="AF3" s="58"/>
-      <c r="AG3" s="58"/>
-      <c r="AH3" s="58" t="s">
+      <c r="AF3" s="65"/>
+      <c r="AG3" s="65"/>
+      <c r="AH3" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="AI3" s="58"/>
-      <c r="AJ3" s="58"/>
-      <c r="AK3" s="64" t="s">
+      <c r="AI3" s="65"/>
+      <c r="AJ3" s="65"/>
+      <c r="AK3" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="AL3" s="64"/>
-      <c r="AM3" s="64"/>
-      <c r="AN3" s="58" t="s">
+      <c r="AL3" s="69"/>
+      <c r="AM3" s="69"/>
+      <c r="AN3" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="AO3" s="58"/>
-      <c r="AP3" s="58"/>
-      <c r="AQ3" s="58" t="s">
+      <c r="AO3" s="65"/>
+      <c r="AP3" s="65"/>
+      <c r="AQ3" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="AR3" s="58"/>
-      <c r="AS3" s="58"/>
-      <c r="AT3" s="58" t="s">
+      <c r="AR3" s="65"/>
+      <c r="AS3" s="65"/>
+      <c r="AT3" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="AU3" s="58"/>
-      <c r="AV3" s="58"/>
-      <c r="AW3" s="58" t="s">
-        <v>72</v>
-      </c>
-      <c r="AX3" s="58"/>
-      <c r="AY3" s="58"/>
-      <c r="AZ3" s="58" t="s">
-        <v>81</v>
-      </c>
-      <c r="BA3" s="58"/>
-      <c r="BB3" s="58"/>
-      <c r="BC3" s="58"/>
-      <c r="BD3" s="58"/>
-      <c r="BE3" s="58"/>
+      <c r="AU3" s="65"/>
+      <c r="AV3" s="65"/>
+      <c r="AW3" s="65" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX3" s="65"/>
+      <c r="AY3" s="65"/>
+      <c r="AZ3" s="65" t="s">
+        <v>79</v>
+      </c>
+      <c r="BA3" s="65"/>
+      <c r="BB3" s="65"/>
+      <c r="BC3" s="65"/>
+      <c r="BD3" s="65"/>
+      <c r="BE3" s="65"/>
     </row>
     <row r="4" spans="1:57" s="15" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A4" s="12"/>
@@ -1472,79 +1595,79 @@
       </c>
       <c r="K4" s="66"/>
       <c r="L4" s="66"/>
-      <c r="M4" s="59" t="s">
+      <c r="M4" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="59"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="59" t="s">
+      <c r="N4" s="67"/>
+      <c r="O4" s="67"/>
+      <c r="P4" s="67" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q4" s="67"/>
+      <c r="R4" s="67"/>
+      <c r="S4" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="Q4" s="59"/>
-      <c r="R4" s="59"/>
-      <c r="S4" s="59" t="s">
+      <c r="T4" s="67"/>
+      <c r="U4" s="67"/>
+      <c r="V4" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="W4" s="68"/>
+      <c r="X4" s="68"/>
+      <c r="Y4" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="T4" s="59"/>
-      <c r="U4" s="59"/>
-      <c r="V4" s="67" t="s">
-        <v>79</v>
-      </c>
-      <c r="W4" s="67"/>
-      <c r="X4" s="67"/>
-      <c r="Y4" s="59" t="s">
+      <c r="Z4" s="67"/>
+      <c r="AA4" s="67"/>
+      <c r="AB4" s="67">
+        <v>2.4</v>
+      </c>
+      <c r="AC4" s="67"/>
+      <c r="AD4" s="67"/>
+      <c r="AE4" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="Z4" s="59"/>
-      <c r="AA4" s="59"/>
-      <c r="AB4" s="59">
-        <v>2.4</v>
-      </c>
-      <c r="AC4" s="59"/>
-      <c r="AD4" s="59"/>
-      <c r="AE4" s="59" t="s">
+      <c r="AF4" s="67"/>
+      <c r="AG4" s="67"/>
+      <c r="AH4" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="AF4" s="59"/>
-      <c r="AG4" s="59"/>
-      <c r="AH4" s="59" t="s">
+      <c r="AI4" s="67"/>
+      <c r="AJ4" s="67"/>
+      <c r="AK4" s="67" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL4" s="67"/>
+      <c r="AM4" s="67"/>
+      <c r="AN4" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="AI4" s="59"/>
-      <c r="AJ4" s="59"/>
-      <c r="AK4" s="59" t="s">
-        <v>78</v>
-      </c>
-      <c r="AL4" s="59"/>
-      <c r="AM4" s="59"/>
-      <c r="AN4" s="59" t="s">
+      <c r="AO4" s="67"/>
+      <c r="AP4" s="67"/>
+      <c r="AQ4" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="AO4" s="59"/>
-      <c r="AP4" s="59"/>
-      <c r="AQ4" s="59" t="s">
+      <c r="AR4" s="67"/>
+      <c r="AS4" s="67"/>
+      <c r="AT4" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="AR4" s="59"/>
-      <c r="AS4" s="59"/>
-      <c r="AT4" s="59" t="s">
-        <v>34</v>
-      </c>
-      <c r="AU4" s="59"/>
-      <c r="AV4" s="59"/>
-      <c r="AW4" s="59" t="s">
-        <v>73</v>
-      </c>
-      <c r="AX4" s="59"/>
-      <c r="AY4" s="59"/>
-      <c r="AZ4" s="59" t="s">
+      <c r="AU4" s="67"/>
+      <c r="AV4" s="67"/>
+      <c r="AW4" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="BA4" s="59"/>
-      <c r="BB4" s="59"/>
-      <c r="BC4" s="59"/>
-      <c r="BD4" s="59"/>
-      <c r="BE4" s="59"/>
+      <c r="AX4" s="67"/>
+      <c r="AY4" s="67"/>
+      <c r="AZ4" s="67" t="s">
+        <v>80</v>
+      </c>
+      <c r="BA4" s="67"/>
+      <c r="BB4" s="67"/>
+      <c r="BC4" s="67"/>
+      <c r="BD4" s="67"/>
+      <c r="BE4" s="67"/>
     </row>
     <row r="5" spans="1:57" ht="16.5" thickTop="1" thickBot="1">
       <c r="A5" s="16"/>
@@ -1556,222 +1679,222 @@
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
       <c r="I5" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" s="71">
+        <v>34</v>
+      </c>
+      <c r="J5" s="62">
         <v>41380</v>
       </c>
-      <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="72">
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="63">
         <v>41373</v>
       </c>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
-      <c r="P5" s="60">
-        <v>41396</v>
-      </c>
-      <c r="Q5" s="60"/>
-      <c r="R5" s="60"/>
-      <c r="S5" s="65">
+      <c r="N5" s="63"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="58">
+        <v>41591</v>
+      </c>
+      <c r="Q5" s="58"/>
+      <c r="R5" s="58"/>
+      <c r="S5" s="64">
         <v>41383</v>
       </c>
-      <c r="T5" s="65"/>
-      <c r="U5" s="65"/>
-      <c r="V5" s="65">
+      <c r="T5" s="64"/>
+      <c r="U5" s="64"/>
+      <c r="V5" s="64">
         <v>41491</v>
       </c>
-      <c r="W5" s="65"/>
-      <c r="X5" s="65"/>
-      <c r="Y5" s="60">
+      <c r="W5" s="64"/>
+      <c r="X5" s="64"/>
+      <c r="Y5" s="58">
         <v>41394</v>
       </c>
-      <c r="Z5" s="60"/>
-      <c r="AA5" s="60"/>
-      <c r="AB5" s="60">
+      <c r="Z5" s="58"/>
+      <c r="AA5" s="58"/>
+      <c r="AB5" s="58">
         <v>41388</v>
       </c>
-      <c r="AC5" s="60"/>
-      <c r="AD5" s="60"/>
-      <c r="AE5" s="60">
+      <c r="AC5" s="58"/>
+      <c r="AD5" s="58"/>
+      <c r="AE5" s="58">
         <v>41388</v>
       </c>
-      <c r="AF5" s="60"/>
-      <c r="AG5" s="60"/>
-      <c r="AH5" s="60">
+      <c r="AF5" s="58"/>
+      <c r="AG5" s="58"/>
+      <c r="AH5" s="58">
         <v>41431</v>
       </c>
-      <c r="AI5" s="60"/>
-      <c r="AJ5" s="60"/>
-      <c r="AK5" s="60">
+      <c r="AI5" s="58"/>
+      <c r="AJ5" s="58"/>
+      <c r="AK5" s="58">
         <v>41467</v>
       </c>
-      <c r="AL5" s="60"/>
-      <c r="AM5" s="60"/>
-      <c r="AN5" s="60">
+      <c r="AL5" s="58"/>
+      <c r="AM5" s="58"/>
+      <c r="AN5" s="58">
         <v>41435</v>
       </c>
-      <c r="AO5" s="60"/>
-      <c r="AP5" s="60"/>
-      <c r="AQ5" s="60">
+      <c r="AO5" s="58"/>
+      <c r="AP5" s="58"/>
+      <c r="AQ5" s="58">
         <v>41449</v>
       </c>
-      <c r="AR5" s="60"/>
-      <c r="AS5" s="60"/>
-      <c r="AT5" s="60">
+      <c r="AR5" s="58"/>
+      <c r="AS5" s="58"/>
+      <c r="AT5" s="58">
         <v>41444</v>
       </c>
-      <c r="AU5" s="60"/>
-      <c r="AV5" s="60"/>
-      <c r="AW5" s="60">
-        <v>41465</v>
-      </c>
-      <c r="AX5" s="60"/>
-      <c r="AY5" s="60"/>
-      <c r="AZ5" s="60">
+      <c r="AU5" s="58"/>
+      <c r="AV5" s="58"/>
+      <c r="AW5" s="58">
+        <v>41591</v>
+      </c>
+      <c r="AX5" s="58"/>
+      <c r="AY5" s="58"/>
+      <c r="AZ5" s="58">
         <v>41571</v>
       </c>
-      <c r="BA5" s="60"/>
-      <c r="BB5" s="60"/>
-      <c r="BC5" s="60"/>
-      <c r="BD5" s="60"/>
-      <c r="BE5" s="60"/>
+      <c r="BA5" s="58"/>
+      <c r="BB5" s="58"/>
+      <c r="BC5" s="58"/>
+      <c r="BD5" s="58"/>
+      <c r="BE5" s="58"/>
     </row>
     <row r="6" spans="1:57" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="19" t="s">
         <v>36</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>37</v>
       </c>
       <c r="C6" s="20">
         <v>1</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" s="22">
         <v>0</v>
       </c>
       <c r="F6" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="H6" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="I6" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="I6" s="26" t="s">
-        <v>42</v>
-      </c>
       <c r="J6" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M6" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N6" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O6" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P6" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q6" s="24"/>
       <c r="R6" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="S6" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="T6" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="U6" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="V6" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="W6" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="X6" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y6" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="S6" s="28" t="s">
+      <c r="Z6" s="60"/>
+      <c r="AA6" s="60"/>
+      <c r="AB6" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="T6" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="U6" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="V6" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="W6" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="X6" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y6" s="69" t="s">
+      <c r="AC6" s="60"/>
+      <c r="AD6" s="60"/>
+      <c r="AE6" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="Z6" s="69"/>
-      <c r="AA6" s="69"/>
-      <c r="AB6" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC6" s="69"/>
-      <c r="AD6" s="69"/>
-      <c r="AE6" s="69" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF6" s="69"/>
-      <c r="AG6" s="69"/>
+      <c r="AF6" s="60"/>
+      <c r="AG6" s="60"/>
       <c r="AH6" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AI6" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AJ6" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AK6" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AL6" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AM6" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AN6" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AO6" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AP6" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AQ6" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AR6" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AS6" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AT6" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AU6" s="24"/>
       <c r="AV6" s="24"/>
       <c r="AW6" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AX6" s="24"/>
       <c r="AY6" s="24"/>
       <c r="AZ6" s="27"/>
       <c r="BA6" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="BB6" s="24"/>
       <c r="BC6" s="27"/>
@@ -1779,132 +1902,132 @@
       <c r="BE6" s="24"/>
     </row>
     <row r="7" spans="1:57" ht="42.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="68"/>
+      <c r="A7" s="59"/>
       <c r="B7" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="20">
         <v>2</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" s="22">
         <v>0</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G7" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="31" t="s">
-        <v>50</v>
-      </c>
       <c r="I7" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J7" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K7" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M7" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N7" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O7" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P7" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q7" s="24"/>
       <c r="R7" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="S7" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T7" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U7" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V7" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="W7" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="X7" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y7" s="69"/>
-      <c r="Z7" s="69"/>
-      <c r="AA7" s="69"/>
-      <c r="AB7" s="69"/>
-      <c r="AC7" s="69"/>
-      <c r="AD7" s="69"/>
-      <c r="AE7" s="69"/>
-      <c r="AF7" s="69"/>
-      <c r="AG7" s="69"/>
+        <v>43</v>
+      </c>
+      <c r="Y7" s="60"/>
+      <c r="Z7" s="60"/>
+      <c r="AA7" s="60"/>
+      <c r="AB7" s="60"/>
+      <c r="AC7" s="60"/>
+      <c r="AD7" s="60"/>
+      <c r="AE7" s="60"/>
+      <c r="AF7" s="60"/>
+      <c r="AG7" s="60"/>
       <c r="AH7" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AI7" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AJ7" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AK7" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AL7" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AM7" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AN7" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AO7" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AP7" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AQ7" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AR7" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AS7" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AT7" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AU7" s="24"/>
       <c r="AV7" s="24"/>
       <c r="AW7" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AX7" s="24"/>
       <c r="AY7" s="24"/>
       <c r="AZ7" s="27"/>
       <c r="BA7" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="BB7" s="24"/>
       <c r="BC7" s="27"/>
@@ -1912,130 +2035,130 @@
       <c r="BE7" s="24"/>
     </row>
     <row r="8" spans="1:57" ht="43.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A8" s="68"/>
+      <c r="A8" s="59"/>
       <c r="B8" s="30"/>
       <c r="C8" s="20">
         <v>3</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8" s="22">
         <v>0</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G8" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="31" t="s">
-        <v>53</v>
-      </c>
       <c r="I8" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J8" s="32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L8" s="33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M8" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N8" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O8" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P8" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q8" s="24"/>
       <c r="R8" s="22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="S8" s="34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T8" s="34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U8" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V8" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="W8" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="X8" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y8" s="69"/>
-      <c r="Z8" s="69"/>
-      <c r="AA8" s="69"/>
-      <c r="AB8" s="69"/>
-      <c r="AC8" s="69"/>
-      <c r="AD8" s="69"/>
-      <c r="AE8" s="69"/>
-      <c r="AF8" s="69"/>
-      <c r="AG8" s="69"/>
+        <v>43</v>
+      </c>
+      <c r="Y8" s="60"/>
+      <c r="Z8" s="60"/>
+      <c r="AA8" s="60"/>
+      <c r="AB8" s="60"/>
+      <c r="AC8" s="60"/>
+      <c r="AD8" s="60"/>
+      <c r="AE8" s="60"/>
+      <c r="AF8" s="60"/>
+      <c r="AG8" s="60"/>
       <c r="AH8" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AI8" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AJ8" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AK8" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AL8" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AM8" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AN8" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AO8" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AP8" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AQ8" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AR8" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AS8" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AT8" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AU8" s="24"/>
       <c r="AV8" s="24"/>
       <c r="AW8" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AX8" s="24"/>
       <c r="AY8" s="24"/>
       <c r="AZ8" s="27"/>
       <c r="BA8" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="BB8" s="24"/>
       <c r="BC8" s="27"/>
@@ -2043,130 +2166,130 @@
       <c r="BE8" s="24"/>
     </row>
     <row r="9" spans="1:57" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A9" s="68"/>
+      <c r="A9" s="59"/>
       <c r="B9" s="30"/>
       <c r="C9" s="20">
         <v>4</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E9" s="22">
         <v>0</v>
       </c>
       <c r="F9" s="56" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G9" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="57" t="s">
-        <v>56</v>
-      </c>
       <c r="I9" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J9" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L9" s="40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M9" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N9" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O9" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P9" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q9" s="20"/>
       <c r="R9" s="41" t="s">
         <v>43</v>
       </c>
       <c r="S9" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T9" s="43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U9" s="44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V9" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="W9" s="21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="X9" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y9" s="69"/>
-      <c r="Z9" s="69"/>
-      <c r="AA9" s="69"/>
-      <c r="AB9" s="69"/>
-      <c r="AC9" s="69"/>
-      <c r="AD9" s="69"/>
-      <c r="AE9" s="69"/>
-      <c r="AF9" s="69"/>
-      <c r="AG9" s="69"/>
+        <v>43</v>
+      </c>
+      <c r="Y9" s="60"/>
+      <c r="Z9" s="60"/>
+      <c r="AA9" s="60"/>
+      <c r="AB9" s="60"/>
+      <c r="AC9" s="60"/>
+      <c r="AD9" s="60"/>
+      <c r="AE9" s="60"/>
+      <c r="AF9" s="60"/>
+      <c r="AG9" s="60"/>
       <c r="AH9" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AI9" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AJ9" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AK9" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AL9" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AM9" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AN9" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AO9" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AP9" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AQ9" s="45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AR9" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AS9" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AT9" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AU9" s="20"/>
       <c r="AV9" s="24"/>
       <c r="AW9" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AX9" s="20"/>
       <c r="AY9" s="24"/>
       <c r="AZ9" s="27"/>
       <c r="BA9" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="BB9" s="24"/>
       <c r="BC9" s="27"/>
@@ -2180,22 +2303,22 @@
         <v>4</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E10" s="35">
         <v>1</v>
       </c>
       <c r="F10" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="G10" s="37" t="s">
+      <c r="I10" s="26" t="s">
         <v>75</v>
-      </c>
-      <c r="H10" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="I10" s="26" t="s">
-        <v>77</v>
       </c>
       <c r="J10" s="39"/>
       <c r="K10" s="20"/>
@@ -2216,15 +2339,15 @@
       <c r="V10" s="21"/>
       <c r="W10" s="21"/>
       <c r="X10" s="21"/>
-      <c r="Y10" s="69"/>
-      <c r="Z10" s="69"/>
-      <c r="AA10" s="69"/>
-      <c r="AB10" s="69"/>
-      <c r="AC10" s="69"/>
-      <c r="AD10" s="69"/>
-      <c r="AE10" s="69"/>
-      <c r="AF10" s="69"/>
-      <c r="AG10" s="69"/>
+      <c r="Y10" s="60"/>
+      <c r="Z10" s="60"/>
+      <c r="AA10" s="60"/>
+      <c r="AB10" s="60"/>
+      <c r="AC10" s="60"/>
+      <c r="AD10" s="60"/>
+      <c r="AE10" s="60"/>
+      <c r="AF10" s="60"/>
+      <c r="AG10" s="60"/>
       <c r="AH10" s="24"/>
       <c r="AI10" s="20"/>
       <c r="AJ10" s="24"/>
@@ -2253,116 +2376,116 @@
       <c r="BE10" s="24"/>
     </row>
     <row r="11" spans="1:57" s="47" customFormat="1" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A11" s="70" t="s">
+      <c r="A11" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>57</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>58</v>
       </c>
       <c r="C11" s="24">
         <v>1</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E11" s="24">
         <v>0</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G11" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="H11" s="46" t="s">
-        <v>61</v>
-      </c>
       <c r="I11" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K11" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L11" s="24"/>
       <c r="M11" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N11" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O11" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P11" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q11" s="24"/>
       <c r="R11" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S11" s="24"/>
       <c r="T11" s="24"/>
       <c r="U11" s="24"/>
       <c r="V11" s="23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="W11" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="X11" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y11" s="69"/>
-      <c r="Z11" s="69"/>
-      <c r="AA11" s="69"/>
-      <c r="AB11" s="69"/>
-      <c r="AC11" s="69"/>
-      <c r="AD11" s="69"/>
-      <c r="AE11" s="69"/>
-      <c r="AF11" s="69"/>
-      <c r="AG11" s="69"/>
+        <v>43</v>
+      </c>
+      <c r="Y11" s="60"/>
+      <c r="Z11" s="60"/>
+      <c r="AA11" s="60"/>
+      <c r="AB11" s="60"/>
+      <c r="AC11" s="60"/>
+      <c r="AD11" s="60"/>
+      <c r="AE11" s="60"/>
+      <c r="AF11" s="60"/>
+      <c r="AG11" s="60"/>
       <c r="AH11" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AI11" s="24"/>
       <c r="AJ11" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AK11" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AL11" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AM11" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AN11" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AO11" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AP11" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AQ11" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AR11" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AS11" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AT11" s="24"/>
       <c r="AU11" s="24"/>
       <c r="AV11" s="24"/>
       <c r="AW11" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AX11" s="24"/>
       <c r="AY11" s="24"/>
@@ -2374,110 +2497,110 @@
       <c r="BE11" s="24"/>
     </row>
     <row r="12" spans="1:57" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A12" s="70"/>
+      <c r="A12" s="61"/>
       <c r="B12" s="30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" s="24">
         <v>2</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E12" s="24">
         <v>0</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G12" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="H12" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="H12" s="46" t="s">
-        <v>65</v>
-      </c>
       <c r="I12" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J12" s="24"/>
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N12" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O12" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P12" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q12" s="24"/>
       <c r="R12" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S12" s="24"/>
       <c r="T12" s="24"/>
       <c r="U12" s="24"/>
       <c r="V12" s="23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="W12" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="X12" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y12" s="69"/>
-      <c r="Z12" s="69"/>
-      <c r="AA12" s="69"/>
-      <c r="AB12" s="69"/>
-      <c r="AC12" s="69"/>
-      <c r="AD12" s="69"/>
-      <c r="AE12" s="69"/>
-      <c r="AF12" s="69"/>
-      <c r="AG12" s="69"/>
+        <v>43</v>
+      </c>
+      <c r="Y12" s="60"/>
+      <c r="Z12" s="60"/>
+      <c r="AA12" s="60"/>
+      <c r="AB12" s="60"/>
+      <c r="AC12" s="60"/>
+      <c r="AD12" s="60"/>
+      <c r="AE12" s="60"/>
+      <c r="AF12" s="60"/>
+      <c r="AG12" s="60"/>
       <c r="AH12" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AI12" s="24"/>
       <c r="AJ12" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AK12" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AL12" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AM12" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AN12" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AO12" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AP12" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AQ12" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AR12" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AS12" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AT12" s="24"/>
       <c r="AU12" s="24"/>
       <c r="AV12" s="24"/>
       <c r="AW12" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AX12" s="24"/>
       <c r="AY12" s="24"/>
@@ -2489,28 +2612,28 @@
       <c r="BE12" s="24"/>
     </row>
     <row r="13" spans="1:57" ht="63" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A13" s="70"/>
+      <c r="A13" s="61"/>
       <c r="B13" s="30"/>
       <c r="C13" s="48">
         <v>3</v>
       </c>
       <c r="D13" s="49" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E13" s="50">
         <v>0</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G13" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="H13" s="31" t="s">
-        <v>68</v>
-      </c>
       <c r="I13" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J13" s="24"/>
       <c r="K13" s="24"/>
@@ -2527,15 +2650,15 @@
       <c r="V13" s="24"/>
       <c r="W13" s="24"/>
       <c r="X13" s="24"/>
-      <c r="Y13" s="69"/>
-      <c r="Z13" s="69"/>
-      <c r="AA13" s="69"/>
-      <c r="AB13" s="69"/>
-      <c r="AC13" s="69"/>
-      <c r="AD13" s="69"/>
-      <c r="AE13" s="69"/>
-      <c r="AF13" s="69"/>
-      <c r="AG13" s="69"/>
+      <c r="Y13" s="60"/>
+      <c r="Z13" s="60"/>
+      <c r="AA13" s="60"/>
+      <c r="AB13" s="60"/>
+      <c r="AC13" s="60"/>
+      <c r="AD13" s="60"/>
+      <c r="AE13" s="60"/>
+      <c r="AF13" s="60"/>
+      <c r="AG13" s="60"/>
       <c r="AH13" s="24"/>
       <c r="AI13" s="24"/>
       <c r="AJ13" s="24"/>
@@ -2562,28 +2685,28 @@
       <c r="BE13" s="24"/>
     </row>
     <row r="14" spans="1:57" ht="45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A14" s="70"/>
+      <c r="A14" s="61"/>
       <c r="B14" s="52"/>
       <c r="C14" s="51">
         <v>4</v>
       </c>
       <c r="D14" s="49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E14" s="50">
         <v>0</v>
       </c>
       <c r="F14" s="49" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G14" s="51" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="H14" s="53" t="s">
-        <v>71</v>
-      </c>
       <c r="I14" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J14" s="54"/>
       <c r="K14" s="54"/>
@@ -2600,15 +2723,15 @@
       <c r="V14" s="54"/>
       <c r="W14" s="54"/>
       <c r="X14" s="54"/>
-      <c r="Y14" s="69"/>
-      <c r="Z14" s="69"/>
-      <c r="AA14" s="69"/>
-      <c r="AB14" s="69"/>
-      <c r="AC14" s="69"/>
-      <c r="AD14" s="69"/>
-      <c r="AE14" s="69"/>
-      <c r="AF14" s="69"/>
-      <c r="AG14" s="69"/>
+      <c r="Y14" s="60"/>
+      <c r="Z14" s="60"/>
+      <c r="AA14" s="60"/>
+      <c r="AB14" s="60"/>
+      <c r="AC14" s="60"/>
+      <c r="AD14" s="60"/>
+      <c r="AE14" s="60"/>
+      <c r="AF14" s="60"/>
+      <c r="AG14" s="60"/>
       <c r="AH14" s="54"/>
       <c r="AI14" s="54"/>
       <c r="AJ14" s="54"/>
@@ -2637,6 +2760,46 @@
     <row r="15" spans="1:57" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="BC3:BE3"/>
+    <mergeCell ref="BC4:BE4"/>
+    <mergeCell ref="BC5:BE5"/>
+    <mergeCell ref="AW3:AY3"/>
+    <mergeCell ref="AW4:AY4"/>
+    <mergeCell ref="AW5:AY5"/>
+    <mergeCell ref="AZ3:BB3"/>
+    <mergeCell ref="AZ4:BB4"/>
+    <mergeCell ref="AZ5:BB5"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="Y3:AA3"/>
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="AH3:AJ3"/>
+    <mergeCell ref="AK3:AM3"/>
+    <mergeCell ref="AN3:AP3"/>
+    <mergeCell ref="AQ3:AS3"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="AT3:AV3"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="AB4:AD4"/>
+    <mergeCell ref="AE4:AG4"/>
+    <mergeCell ref="AH4:AJ4"/>
+    <mergeCell ref="AK4:AM4"/>
+    <mergeCell ref="AN4:AP4"/>
+    <mergeCell ref="AQ4:AS4"/>
+    <mergeCell ref="AT4:AV4"/>
     <mergeCell ref="AN5:AP5"/>
     <mergeCell ref="AQ5:AS5"/>
     <mergeCell ref="AT5:AV5"/>
@@ -2653,49 +2816,10 @@
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="M5:O5"/>
     <mergeCell ref="P5:R5"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="V5:X5"/>
-    <mergeCell ref="AT3:AV3"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="V4:X4"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="AB4:AD4"/>
-    <mergeCell ref="AE4:AG4"/>
-    <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="AK4:AM4"/>
-    <mergeCell ref="AN4:AP4"/>
-    <mergeCell ref="AQ4:AS4"/>
-    <mergeCell ref="AT4:AV4"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="AK3:AM3"/>
-    <mergeCell ref="AN3:AP3"/>
-    <mergeCell ref="AQ3:AS3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="Y3:AA3"/>
-    <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="BC3:BE3"/>
-    <mergeCell ref="BC4:BE4"/>
-    <mergeCell ref="BC5:BE5"/>
-    <mergeCell ref="AW3:AY3"/>
-    <mergeCell ref="AW4:AY4"/>
-    <mergeCell ref="AW5:AY5"/>
-    <mergeCell ref="AZ3:BB3"/>
-    <mergeCell ref="AZ4:BB4"/>
-    <mergeCell ref="AZ5:BB5"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added iGrafx Process 2013 for Six Sigma v15.0.4.1565 testing done on 2013-11-07	by Fatma Dandashi from Mitre.
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="631"/>
+    <workbookView xWindow="3360" yWindow="-75" windowWidth="20925" windowHeight="9405" tabRatio="631"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case Structure" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="85">
   <si>
     <t>Note: Tools that are not listed here have either not been tested or may not support both BPMN import and export.</t>
   </si>
@@ -469,6 +469,12 @@
   </si>
   <si>
     <t>c906a7c941b82dbb832ed9be62989c171c724199</t>
+  </si>
+  <si>
+    <t>iGrafx Process 2013 for Six Sigma</t>
+  </si>
+  <si>
+    <t>15.0.4.1565</t>
   </si>
 </sst>
 </file>
@@ -707,7 +713,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -874,9 +880,36 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -892,36 +925,18 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="TableStyleLight1" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1006,9 +1021,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1046,7 +1061,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1118,7 +1133,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1297,11 +1312,11 @@
   </sheetPr>
   <dimension ref="A1:AMK15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AH4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AW11" sqref="AW11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AO3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BD6" sqref="BD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="44.85546875" style="1"/>
@@ -1312,27 +1327,29 @@
     <col min="7" max="7" width="16.5703125" style="1"/>
     <col min="8" max="8" width="54.85546875" style="1"/>
     <col min="9" max="9" width="22.5703125" style="1"/>
-    <col min="10" max="1025" width="9.140625" style="1"/>
+    <col min="10" max="54" width="9.140625" style="1"/>
+    <col min="55" max="57" width="10" style="1" customWidth="1"/>
+    <col min="58" max="1025" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="15.75" thickBot="1">
+    <row r="1" spans="1:60" ht="15.75" thickBot="1">
       <c r="K1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:57" ht="47.25" thickTop="1" thickBot="1">
-      <c r="A2" s="70" t="s">
+    <row r="2" spans="1:60" ht="47.25" thickTop="1" thickBot="1">
+      <c r="A2" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70" t="s">
+      <c r="B2" s="61"/>
+      <c r="C2" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70" t="s">
+      <c r="D2" s="61"/>
+      <c r="E2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="70"/>
+      <c r="F2" s="61"/>
       <c r="G2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1486,8 +1503,17 @@
       <c r="BE2" s="8" t="s">
         <v>9</v>
       </c>
+      <c r="BF2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="BG2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="BH2" s="8" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:57" ht="25.35" customHeight="1" thickTop="1" thickBot="1">
+    <row r="3" spans="1:60" ht="25.35" customHeight="1" thickTop="1" thickBot="1">
       <c r="A3" s="9"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -1499,86 +1525,91 @@
       <c r="I3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="71" t="s">
+      <c r="J3" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="72" t="s">
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="65" t="s">
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="65" t="s">
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="T3" s="65"/>
-      <c r="U3" s="65"/>
-      <c r="V3" s="65" t="s">
+      <c r="T3" s="58"/>
+      <c r="U3" s="58"/>
+      <c r="V3" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="W3" s="65"/>
-      <c r="X3" s="65"/>
-      <c r="Y3" s="65" t="s">
+      <c r="W3" s="58"/>
+      <c r="X3" s="58"/>
+      <c r="Y3" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="Z3" s="65"/>
-      <c r="AA3" s="65"/>
-      <c r="AB3" s="65" t="s">
+      <c r="Z3" s="58"/>
+      <c r="AA3" s="58"/>
+      <c r="AB3" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="AC3" s="65"/>
-      <c r="AD3" s="65"/>
-      <c r="AE3" s="65" t="s">
+      <c r="AC3" s="58"/>
+      <c r="AD3" s="58"/>
+      <c r="AE3" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="AF3" s="65"/>
-      <c r="AG3" s="65"/>
-      <c r="AH3" s="65" t="s">
+      <c r="AF3" s="58"/>
+      <c r="AG3" s="58"/>
+      <c r="AH3" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="AI3" s="65"/>
-      <c r="AJ3" s="65"/>
-      <c r="AK3" s="69" t="s">
+      <c r="AI3" s="58"/>
+      <c r="AJ3" s="58"/>
+      <c r="AK3" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="AL3" s="69"/>
-      <c r="AM3" s="69"/>
-      <c r="AN3" s="65" t="s">
+      <c r="AL3" s="64"/>
+      <c r="AM3" s="64"/>
+      <c r="AN3" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="AO3" s="65"/>
-      <c r="AP3" s="65"/>
-      <c r="AQ3" s="65" t="s">
+      <c r="AO3" s="58"/>
+      <c r="AP3" s="58"/>
+      <c r="AQ3" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="AR3" s="65"/>
-      <c r="AS3" s="65"/>
-      <c r="AT3" s="65" t="s">
+      <c r="AR3" s="58"/>
+      <c r="AS3" s="58"/>
+      <c r="AT3" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="AU3" s="65"/>
-      <c r="AV3" s="65"/>
-      <c r="AW3" s="65" t="s">
+      <c r="AU3" s="58"/>
+      <c r="AV3" s="58"/>
+      <c r="AW3" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="AX3" s="65"/>
-      <c r="AY3" s="65"/>
-      <c r="AZ3" s="65" t="s">
+      <c r="AX3" s="58"/>
+      <c r="AY3" s="58"/>
+      <c r="AZ3" s="58" t="s">
         <v>79</v>
       </c>
-      <c r="BA3" s="65"/>
-      <c r="BB3" s="65"/>
-      <c r="BC3" s="65"/>
-      <c r="BD3" s="65"/>
-      <c r="BE3" s="65"/>
+      <c r="BA3" s="58"/>
+      <c r="BB3" s="58"/>
+      <c r="BC3" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="BD3" s="73"/>
+      <c r="BE3" s="73"/>
+      <c r="BF3" s="58"/>
+      <c r="BG3" s="58"/>
+      <c r="BH3" s="58"/>
     </row>
-    <row r="4" spans="1:57" s="15" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1">
+    <row r="4" spans="1:60" s="15" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A4" s="12"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -1595,81 +1626,86 @@
       </c>
       <c r="K4" s="66"/>
       <c r="L4" s="66"/>
-      <c r="M4" s="67" t="s">
+      <c r="M4" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="67"/>
-      <c r="O4" s="67"/>
-      <c r="P4" s="67" t="s">
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67" t="s">
+      <c r="Q4" s="59"/>
+      <c r="R4" s="59"/>
+      <c r="S4" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="T4" s="67"/>
-      <c r="U4" s="67"/>
-      <c r="V4" s="68" t="s">
+      <c r="T4" s="59"/>
+      <c r="U4" s="59"/>
+      <c r="V4" s="67" t="s">
         <v>77</v>
       </c>
-      <c r="W4" s="68"/>
-      <c r="X4" s="68"/>
-      <c r="Y4" s="67" t="s">
+      <c r="W4" s="67"/>
+      <c r="X4" s="67"/>
+      <c r="Y4" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="Z4" s="67"/>
-      <c r="AA4" s="67"/>
-      <c r="AB4" s="67">
+      <c r="Z4" s="59"/>
+      <c r="AA4" s="59"/>
+      <c r="AB4" s="59">
         <v>2.4</v>
       </c>
-      <c r="AC4" s="67"/>
-      <c r="AD4" s="67"/>
-      <c r="AE4" s="67" t="s">
+      <c r="AC4" s="59"/>
+      <c r="AD4" s="59"/>
+      <c r="AE4" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="AF4" s="67"/>
-      <c r="AG4" s="67"/>
-      <c r="AH4" s="67" t="s">
+      <c r="AF4" s="59"/>
+      <c r="AG4" s="59"/>
+      <c r="AH4" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="AI4" s="67"/>
-      <c r="AJ4" s="67"/>
-      <c r="AK4" s="67" t="s">
+      <c r="AI4" s="59"/>
+      <c r="AJ4" s="59"/>
+      <c r="AK4" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="AL4" s="67"/>
-      <c r="AM4" s="67"/>
-      <c r="AN4" s="67" t="s">
+      <c r="AL4" s="59"/>
+      <c r="AM4" s="59"/>
+      <c r="AN4" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="AO4" s="67"/>
-      <c r="AP4" s="67"/>
-      <c r="AQ4" s="67" t="s">
+      <c r="AO4" s="59"/>
+      <c r="AP4" s="59"/>
+      <c r="AQ4" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="AR4" s="67"/>
-      <c r="AS4" s="67"/>
-      <c r="AT4" s="67" t="s">
+      <c r="AR4" s="59"/>
+      <c r="AS4" s="59"/>
+      <c r="AT4" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="AU4" s="67"/>
-      <c r="AV4" s="67"/>
-      <c r="AW4" s="67" t="s">
+      <c r="AU4" s="59"/>
+      <c r="AV4" s="59"/>
+      <c r="AW4" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="AX4" s="67"/>
-      <c r="AY4" s="67"/>
-      <c r="AZ4" s="67" t="s">
+      <c r="AX4" s="59"/>
+      <c r="AY4" s="59"/>
+      <c r="AZ4" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="BA4" s="67"/>
-      <c r="BB4" s="67"/>
-      <c r="BC4" s="67"/>
-      <c r="BD4" s="67"/>
-      <c r="BE4" s="67"/>
+      <c r="BA4" s="59"/>
+      <c r="BB4" s="59"/>
+      <c r="BC4" s="74" t="s">
+        <v>84</v>
+      </c>
+      <c r="BD4" s="74"/>
+      <c r="BE4" s="74"/>
+      <c r="BF4" s="59"/>
+      <c r="BG4" s="59"/>
+      <c r="BH4" s="59"/>
     </row>
-    <row r="5" spans="1:57" ht="16.5" thickTop="1" thickBot="1">
+    <row r="5" spans="1:60" ht="16.5" thickTop="1" thickBot="1">
       <c r="A5" s="16"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -1681,87 +1717,92 @@
       <c r="I5" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="62">
+      <c r="J5" s="71">
         <v>41380</v>
       </c>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="63">
+      <c r="K5" s="71"/>
+      <c r="L5" s="71"/>
+      <c r="M5" s="72">
         <v>41373</v>
       </c>
-      <c r="N5" s="63"/>
-      <c r="O5" s="63"/>
-      <c r="P5" s="58">
+      <c r="N5" s="72"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="60">
         <v>41591</v>
       </c>
-      <c r="Q5" s="58"/>
-      <c r="R5" s="58"/>
-      <c r="S5" s="64">
+      <c r="Q5" s="60"/>
+      <c r="R5" s="60"/>
+      <c r="S5" s="65">
         <v>41383</v>
       </c>
-      <c r="T5" s="64"/>
-      <c r="U5" s="64"/>
-      <c r="V5" s="64">
+      <c r="T5" s="65"/>
+      <c r="U5" s="65"/>
+      <c r="V5" s="65">
         <v>41491</v>
       </c>
-      <c r="W5" s="64"/>
-      <c r="X5" s="64"/>
-      <c r="Y5" s="58">
+      <c r="W5" s="65"/>
+      <c r="X5" s="65"/>
+      <c r="Y5" s="60">
         <v>41394</v>
       </c>
-      <c r="Z5" s="58"/>
-      <c r="AA5" s="58"/>
-      <c r="AB5" s="58">
+      <c r="Z5" s="60"/>
+      <c r="AA5" s="60"/>
+      <c r="AB5" s="60">
         <v>41388</v>
       </c>
-      <c r="AC5" s="58"/>
-      <c r="AD5" s="58"/>
-      <c r="AE5" s="58">
+      <c r="AC5" s="60"/>
+      <c r="AD5" s="60"/>
+      <c r="AE5" s="60">
         <v>41388</v>
       </c>
-      <c r="AF5" s="58"/>
-      <c r="AG5" s="58"/>
-      <c r="AH5" s="58">
+      <c r="AF5" s="60"/>
+      <c r="AG5" s="60"/>
+      <c r="AH5" s="60">
         <v>41431</v>
       </c>
-      <c r="AI5" s="58"/>
-      <c r="AJ5" s="58"/>
-      <c r="AK5" s="58">
+      <c r="AI5" s="60"/>
+      <c r="AJ5" s="60"/>
+      <c r="AK5" s="60">
         <v>41467</v>
       </c>
-      <c r="AL5" s="58"/>
-      <c r="AM5" s="58"/>
-      <c r="AN5" s="58">
+      <c r="AL5" s="60"/>
+      <c r="AM5" s="60"/>
+      <c r="AN5" s="60">
         <v>41435</v>
       </c>
-      <c r="AO5" s="58"/>
-      <c r="AP5" s="58"/>
-      <c r="AQ5" s="58">
+      <c r="AO5" s="60"/>
+      <c r="AP5" s="60"/>
+      <c r="AQ5" s="60">
         <v>41449</v>
       </c>
-      <c r="AR5" s="58"/>
-      <c r="AS5" s="58"/>
-      <c r="AT5" s="58">
+      <c r="AR5" s="60"/>
+      <c r="AS5" s="60"/>
+      <c r="AT5" s="60">
         <v>41444</v>
       </c>
-      <c r="AU5" s="58"/>
-      <c r="AV5" s="58"/>
-      <c r="AW5" s="58">
+      <c r="AU5" s="60"/>
+      <c r="AV5" s="60"/>
+      <c r="AW5" s="60">
         <v>41591</v>
       </c>
-      <c r="AX5" s="58"/>
-      <c r="AY5" s="58"/>
-      <c r="AZ5" s="58">
+      <c r="AX5" s="60"/>
+      <c r="AY5" s="60"/>
+      <c r="AZ5" s="60">
         <v>41571</v>
       </c>
-      <c r="BA5" s="58"/>
-      <c r="BB5" s="58"/>
-      <c r="BC5" s="58"/>
-      <c r="BD5" s="58"/>
-      <c r="BE5" s="58"/>
+      <c r="BA5" s="60"/>
+      <c r="BB5" s="60"/>
+      <c r="BC5" s="75">
+        <v>41585</v>
+      </c>
+      <c r="BD5" s="75"/>
+      <c r="BE5" s="75"/>
+      <c r="BF5" s="60"/>
+      <c r="BG5" s="60"/>
+      <c r="BH5" s="60"/>
     </row>
-    <row r="6" spans="1:57" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="59" t="s">
+    <row r="6" spans="1:60" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A6" s="68" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="19" t="s">
@@ -1831,21 +1872,21 @@
       <c r="X6" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="Y6" s="60" t="s">
+      <c r="Y6" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="Z6" s="60"/>
-      <c r="AA6" s="60"/>
-      <c r="AB6" s="60" t="s">
+      <c r="Z6" s="69"/>
+      <c r="AA6" s="69"/>
+      <c r="AB6" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="AC6" s="60"/>
-      <c r="AD6" s="60"/>
-      <c r="AE6" s="60" t="s">
+      <c r="AC6" s="69"/>
+      <c r="AD6" s="69"/>
+      <c r="AE6" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="AF6" s="60"/>
-      <c r="AG6" s="60"/>
+      <c r="AF6" s="69"/>
+      <c r="AG6" s="69"/>
       <c r="AH6" s="27" t="s">
         <v>43</v>
       </c>
@@ -1897,12 +1938,21 @@
         <v>43</v>
       </c>
       <c r="BB6" s="24"/>
-      <c r="BC6" s="27"/>
-      <c r="BD6" s="24"/>
-      <c r="BE6" s="24"/>
+      <c r="BC6" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BD6" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BE6" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BF6" s="27"/>
+      <c r="BG6" s="24"/>
+      <c r="BH6" s="24"/>
     </row>
-    <row r="7" spans="1:57" ht="42.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="59"/>
+    <row r="7" spans="1:60" ht="42.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A7" s="68"/>
       <c r="B7" s="30" t="s">
         <v>46</v>
       </c>
@@ -1970,15 +2020,15 @@
       <c r="X7" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="Y7" s="60"/>
-      <c r="Z7" s="60"/>
-      <c r="AA7" s="60"/>
-      <c r="AB7" s="60"/>
-      <c r="AC7" s="60"/>
-      <c r="AD7" s="60"/>
-      <c r="AE7" s="60"/>
-      <c r="AF7" s="60"/>
-      <c r="AG7" s="60"/>
+      <c r="Y7" s="69"/>
+      <c r="Z7" s="69"/>
+      <c r="AA7" s="69"/>
+      <c r="AB7" s="69"/>
+      <c r="AC7" s="69"/>
+      <c r="AD7" s="69"/>
+      <c r="AE7" s="69"/>
+      <c r="AF7" s="69"/>
+      <c r="AG7" s="69"/>
       <c r="AH7" s="27" t="s">
         <v>43</v>
       </c>
@@ -2030,12 +2080,21 @@
         <v>43</v>
       </c>
       <c r="BB7" s="24"/>
-      <c r="BC7" s="27"/>
-      <c r="BD7" s="24"/>
-      <c r="BE7" s="24"/>
+      <c r="BC7" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BD7" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BE7" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BF7" s="27"/>
+      <c r="BG7" s="24"/>
+      <c r="BH7" s="24"/>
     </row>
-    <row r="8" spans="1:57" ht="43.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A8" s="59"/>
+    <row r="8" spans="1:60" ht="43.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A8" s="68"/>
       <c r="B8" s="30"/>
       <c r="C8" s="20">
         <v>3</v>
@@ -2101,15 +2160,15 @@
       <c r="X8" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="Y8" s="60"/>
-      <c r="Z8" s="60"/>
-      <c r="AA8" s="60"/>
-      <c r="AB8" s="60"/>
-      <c r="AC8" s="60"/>
-      <c r="AD8" s="60"/>
-      <c r="AE8" s="60"/>
-      <c r="AF8" s="60"/>
-      <c r="AG8" s="60"/>
+      <c r="Y8" s="69"/>
+      <c r="Z8" s="69"/>
+      <c r="AA8" s="69"/>
+      <c r="AB8" s="69"/>
+      <c r="AC8" s="69"/>
+      <c r="AD8" s="69"/>
+      <c r="AE8" s="69"/>
+      <c r="AF8" s="69"/>
+      <c r="AG8" s="69"/>
       <c r="AH8" s="27" t="s">
         <v>42</v>
       </c>
@@ -2161,12 +2220,21 @@
         <v>42</v>
       </c>
       <c r="BB8" s="24"/>
-      <c r="BC8" s="27"/>
-      <c r="BD8" s="24"/>
-      <c r="BE8" s="24"/>
+      <c r="BC8" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BD8" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BE8" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BF8" s="27"/>
+      <c r="BG8" s="24"/>
+      <c r="BH8" s="24"/>
     </row>
-    <row r="9" spans="1:57" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A9" s="59"/>
+    <row r="9" spans="1:60" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A9" s="68"/>
       <c r="B9" s="30"/>
       <c r="C9" s="20">
         <v>4</v>
@@ -2232,15 +2300,15 @@
       <c r="X9" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="Y9" s="60"/>
-      <c r="Z9" s="60"/>
-      <c r="AA9" s="60"/>
-      <c r="AB9" s="60"/>
-      <c r="AC9" s="60"/>
-      <c r="AD9" s="60"/>
-      <c r="AE9" s="60"/>
-      <c r="AF9" s="60"/>
-      <c r="AG9" s="60"/>
+      <c r="Y9" s="69"/>
+      <c r="Z9" s="69"/>
+      <c r="AA9" s="69"/>
+      <c r="AB9" s="69"/>
+      <c r="AC9" s="69"/>
+      <c r="AD9" s="69"/>
+      <c r="AE9" s="69"/>
+      <c r="AF9" s="69"/>
+      <c r="AG9" s="69"/>
       <c r="AH9" s="24" t="s">
         <v>42</v>
       </c>
@@ -2292,11 +2360,20 @@
         <v>42</v>
       </c>
       <c r="BB9" s="24"/>
-      <c r="BC9" s="27"/>
-      <c r="BD9" s="20"/>
-      <c r="BE9" s="24"/>
+      <c r="BC9" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BD9" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BE9" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BF9" s="27"/>
+      <c r="BG9" s="20"/>
+      <c r="BH9" s="24"/>
     </row>
-    <row r="10" spans="1:57" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
+    <row r="10" spans="1:60" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A10" s="55"/>
       <c r="B10" s="30"/>
       <c r="C10" s="20">
@@ -2339,15 +2416,15 @@
       <c r="V10" s="21"/>
       <c r="W10" s="21"/>
       <c r="X10" s="21"/>
-      <c r="Y10" s="60"/>
-      <c r="Z10" s="60"/>
-      <c r="AA10" s="60"/>
-      <c r="AB10" s="60"/>
-      <c r="AC10" s="60"/>
-      <c r="AD10" s="60"/>
-      <c r="AE10" s="60"/>
-      <c r="AF10" s="60"/>
-      <c r="AG10" s="60"/>
+      <c r="Y10" s="69"/>
+      <c r="Z10" s="69"/>
+      <c r="AA10" s="69"/>
+      <c r="AB10" s="69"/>
+      <c r="AC10" s="69"/>
+      <c r="AD10" s="69"/>
+      <c r="AE10" s="69"/>
+      <c r="AF10" s="69"/>
+      <c r="AG10" s="69"/>
       <c r="AH10" s="24"/>
       <c r="AI10" s="20"/>
       <c r="AJ10" s="24"/>
@@ -2371,12 +2448,21 @@
       <c r="AZ10" s="27"/>
       <c r="BA10" s="20"/>
       <c r="BB10" s="24"/>
-      <c r="BC10" s="27"/>
-      <c r="BD10" s="20"/>
-      <c r="BE10" s="24"/>
+      <c r="BC10" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BD10" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BE10" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BF10" s="27"/>
+      <c r="BG10" s="20"/>
+      <c r="BH10" s="24"/>
     </row>
-    <row r="11" spans="1:57" s="47" customFormat="1" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A11" s="61" t="s">
+    <row r="11" spans="1:60" s="47" customFormat="1" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A11" s="70" t="s">
         <v>56</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -2438,15 +2524,15 @@
       <c r="X11" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="Y11" s="60"/>
-      <c r="Z11" s="60"/>
-      <c r="AA11" s="60"/>
-      <c r="AB11" s="60"/>
-      <c r="AC11" s="60"/>
-      <c r="AD11" s="60"/>
-      <c r="AE11" s="60"/>
-      <c r="AF11" s="60"/>
-      <c r="AG11" s="60"/>
+      <c r="Y11" s="69"/>
+      <c r="Z11" s="69"/>
+      <c r="AA11" s="69"/>
+      <c r="AB11" s="69"/>
+      <c r="AC11" s="69"/>
+      <c r="AD11" s="69"/>
+      <c r="AE11" s="69"/>
+      <c r="AF11" s="69"/>
+      <c r="AG11" s="69"/>
       <c r="AH11" s="24" t="s">
         <v>42</v>
       </c>
@@ -2492,12 +2578,21 @@
       <c r="AZ11" s="24"/>
       <c r="BA11" s="24"/>
       <c r="BB11" s="24"/>
-      <c r="BC11" s="24"/>
-      <c r="BD11" s="24"/>
-      <c r="BE11" s="24"/>
+      <c r="BC11" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BD11" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BE11" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BF11" s="24"/>
+      <c r="BG11" s="24"/>
+      <c r="BH11" s="24"/>
     </row>
-    <row r="12" spans="1:57" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A12" s="61"/>
+    <row r="12" spans="1:60" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A12" s="70"/>
       <c r="B12" s="30" t="s">
         <v>61</v>
       </c>
@@ -2553,15 +2648,15 @@
       <c r="X12" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="Y12" s="60"/>
-      <c r="Z12" s="60"/>
-      <c r="AA12" s="60"/>
-      <c r="AB12" s="60"/>
-      <c r="AC12" s="60"/>
-      <c r="AD12" s="60"/>
-      <c r="AE12" s="60"/>
-      <c r="AF12" s="60"/>
-      <c r="AG12" s="60"/>
+      <c r="Y12" s="69"/>
+      <c r="Z12" s="69"/>
+      <c r="AA12" s="69"/>
+      <c r="AB12" s="69"/>
+      <c r="AC12" s="69"/>
+      <c r="AD12" s="69"/>
+      <c r="AE12" s="69"/>
+      <c r="AF12" s="69"/>
+      <c r="AG12" s="69"/>
       <c r="AH12" s="24" t="s">
         <v>42</v>
       </c>
@@ -2607,12 +2702,21 @@
       <c r="AZ12" s="24"/>
       <c r="BA12" s="24"/>
       <c r="BB12" s="24"/>
-      <c r="BC12" s="24"/>
-      <c r="BD12" s="24"/>
-      <c r="BE12" s="24"/>
+      <c r="BC12" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BD12" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BE12" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BF12" s="24"/>
+      <c r="BG12" s="24"/>
+      <c r="BH12" s="24"/>
     </row>
-    <row r="13" spans="1:57" ht="63" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A13" s="61"/>
+    <row r="13" spans="1:60" ht="63" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A13" s="70"/>
       <c r="B13" s="30"/>
       <c r="C13" s="48">
         <v>3</v>
@@ -2650,15 +2754,15 @@
       <c r="V13" s="24"/>
       <c r="W13" s="24"/>
       <c r="X13" s="24"/>
-      <c r="Y13" s="60"/>
-      <c r="Z13" s="60"/>
-      <c r="AA13" s="60"/>
-      <c r="AB13" s="60"/>
-      <c r="AC13" s="60"/>
-      <c r="AD13" s="60"/>
-      <c r="AE13" s="60"/>
-      <c r="AF13" s="60"/>
-      <c r="AG13" s="60"/>
+      <c r="Y13" s="69"/>
+      <c r="Z13" s="69"/>
+      <c r="AA13" s="69"/>
+      <c r="AB13" s="69"/>
+      <c r="AC13" s="69"/>
+      <c r="AD13" s="69"/>
+      <c r="AE13" s="69"/>
+      <c r="AF13" s="69"/>
+      <c r="AG13" s="69"/>
       <c r="AH13" s="24"/>
       <c r="AI13" s="24"/>
       <c r="AJ13" s="24"/>
@@ -2683,9 +2787,12 @@
       <c r="BC13" s="24"/>
       <c r="BD13" s="24"/>
       <c r="BE13" s="24"/>
+      <c r="BF13" s="24"/>
+      <c r="BG13" s="24"/>
+      <c r="BH13" s="24"/>
     </row>
-    <row r="14" spans="1:57" ht="45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A14" s="61"/>
+    <row r="14" spans="1:60" ht="45" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A14" s="70"/>
       <c r="B14" s="52"/>
       <c r="C14" s="51">
         <v>4</v>
@@ -2723,15 +2830,15 @@
       <c r="V14" s="54"/>
       <c r="W14" s="54"/>
       <c r="X14" s="54"/>
-      <c r="Y14" s="60"/>
-      <c r="Z14" s="60"/>
-      <c r="AA14" s="60"/>
-      <c r="AB14" s="60"/>
-      <c r="AC14" s="60"/>
-      <c r="AD14" s="60"/>
-      <c r="AE14" s="60"/>
-      <c r="AF14" s="60"/>
-      <c r="AG14" s="60"/>
+      <c r="Y14" s="69"/>
+      <c r="Z14" s="69"/>
+      <c r="AA14" s="69"/>
+      <c r="AB14" s="69"/>
+      <c r="AC14" s="69"/>
+      <c r="AD14" s="69"/>
+      <c r="AE14" s="69"/>
+      <c r="AF14" s="69"/>
+      <c r="AG14" s="69"/>
       <c r="AH14" s="54"/>
       <c r="AI14" s="54"/>
       <c r="AJ14" s="54"/>
@@ -2756,34 +2863,32 @@
       <c r="BC14" s="54"/>
       <c r="BD14" s="54"/>
       <c r="BE14" s="54"/>
+      <c r="BF14" s="54"/>
+      <c r="BG14" s="54"/>
+      <c r="BH14" s="54"/>
     </row>
-    <row r="15" spans="1:57" ht="15.75" thickTop="1"/>
+    <row r="15" spans="1:60" ht="15.75" thickTop="1"/>
   </sheetData>
-  <mergeCells count="56">
-    <mergeCell ref="BC3:BE3"/>
-    <mergeCell ref="BC4:BE4"/>
-    <mergeCell ref="BC5:BE5"/>
-    <mergeCell ref="AW3:AY3"/>
-    <mergeCell ref="AW4:AY4"/>
-    <mergeCell ref="AW5:AY5"/>
-    <mergeCell ref="AZ3:BB3"/>
-    <mergeCell ref="AZ4:BB4"/>
-    <mergeCell ref="AZ5:BB5"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="Y3:AA3"/>
-    <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="AK3:AM3"/>
-    <mergeCell ref="AN3:AP3"/>
-    <mergeCell ref="AQ3:AS3"/>
+  <mergeCells count="59">
+    <mergeCell ref="BF3:BH3"/>
+    <mergeCell ref="BF4:BH4"/>
+    <mergeCell ref="BF5:BH5"/>
+    <mergeCell ref="AN5:AP5"/>
+    <mergeCell ref="AQ5:AS5"/>
+    <mergeCell ref="AT5:AV5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="Y6:AA14"/>
+    <mergeCell ref="AB6:AD14"/>
+    <mergeCell ref="AE6:AG14"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="Y5:AA5"/>
+    <mergeCell ref="AB5:AD5"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AK5:AM5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="P5:R5"/>
     <mergeCell ref="S5:U5"/>
     <mergeCell ref="V5:X5"/>
     <mergeCell ref="AT3:AV3"/>
@@ -2800,22 +2905,30 @@
     <mergeCell ref="AN4:AP4"/>
     <mergeCell ref="AQ4:AS4"/>
     <mergeCell ref="AT4:AV4"/>
-    <mergeCell ref="AN5:AP5"/>
-    <mergeCell ref="AQ5:AS5"/>
-    <mergeCell ref="AT5:AV5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="Y6:AA14"/>
-    <mergeCell ref="AB6:AD14"/>
-    <mergeCell ref="AE6:AG14"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="Y5:AA5"/>
-    <mergeCell ref="AB5:AD5"/>
-    <mergeCell ref="AE5:AG5"/>
-    <mergeCell ref="AH5:AJ5"/>
-    <mergeCell ref="AK5:AM5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="AH3:AJ3"/>
+    <mergeCell ref="AK3:AM3"/>
+    <mergeCell ref="AN3:AP3"/>
+    <mergeCell ref="AQ3:AS3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="Y3:AA3"/>
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="BC3:BE3"/>
+    <mergeCell ref="BC4:BE4"/>
+    <mergeCell ref="BC5:BE5"/>
+    <mergeCell ref="AW3:AY3"/>
+    <mergeCell ref="AW4:AY4"/>
+    <mergeCell ref="AW5:AY5"/>
+    <mergeCell ref="AZ3:BB3"/>
+    <mergeCell ref="AZ4:BB4"/>
+    <mergeCell ref="AZ5:BB5"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Added Yaoqiang 3.0.1 test results
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="86">
   <si>
     <t>Note: Tools that are not listed here have either not been tested or may not support both BPMN import and export.</t>
   </si>
@@ -451,10 +451,6 @@
     <t>4.1.1</t>
   </si>
   <si>
-    <t>2.2.6</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>OK</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -475,6 +471,14 @@
   </si>
   <si>
     <t>15.0.4.1565</t>
+  </si>
+  <si>
+    <t>OK</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.0.1</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -482,9 +486,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -886,8 +890,35 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -899,45 +930,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="TableStyleLight1" xfId="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1021,7 +1025,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1312,11 +1316,11 @@
   </sheetPr>
   <dimension ref="A1:AMK15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AO3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BD6" sqref="BD6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="V3" sqref="V3:X3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="44.85546875" style="1"/>
@@ -1332,24 +1336,24 @@
     <col min="58" max="1025" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" ht="15.75" thickBot="1">
+    <row r="1" spans="1:60" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:60" ht="47.25" thickTop="1" thickBot="1">
-      <c r="A2" s="61" t="s">
+    <row r="2" spans="1:60" ht="47.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61" t="s">
+      <c r="B2" s="70"/>
+      <c r="C2" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61" t="s">
+      <c r="D2" s="70"/>
+      <c r="E2" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="61"/>
+      <c r="F2" s="70"/>
       <c r="G2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1513,7 +1517,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:60" ht="25.35" customHeight="1" thickTop="1" thickBot="1">
+    <row r="3" spans="1:60" ht="25.35" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -1525,16 +1529,16 @@
       <c r="I3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="62" t="s">
+      <c r="J3" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="63" t="s">
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="72"/>
       <c r="P3" s="58" t="s">
         <v>13</v>
       </c>
@@ -1570,11 +1574,11 @@
       </c>
       <c r="AI3" s="58"/>
       <c r="AJ3" s="58"/>
-      <c r="AK3" s="64" t="s">
+      <c r="AK3" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="AL3" s="64"/>
-      <c r="AM3" s="64"/>
+      <c r="AL3" s="69"/>
+      <c r="AM3" s="69"/>
       <c r="AN3" s="58" t="s">
         <v>21</v>
       </c>
@@ -1596,12 +1600,12 @@
       <c r="AX3" s="58"/>
       <c r="AY3" s="58"/>
       <c r="AZ3" s="58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="BA3" s="58"/>
       <c r="BB3" s="58"/>
       <c r="BC3" s="73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="BD3" s="73"/>
       <c r="BE3" s="73"/>
@@ -1609,7 +1613,7 @@
       <c r="BG3" s="58"/>
       <c r="BH3" s="58"/>
     </row>
-    <row r="4" spans="1:60" s="15" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1">
+    <row r="4" spans="1:60" s="15" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -1621,18 +1625,18 @@
       <c r="I4" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="66" t="s">
+      <c r="J4" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="66"/>
-      <c r="L4" s="66"/>
+      <c r="K4" s="67"/>
+      <c r="L4" s="67"/>
       <c r="M4" s="59" t="s">
         <v>26</v>
       </c>
       <c r="N4" s="59"/>
       <c r="O4" s="59"/>
       <c r="P4" s="59" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q4" s="59"/>
       <c r="R4" s="59"/>
@@ -1641,11 +1645,11 @@
       </c>
       <c r="T4" s="59"/>
       <c r="U4" s="59"/>
-      <c r="V4" s="67" t="s">
-        <v>77</v>
-      </c>
-      <c r="W4" s="67"/>
-      <c r="X4" s="67"/>
+      <c r="V4" s="68" t="s">
+        <v>85</v>
+      </c>
+      <c r="W4" s="68"/>
+      <c r="X4" s="68"/>
       <c r="Y4" s="59" t="s">
         <v>28</v>
       </c>
@@ -1687,17 +1691,17 @@
       <c r="AU4" s="59"/>
       <c r="AV4" s="59"/>
       <c r="AW4" s="59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AX4" s="59"/>
       <c r="AY4" s="59"/>
       <c r="AZ4" s="59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="BA4" s="59"/>
       <c r="BB4" s="59"/>
       <c r="BC4" s="74" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="BD4" s="74"/>
       <c r="BE4" s="74"/>
@@ -1705,7 +1709,7 @@
       <c r="BG4" s="59"/>
       <c r="BH4" s="59"/>
     </row>
-    <row r="5" spans="1:60" ht="16.5" thickTop="1" thickBot="1">
+    <row r="5" spans="1:60" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -1717,31 +1721,31 @@
       <c r="I5" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="71">
+      <c r="J5" s="64">
         <v>41380</v>
       </c>
-      <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="72">
+      <c r="K5" s="64"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="65">
         <v>41373</v>
       </c>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="65"/>
       <c r="P5" s="60">
         <v>41591</v>
       </c>
       <c r="Q5" s="60"/>
       <c r="R5" s="60"/>
-      <c r="S5" s="65">
+      <c r="S5" s="66">
         <v>41383</v>
       </c>
-      <c r="T5" s="65"/>
-      <c r="U5" s="65"/>
-      <c r="V5" s="65">
-        <v>41491</v>
-      </c>
-      <c r="W5" s="65"/>
-      <c r="X5" s="65"/>
+      <c r="T5" s="66"/>
+      <c r="U5" s="66"/>
+      <c r="V5" s="66">
+        <v>41599</v>
+      </c>
+      <c r="W5" s="66"/>
+      <c r="X5" s="66"/>
       <c r="Y5" s="60">
         <v>41394</v>
       </c>
@@ -1801,8 +1805,8 @@
       <c r="BG5" s="60"/>
       <c r="BH5" s="60"/>
     </row>
-    <row r="6" spans="1:60" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="68" t="s">
+    <row r="6" spans="1:60" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="61" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="19" t="s">
@@ -1872,21 +1876,21 @@
       <c r="X6" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="Y6" s="69" t="s">
+      <c r="Y6" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="Z6" s="69"/>
-      <c r="AA6" s="69"/>
-      <c r="AB6" s="69" t="s">
+      <c r="Z6" s="62"/>
+      <c r="AA6" s="62"/>
+      <c r="AB6" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="AC6" s="69"/>
-      <c r="AD6" s="69"/>
-      <c r="AE6" s="69" t="s">
+      <c r="AC6" s="62"/>
+      <c r="AD6" s="62"/>
+      <c r="AE6" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="AF6" s="69"/>
-      <c r="AG6" s="69"/>
+      <c r="AF6" s="62"/>
+      <c r="AG6" s="62"/>
       <c r="AH6" s="27" t="s">
         <v>43</v>
       </c>
@@ -1951,8 +1955,8 @@
       <c r="BG6" s="24"/>
       <c r="BH6" s="24"/>
     </row>
-    <row r="7" spans="1:60" ht="42.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="68"/>
+    <row r="7" spans="1:60" ht="42.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="61"/>
       <c r="B7" s="30" t="s">
         <v>46</v>
       </c>
@@ -2020,15 +2024,15 @@
       <c r="X7" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="Y7" s="69"/>
-      <c r="Z7" s="69"/>
-      <c r="AA7" s="69"/>
-      <c r="AB7" s="69"/>
-      <c r="AC7" s="69"/>
-      <c r="AD7" s="69"/>
-      <c r="AE7" s="69"/>
-      <c r="AF7" s="69"/>
-      <c r="AG7" s="69"/>
+      <c r="Y7" s="62"/>
+      <c r="Z7" s="62"/>
+      <c r="AA7" s="62"/>
+      <c r="AB7" s="62"/>
+      <c r="AC7" s="62"/>
+      <c r="AD7" s="62"/>
+      <c r="AE7" s="62"/>
+      <c r="AF7" s="62"/>
+      <c r="AG7" s="62"/>
       <c r="AH7" s="27" t="s">
         <v>43</v>
       </c>
@@ -2093,8 +2097,8 @@
       <c r="BG7" s="24"/>
       <c r="BH7" s="24"/>
     </row>
-    <row r="8" spans="1:60" ht="43.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A8" s="68"/>
+    <row r="8" spans="1:60" ht="43.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="61"/>
       <c r="B8" s="30"/>
       <c r="C8" s="20">
         <v>3</v>
@@ -2160,15 +2164,15 @@
       <c r="X8" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="Y8" s="69"/>
-      <c r="Z8" s="69"/>
-      <c r="AA8" s="69"/>
-      <c r="AB8" s="69"/>
-      <c r="AC8" s="69"/>
-      <c r="AD8" s="69"/>
-      <c r="AE8" s="69"/>
-      <c r="AF8" s="69"/>
-      <c r="AG8" s="69"/>
+      <c r="Y8" s="62"/>
+      <c r="Z8" s="62"/>
+      <c r="AA8" s="62"/>
+      <c r="AB8" s="62"/>
+      <c r="AC8" s="62"/>
+      <c r="AD8" s="62"/>
+      <c r="AE8" s="62"/>
+      <c r="AF8" s="62"/>
+      <c r="AG8" s="62"/>
       <c r="AH8" s="27" t="s">
         <v>42</v>
       </c>
@@ -2233,8 +2237,8 @@
       <c r="BG8" s="24"/>
       <c r="BH8" s="24"/>
     </row>
-    <row r="9" spans="1:60" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A9" s="68"/>
+    <row r="9" spans="1:60" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="61"/>
       <c r="B9" s="30"/>
       <c r="C9" s="20">
         <v>4</v>
@@ -2292,23 +2296,23 @@
         <v>42</v>
       </c>
       <c r="V9" s="21" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="W9" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="X9" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="Y9" s="69"/>
-      <c r="Z9" s="69"/>
-      <c r="AA9" s="69"/>
-      <c r="AB9" s="69"/>
-      <c r="AC9" s="69"/>
-      <c r="AD9" s="69"/>
-      <c r="AE9" s="69"/>
-      <c r="AF9" s="69"/>
-      <c r="AG9" s="69"/>
+      <c r="Y9" s="62"/>
+      <c r="Z9" s="62"/>
+      <c r="AA9" s="62"/>
+      <c r="AB9" s="62"/>
+      <c r="AC9" s="62"/>
+      <c r="AD9" s="62"/>
+      <c r="AE9" s="62"/>
+      <c r="AF9" s="62"/>
+      <c r="AG9" s="62"/>
       <c r="AH9" s="24" t="s">
         <v>42</v>
       </c>
@@ -2373,7 +2377,7 @@
       <c r="BG9" s="20"/>
       <c r="BH9" s="24"/>
     </row>
-    <row r="10" spans="1:60" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
+    <row r="10" spans="1:60" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="55"/>
       <c r="B10" s="30"/>
       <c r="C10" s="20">
@@ -2413,18 +2417,24 @@
       <c r="S10" s="42"/>
       <c r="T10" s="43"/>
       <c r="U10" s="44"/>
-      <c r="V10" s="21"/>
-      <c r="W10" s="21"/>
-      <c r="X10" s="21"/>
-      <c r="Y10" s="69"/>
-      <c r="Z10" s="69"/>
-      <c r="AA10" s="69"/>
-      <c r="AB10" s="69"/>
-      <c r="AC10" s="69"/>
-      <c r="AD10" s="69"/>
-      <c r="AE10" s="69"/>
-      <c r="AF10" s="69"/>
-      <c r="AG10" s="69"/>
+      <c r="V10" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="W10" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="X10" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y10" s="62"/>
+      <c r="Z10" s="62"/>
+      <c r="AA10" s="62"/>
+      <c r="AB10" s="62"/>
+      <c r="AC10" s="62"/>
+      <c r="AD10" s="62"/>
+      <c r="AE10" s="62"/>
+      <c r="AF10" s="62"/>
+      <c r="AG10" s="62"/>
       <c r="AH10" s="24"/>
       <c r="AI10" s="20"/>
       <c r="AJ10" s="24"/>
@@ -2461,8 +2471,8 @@
       <c r="BG10" s="20"/>
       <c r="BH10" s="24"/>
     </row>
-    <row r="11" spans="1:60" s="47" customFormat="1" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A11" s="70" t="s">
+    <row r="11" spans="1:60" s="47" customFormat="1" ht="58.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="63" t="s">
         <v>56</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -2516,7 +2526,7 @@
       <c r="T11" s="24"/>
       <c r="U11" s="24"/>
       <c r="V11" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="W11" s="23" t="s">
         <v>42</v>
@@ -2524,15 +2534,15 @@
       <c r="X11" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="Y11" s="69"/>
-      <c r="Z11" s="69"/>
-      <c r="AA11" s="69"/>
-      <c r="AB11" s="69"/>
-      <c r="AC11" s="69"/>
-      <c r="AD11" s="69"/>
-      <c r="AE11" s="69"/>
-      <c r="AF11" s="69"/>
-      <c r="AG11" s="69"/>
+      <c r="Y11" s="62"/>
+      <c r="Z11" s="62"/>
+      <c r="AA11" s="62"/>
+      <c r="AB11" s="62"/>
+      <c r="AC11" s="62"/>
+      <c r="AD11" s="62"/>
+      <c r="AE11" s="62"/>
+      <c r="AF11" s="62"/>
+      <c r="AG11" s="62"/>
       <c r="AH11" s="24" t="s">
         <v>42</v>
       </c>
@@ -2591,8 +2601,8 @@
       <c r="BG11" s="24"/>
       <c r="BH11" s="24"/>
     </row>
-    <row r="12" spans="1:60" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A12" s="70"/>
+    <row r="12" spans="1:60" ht="58.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="63"/>
       <c r="B12" s="30" t="s">
         <v>61</v>
       </c>
@@ -2640,7 +2650,7 @@
       <c r="T12" s="24"/>
       <c r="U12" s="24"/>
       <c r="V12" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="W12" s="23" t="s">
         <v>42</v>
@@ -2648,15 +2658,15 @@
       <c r="X12" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="Y12" s="69"/>
-      <c r="Z12" s="69"/>
-      <c r="AA12" s="69"/>
-      <c r="AB12" s="69"/>
-      <c r="AC12" s="69"/>
-      <c r="AD12" s="69"/>
-      <c r="AE12" s="69"/>
-      <c r="AF12" s="69"/>
-      <c r="AG12" s="69"/>
+      <c r="Y12" s="62"/>
+      <c r="Z12" s="62"/>
+      <c r="AA12" s="62"/>
+      <c r="AB12" s="62"/>
+      <c r="AC12" s="62"/>
+      <c r="AD12" s="62"/>
+      <c r="AE12" s="62"/>
+      <c r="AF12" s="62"/>
+      <c r="AG12" s="62"/>
       <c r="AH12" s="24" t="s">
         <v>42</v>
       </c>
@@ -2715,8 +2725,8 @@
       <c r="BG12" s="24"/>
       <c r="BH12" s="24"/>
     </row>
-    <row r="13" spans="1:60" ht="63" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A13" s="70"/>
+    <row r="13" spans="1:60" ht="63" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="63"/>
       <c r="B13" s="30"/>
       <c r="C13" s="48">
         <v>3</v>
@@ -2754,15 +2764,15 @@
       <c r="V13" s="24"/>
       <c r="W13" s="24"/>
       <c r="X13" s="24"/>
-      <c r="Y13" s="69"/>
-      <c r="Z13" s="69"/>
-      <c r="AA13" s="69"/>
-      <c r="AB13" s="69"/>
-      <c r="AC13" s="69"/>
-      <c r="AD13" s="69"/>
-      <c r="AE13" s="69"/>
-      <c r="AF13" s="69"/>
-      <c r="AG13" s="69"/>
+      <c r="Y13" s="62"/>
+      <c r="Z13" s="62"/>
+      <c r="AA13" s="62"/>
+      <c r="AB13" s="62"/>
+      <c r="AC13" s="62"/>
+      <c r="AD13" s="62"/>
+      <c r="AE13" s="62"/>
+      <c r="AF13" s="62"/>
+      <c r="AG13" s="62"/>
       <c r="AH13" s="24"/>
       <c r="AI13" s="24"/>
       <c r="AJ13" s="24"/>
@@ -2791,8 +2801,8 @@
       <c r="BG13" s="24"/>
       <c r="BH13" s="24"/>
     </row>
-    <row r="14" spans="1:60" ht="45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A14" s="70"/>
+    <row r="14" spans="1:60" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="63"/>
       <c r="B14" s="52"/>
       <c r="C14" s="51">
         <v>4</v>
@@ -2830,15 +2840,15 @@
       <c r="V14" s="54"/>
       <c r="W14" s="54"/>
       <c r="X14" s="54"/>
-      <c r="Y14" s="69"/>
-      <c r="Z14" s="69"/>
-      <c r="AA14" s="69"/>
-      <c r="AB14" s="69"/>
-      <c r="AC14" s="69"/>
-      <c r="AD14" s="69"/>
-      <c r="AE14" s="69"/>
-      <c r="AF14" s="69"/>
-      <c r="AG14" s="69"/>
+      <c r="Y14" s="62"/>
+      <c r="Z14" s="62"/>
+      <c r="AA14" s="62"/>
+      <c r="AB14" s="62"/>
+      <c r="AC14" s="62"/>
+      <c r="AD14" s="62"/>
+      <c r="AE14" s="62"/>
+      <c r="AF14" s="62"/>
+      <c r="AG14" s="62"/>
       <c r="AH14" s="54"/>
       <c r="AI14" s="54"/>
       <c r="AJ14" s="54"/>
@@ -2867,68 +2877,68 @@
       <c r="BG14" s="54"/>
       <c r="BH14" s="54"/>
     </row>
-    <row r="15" spans="1:60" ht="15.75" thickTop="1"/>
+    <row r="15" spans="1:60" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="59">
+    <mergeCell ref="AZ3:BB3"/>
+    <mergeCell ref="AZ4:BB4"/>
+    <mergeCell ref="AZ5:BB5"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="Y3:AA3"/>
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="AH3:AJ3"/>
+    <mergeCell ref="AK3:AM3"/>
+    <mergeCell ref="AN3:AP3"/>
+    <mergeCell ref="AQ3:AS3"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="AB4:AD4"/>
+    <mergeCell ref="AE4:AG4"/>
+    <mergeCell ref="AH4:AJ4"/>
+    <mergeCell ref="AK4:AM4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="Y5:AA5"/>
+    <mergeCell ref="AB5:AD5"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AK5:AM5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="Y6:AA14"/>
+    <mergeCell ref="AB6:AD14"/>
+    <mergeCell ref="AE6:AG14"/>
+    <mergeCell ref="A11:A14"/>
     <mergeCell ref="BF3:BH3"/>
     <mergeCell ref="BF4:BH4"/>
     <mergeCell ref="BF5:BH5"/>
     <mergeCell ref="AN5:AP5"/>
     <mergeCell ref="AQ5:AS5"/>
     <mergeCell ref="AT5:AV5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="Y6:AA14"/>
-    <mergeCell ref="AB6:AD14"/>
-    <mergeCell ref="AE6:AG14"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="Y5:AA5"/>
-    <mergeCell ref="AB5:AD5"/>
-    <mergeCell ref="AE5:AG5"/>
-    <mergeCell ref="AH5:AJ5"/>
-    <mergeCell ref="AK5:AM5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="V5:X5"/>
     <mergeCell ref="AT3:AV3"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="V4:X4"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="AB4:AD4"/>
-    <mergeCell ref="AE4:AG4"/>
-    <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="AK4:AM4"/>
     <mergeCell ref="AN4:AP4"/>
     <mergeCell ref="AQ4:AS4"/>
     <mergeCell ref="AT4:AV4"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="AK3:AM3"/>
-    <mergeCell ref="AN3:AP3"/>
-    <mergeCell ref="AQ3:AS3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="Y3:AA3"/>
-    <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:O3"/>
     <mergeCell ref="BC3:BE3"/>
     <mergeCell ref="BC4:BE4"/>
     <mergeCell ref="BC5:BE5"/>
     <mergeCell ref="AW3:AY3"/>
     <mergeCell ref="AW4:AY4"/>
     <mergeCell ref="AW5:AY5"/>
-    <mergeCell ref="AZ3:BB3"/>
-    <mergeCell ref="AZ4:BB4"/>
-    <mergeCell ref="AZ5:BB5"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Add export test results camunda Modeler 2.2.0
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -13,118 +13,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>mschoe</author>
-  </authors>
-  <commentList>
-    <comment ref="P8" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>mschoe:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-sub process not collapsed. Wrong interpretaion of missing isExpanded attribute </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P9" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>mschoe:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-modeler cannot display lanes without pools</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P11" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>mschoe:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-- collapsed Call Activities can be displayed only
-- Group is missing
-- collapsed sub process is displayed as expanded</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P12" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>mschoe:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-- collapsed Call Activities can be displayed only
-- collapsed sub process is displayed as expanded
-- group is missing</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="83">
   <si>
     <t>Note: Tools that are not listed here have either not been tested or may not support both BPMN import and export.</t>
   </si>
@@ -478,7 +368,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -523,19 +413,6 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -874,9 +751,36 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -890,33 +794,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1291,14 +1168,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AMK15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AH4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AW11" sqref="AW11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1321,18 +1198,18 @@
       </c>
     </row>
     <row r="2" spans="1:57" ht="47.25" thickTop="1" thickBot="1">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70" t="s">
+      <c r="B2" s="61"/>
+      <c r="C2" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70" t="s">
+      <c r="D2" s="61"/>
+      <c r="E2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="70"/>
+      <c r="F2" s="61"/>
       <c r="G2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1499,84 +1376,84 @@
       <c r="I3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="71" t="s">
+      <c r="J3" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="72" t="s">
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="65" t="s">
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="65" t="s">
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="T3" s="65"/>
-      <c r="U3" s="65"/>
-      <c r="V3" s="65" t="s">
+      <c r="T3" s="58"/>
+      <c r="U3" s="58"/>
+      <c r="V3" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="W3" s="65"/>
-      <c r="X3" s="65"/>
-      <c r="Y3" s="65" t="s">
+      <c r="W3" s="58"/>
+      <c r="X3" s="58"/>
+      <c r="Y3" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="Z3" s="65"/>
-      <c r="AA3" s="65"/>
-      <c r="AB3" s="65" t="s">
+      <c r="Z3" s="58"/>
+      <c r="AA3" s="58"/>
+      <c r="AB3" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="AC3" s="65"/>
-      <c r="AD3" s="65"/>
-      <c r="AE3" s="65" t="s">
+      <c r="AC3" s="58"/>
+      <c r="AD3" s="58"/>
+      <c r="AE3" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="AF3" s="65"/>
-      <c r="AG3" s="65"/>
-      <c r="AH3" s="65" t="s">
+      <c r="AF3" s="58"/>
+      <c r="AG3" s="58"/>
+      <c r="AH3" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="AI3" s="65"/>
-      <c r="AJ3" s="65"/>
-      <c r="AK3" s="69" t="s">
+      <c r="AI3" s="58"/>
+      <c r="AJ3" s="58"/>
+      <c r="AK3" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="AL3" s="69"/>
-      <c r="AM3" s="69"/>
-      <c r="AN3" s="65" t="s">
+      <c r="AL3" s="64"/>
+      <c r="AM3" s="64"/>
+      <c r="AN3" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="AO3" s="65"/>
-      <c r="AP3" s="65"/>
-      <c r="AQ3" s="65" t="s">
+      <c r="AO3" s="58"/>
+      <c r="AP3" s="58"/>
+      <c r="AQ3" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="AR3" s="65"/>
-      <c r="AS3" s="65"/>
-      <c r="AT3" s="65" t="s">
+      <c r="AR3" s="58"/>
+      <c r="AS3" s="58"/>
+      <c r="AT3" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="AU3" s="65"/>
-      <c r="AV3" s="65"/>
-      <c r="AW3" s="65" t="s">
+      <c r="AU3" s="58"/>
+      <c r="AV3" s="58"/>
+      <c r="AW3" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="AX3" s="65"/>
-      <c r="AY3" s="65"/>
-      <c r="AZ3" s="65" t="s">
+      <c r="AX3" s="58"/>
+      <c r="AY3" s="58"/>
+      <c r="AZ3" s="58" t="s">
         <v>79</v>
       </c>
-      <c r="BA3" s="65"/>
-      <c r="BB3" s="65"/>
-      <c r="BC3" s="65"/>
-      <c r="BD3" s="65"/>
-      <c r="BE3" s="65"/>
+      <c r="BA3" s="58"/>
+      <c r="BB3" s="58"/>
+      <c r="BC3" s="58"/>
+      <c r="BD3" s="58"/>
+      <c r="BE3" s="58"/>
     </row>
     <row r="4" spans="1:57" s="15" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A4" s="12"/>
@@ -1595,79 +1472,79 @@
       </c>
       <c r="K4" s="66"/>
       <c r="L4" s="66"/>
-      <c r="M4" s="67" t="s">
+      <c r="M4" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="67"/>
-      <c r="O4" s="67"/>
-      <c r="P4" s="67" t="s">
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67" t="s">
+      <c r="Q4" s="59"/>
+      <c r="R4" s="59"/>
+      <c r="S4" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="T4" s="67"/>
-      <c r="U4" s="67"/>
-      <c r="V4" s="68" t="s">
+      <c r="T4" s="59"/>
+      <c r="U4" s="59"/>
+      <c r="V4" s="67" t="s">
         <v>77</v>
       </c>
-      <c r="W4" s="68"/>
-      <c r="X4" s="68"/>
-      <c r="Y4" s="67" t="s">
+      <c r="W4" s="67"/>
+      <c r="X4" s="67"/>
+      <c r="Y4" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="Z4" s="67"/>
-      <c r="AA4" s="67"/>
-      <c r="AB4" s="67">
+      <c r="Z4" s="59"/>
+      <c r="AA4" s="59"/>
+      <c r="AB4" s="59">
         <v>2.4</v>
       </c>
-      <c r="AC4" s="67"/>
-      <c r="AD4" s="67"/>
-      <c r="AE4" s="67" t="s">
+      <c r="AC4" s="59"/>
+      <c r="AD4" s="59"/>
+      <c r="AE4" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="AF4" s="67"/>
-      <c r="AG4" s="67"/>
-      <c r="AH4" s="67" t="s">
+      <c r="AF4" s="59"/>
+      <c r="AG4" s="59"/>
+      <c r="AH4" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="AI4" s="67"/>
-      <c r="AJ4" s="67"/>
-      <c r="AK4" s="67" t="s">
+      <c r="AI4" s="59"/>
+      <c r="AJ4" s="59"/>
+      <c r="AK4" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="AL4" s="67"/>
-      <c r="AM4" s="67"/>
-      <c r="AN4" s="67" t="s">
+      <c r="AL4" s="59"/>
+      <c r="AM4" s="59"/>
+      <c r="AN4" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="AO4" s="67"/>
-      <c r="AP4" s="67"/>
-      <c r="AQ4" s="67" t="s">
+      <c r="AO4" s="59"/>
+      <c r="AP4" s="59"/>
+      <c r="AQ4" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="AR4" s="67"/>
-      <c r="AS4" s="67"/>
-      <c r="AT4" s="67" t="s">
+      <c r="AR4" s="59"/>
+      <c r="AS4" s="59"/>
+      <c r="AT4" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="AU4" s="67"/>
-      <c r="AV4" s="67"/>
-      <c r="AW4" s="67" t="s">
+      <c r="AU4" s="59"/>
+      <c r="AV4" s="59"/>
+      <c r="AW4" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="AX4" s="67"/>
-      <c r="AY4" s="67"/>
-      <c r="AZ4" s="67" t="s">
+      <c r="AX4" s="59"/>
+      <c r="AY4" s="59"/>
+      <c r="AZ4" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="BA4" s="67"/>
-      <c r="BB4" s="67"/>
-      <c r="BC4" s="67"/>
-      <c r="BD4" s="67"/>
-      <c r="BE4" s="67"/>
+      <c r="BA4" s="59"/>
+      <c r="BB4" s="59"/>
+      <c r="BC4" s="59"/>
+      <c r="BD4" s="59"/>
+      <c r="BE4" s="59"/>
     </row>
     <row r="5" spans="1:57" ht="16.5" thickTop="1" thickBot="1">
       <c r="A5" s="16"/>
@@ -1681,87 +1558,87 @@
       <c r="I5" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="62">
+      <c r="J5" s="71">
         <v>41380</v>
       </c>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="63">
+      <c r="K5" s="71"/>
+      <c r="L5" s="71"/>
+      <c r="M5" s="72">
         <v>41373</v>
       </c>
-      <c r="N5" s="63"/>
-      <c r="O5" s="63"/>
-      <c r="P5" s="58">
+      <c r="N5" s="72"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="60">
         <v>41591</v>
       </c>
-      <c r="Q5" s="58"/>
-      <c r="R5" s="58"/>
-      <c r="S5" s="64">
+      <c r="Q5" s="60"/>
+      <c r="R5" s="60"/>
+      <c r="S5" s="65">
         <v>41383</v>
       </c>
-      <c r="T5" s="64"/>
-      <c r="U5" s="64"/>
-      <c r="V5" s="64">
+      <c r="T5" s="65"/>
+      <c r="U5" s="65"/>
+      <c r="V5" s="65">
         <v>41491</v>
       </c>
-      <c r="W5" s="64"/>
-      <c r="X5" s="64"/>
-      <c r="Y5" s="58">
+      <c r="W5" s="65"/>
+      <c r="X5" s="65"/>
+      <c r="Y5" s="60">
         <v>41394</v>
       </c>
-      <c r="Z5" s="58"/>
-      <c r="AA5" s="58"/>
-      <c r="AB5" s="58">
+      <c r="Z5" s="60"/>
+      <c r="AA5" s="60"/>
+      <c r="AB5" s="60">
         <v>41388</v>
       </c>
-      <c r="AC5" s="58"/>
-      <c r="AD5" s="58"/>
-      <c r="AE5" s="58">
+      <c r="AC5" s="60"/>
+      <c r="AD5" s="60"/>
+      <c r="AE5" s="60">
         <v>41388</v>
       </c>
-      <c r="AF5" s="58"/>
-      <c r="AG5" s="58"/>
-      <c r="AH5" s="58">
+      <c r="AF5" s="60"/>
+      <c r="AG5" s="60"/>
+      <c r="AH5" s="60">
         <v>41431</v>
       </c>
-      <c r="AI5" s="58"/>
-      <c r="AJ5" s="58"/>
-      <c r="AK5" s="58">
+      <c r="AI5" s="60"/>
+      <c r="AJ5" s="60"/>
+      <c r="AK5" s="60">
         <v>41467</v>
       </c>
-      <c r="AL5" s="58"/>
-      <c r="AM5" s="58"/>
-      <c r="AN5" s="58">
+      <c r="AL5" s="60"/>
+      <c r="AM5" s="60"/>
+      <c r="AN5" s="60">
         <v>41435</v>
       </c>
-      <c r="AO5" s="58"/>
-      <c r="AP5" s="58"/>
-      <c r="AQ5" s="58">
+      <c r="AO5" s="60"/>
+      <c r="AP5" s="60"/>
+      <c r="AQ5" s="60">
         <v>41449</v>
       </c>
-      <c r="AR5" s="58"/>
-      <c r="AS5" s="58"/>
-      <c r="AT5" s="58">
+      <c r="AR5" s="60"/>
+      <c r="AS5" s="60"/>
+      <c r="AT5" s="60">
         <v>41444</v>
       </c>
-      <c r="AU5" s="58"/>
-      <c r="AV5" s="58"/>
-      <c r="AW5" s="58">
+      <c r="AU5" s="60"/>
+      <c r="AV5" s="60"/>
+      <c r="AW5" s="60">
         <v>41591</v>
       </c>
-      <c r="AX5" s="58"/>
-      <c r="AY5" s="58"/>
-      <c r="AZ5" s="58">
+      <c r="AX5" s="60"/>
+      <c r="AY5" s="60"/>
+      <c r="AZ5" s="60">
         <v>41571</v>
       </c>
-      <c r="BA5" s="58"/>
-      <c r="BB5" s="58"/>
-      <c r="BC5" s="58"/>
-      <c r="BD5" s="58"/>
-      <c r="BE5" s="58"/>
+      <c r="BA5" s="60"/>
+      <c r="BB5" s="60"/>
+      <c r="BC5" s="60"/>
+      <c r="BD5" s="60"/>
+      <c r="BE5" s="60"/>
     </row>
     <row r="6" spans="1:57" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="68" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="19" t="s">
@@ -1809,7 +1686,9 @@
       <c r="P6" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="Q6" s="24"/>
+      <c r="Q6" s="24" t="s">
+        <v>43</v>
+      </c>
       <c r="R6" s="22" t="s">
         <v>43</v>
       </c>
@@ -1831,21 +1710,21 @@
       <c r="X6" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="Y6" s="60" t="s">
+      <c r="Y6" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="Z6" s="60"/>
-      <c r="AA6" s="60"/>
-      <c r="AB6" s="60" t="s">
+      <c r="Z6" s="69"/>
+      <c r="AA6" s="69"/>
+      <c r="AB6" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="AC6" s="60"/>
-      <c r="AD6" s="60"/>
-      <c r="AE6" s="60" t="s">
+      <c r="AC6" s="69"/>
+      <c r="AD6" s="69"/>
+      <c r="AE6" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="AF6" s="60"/>
-      <c r="AG6" s="60"/>
+      <c r="AF6" s="69"/>
+      <c r="AG6" s="69"/>
       <c r="AH6" s="27" t="s">
         <v>43</v>
       </c>
@@ -1902,7 +1781,7 @@
       <c r="BE6" s="24"/>
     </row>
     <row r="7" spans="1:57" ht="42.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="59"/>
+      <c r="A7" s="68"/>
       <c r="B7" s="30" t="s">
         <v>46</v>
       </c>
@@ -1948,7 +1827,9 @@
       <c r="P7" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="Q7" s="24"/>
+      <c r="Q7" s="24" t="s">
+        <v>43</v>
+      </c>
       <c r="R7" s="22" t="s">
         <v>43</v>
       </c>
@@ -1970,15 +1851,15 @@
       <c r="X7" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="Y7" s="60"/>
-      <c r="Z7" s="60"/>
-      <c r="AA7" s="60"/>
-      <c r="AB7" s="60"/>
-      <c r="AC7" s="60"/>
-      <c r="AD7" s="60"/>
-      <c r="AE7" s="60"/>
-      <c r="AF7" s="60"/>
-      <c r="AG7" s="60"/>
+      <c r="Y7" s="69"/>
+      <c r="Z7" s="69"/>
+      <c r="AA7" s="69"/>
+      <c r="AB7" s="69"/>
+      <c r="AC7" s="69"/>
+      <c r="AD7" s="69"/>
+      <c r="AE7" s="69"/>
+      <c r="AF7" s="69"/>
+      <c r="AG7" s="69"/>
       <c r="AH7" s="27" t="s">
         <v>43</v>
       </c>
@@ -2035,7 +1916,7 @@
       <c r="BE7" s="24"/>
     </row>
     <row r="8" spans="1:57" ht="43.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A8" s="59"/>
+      <c r="A8" s="68"/>
       <c r="B8" s="30"/>
       <c r="C8" s="20">
         <v>3</v>
@@ -2079,7 +1960,9 @@
       <c r="P8" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="24"/>
+      <c r="Q8" s="24" t="s">
+        <v>43</v>
+      </c>
       <c r="R8" s="22" t="s">
         <v>42</v>
       </c>
@@ -2101,15 +1984,15 @@
       <c r="X8" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="Y8" s="60"/>
-      <c r="Z8" s="60"/>
-      <c r="AA8" s="60"/>
-      <c r="AB8" s="60"/>
-      <c r="AC8" s="60"/>
-      <c r="AD8" s="60"/>
-      <c r="AE8" s="60"/>
-      <c r="AF8" s="60"/>
-      <c r="AG8" s="60"/>
+      <c r="Y8" s="69"/>
+      <c r="Z8" s="69"/>
+      <c r="AA8" s="69"/>
+      <c r="AB8" s="69"/>
+      <c r="AC8" s="69"/>
+      <c r="AD8" s="69"/>
+      <c r="AE8" s="69"/>
+      <c r="AF8" s="69"/>
+      <c r="AG8" s="69"/>
       <c r="AH8" s="27" t="s">
         <v>42</v>
       </c>
@@ -2166,7 +2049,7 @@
       <c r="BE8" s="24"/>
     </row>
     <row r="9" spans="1:57" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A9" s="59"/>
+      <c r="A9" s="68"/>
       <c r="B9" s="30"/>
       <c r="C9" s="20">
         <v>4</v>
@@ -2210,7 +2093,9 @@
       <c r="P9" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="Q9" s="20"/>
+      <c r="Q9" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="R9" s="41" t="s">
         <v>43</v>
       </c>
@@ -2232,15 +2117,15 @@
       <c r="X9" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="Y9" s="60"/>
-      <c r="Z9" s="60"/>
-      <c r="AA9" s="60"/>
-      <c r="AB9" s="60"/>
-      <c r="AC9" s="60"/>
-      <c r="AD9" s="60"/>
-      <c r="AE9" s="60"/>
-      <c r="AF9" s="60"/>
-      <c r="AG9" s="60"/>
+      <c r="Y9" s="69"/>
+      <c r="Z9" s="69"/>
+      <c r="AA9" s="69"/>
+      <c r="AB9" s="69"/>
+      <c r="AC9" s="69"/>
+      <c r="AD9" s="69"/>
+      <c r="AE9" s="69"/>
+      <c r="AF9" s="69"/>
+      <c r="AG9" s="69"/>
       <c r="AH9" s="24" t="s">
         <v>42</v>
       </c>
@@ -2329,7 +2214,9 @@
       <c r="P10" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="Q10" s="20"/>
+      <c r="Q10" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="R10" s="41" t="s">
         <v>43</v>
       </c>
@@ -2339,15 +2226,15 @@
       <c r="V10" s="21"/>
       <c r="W10" s="21"/>
       <c r="X10" s="21"/>
-      <c r="Y10" s="60"/>
-      <c r="Z10" s="60"/>
-      <c r="AA10" s="60"/>
-      <c r="AB10" s="60"/>
-      <c r="AC10" s="60"/>
-      <c r="AD10" s="60"/>
-      <c r="AE10" s="60"/>
-      <c r="AF10" s="60"/>
-      <c r="AG10" s="60"/>
+      <c r="Y10" s="69"/>
+      <c r="Z10" s="69"/>
+      <c r="AA10" s="69"/>
+      <c r="AB10" s="69"/>
+      <c r="AC10" s="69"/>
+      <c r="AD10" s="69"/>
+      <c r="AE10" s="69"/>
+      <c r="AF10" s="69"/>
+      <c r="AG10" s="69"/>
       <c r="AH10" s="24"/>
       <c r="AI10" s="20"/>
       <c r="AJ10" s="24"/>
@@ -2376,7 +2263,7 @@
       <c r="BE10" s="24"/>
     </row>
     <row r="11" spans="1:57" s="47" customFormat="1" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A11" s="61" t="s">
+      <c r="A11" s="70" t="s">
         <v>56</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -2422,7 +2309,9 @@
       <c r="P11" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="Q11" s="24"/>
+      <c r="Q11" s="24" t="s">
+        <v>42</v>
+      </c>
       <c r="R11" s="24" t="s">
         <v>42</v>
       </c>
@@ -2438,15 +2327,15 @@
       <c r="X11" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="Y11" s="60"/>
-      <c r="Z11" s="60"/>
-      <c r="AA11" s="60"/>
-      <c r="AB11" s="60"/>
-      <c r="AC11" s="60"/>
-      <c r="AD11" s="60"/>
-      <c r="AE11" s="60"/>
-      <c r="AF11" s="60"/>
-      <c r="AG11" s="60"/>
+      <c r="Y11" s="69"/>
+      <c r="Z11" s="69"/>
+      <c r="AA11" s="69"/>
+      <c r="AB11" s="69"/>
+      <c r="AC11" s="69"/>
+      <c r="AD11" s="69"/>
+      <c r="AE11" s="69"/>
+      <c r="AF11" s="69"/>
+      <c r="AG11" s="69"/>
       <c r="AH11" s="24" t="s">
         <v>42</v>
       </c>
@@ -2497,7 +2386,7 @@
       <c r="BE11" s="24"/>
     </row>
     <row r="12" spans="1:57" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A12" s="61"/>
+      <c r="A12" s="70"/>
       <c r="B12" s="30" t="s">
         <v>61</v>
       </c>
@@ -2537,7 +2426,9 @@
       <c r="P12" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="Q12" s="24"/>
+      <c r="Q12" s="24" t="s">
+        <v>42</v>
+      </c>
       <c r="R12" s="24" t="s">
         <v>42</v>
       </c>
@@ -2553,15 +2444,15 @@
       <c r="X12" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="Y12" s="60"/>
-      <c r="Z12" s="60"/>
-      <c r="AA12" s="60"/>
-      <c r="AB12" s="60"/>
-      <c r="AC12" s="60"/>
-      <c r="AD12" s="60"/>
-      <c r="AE12" s="60"/>
-      <c r="AF12" s="60"/>
-      <c r="AG12" s="60"/>
+      <c r="Y12" s="69"/>
+      <c r="Z12" s="69"/>
+      <c r="AA12" s="69"/>
+      <c r="AB12" s="69"/>
+      <c r="AC12" s="69"/>
+      <c r="AD12" s="69"/>
+      <c r="AE12" s="69"/>
+      <c r="AF12" s="69"/>
+      <c r="AG12" s="69"/>
       <c r="AH12" s="24" t="s">
         <v>42</v>
       </c>
@@ -2612,7 +2503,7 @@
       <c r="BE12" s="24"/>
     </row>
     <row r="13" spans="1:57" ht="63" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A13" s="61"/>
+      <c r="A13" s="70"/>
       <c r="B13" s="30"/>
       <c r="C13" s="48">
         <v>3</v>
@@ -2650,15 +2541,15 @@
       <c r="V13" s="24"/>
       <c r="W13" s="24"/>
       <c r="X13" s="24"/>
-      <c r="Y13" s="60"/>
-      <c r="Z13" s="60"/>
-      <c r="AA13" s="60"/>
-      <c r="AB13" s="60"/>
-      <c r="AC13" s="60"/>
-      <c r="AD13" s="60"/>
-      <c r="AE13" s="60"/>
-      <c r="AF13" s="60"/>
-      <c r="AG13" s="60"/>
+      <c r="Y13" s="69"/>
+      <c r="Z13" s="69"/>
+      <c r="AA13" s="69"/>
+      <c r="AB13" s="69"/>
+      <c r="AC13" s="69"/>
+      <c r="AD13" s="69"/>
+      <c r="AE13" s="69"/>
+      <c r="AF13" s="69"/>
+      <c r="AG13" s="69"/>
       <c r="AH13" s="24"/>
       <c r="AI13" s="24"/>
       <c r="AJ13" s="24"/>
@@ -2685,7 +2576,7 @@
       <c r="BE13" s="24"/>
     </row>
     <row r="14" spans="1:57" ht="45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A14" s="61"/>
+      <c r="A14" s="70"/>
       <c r="B14" s="52"/>
       <c r="C14" s="51">
         <v>4</v>
@@ -2723,15 +2614,15 @@
       <c r="V14" s="54"/>
       <c r="W14" s="54"/>
       <c r="X14" s="54"/>
-      <c r="Y14" s="60"/>
-      <c r="Z14" s="60"/>
-      <c r="AA14" s="60"/>
-      <c r="AB14" s="60"/>
-      <c r="AC14" s="60"/>
-      <c r="AD14" s="60"/>
-      <c r="AE14" s="60"/>
-      <c r="AF14" s="60"/>
-      <c r="AG14" s="60"/>
+      <c r="Y14" s="69"/>
+      <c r="Z14" s="69"/>
+      <c r="AA14" s="69"/>
+      <c r="AB14" s="69"/>
+      <c r="AC14" s="69"/>
+      <c r="AD14" s="69"/>
+      <c r="AE14" s="69"/>
+      <c r="AF14" s="69"/>
+      <c r="AG14" s="69"/>
       <c r="AH14" s="54"/>
       <c r="AI14" s="54"/>
       <c r="AJ14" s="54"/>
@@ -2760,30 +2651,22 @@
     <row r="15" spans="1:57" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="BC3:BE3"/>
-    <mergeCell ref="BC4:BE4"/>
-    <mergeCell ref="BC5:BE5"/>
-    <mergeCell ref="AW3:AY3"/>
-    <mergeCell ref="AW4:AY4"/>
-    <mergeCell ref="AW5:AY5"/>
-    <mergeCell ref="AZ3:BB3"/>
-    <mergeCell ref="AZ4:BB4"/>
-    <mergeCell ref="AZ5:BB5"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="Y3:AA3"/>
-    <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="AK3:AM3"/>
-    <mergeCell ref="AN3:AP3"/>
-    <mergeCell ref="AQ3:AS3"/>
+    <mergeCell ref="AN5:AP5"/>
+    <mergeCell ref="AQ5:AS5"/>
+    <mergeCell ref="AT5:AV5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="Y6:AA14"/>
+    <mergeCell ref="AB6:AD14"/>
+    <mergeCell ref="AE6:AG14"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="Y5:AA5"/>
+    <mergeCell ref="AB5:AD5"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AK5:AM5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="P5:R5"/>
     <mergeCell ref="S5:U5"/>
     <mergeCell ref="V5:X5"/>
     <mergeCell ref="AT3:AV3"/>
@@ -2800,26 +2683,33 @@
     <mergeCell ref="AN4:AP4"/>
     <mergeCell ref="AQ4:AS4"/>
     <mergeCell ref="AT4:AV4"/>
-    <mergeCell ref="AN5:AP5"/>
-    <mergeCell ref="AQ5:AS5"/>
-    <mergeCell ref="AT5:AV5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="Y6:AA14"/>
-    <mergeCell ref="AB6:AD14"/>
-    <mergeCell ref="AE6:AG14"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="Y5:AA5"/>
-    <mergeCell ref="AB5:AD5"/>
-    <mergeCell ref="AE5:AG5"/>
-    <mergeCell ref="AH5:AJ5"/>
-    <mergeCell ref="AK5:AM5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="AH3:AJ3"/>
+    <mergeCell ref="AK3:AM3"/>
+    <mergeCell ref="AN3:AP3"/>
+    <mergeCell ref="AQ3:AS3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="Y3:AA3"/>
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="BC3:BE3"/>
+    <mergeCell ref="BC4:BE4"/>
+    <mergeCell ref="BC5:BE5"/>
+    <mergeCell ref="AW3:AY3"/>
+    <mergeCell ref="AW4:AY4"/>
+    <mergeCell ref="AW5:AY5"/>
+    <mergeCell ref="AZ3:BB3"/>
+    <mergeCell ref="AZ4:BB4"/>
+    <mergeCell ref="AZ5:BB5"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added ARIS Architect 9.5.0 import results to spreadsheet
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="88">
   <si>
     <t>Note: Tools that are not listed here have either not been tested or may not support both BPMN import and export.</t>
   </si>
@@ -479,6 +479,12 @@
   </si>
   <si>
     <t>2.2.0</t>
+  </si>
+  <si>
+    <t>ARIS Architect</t>
+  </si>
+  <si>
+    <t>9.5.0</t>
   </si>
 </sst>
 </file>
@@ -728,7 +734,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -844,9 +850,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -895,6 +898,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -904,6 +910,45 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -913,47 +958,26 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1331,10 +1355,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AMK15"/>
+  <dimension ref="A1:AMN15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AZ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AE1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AL10" sqref="AL10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1348,29 +1372,29 @@
     <col min="7" max="7" width="16.5703125" style="1"/>
     <col min="8" max="8" width="54.85546875" style="1"/>
     <col min="9" max="9" width="22.5703125" style="1"/>
-    <col min="10" max="54" width="9.140625" style="1"/>
-    <col min="55" max="57" width="10" style="1" customWidth="1"/>
-    <col min="58" max="1025" width="9.140625" style="1"/>
+    <col min="10" max="57" width="9.140625" style="1"/>
+    <col min="58" max="60" width="10" style="1" customWidth="1"/>
+    <col min="61" max="1028" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" ht="15.75" thickBot="1">
+    <row r="1" spans="1:63" ht="15.75" thickBot="1">
       <c r="K1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:60" ht="47.25" thickTop="1" thickBot="1">
-      <c r="A2" s="61" t="s">
+    <row r="2" spans="1:63" ht="47.25" thickTop="1" thickBot="1">
+      <c r="A2" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61" t="s">
+      <c r="B2" s="74"/>
+      <c r="C2" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61" t="s">
+      <c r="D2" s="74"/>
+      <c r="E2" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="61"/>
+      <c r="F2" s="74"/>
       <c r="G2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1533,8 +1557,17 @@
       <c r="BH2" s="8" t="s">
         <v>9</v>
       </c>
+      <c r="BI2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="BJ2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="BK2" s="8" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:60" ht="25.35" customHeight="1" thickTop="1" thickBot="1">
+    <row r="3" spans="1:63" ht="25.35" customHeight="1" thickTop="1" thickBot="1">
       <c r="A3" s="9"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -1546,91 +1579,96 @@
       <c r="I3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="62" t="s">
+      <c r="J3" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="63" t="s">
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63"/>
+      <c r="N3" s="76"/>
+      <c r="O3" s="76"/>
       <c r="P3" s="58" t="s">
         <v>13</v>
       </c>
       <c r="Q3" s="58"/>
       <c r="R3" s="58"/>
-      <c r="S3" s="58" t="s">
+      <c r="S3" s="75" t="s">
+        <v>71</v>
+      </c>
+      <c r="T3" s="82"/>
+      <c r="U3" s="83"/>
+      <c r="V3" s="58" t="s">
         <v>14</v>
-      </c>
-      <c r="T3" s="58"/>
-      <c r="U3" s="58"/>
-      <c r="V3" s="58" t="s">
-        <v>15</v>
       </c>
       <c r="W3" s="58"/>
       <c r="X3" s="58"/>
       <c r="Y3" s="58" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Z3" s="58"/>
       <c r="AA3" s="58"/>
       <c r="AB3" s="58" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AC3" s="58"/>
       <c r="AD3" s="58"/>
       <c r="AE3" s="58" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AF3" s="58"/>
       <c r="AG3" s="58"/>
       <c r="AH3" s="58" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AI3" s="58"/>
       <c r="AJ3" s="58"/>
-      <c r="AK3" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="AL3" s="64"/>
-      <c r="AM3" s="64"/>
+      <c r="AK3" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL3" s="58"/>
+      <c r="AM3" s="58"/>
       <c r="AN3" s="58" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="AO3" s="58"/>
       <c r="AP3" s="58"/>
       <c r="AQ3" s="58" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="AR3" s="58"/>
       <c r="AS3" s="58"/>
-      <c r="AT3" s="58" t="s">
+      <c r="AT3" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="AU3" s="62"/>
+      <c r="AV3" s="63"/>
+      <c r="AW3" s="75" t="s">
+        <v>21</v>
+      </c>
+      <c r="AX3" s="82"/>
+      <c r="AY3" s="83"/>
+      <c r="AZ3" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="BA3" s="82"/>
+      <c r="BB3" s="83"/>
+      <c r="BC3" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="AU3" s="58"/>
-      <c r="AV3" s="58"/>
-      <c r="AW3" s="58" t="s">
-        <v>71</v>
-      </c>
-      <c r="AX3" s="58"/>
-      <c r="AY3" s="58"/>
-      <c r="AZ3" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="BA3" s="58"/>
-      <c r="BB3" s="58"/>
-      <c r="BC3" s="75" t="s">
+      <c r="BD3" s="82"/>
+      <c r="BE3" s="83"/>
+      <c r="BF3" s="61" t="s">
         <v>81</v>
       </c>
-      <c r="BD3" s="76"/>
-      <c r="BE3" s="77"/>
-      <c r="BF3" s="58"/>
-      <c r="BG3" s="58"/>
-      <c r="BH3" s="58"/>
+      <c r="BG3" s="62"/>
+      <c r="BH3" s="63"/>
+      <c r="BI3" s="58"/>
+      <c r="BJ3" s="58"/>
+      <c r="BK3" s="58"/>
     </row>
-    <row r="4" spans="1:60" s="15" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1">
+    <row r="4" spans="1:63" s="15" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A4" s="12"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -1642,11 +1680,11 @@
       <c r="I4" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="65" t="s">
+      <c r="J4" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="65"/>
-      <c r="L4" s="65"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="72"/>
       <c r="M4" s="59" t="s">
         <v>26</v>
       </c>
@@ -1657,76 +1695,81 @@
       </c>
       <c r="Q4" s="59"/>
       <c r="R4" s="59"/>
-      <c r="S4" s="59" t="s">
+      <c r="S4" s="72" t="s">
+        <v>80</v>
+      </c>
+      <c r="T4" s="80"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="T4" s="59"/>
-      <c r="U4" s="59"/>
-      <c r="V4" s="66" t="s">
+      <c r="W4" s="59"/>
+      <c r="X4" s="59"/>
+      <c r="Y4" s="73" t="s">
         <v>84</v>
       </c>
-      <c r="W4" s="66"/>
-      <c r="X4" s="66"/>
-      <c r="Y4" s="59" t="s">
+      <c r="Z4" s="73"/>
+      <c r="AA4" s="73"/>
+      <c r="AB4" s="59" t="s">
         <v>28</v>
-      </c>
-      <c r="Z4" s="59"/>
-      <c r="AA4" s="59"/>
-      <c r="AB4" s="59">
-        <v>2.4</v>
       </c>
       <c r="AC4" s="59"/>
       <c r="AD4" s="59"/>
-      <c r="AE4" s="59" t="s">
-        <v>29</v>
+      <c r="AE4" s="59">
+        <v>2.4</v>
       </c>
       <c r="AF4" s="59"/>
       <c r="AG4" s="59"/>
       <c r="AH4" s="59" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AI4" s="59"/>
       <c r="AJ4" s="59"/>
       <c r="AK4" s="59" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AL4" s="59"/>
       <c r="AM4" s="59"/>
       <c r="AN4" s="59" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="AO4" s="59"/>
       <c r="AP4" s="59"/>
       <c r="AQ4" s="59" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="AR4" s="59"/>
       <c r="AS4" s="59"/>
-      <c r="AT4" s="59" t="s">
+      <c r="AT4" s="72" t="s">
+        <v>76</v>
+      </c>
+      <c r="AU4" s="80"/>
+      <c r="AV4" s="81"/>
+      <c r="AW4" s="72" t="s">
+        <v>31</v>
+      </c>
+      <c r="AX4" s="80"/>
+      <c r="AY4" s="81"/>
+      <c r="AZ4" s="72" t="s">
+        <v>32</v>
+      </c>
+      <c r="BA4" s="80"/>
+      <c r="BB4" s="81"/>
+      <c r="BC4" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="AU4" s="59"/>
-      <c r="AV4" s="59"/>
-      <c r="AW4" s="59" t="s">
-        <v>80</v>
-      </c>
-      <c r="AX4" s="59"/>
-      <c r="AY4" s="59"/>
-      <c r="AZ4" s="59" t="s">
-        <v>79</v>
-      </c>
-      <c r="BA4" s="59"/>
-      <c r="BB4" s="59"/>
-      <c r="BC4" s="73" t="s">
+      <c r="BD4" s="80"/>
+      <c r="BE4" s="81"/>
+      <c r="BF4" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="BD4" s="73"/>
-      <c r="BE4" s="73"/>
-      <c r="BF4" s="59"/>
-      <c r="BG4" s="59"/>
-      <c r="BH4" s="59"/>
+      <c r="BG4" s="64"/>
+      <c r="BH4" s="64"/>
+      <c r="BI4" s="59"/>
+      <c r="BJ4" s="59"/>
+      <c r="BK4" s="59"/>
     </row>
-    <row r="5" spans="1:60" ht="16.5" thickTop="1" thickBot="1">
+    <row r="5" spans="1:63" ht="16.5" thickTop="1" thickBot="1">
       <c r="A5" s="16"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -1738,38 +1781,38 @@
       <c r="I5" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="67">
+      <c r="J5" s="69">
         <v>41380</v>
       </c>
-      <c r="K5" s="67"/>
-      <c r="L5" s="67"/>
-      <c r="M5" s="68">
+      <c r="K5" s="69"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="70">
         <v>41373</v>
       </c>
-      <c r="N5" s="68"/>
-      <c r="O5" s="68"/>
+      <c r="N5" s="70"/>
+      <c r="O5" s="70"/>
       <c r="P5" s="60">
         <v>41591</v>
       </c>
       <c r="Q5" s="60"/>
-      <c r="R5" s="60"/>
-      <c r="S5" s="69">
+      <c r="R5" s="71"/>
+      <c r="S5" s="77">
+        <v>41591</v>
+      </c>
+      <c r="T5" s="78"/>
+      <c r="U5" s="79"/>
+      <c r="V5" s="71">
         <v>41383</v>
       </c>
-      <c r="T5" s="69"/>
-      <c r="U5" s="69"/>
-      <c r="V5" s="69">
+      <c r="W5" s="71"/>
+      <c r="X5" s="71"/>
+      <c r="Y5" s="71">
         <v>41599</v>
       </c>
-      <c r="W5" s="69"/>
-      <c r="X5" s="69"/>
-      <c r="Y5" s="60">
+      <c r="Z5" s="71"/>
+      <c r="AA5" s="71"/>
+      <c r="AB5" s="60">
         <v>41394</v>
-      </c>
-      <c r="Z5" s="60"/>
-      <c r="AA5" s="60"/>
-      <c r="AB5" s="60">
-        <v>41388</v>
       </c>
       <c r="AC5" s="60"/>
       <c r="AD5" s="60"/>
@@ -1779,51 +1822,56 @@
       <c r="AF5" s="60"/>
       <c r="AG5" s="60"/>
       <c r="AH5" s="60">
-        <v>41431</v>
+        <v>41388</v>
       </c>
       <c r="AI5" s="60"/>
       <c r="AJ5" s="60"/>
       <c r="AK5" s="60">
-        <v>41467</v>
+        <v>41571</v>
       </c>
       <c r="AL5" s="60"/>
       <c r="AM5" s="60"/>
       <c r="AN5" s="60">
-        <v>41435</v>
+        <v>41600</v>
       </c>
       <c r="AO5" s="60"/>
       <c r="AP5" s="60"/>
       <c r="AQ5" s="60">
-        <v>41449</v>
+        <v>41431</v>
       </c>
       <c r="AR5" s="60"/>
       <c r="AS5" s="60"/>
-      <c r="AT5" s="60">
+      <c r="AT5" s="77">
+        <v>41467</v>
+      </c>
+      <c r="AU5" s="78"/>
+      <c r="AV5" s="79"/>
+      <c r="AW5" s="77">
+        <v>41435</v>
+      </c>
+      <c r="AX5" s="78"/>
+      <c r="AY5" s="79"/>
+      <c r="AZ5" s="77">
+        <v>41449</v>
+      </c>
+      <c r="BA5" s="78"/>
+      <c r="BB5" s="79"/>
+      <c r="BC5" s="77">
         <v>41444</v>
       </c>
-      <c r="AU5" s="60"/>
-      <c r="AV5" s="60"/>
-      <c r="AW5" s="60">
-        <v>41591</v>
-      </c>
-      <c r="AX5" s="60"/>
-      <c r="AY5" s="60"/>
-      <c r="AZ5" s="60">
-        <v>41571</v>
-      </c>
-      <c r="BA5" s="60"/>
-      <c r="BB5" s="60"/>
-      <c r="BC5" s="74">
+      <c r="BD5" s="78"/>
+      <c r="BE5" s="79"/>
+      <c r="BF5" s="65">
         <v>41585</v>
       </c>
-      <c r="BD5" s="74"/>
-      <c r="BE5" s="74"/>
-      <c r="BF5" s="60"/>
-      <c r="BG5" s="60"/>
-      <c r="BH5" s="60"/>
+      <c r="BG5" s="65"/>
+      <c r="BH5" s="65"/>
+      <c r="BI5" s="60"/>
+      <c r="BJ5" s="60"/>
+      <c r="BK5" s="60"/>
     </row>
-    <row r="6" spans="1:60" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="70" t="s">
+    <row r="6" spans="1:63" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A6" s="66" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="19" t="s">
@@ -1874,69 +1922,57 @@
       <c r="Q6" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="R6" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="S6" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="T6" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="U6" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="V6" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="W6" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="X6" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y6" s="71" t="s">
+      <c r="R6" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="S6" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="W6" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="X6" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y6" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z6" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA6" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB6" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="Z6" s="71"/>
-      <c r="AA6" s="71"/>
-      <c r="AB6" s="71" t="s">
+      <c r="AC6" s="67"/>
+      <c r="AD6" s="67"/>
+      <c r="AE6" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="AC6" s="71"/>
-      <c r="AD6" s="71"/>
-      <c r="AE6" s="71" t="s">
+      <c r="AF6" s="67"/>
+      <c r="AG6" s="67"/>
+      <c r="AH6" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="AF6" s="71"/>
-      <c r="AG6" s="71"/>
-      <c r="AH6" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="AI6" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="AJ6" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="AK6" s="24" t="s">
-        <v>43</v>
-      </c>
+      <c r="AI6" s="67"/>
+      <c r="AJ6" s="67"/>
+      <c r="AK6" s="27"/>
       <c r="AL6" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="AM6" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="AN6" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="AO6" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="AP6" s="23" t="s">
-        <v>43</v>
-      </c>
+      <c r="AM6" s="24"/>
+      <c r="AN6" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="AO6" s="24"/>
+      <c r="AP6" s="24"/>
       <c r="AQ6" s="27" t="s">
         <v>43</v>
       </c>
@@ -1946,36 +1982,53 @@
       <c r="AS6" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AT6" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="AU6" s="24"/>
-      <c r="AV6" s="24"/>
-      <c r="AW6" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="AX6" s="24"/>
-      <c r="AY6" s="24"/>
-      <c r="AZ6" s="27"/>
+      <c r="AT6" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="AU6" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="AV6" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="AW6" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="AX6" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="AY6" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="AZ6" s="27" t="s">
+        <v>43</v>
+      </c>
       <c r="BA6" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="BB6" s="24"/>
+      <c r="BB6" s="24" t="s">
+        <v>42</v>
+      </c>
       <c r="BC6" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="BD6" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE6" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="BF6" s="27"/>
-      <c r="BG6" s="24"/>
-      <c r="BH6" s="24"/>
+      <c r="BD6" s="24"/>
+      <c r="BE6" s="24"/>
+      <c r="BF6" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG6" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH6" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI6" s="27"/>
+      <c r="BJ6" s="24"/>
+      <c r="BK6" s="24"/>
     </row>
-    <row r="7" spans="1:60" ht="42.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="70"/>
+    <row r="7" spans="1:63" ht="42.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A7" s="66"/>
       <c r="B7" s="30" t="s">
         <v>46</v>
       </c>
@@ -2021,66 +2074,54 @@
       <c r="P7" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="Q7" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="R7" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="S7" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="T7" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="U7" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="V7" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="W7" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="X7" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y7" s="71"/>
-      <c r="Z7" s="71"/>
-      <c r="AA7" s="71"/>
-      <c r="AB7" s="71"/>
-      <c r="AC7" s="71"/>
-      <c r="AD7" s="71"/>
-      <c r="AE7" s="71"/>
-      <c r="AF7" s="71"/>
-      <c r="AG7" s="71"/>
-      <c r="AH7" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="AI7" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="AJ7" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="AK7" s="24" t="s">
-        <v>43</v>
-      </c>
+      <c r="Q7" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="R7" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="S7" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="T7" s="24"/>
+      <c r="U7" s="24"/>
+      <c r="V7" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="W7" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="X7" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y7" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z7" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA7" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB7" s="67"/>
+      <c r="AC7" s="67"/>
+      <c r="AD7" s="67"/>
+      <c r="AE7" s="67"/>
+      <c r="AF7" s="67"/>
+      <c r="AG7" s="67"/>
+      <c r="AH7" s="67"/>
+      <c r="AI7" s="67"/>
+      <c r="AJ7" s="67"/>
+      <c r="AK7" s="27"/>
       <c r="AL7" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="AM7" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="AN7" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="AO7" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="AP7" s="23" t="s">
-        <v>43</v>
-      </c>
+      <c r="AM7" s="24"/>
+      <c r="AN7" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="AO7" s="24"/>
+      <c r="AP7" s="24"/>
       <c r="AQ7" s="27" t="s">
         <v>43</v>
       </c>
@@ -2090,36 +2131,53 @@
       <c r="AS7" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AT7" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="AU7" s="24"/>
-      <c r="AV7" s="24"/>
-      <c r="AW7" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="AX7" s="24"/>
-      <c r="AY7" s="24"/>
-      <c r="AZ7" s="27"/>
+      <c r="AT7" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="AU7" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="AV7" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="AW7" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="AX7" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="AY7" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="AZ7" s="27" t="s">
+        <v>43</v>
+      </c>
       <c r="BA7" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="BB7" s="24"/>
+      <c r="BB7" s="24" t="s">
+        <v>42</v>
+      </c>
       <c r="BC7" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="BD7" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE7" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="BF7" s="27"/>
-      <c r="BG7" s="24"/>
-      <c r="BH7" s="24"/>
+      <c r="BD7" s="24"/>
+      <c r="BE7" s="24"/>
+      <c r="BF7" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG7" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH7" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI7" s="27"/>
+      <c r="BJ7" s="24"/>
+      <c r="BK7" s="24"/>
     </row>
-    <row r="8" spans="1:60" ht="43.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A8" s="70"/>
+    <row r="8" spans="1:63" ht="43.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A8" s="66"/>
       <c r="B8" s="30"/>
       <c r="C8" s="20">
         <v>3</v>
@@ -2163,105 +2221,110 @@
       <c r="P8" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="R8" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="S8" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="T8" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="U8" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="V8" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="W8" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="X8" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y8" s="71"/>
-      <c r="Z8" s="71"/>
-      <c r="AA8" s="71"/>
-      <c r="AB8" s="71"/>
-      <c r="AC8" s="71"/>
-      <c r="AD8" s="71"/>
-      <c r="AE8" s="71"/>
-      <c r="AF8" s="71"/>
-      <c r="AG8" s="71"/>
-      <c r="AH8" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="AI8" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="AJ8" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="AK8" s="24" t="s">
-        <v>43</v>
-      </c>
+      <c r="Q8" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="R8" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="S8" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="T8" s="24"/>
+      <c r="U8" s="24"/>
+      <c r="V8" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="W8" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="X8" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y8" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z8" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA8" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB8" s="67"/>
+      <c r="AC8" s="67"/>
+      <c r="AD8" s="67"/>
+      <c r="AE8" s="67"/>
+      <c r="AF8" s="67"/>
+      <c r="AG8" s="67"/>
+      <c r="AH8" s="67"/>
+      <c r="AI8" s="67"/>
+      <c r="AJ8" s="67"/>
+      <c r="AK8" s="27"/>
       <c r="AL8" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="AM8" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="AN8" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="AO8" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="AP8" s="23" t="s">
-        <v>43</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="AM8" s="24"/>
+      <c r="AN8" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="AO8" s="24"/>
+      <c r="AP8" s="24"/>
       <c r="AQ8" s="27" t="s">
         <v>42</v>
       </c>
       <c r="AR8" s="24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AS8" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AT8" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="AU8" s="24"/>
-      <c r="AV8" s="24"/>
-      <c r="AW8" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="AX8" s="24"/>
-      <c r="AY8" s="24"/>
-      <c r="AZ8" s="27"/>
+      <c r="AT8" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="AU8" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="AV8" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="AW8" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="AX8" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="AY8" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="AZ8" s="27" t="s">
+        <v>42</v>
+      </c>
       <c r="BA8" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="BB8" s="24"/>
+      <c r="BB8" s="24" t="s">
+        <v>42</v>
+      </c>
       <c r="BC8" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="BD8" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE8" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="BF8" s="27"/>
-      <c r="BG8" s="24"/>
-      <c r="BH8" s="24"/>
+      <c r="BD8" s="24"/>
+      <c r="BE8" s="24"/>
+      <c r="BF8" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG8" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH8" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI8" s="27"/>
+      <c r="BJ8" s="24"/>
+      <c r="BK8" s="24"/>
     </row>
-    <row r="9" spans="1:60" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A9" s="70"/>
+    <row r="9" spans="1:63" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A9" s="66"/>
       <c r="B9" s="30"/>
       <c r="C9" s="20">
         <v>4</v>
@@ -2272,13 +2335,13 @@
       <c r="E9" s="22">
         <v>0</v>
       </c>
-      <c r="F9" s="56" t="s">
+      <c r="F9" s="55" t="s">
         <v>38</v>
       </c>
       <c r="G9" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="57" t="s">
+      <c r="H9" s="56" t="s">
         <v>55</v>
       </c>
       <c r="I9" s="26" t="s">
@@ -2305,105 +2368,110 @@
       <c r="P9" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="Q9" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="R9" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="S9" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="T9" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="U9" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="V9" s="21" t="s">
+      <c r="Q9" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="R9" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="S9" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="T9" s="20"/>
+      <c r="U9" s="24"/>
+      <c r="V9" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="W9" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="X9" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y9" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="W9" s="21" t="s">
+      <c r="Z9" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="X9" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y9" s="71"/>
-      <c r="Z9" s="71"/>
-      <c r="AA9" s="71"/>
-      <c r="AB9" s="71"/>
-      <c r="AC9" s="71"/>
-      <c r="AD9" s="71"/>
-      <c r="AE9" s="71"/>
-      <c r="AF9" s="71"/>
-      <c r="AG9" s="71"/>
-      <c r="AH9" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="AI9" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AJ9" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="AK9" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="AL9" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="AM9" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="AN9" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="AO9" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="AP9" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="AQ9" s="45" t="s">
-        <v>43</v>
+      <c r="AA9" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB9" s="67"/>
+      <c r="AC9" s="67"/>
+      <c r="AD9" s="67"/>
+      <c r="AE9" s="67"/>
+      <c r="AF9" s="67"/>
+      <c r="AG9" s="67"/>
+      <c r="AH9" s="67"/>
+      <c r="AI9" s="67"/>
+      <c r="AJ9" s="67"/>
+      <c r="AK9" s="27"/>
+      <c r="AL9" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM9" s="24"/>
+      <c r="AN9" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="AO9" s="20"/>
+      <c r="AP9" s="24"/>
+      <c r="AQ9" s="24" t="s">
+        <v>42</v>
       </c>
       <c r="AR9" s="20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AS9" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AT9" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="AU9" s="20"/>
-      <c r="AV9" s="24"/>
-      <c r="AW9" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="AX9" s="20"/>
-      <c r="AY9" s="24"/>
-      <c r="AZ9" s="27"/>
+      <c r="AT9" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="AU9" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="AV9" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="AW9" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="AX9" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="AY9" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="AZ9" s="44" t="s">
+        <v>43</v>
+      </c>
       <c r="BA9" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="BB9" s="24"/>
+      <c r="BB9" s="24" t="s">
+        <v>42</v>
+      </c>
       <c r="BC9" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="BD9" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE9" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="BF9" s="27"/>
-      <c r="BG9" s="20"/>
-      <c r="BH9" s="24"/>
+      <c r="BD9" s="20"/>
+      <c r="BE9" s="24"/>
+      <c r="BF9" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG9" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH9" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI9" s="27"/>
+      <c r="BJ9" s="20"/>
+      <c r="BK9" s="24"/>
     </row>
-    <row r="10" spans="1:60" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A10" s="55"/>
+    <row r="10" spans="1:63" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A10" s="54"/>
       <c r="B10" s="30"/>
       <c r="C10" s="20">
         <v>4</v>
@@ -2435,71 +2503,76 @@
       <c r="P10" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="Q10" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="R10" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="S10" s="42"/>
-      <c r="T10" s="43"/>
-      <c r="U10" s="44"/>
-      <c r="V10" s="21" t="s">
+      <c r="Q10" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="R10" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="S10" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="T10" s="20"/>
+      <c r="U10" s="24"/>
+      <c r="V10" s="41"/>
+      <c r="W10" s="42"/>
+      <c r="X10" s="43"/>
+      <c r="Y10" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="W10" s="21" t="s">
+      <c r="Z10" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="X10" s="21" t="s">
+      <c r="AA10" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="Y10" s="71"/>
-      <c r="Z10" s="71"/>
-      <c r="AA10" s="71"/>
-      <c r="AB10" s="71"/>
-      <c r="AC10" s="71"/>
-      <c r="AD10" s="71"/>
-      <c r="AE10" s="71"/>
-      <c r="AF10" s="71"/>
-      <c r="AG10" s="71"/>
-      <c r="AH10" s="24"/>
-      <c r="AI10" s="20"/>
-      <c r="AJ10" s="24"/>
-      <c r="AK10" s="24"/>
-      <c r="AL10" s="24"/>
+      <c r="AB10" s="67"/>
+      <c r="AC10" s="67"/>
+      <c r="AD10" s="67"/>
+      <c r="AE10" s="67"/>
+      <c r="AF10" s="67"/>
+      <c r="AG10" s="67"/>
+      <c r="AH10" s="67"/>
+      <c r="AI10" s="67"/>
+      <c r="AJ10" s="67"/>
+      <c r="AK10" s="27"/>
+      <c r="AL10" s="20"/>
       <c r="AM10" s="24"/>
-      <c r="AN10" s="21"/>
-      <c r="AO10" s="21"/>
-      <c r="AP10" s="21"/>
-      <c r="AQ10" s="45"/>
+      <c r="AN10" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="AO10" s="20"/>
+      <c r="AP10" s="24"/>
+      <c r="AQ10" s="24"/>
       <c r="AR10" s="20"/>
       <c r="AS10" s="24"/>
-      <c r="AT10" s="27"/>
-      <c r="AU10" s="20"/>
+      <c r="AT10" s="24"/>
+      <c r="AU10" s="24"/>
       <c r="AV10" s="24"/>
-      <c r="AW10" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="AX10" s="20"/>
-      <c r="AY10" s="24"/>
-      <c r="AZ10" s="27"/>
+      <c r="AW10" s="21"/>
+      <c r="AX10" s="21"/>
+      <c r="AY10" s="21"/>
+      <c r="AZ10" s="44"/>
       <c r="BA10" s="20"/>
       <c r="BB10" s="24"/>
-      <c r="BC10" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="BD10" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE10" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="BF10" s="27"/>
-      <c r="BG10" s="20"/>
-      <c r="BH10" s="24"/>
+      <c r="BC10" s="27"/>
+      <c r="BD10" s="20"/>
+      <c r="BE10" s="24"/>
+      <c r="BF10" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG10" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH10" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI10" s="27"/>
+      <c r="BJ10" s="20"/>
+      <c r="BK10" s="24"/>
     </row>
-    <row r="11" spans="1:60" s="47" customFormat="1" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A11" s="72" t="s">
+    <row r="11" spans="1:63" s="46" customFormat="1" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A11" s="68" t="s">
         <v>56</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -2520,7 +2593,7 @@
       <c r="G11" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="H11" s="46" t="s">
+      <c r="H11" s="45" t="s">
         <v>60</v>
       </c>
       <c r="I11" s="26" t="s">
@@ -2545,93 +2618,96 @@
       <c r="P11" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="Q11" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="R11" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="S11" s="24"/>
+      <c r="Q11" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="R11" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="S11" s="57" t="s">
+        <v>42</v>
+      </c>
       <c r="T11" s="24"/>
       <c r="U11" s="24"/>
-      <c r="V11" s="23" t="s">
+      <c r="V11" s="24"/>
+      <c r="W11" s="24"/>
+      <c r="X11" s="24"/>
+      <c r="Y11" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="W11" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="X11" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y11" s="71"/>
-      <c r="Z11" s="71"/>
-      <c r="AA11" s="71"/>
-      <c r="AB11" s="71"/>
-      <c r="AC11" s="71"/>
-      <c r="AD11" s="71"/>
-      <c r="AE11" s="71"/>
-      <c r="AF11" s="71"/>
-      <c r="AG11" s="71"/>
-      <c r="AH11" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="AI11" s="24"/>
-      <c r="AJ11" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="AK11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="AL11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="AM11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="AN11" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="AO11" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="AP11" s="23" t="s">
-        <v>42</v>
-      </c>
+      <c r="Z11" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA11" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB11" s="67"/>
+      <c r="AC11" s="67"/>
+      <c r="AD11" s="67"/>
+      <c r="AE11" s="67"/>
+      <c r="AF11" s="67"/>
+      <c r="AG11" s="67"/>
+      <c r="AH11" s="67"/>
+      <c r="AI11" s="67"/>
+      <c r="AJ11" s="67"/>
+      <c r="AK11" s="24"/>
+      <c r="AL11" s="24"/>
+      <c r="AM11" s="24"/>
+      <c r="AN11" s="24"/>
+      <c r="AO11" s="24"/>
+      <c r="AP11" s="24"/>
       <c r="AQ11" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AR11" s="24" t="s">
-        <v>42</v>
-      </c>
+      <c r="AR11" s="24"/>
       <c r="AS11" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AT11" s="24"/>
-      <c r="AU11" s="24"/>
-      <c r="AV11" s="24"/>
-      <c r="AW11" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="AX11" s="24"/>
-      <c r="AY11" s="24"/>
-      <c r="AZ11" s="24"/>
-      <c r="BA11" s="24"/>
-      <c r="BB11" s="24"/>
-      <c r="BC11" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="BD11" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE11" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="BF11" s="24"/>
-      <c r="BG11" s="24"/>
-      <c r="BH11" s="24"/>
+      <c r="AT11" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="AU11" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="AV11" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="AW11" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="AX11" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="AY11" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="AZ11" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="BA11" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="BB11" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="BC11" s="24"/>
+      <c r="BD11" s="24"/>
+      <c r="BE11" s="24"/>
+      <c r="BF11" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG11" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH11" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI11" s="24"/>
+      <c r="BJ11" s="24"/>
+      <c r="BK11" s="24"/>
     </row>
-    <row r="12" spans="1:60" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A12" s="72"/>
+    <row r="12" spans="1:63" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A12" s="68"/>
       <c r="B12" s="30" t="s">
         <v>61</v>
       </c>
@@ -2650,7 +2726,7 @@
       <c r="G12" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="H12" s="46" t="s">
+      <c r="H12" s="45" t="s">
         <v>64</v>
       </c>
       <c r="I12" s="26" t="s">
@@ -2671,107 +2747,110 @@
       <c r="P12" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="Q12" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="R12" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="S12" s="24"/>
+      <c r="Q12" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="R12" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="S12" s="57" t="s">
+        <v>42</v>
+      </c>
       <c r="T12" s="24"/>
       <c r="U12" s="24"/>
-      <c r="V12" s="23" t="s">
+      <c r="V12" s="24"/>
+      <c r="W12" s="24"/>
+      <c r="X12" s="24"/>
+      <c r="Y12" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="W12" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="X12" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y12" s="71"/>
-      <c r="Z12" s="71"/>
-      <c r="AA12" s="71"/>
-      <c r="AB12" s="71"/>
-      <c r="AC12" s="71"/>
-      <c r="AD12" s="71"/>
-      <c r="AE12" s="71"/>
-      <c r="AF12" s="71"/>
-      <c r="AG12" s="71"/>
-      <c r="AH12" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="AI12" s="24"/>
-      <c r="AJ12" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="AK12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="AL12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="AM12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="AN12" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="AO12" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="AP12" s="23" t="s">
-        <v>42</v>
-      </c>
+      <c r="Z12" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA12" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB12" s="67"/>
+      <c r="AC12" s="67"/>
+      <c r="AD12" s="67"/>
+      <c r="AE12" s="67"/>
+      <c r="AF12" s="67"/>
+      <c r="AG12" s="67"/>
+      <c r="AH12" s="67"/>
+      <c r="AI12" s="67"/>
+      <c r="AJ12" s="67"/>
+      <c r="AK12" s="24"/>
+      <c r="AL12" s="24"/>
+      <c r="AM12" s="24"/>
+      <c r="AN12" s="24"/>
+      <c r="AO12" s="24"/>
+      <c r="AP12" s="24"/>
       <c r="AQ12" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AR12" s="24" t="s">
-        <v>42</v>
-      </c>
+      <c r="AR12" s="24"/>
       <c r="AS12" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AT12" s="24"/>
-      <c r="AU12" s="24"/>
-      <c r="AV12" s="24"/>
-      <c r="AW12" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="AX12" s="24"/>
-      <c r="AY12" s="24"/>
-      <c r="AZ12" s="24"/>
-      <c r="BA12" s="24"/>
-      <c r="BB12" s="24"/>
-      <c r="BC12" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="BD12" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE12" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="BF12" s="24"/>
-      <c r="BG12" s="24"/>
-      <c r="BH12" s="24"/>
+      <c r="AT12" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="AU12" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="AV12" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="AW12" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="AX12" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="AY12" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="AZ12" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="BA12" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="BB12" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="BC12" s="24"/>
+      <c r="BD12" s="24"/>
+      <c r="BE12" s="24"/>
+      <c r="BF12" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG12" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BH12" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI12" s="24"/>
+      <c r="BJ12" s="24"/>
+      <c r="BK12" s="24"/>
     </row>
-    <row r="13" spans="1:60" ht="63" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A13" s="72"/>
+    <row r="13" spans="1:63" ht="63" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A13" s="68"/>
       <c r="B13" s="30"/>
-      <c r="C13" s="48">
+      <c r="C13" s="47">
         <v>3</v>
       </c>
-      <c r="D13" s="49" t="s">
+      <c r="D13" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="50">
+      <c r="E13" s="49">
         <v>0</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="51" t="s">
+      <c r="G13" s="50" t="s">
         <v>66</v>
       </c>
       <c r="H13" s="31" t="s">
@@ -2795,18 +2874,18 @@
       <c r="V13" s="24"/>
       <c r="W13" s="24"/>
       <c r="X13" s="24"/>
-      <c r="Y13" s="71"/>
-      <c r="Z13" s="71"/>
-      <c r="AA13" s="71"/>
-      <c r="AB13" s="71"/>
-      <c r="AC13" s="71"/>
-      <c r="AD13" s="71"/>
-      <c r="AE13" s="71"/>
-      <c r="AF13" s="71"/>
-      <c r="AG13" s="71"/>
-      <c r="AH13" s="24"/>
-      <c r="AI13" s="24"/>
-      <c r="AJ13" s="24"/>
+      <c r="Y13" s="24"/>
+      <c r="Z13" s="24"/>
+      <c r="AA13" s="24"/>
+      <c r="AB13" s="67"/>
+      <c r="AC13" s="67"/>
+      <c r="AD13" s="67"/>
+      <c r="AE13" s="67"/>
+      <c r="AF13" s="67"/>
+      <c r="AG13" s="67"/>
+      <c r="AH13" s="67"/>
+      <c r="AI13" s="67"/>
+      <c r="AJ13" s="67"/>
       <c r="AK13" s="24"/>
       <c r="AL13" s="24"/>
       <c r="AM13" s="24"/>
@@ -2831,145 +2910,154 @@
       <c r="BF13" s="24"/>
       <c r="BG13" s="24"/>
       <c r="BH13" s="24"/>
+      <c r="BI13" s="24"/>
+      <c r="BJ13" s="24"/>
+      <c r="BK13" s="24"/>
     </row>
-    <row r="14" spans="1:60" ht="45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A14" s="72"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="51">
+    <row r="14" spans="1:63" ht="45" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A14" s="68"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="50">
         <v>4</v>
       </c>
-      <c r="D14" s="49" t="s">
+      <c r="D14" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="50">
+      <c r="E14" s="49">
         <v>0</v>
       </c>
-      <c r="F14" s="49" t="s">
+      <c r="F14" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="51" t="s">
+      <c r="G14" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="H14" s="53" t="s">
+      <c r="H14" s="52" t="s">
         <v>70</v>
       </c>
       <c r="I14" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="54"/>
-      <c r="M14" s="54"/>
-      <c r="N14" s="54"/>
-      <c r="O14" s="54"/>
-      <c r="P14" s="54"/>
-      <c r="Q14" s="54"/>
-      <c r="R14" s="54"/>
-      <c r="S14" s="54"/>
-      <c r="T14" s="54"/>
-      <c r="U14" s="54"/>
-      <c r="V14" s="54"/>
-      <c r="W14" s="54"/>
-      <c r="X14" s="54"/>
-      <c r="Y14" s="71"/>
-      <c r="Z14" s="71"/>
-      <c r="AA14" s="71"/>
-      <c r="AB14" s="71"/>
-      <c r="AC14" s="71"/>
-      <c r="AD14" s="71"/>
-      <c r="AE14" s="71"/>
-      <c r="AF14" s="71"/>
-      <c r="AG14" s="71"/>
-      <c r="AH14" s="54"/>
-      <c r="AI14" s="54"/>
-      <c r="AJ14" s="54"/>
-      <c r="AK14" s="54"/>
-      <c r="AL14" s="54"/>
-      <c r="AM14" s="54"/>
-      <c r="AN14" s="54"/>
-      <c r="AO14" s="54"/>
-      <c r="AP14" s="54"/>
-      <c r="AQ14" s="54"/>
-      <c r="AR14" s="54"/>
-      <c r="AS14" s="54"/>
-      <c r="AT14" s="54"/>
-      <c r="AU14" s="54"/>
-      <c r="AV14" s="54"/>
-      <c r="AW14" s="54"/>
-      <c r="AX14" s="54"/>
-      <c r="AY14" s="54"/>
-      <c r="AZ14" s="54"/>
-      <c r="BA14" s="54"/>
-      <c r="BB14" s="54"/>
-      <c r="BC14" s="54"/>
-      <c r="BD14" s="54"/>
-      <c r="BE14" s="54"/>
-      <c r="BF14" s="54"/>
-      <c r="BG14" s="54"/>
-      <c r="BH14" s="54"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="53"/>
+      <c r="M14" s="53"/>
+      <c r="N14" s="53"/>
+      <c r="O14" s="53"/>
+      <c r="P14" s="53"/>
+      <c r="Q14" s="53"/>
+      <c r="R14" s="53"/>
+      <c r="S14" s="53"/>
+      <c r="T14" s="53"/>
+      <c r="U14" s="53"/>
+      <c r="V14" s="53"/>
+      <c r="W14" s="53"/>
+      <c r="X14" s="53"/>
+      <c r="Y14" s="53"/>
+      <c r="Z14" s="53"/>
+      <c r="AA14" s="53"/>
+      <c r="AB14" s="67"/>
+      <c r="AC14" s="67"/>
+      <c r="AD14" s="67"/>
+      <c r="AE14" s="67"/>
+      <c r="AF14" s="67"/>
+      <c r="AG14" s="67"/>
+      <c r="AH14" s="67"/>
+      <c r="AI14" s="67"/>
+      <c r="AJ14" s="67"/>
+      <c r="AK14" s="53"/>
+      <c r="AL14" s="53"/>
+      <c r="AM14" s="53"/>
+      <c r="AN14" s="53"/>
+      <c r="AO14" s="53"/>
+      <c r="AP14" s="53"/>
+      <c r="AQ14" s="53"/>
+      <c r="AR14" s="53"/>
+      <c r="AS14" s="53"/>
+      <c r="AT14" s="53"/>
+      <c r="AU14" s="53"/>
+      <c r="AV14" s="53"/>
+      <c r="AW14" s="53"/>
+      <c r="AX14" s="53"/>
+      <c r="AY14" s="53"/>
+      <c r="AZ14" s="53"/>
+      <c r="BA14" s="53"/>
+      <c r="BB14" s="53"/>
+      <c r="BC14" s="53"/>
+      <c r="BD14" s="53"/>
+      <c r="BE14" s="53"/>
+      <c r="BF14" s="53"/>
+      <c r="BG14" s="53"/>
+      <c r="BH14" s="53"/>
+      <c r="BI14" s="53"/>
+      <c r="BJ14" s="53"/>
+      <c r="BK14" s="53"/>
     </row>
-    <row r="15" spans="1:60" ht="15.75" thickTop="1"/>
+    <row r="15" spans="1:63" ht="15.75" thickTop="1"/>
   </sheetData>
-  <mergeCells count="59">
-    <mergeCell ref="BF3:BH3"/>
-    <mergeCell ref="BF4:BH4"/>
-    <mergeCell ref="BF5:BH5"/>
-    <mergeCell ref="AN5:AP5"/>
-    <mergeCell ref="AQ5:AS5"/>
+  <mergeCells count="62">
+    <mergeCell ref="AW5:AY5"/>
     <mergeCell ref="AT5:AV5"/>
     <mergeCell ref="AT3:AV3"/>
+    <mergeCell ref="AN3:AP3"/>
     <mergeCell ref="AN4:AP4"/>
-    <mergeCell ref="AQ4:AS4"/>
-    <mergeCell ref="AT4:AV4"/>
+    <mergeCell ref="AN5:AP5"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="BC4:BE4"/>
+    <mergeCell ref="AZ4:BB4"/>
     <mergeCell ref="BC3:BE3"/>
-    <mergeCell ref="BC4:BE4"/>
     <mergeCell ref="BC5:BE5"/>
-    <mergeCell ref="AW3:AY3"/>
-    <mergeCell ref="AW4:AY4"/>
-    <mergeCell ref="AW5:AY5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="Y6:AA14"/>
-    <mergeCell ref="AB6:AD14"/>
-    <mergeCell ref="AE6:AG14"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="Y5:AA5"/>
-    <mergeCell ref="AB5:AD5"/>
-    <mergeCell ref="AE5:AG5"/>
-    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AZ5:BB5"/>
+    <mergeCell ref="AK3:AM3"/>
+    <mergeCell ref="AK4:AM4"/>
     <mergeCell ref="AK5:AM5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="V5:X5"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="V4:X4"/>
-    <mergeCell ref="AN3:AP3"/>
-    <mergeCell ref="AQ3:AS3"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="AB4:AD4"/>
-    <mergeCell ref="AE4:AG4"/>
-    <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="AK4:AM4"/>
-    <mergeCell ref="AZ3:BB3"/>
-    <mergeCell ref="AZ4:BB4"/>
-    <mergeCell ref="AZ5:BB5"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="J3:L3"/>
     <mergeCell ref="M3:O3"/>
     <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:U3"/>
     <mergeCell ref="V3:X3"/>
     <mergeCell ref="Y3:AA3"/>
     <mergeCell ref="AB3:AD3"/>
     <mergeCell ref="AE3:AG3"/>
     <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="AK3:AM3"/>
+    <mergeCell ref="AQ3:AS3"/>
+    <mergeCell ref="AW3:AY3"/>
+    <mergeCell ref="AZ3:BB3"/>
+    <mergeCell ref="AB4:AD4"/>
+    <mergeCell ref="AE4:AG4"/>
+    <mergeCell ref="AH4:AJ4"/>
+    <mergeCell ref="AQ4:AS4"/>
+    <mergeCell ref="AT4:AV4"/>
+    <mergeCell ref="AW4:AY4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="Y5:AA5"/>
+    <mergeCell ref="AB5:AD5"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AQ5:AS5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="AB6:AD14"/>
+    <mergeCell ref="AE6:AG14"/>
+    <mergeCell ref="AH6:AJ14"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="BI3:BK3"/>
+    <mergeCell ref="BI4:BK4"/>
+    <mergeCell ref="BI5:BK5"/>
+    <mergeCell ref="BF3:BH3"/>
+    <mergeCell ref="BF4:BH4"/>
+    <mergeCell ref="BF5:BH5"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Add test results camunda Modeler 2.3.0
import and roundtrip test
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="13830" yWindow="-15" windowWidth="13890" windowHeight="12870" tabRatio="631"/>
@@ -11,116 +11,6 @@
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>mschoe</author>
-  </authors>
-  <commentList>
-    <comment ref="P8" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>mschoe:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-sub process not collapsed. Wrong interpretaion of missing isExpanded attribute </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P9" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>mschoe:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-modeler cannot display lanes without pools</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P11" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>mschoe:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-- collapsed Call Activities can be displayed only
-- Group is missing
-- collapsed sub process is displayed as expanded</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P12" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>mschoe:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-- collapsed Call Activities can be displayed only
-- collapsed sub process is displayed as expanded
-- group is missing</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -478,13 +368,13 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>2.2.0</t>
-  </si>
-  <si>
     <t>ARIS Architect</t>
   </si>
   <si>
     <t>9.5.0</t>
+  </si>
+  <si>
+    <t>2.3.0</t>
   </si>
 </sst>
 </file>
@@ -494,7 +384,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -539,19 +429,6 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -901,6 +778,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -910,14 +805,50 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -925,63 +856,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="TableStyleLight1" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1066,9 +943,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1106,7 +983,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1178,7 +1055,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1351,17 +1228,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AMN15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AE1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AL10" sqref="AL10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="44.85546875" style="1"/>
@@ -1383,18 +1260,18 @@
       </c>
     </row>
     <row r="2" spans="1:63" ht="47.25" thickTop="1" thickBot="1">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74" t="s">
+      <c r="B2" s="73"/>
+      <c r="C2" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74" t="s">
+      <c r="D2" s="73"/>
+      <c r="E2" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="74"/>
+      <c r="F2" s="73"/>
       <c r="G2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1579,94 +1456,94 @@
       <c r="I3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="75" t="s">
+      <c r="J3" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
-      <c r="M3" s="76" t="s">
+      <c r="K3" s="70"/>
+      <c r="L3" s="70"/>
+      <c r="M3" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="76"/>
-      <c r="O3" s="76"/>
-      <c r="P3" s="58" t="s">
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="58"/>
-      <c r="S3" s="75" t="s">
+      <c r="Q3" s="64"/>
+      <c r="R3" s="64"/>
+      <c r="S3" s="70" t="s">
         <v>71</v>
       </c>
-      <c r="T3" s="82"/>
-      <c r="U3" s="83"/>
-      <c r="V3" s="58" t="s">
+      <c r="T3" s="71"/>
+      <c r="U3" s="72"/>
+      <c r="V3" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="W3" s="58"/>
-      <c r="X3" s="58"/>
-      <c r="Y3" s="58" t="s">
+      <c r="W3" s="64"/>
+      <c r="X3" s="64"/>
+      <c r="Y3" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="Z3" s="58"/>
-      <c r="AA3" s="58"/>
-      <c r="AB3" s="58" t="s">
+      <c r="Z3" s="64"/>
+      <c r="AA3" s="64"/>
+      <c r="AB3" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="AC3" s="58"/>
-      <c r="AD3" s="58"/>
-      <c r="AE3" s="58" t="s">
+      <c r="AC3" s="64"/>
+      <c r="AD3" s="64"/>
+      <c r="AE3" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="AF3" s="58"/>
-      <c r="AG3" s="58"/>
-      <c r="AH3" s="58" t="s">
+      <c r="AF3" s="64"/>
+      <c r="AG3" s="64"/>
+      <c r="AH3" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="AI3" s="58"/>
-      <c r="AJ3" s="58"/>
-      <c r="AK3" s="58" t="s">
+      <c r="AI3" s="64"/>
+      <c r="AJ3" s="64"/>
+      <c r="AK3" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="AL3" s="58"/>
-      <c r="AM3" s="58"/>
-      <c r="AN3" s="58" t="s">
-        <v>86</v>
-      </c>
-      <c r="AO3" s="58"/>
-      <c r="AP3" s="58"/>
-      <c r="AQ3" s="58" t="s">
+      <c r="AL3" s="64"/>
+      <c r="AM3" s="64"/>
+      <c r="AN3" s="64" t="s">
+        <v>85</v>
+      </c>
+      <c r="AO3" s="64"/>
+      <c r="AP3" s="64"/>
+      <c r="AQ3" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="AR3" s="58"/>
-      <c r="AS3" s="58"/>
+      <c r="AR3" s="64"/>
+      <c r="AS3" s="64"/>
       <c r="AT3" s="61" t="s">
         <v>20</v>
       </c>
       <c r="AU3" s="62"/>
       <c r="AV3" s="63"/>
-      <c r="AW3" s="75" t="s">
+      <c r="AW3" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="AX3" s="82"/>
-      <c r="AY3" s="83"/>
-      <c r="AZ3" s="75" t="s">
+      <c r="AX3" s="71"/>
+      <c r="AY3" s="72"/>
+      <c r="AZ3" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="BA3" s="82"/>
-      <c r="BB3" s="83"/>
-      <c r="BC3" s="75" t="s">
+      <c r="BA3" s="71"/>
+      <c r="BB3" s="72"/>
+      <c r="BC3" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="BD3" s="82"/>
-      <c r="BE3" s="83"/>
+      <c r="BD3" s="71"/>
+      <c r="BE3" s="72"/>
       <c r="BF3" s="61" t="s">
         <v>81</v>
       </c>
       <c r="BG3" s="62"/>
       <c r="BH3" s="63"/>
-      <c r="BI3" s="58"/>
-      <c r="BJ3" s="58"/>
-      <c r="BK3" s="58"/>
+      <c r="BI3" s="64"/>
+      <c r="BJ3" s="64"/>
+      <c r="BK3" s="64"/>
     </row>
     <row r="4" spans="1:63" s="15" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A4" s="12"/>
@@ -1680,94 +1557,94 @@
       <c r="I4" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="72" t="s">
+      <c r="J4" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="72"/>
-      <c r="L4" s="72"/>
-      <c r="M4" s="59" t="s">
+      <c r="K4" s="67"/>
+      <c r="L4" s="67"/>
+      <c r="M4" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="59"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="59" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q4" s="59"/>
-      <c r="R4" s="59"/>
-      <c r="S4" s="72" t="s">
+      <c r="N4" s="65"/>
+      <c r="O4" s="65"/>
+      <c r="P4" s="65" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q4" s="65"/>
+      <c r="R4" s="65"/>
+      <c r="S4" s="67" t="s">
         <v>80</v>
       </c>
-      <c r="T4" s="80"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="59" t="s">
+      <c r="T4" s="68"/>
+      <c r="U4" s="69"/>
+      <c r="V4" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="W4" s="59"/>
-      <c r="X4" s="59"/>
-      <c r="Y4" s="73" t="s">
+      <c r="W4" s="65"/>
+      <c r="X4" s="65"/>
+      <c r="Y4" s="75" t="s">
         <v>84</v>
       </c>
-      <c r="Z4" s="73"/>
-      <c r="AA4" s="73"/>
-      <c r="AB4" s="59" t="s">
+      <c r="Z4" s="75"/>
+      <c r="AA4" s="75"/>
+      <c r="AB4" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="AC4" s="59"/>
-      <c r="AD4" s="59"/>
-      <c r="AE4" s="59">
+      <c r="AC4" s="65"/>
+      <c r="AD4" s="65"/>
+      <c r="AE4" s="65">
         <v>2.4</v>
       </c>
-      <c r="AF4" s="59"/>
-      <c r="AG4" s="59"/>
-      <c r="AH4" s="59" t="s">
+      <c r="AF4" s="65"/>
+      <c r="AG4" s="65"/>
+      <c r="AH4" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="AI4" s="59"/>
-      <c r="AJ4" s="59"/>
-      <c r="AK4" s="59" t="s">
+      <c r="AI4" s="65"/>
+      <c r="AJ4" s="65"/>
+      <c r="AK4" s="65" t="s">
         <v>79</v>
       </c>
-      <c r="AL4" s="59"/>
-      <c r="AM4" s="59"/>
-      <c r="AN4" s="59" t="s">
-        <v>87</v>
-      </c>
-      <c r="AO4" s="59"/>
-      <c r="AP4" s="59"/>
-      <c r="AQ4" s="59" t="s">
+      <c r="AL4" s="65"/>
+      <c r="AM4" s="65"/>
+      <c r="AN4" s="65" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO4" s="65"/>
+      <c r="AP4" s="65"/>
+      <c r="AQ4" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="AR4" s="59"/>
-      <c r="AS4" s="59"/>
-      <c r="AT4" s="72" t="s">
+      <c r="AR4" s="65"/>
+      <c r="AS4" s="65"/>
+      <c r="AT4" s="67" t="s">
         <v>76</v>
       </c>
-      <c r="AU4" s="80"/>
-      <c r="AV4" s="81"/>
-      <c r="AW4" s="72" t="s">
+      <c r="AU4" s="68"/>
+      <c r="AV4" s="69"/>
+      <c r="AW4" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="AX4" s="80"/>
-      <c r="AY4" s="81"/>
-      <c r="AZ4" s="72" t="s">
+      <c r="AX4" s="68"/>
+      <c r="AY4" s="69"/>
+      <c r="AZ4" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="BA4" s="80"/>
-      <c r="BB4" s="81"/>
-      <c r="BC4" s="72" t="s">
+      <c r="BA4" s="68"/>
+      <c r="BB4" s="69"/>
+      <c r="BC4" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="BD4" s="80"/>
-      <c r="BE4" s="81"/>
-      <c r="BF4" s="64" t="s">
+      <c r="BD4" s="68"/>
+      <c r="BE4" s="69"/>
+      <c r="BF4" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="BG4" s="64"/>
-      <c r="BH4" s="64"/>
-      <c r="BI4" s="59"/>
-      <c r="BJ4" s="59"/>
-      <c r="BK4" s="59"/>
+      <c r="BG4" s="82"/>
+      <c r="BH4" s="82"/>
+      <c r="BI4" s="65"/>
+      <c r="BJ4" s="65"/>
+      <c r="BK4" s="65"/>
     </row>
     <row r="5" spans="1:63" ht="16.5" thickTop="1" thickBot="1">
       <c r="A5" s="16"/>
@@ -1781,97 +1658,97 @@
       <c r="I5" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="69">
+      <c r="J5" s="76">
         <v>41380</v>
       </c>
-      <c r="K5" s="69"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="70">
+      <c r="K5" s="76"/>
+      <c r="L5" s="76"/>
+      <c r="M5" s="77">
         <v>41373</v>
       </c>
-      <c r="N5" s="70"/>
-      <c r="O5" s="70"/>
-      <c r="P5" s="60">
+      <c r="N5" s="77"/>
+      <c r="O5" s="77"/>
+      <c r="P5" s="66">
+        <v>41614</v>
+      </c>
+      <c r="Q5" s="66"/>
+      <c r="R5" s="78"/>
+      <c r="S5" s="58">
         <v>41591</v>
       </c>
-      <c r="Q5" s="60"/>
-      <c r="R5" s="71"/>
-      <c r="S5" s="77">
-        <v>41591</v>
-      </c>
-      <c r="T5" s="78"/>
-      <c r="U5" s="79"/>
-      <c r="V5" s="71">
+      <c r="T5" s="59"/>
+      <c r="U5" s="60"/>
+      <c r="V5" s="78">
         <v>41383</v>
       </c>
-      <c r="W5" s="71"/>
-      <c r="X5" s="71"/>
-      <c r="Y5" s="71">
+      <c r="W5" s="78"/>
+      <c r="X5" s="78"/>
+      <c r="Y5" s="78">
         <v>41599</v>
       </c>
-      <c r="Z5" s="71"/>
-      <c r="AA5" s="71"/>
-      <c r="AB5" s="60">
+      <c r="Z5" s="78"/>
+      <c r="AA5" s="78"/>
+      <c r="AB5" s="66">
         <v>41394</v>
       </c>
-      <c r="AC5" s="60"/>
-      <c r="AD5" s="60"/>
-      <c r="AE5" s="60">
+      <c r="AC5" s="66"/>
+      <c r="AD5" s="66"/>
+      <c r="AE5" s="66">
         <v>41388</v>
       </c>
-      <c r="AF5" s="60"/>
-      <c r="AG5" s="60"/>
-      <c r="AH5" s="60">
+      <c r="AF5" s="66"/>
+      <c r="AG5" s="66"/>
+      <c r="AH5" s="66">
         <v>41388</v>
       </c>
-      <c r="AI5" s="60"/>
-      <c r="AJ5" s="60"/>
-      <c r="AK5" s="60">
+      <c r="AI5" s="66"/>
+      <c r="AJ5" s="66"/>
+      <c r="AK5" s="66">
         <v>41571</v>
       </c>
-      <c r="AL5" s="60"/>
-      <c r="AM5" s="60"/>
-      <c r="AN5" s="60">
+      <c r="AL5" s="66"/>
+      <c r="AM5" s="66"/>
+      <c r="AN5" s="66">
         <v>41600</v>
       </c>
-      <c r="AO5" s="60"/>
-      <c r="AP5" s="60"/>
-      <c r="AQ5" s="60">
+      <c r="AO5" s="66"/>
+      <c r="AP5" s="66"/>
+      <c r="AQ5" s="66">
         <v>41431</v>
       </c>
-      <c r="AR5" s="60"/>
-      <c r="AS5" s="60"/>
-      <c r="AT5" s="77">
+      <c r="AR5" s="66"/>
+      <c r="AS5" s="66"/>
+      <c r="AT5" s="58">
         <v>41467</v>
       </c>
-      <c r="AU5" s="78"/>
-      <c r="AV5" s="79"/>
-      <c r="AW5" s="77">
+      <c r="AU5" s="59"/>
+      <c r="AV5" s="60"/>
+      <c r="AW5" s="58">
         <v>41435</v>
       </c>
-      <c r="AX5" s="78"/>
-      <c r="AY5" s="79"/>
-      <c r="AZ5" s="77">
+      <c r="AX5" s="59"/>
+      <c r="AY5" s="60"/>
+      <c r="AZ5" s="58">
         <v>41449</v>
       </c>
-      <c r="BA5" s="78"/>
-      <c r="BB5" s="79"/>
-      <c r="BC5" s="77">
+      <c r="BA5" s="59"/>
+      <c r="BB5" s="60"/>
+      <c r="BC5" s="58">
         <v>41444</v>
       </c>
-      <c r="BD5" s="78"/>
-      <c r="BE5" s="79"/>
-      <c r="BF5" s="65">
+      <c r="BD5" s="59"/>
+      <c r="BE5" s="60"/>
+      <c r="BF5" s="83">
         <v>41585</v>
       </c>
-      <c r="BG5" s="65"/>
-      <c r="BH5" s="65"/>
-      <c r="BI5" s="60"/>
-      <c r="BJ5" s="60"/>
-      <c r="BK5" s="60"/>
+      <c r="BG5" s="83"/>
+      <c r="BH5" s="83"/>
+      <c r="BI5" s="66"/>
+      <c r="BJ5" s="66"/>
+      <c r="BK5" s="66"/>
     </row>
     <row r="6" spans="1:63" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="79" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="19" t="s">
@@ -1948,21 +1825,21 @@
       <c r="AA6" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="AB6" s="67" t="s">
+      <c r="AB6" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="AC6" s="67"/>
-      <c r="AD6" s="67"/>
-      <c r="AE6" s="67" t="s">
+      <c r="AC6" s="80"/>
+      <c r="AD6" s="80"/>
+      <c r="AE6" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="AF6" s="67"/>
-      <c r="AG6" s="67"/>
-      <c r="AH6" s="67" t="s">
+      <c r="AF6" s="80"/>
+      <c r="AG6" s="80"/>
+      <c r="AH6" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="AI6" s="67"/>
-      <c r="AJ6" s="67"/>
+      <c r="AI6" s="80"/>
+      <c r="AJ6" s="80"/>
       <c r="AK6" s="27"/>
       <c r="AL6" s="24" t="s">
         <v>43</v>
@@ -2028,7 +1905,7 @@
       <c r="BK6" s="24"/>
     </row>
     <row r="7" spans="1:63" ht="42.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="66"/>
+      <c r="A7" s="79"/>
       <c r="B7" s="30" t="s">
         <v>46</v>
       </c>
@@ -2103,15 +1980,15 @@
       <c r="AA7" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="AB7" s="67"/>
-      <c r="AC7" s="67"/>
-      <c r="AD7" s="67"/>
-      <c r="AE7" s="67"/>
-      <c r="AF7" s="67"/>
-      <c r="AG7" s="67"/>
-      <c r="AH7" s="67"/>
-      <c r="AI7" s="67"/>
-      <c r="AJ7" s="67"/>
+      <c r="AB7" s="80"/>
+      <c r="AC7" s="80"/>
+      <c r="AD7" s="80"/>
+      <c r="AE7" s="80"/>
+      <c r="AF7" s="80"/>
+      <c r="AG7" s="80"/>
+      <c r="AH7" s="80"/>
+      <c r="AI7" s="80"/>
+      <c r="AJ7" s="80"/>
       <c r="AK7" s="27"/>
       <c r="AL7" s="24" t="s">
         <v>43</v>
@@ -2177,7 +2054,7 @@
       <c r="BK7" s="24"/>
     </row>
     <row r="8" spans="1:63" ht="43.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A8" s="66"/>
+      <c r="A8" s="79"/>
       <c r="B8" s="30"/>
       <c r="C8" s="20">
         <v>3</v>
@@ -2219,13 +2096,13 @@
         <v>43</v>
       </c>
       <c r="P8" s="24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q8" s="57" t="s">
         <v>43</v>
       </c>
       <c r="R8" s="57" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S8" s="57" t="s">
         <v>43</v>
@@ -2250,15 +2127,15 @@
       <c r="AA8" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="AB8" s="67"/>
-      <c r="AC8" s="67"/>
-      <c r="AD8" s="67"/>
-      <c r="AE8" s="67"/>
-      <c r="AF8" s="67"/>
-      <c r="AG8" s="67"/>
-      <c r="AH8" s="67"/>
-      <c r="AI8" s="67"/>
-      <c r="AJ8" s="67"/>
+      <c r="AB8" s="80"/>
+      <c r="AC8" s="80"/>
+      <c r="AD8" s="80"/>
+      <c r="AE8" s="80"/>
+      <c r="AF8" s="80"/>
+      <c r="AG8" s="80"/>
+      <c r="AH8" s="80"/>
+      <c r="AI8" s="80"/>
+      <c r="AJ8" s="80"/>
       <c r="AK8" s="27"/>
       <c r="AL8" s="24" t="s">
         <v>42</v>
@@ -2324,7 +2201,7 @@
       <c r="BK8" s="24"/>
     </row>
     <row r="9" spans="1:63" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A9" s="66"/>
+      <c r="A9" s="79"/>
       <c r="B9" s="30"/>
       <c r="C9" s="20">
         <v>4</v>
@@ -2397,15 +2274,15 @@
       <c r="AA9" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="AB9" s="67"/>
-      <c r="AC9" s="67"/>
-      <c r="AD9" s="67"/>
-      <c r="AE9" s="67"/>
-      <c r="AF9" s="67"/>
-      <c r="AG9" s="67"/>
-      <c r="AH9" s="67"/>
-      <c r="AI9" s="67"/>
-      <c r="AJ9" s="67"/>
+      <c r="AB9" s="80"/>
+      <c r="AC9" s="80"/>
+      <c r="AD9" s="80"/>
+      <c r="AE9" s="80"/>
+      <c r="AF9" s="80"/>
+      <c r="AG9" s="80"/>
+      <c r="AH9" s="80"/>
+      <c r="AI9" s="80"/>
+      <c r="AJ9" s="80"/>
       <c r="AK9" s="27"/>
       <c r="AL9" s="20" t="s">
         <v>42</v>
@@ -2526,15 +2403,15 @@
       <c r="AA10" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="AB10" s="67"/>
-      <c r="AC10" s="67"/>
-      <c r="AD10" s="67"/>
-      <c r="AE10" s="67"/>
-      <c r="AF10" s="67"/>
-      <c r="AG10" s="67"/>
-      <c r="AH10" s="67"/>
-      <c r="AI10" s="67"/>
-      <c r="AJ10" s="67"/>
+      <c r="AB10" s="80"/>
+      <c r="AC10" s="80"/>
+      <c r="AD10" s="80"/>
+      <c r="AE10" s="80"/>
+      <c r="AF10" s="80"/>
+      <c r="AG10" s="80"/>
+      <c r="AH10" s="80"/>
+      <c r="AI10" s="80"/>
+      <c r="AJ10" s="80"/>
       <c r="AK10" s="27"/>
       <c r="AL10" s="20"/>
       <c r="AM10" s="24"/>
@@ -2572,7 +2449,7 @@
       <c r="BK10" s="24"/>
     </row>
     <row r="11" spans="1:63" s="46" customFormat="1" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A11" s="68" t="s">
+      <c r="A11" s="81" t="s">
         <v>56</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -2641,15 +2518,15 @@
       <c r="AA11" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="AB11" s="67"/>
-      <c r="AC11" s="67"/>
-      <c r="AD11" s="67"/>
-      <c r="AE11" s="67"/>
-      <c r="AF11" s="67"/>
-      <c r="AG11" s="67"/>
-      <c r="AH11" s="67"/>
-      <c r="AI11" s="67"/>
-      <c r="AJ11" s="67"/>
+      <c r="AB11" s="80"/>
+      <c r="AC11" s="80"/>
+      <c r="AD11" s="80"/>
+      <c r="AE11" s="80"/>
+      <c r="AF11" s="80"/>
+      <c r="AG11" s="80"/>
+      <c r="AH11" s="80"/>
+      <c r="AI11" s="80"/>
+      <c r="AJ11" s="80"/>
       <c r="AK11" s="24"/>
       <c r="AL11" s="24"/>
       <c r="AM11" s="24"/>
@@ -2707,7 +2584,7 @@
       <c r="BK11" s="24"/>
     </row>
     <row r="12" spans="1:63" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A12" s="68"/>
+      <c r="A12" s="81"/>
       <c r="B12" s="30" t="s">
         <v>61</v>
       </c>
@@ -2770,15 +2647,15 @@
       <c r="AA12" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="AB12" s="67"/>
-      <c r="AC12" s="67"/>
-      <c r="AD12" s="67"/>
-      <c r="AE12" s="67"/>
-      <c r="AF12" s="67"/>
-      <c r="AG12" s="67"/>
-      <c r="AH12" s="67"/>
-      <c r="AI12" s="67"/>
-      <c r="AJ12" s="67"/>
+      <c r="AB12" s="80"/>
+      <c r="AC12" s="80"/>
+      <c r="AD12" s="80"/>
+      <c r="AE12" s="80"/>
+      <c r="AF12" s="80"/>
+      <c r="AG12" s="80"/>
+      <c r="AH12" s="80"/>
+      <c r="AI12" s="80"/>
+      <c r="AJ12" s="80"/>
       <c r="AK12" s="24"/>
       <c r="AL12" s="24"/>
       <c r="AM12" s="24"/>
@@ -2836,7 +2713,7 @@
       <c r="BK12" s="24"/>
     </row>
     <row r="13" spans="1:63" ht="63" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A13" s="68"/>
+      <c r="A13" s="81"/>
       <c r="B13" s="30"/>
       <c r="C13" s="47">
         <v>3</v>
@@ -2877,15 +2754,15 @@
       <c r="Y13" s="24"/>
       <c r="Z13" s="24"/>
       <c r="AA13" s="24"/>
-      <c r="AB13" s="67"/>
-      <c r="AC13" s="67"/>
-      <c r="AD13" s="67"/>
-      <c r="AE13" s="67"/>
-      <c r="AF13" s="67"/>
-      <c r="AG13" s="67"/>
-      <c r="AH13" s="67"/>
-      <c r="AI13" s="67"/>
-      <c r="AJ13" s="67"/>
+      <c r="AB13" s="80"/>
+      <c r="AC13" s="80"/>
+      <c r="AD13" s="80"/>
+      <c r="AE13" s="80"/>
+      <c r="AF13" s="80"/>
+      <c r="AG13" s="80"/>
+      <c r="AH13" s="80"/>
+      <c r="AI13" s="80"/>
+      <c r="AJ13" s="80"/>
       <c r="AK13" s="24"/>
       <c r="AL13" s="24"/>
       <c r="AM13" s="24"/>
@@ -2915,7 +2792,7 @@
       <c r="BK13" s="24"/>
     </row>
     <row r="14" spans="1:63" ht="45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A14" s="68"/>
+      <c r="A14" s="81"/>
       <c r="B14" s="51"/>
       <c r="C14" s="50">
         <v>4</v>
@@ -2956,15 +2833,15 @@
       <c r="Y14" s="53"/>
       <c r="Z14" s="53"/>
       <c r="AA14" s="53"/>
-      <c r="AB14" s="67"/>
-      <c r="AC14" s="67"/>
-      <c r="AD14" s="67"/>
-      <c r="AE14" s="67"/>
-      <c r="AF14" s="67"/>
-      <c r="AG14" s="67"/>
-      <c r="AH14" s="67"/>
-      <c r="AI14" s="67"/>
-      <c r="AJ14" s="67"/>
+      <c r="AB14" s="80"/>
+      <c r="AC14" s="80"/>
+      <c r="AD14" s="80"/>
+      <c r="AE14" s="80"/>
+      <c r="AF14" s="80"/>
+      <c r="AG14" s="80"/>
+      <c r="AH14" s="80"/>
+      <c r="AI14" s="80"/>
+      <c r="AJ14" s="80"/>
       <c r="AK14" s="53"/>
       <c r="AL14" s="53"/>
       <c r="AM14" s="53"/>
@@ -2996,12 +2873,46 @@
     <row r="15" spans="1:63" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="AW5:AY5"/>
-    <mergeCell ref="AT5:AV5"/>
-    <mergeCell ref="AT3:AV3"/>
-    <mergeCell ref="AN3:AP3"/>
-    <mergeCell ref="AN4:AP4"/>
-    <mergeCell ref="AN5:AP5"/>
+    <mergeCell ref="BI3:BK3"/>
+    <mergeCell ref="BI4:BK4"/>
+    <mergeCell ref="BI5:BK5"/>
+    <mergeCell ref="BF3:BH3"/>
+    <mergeCell ref="BF4:BH4"/>
+    <mergeCell ref="BF5:BH5"/>
+    <mergeCell ref="AB5:AD5"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AQ5:AS5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="AB6:AD14"/>
+    <mergeCell ref="AE6:AG14"/>
+    <mergeCell ref="AH6:AJ14"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="Y5:AA5"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="AE4:AG4"/>
+    <mergeCell ref="AH4:AJ4"/>
+    <mergeCell ref="AQ4:AS4"/>
+    <mergeCell ref="AT4:AV4"/>
+    <mergeCell ref="AW4:AY4"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="Y3:AA3"/>
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
     <mergeCell ref="S5:U5"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="S3:U3"/>
@@ -3013,55 +2924,20 @@
     <mergeCell ref="AK3:AM3"/>
     <mergeCell ref="AK4:AM4"/>
     <mergeCell ref="AK5:AM5"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="Y3:AA3"/>
-    <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="AE3:AG3"/>
     <mergeCell ref="AH3:AJ3"/>
     <mergeCell ref="AQ3:AS3"/>
     <mergeCell ref="AW3:AY3"/>
     <mergeCell ref="AZ3:BB3"/>
     <mergeCell ref="AB4:AD4"/>
-    <mergeCell ref="AE4:AG4"/>
-    <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="AQ4:AS4"/>
-    <mergeCell ref="AT4:AV4"/>
-    <mergeCell ref="AW4:AY4"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="V4:X4"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="V5:X5"/>
-    <mergeCell ref="Y5:AA5"/>
-    <mergeCell ref="AB5:AD5"/>
-    <mergeCell ref="AE5:AG5"/>
-    <mergeCell ref="AH5:AJ5"/>
-    <mergeCell ref="AQ5:AS5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="AB6:AD14"/>
-    <mergeCell ref="AE6:AG14"/>
-    <mergeCell ref="AH6:AJ14"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="BI3:BK3"/>
-    <mergeCell ref="BI4:BK4"/>
-    <mergeCell ref="BI5:BK5"/>
-    <mergeCell ref="BF3:BH3"/>
-    <mergeCell ref="BF4:BH4"/>
-    <mergeCell ref="BF5:BH5"/>
+    <mergeCell ref="AW5:AY5"/>
+    <mergeCell ref="AT5:AV5"/>
+    <mergeCell ref="AT3:AV3"/>
+    <mergeCell ref="AN3:AP3"/>
+    <mergeCell ref="AN4:AP4"/>
+    <mergeCell ref="AN5:AP5"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Trisotech BPMN Web Modeler 4.1.1 to BPMN Web Modeler 4.1.8
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>Process Modeler for Visio (itp-commerce)</t>
-  </si>
-  <si>
-    <t>Business Process Incubator BPMN 2.0 Web Modeler</t>
   </si>
   <si>
     <t>ADONIS</t>
@@ -338,9 +335,6 @@
     <t>Signavio Process Editor 7.1.0</t>
   </si>
   <si>
-    <t>4.1.1</t>
-  </si>
-  <si>
     <t>OK</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -375,6 +369,12 @@
   </si>
   <si>
     <t>2.3.0</t>
+  </si>
+  <si>
+    <t>Trisotech BPMN 2.0 Web Modeler</t>
+  </si>
+  <si>
+    <t>4.1.8</t>
   </si>
 </sst>
 </file>
@@ -611,7 +611,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -778,6 +778,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -787,78 +850,42 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="TableStyleLight1" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -943,9 +970,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -983,7 +1010,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1055,7 +1082,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1234,11 +1261,11 @@
   </sheetPr>
   <dimension ref="A1:AMN15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AB1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AU6" sqref="AU6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="44.85546875" style="1"/>
@@ -1260,18 +1287,18 @@
       </c>
     </row>
     <row r="2" spans="1:63" ht="47.25" thickTop="1" thickBot="1">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73" t="s">
+      <c r="B2" s="76"/>
+      <c r="C2" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73" t="s">
+      <c r="D2" s="76"/>
+      <c r="E2" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="73"/>
+      <c r="F2" s="76"/>
       <c r="G2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1456,94 +1483,94 @@
       <c r="I3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="70" t="s">
+      <c r="J3" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="74" t="s">
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="74"/>
-      <c r="O3" s="74"/>
-      <c r="P3" s="64" t="s">
+      <c r="N3" s="78"/>
+      <c r="O3" s="78"/>
+      <c r="P3" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="70" t="s">
-        <v>71</v>
-      </c>
-      <c r="T3" s="71"/>
-      <c r="U3" s="72"/>
-      <c r="V3" s="64" t="s">
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="T3" s="82"/>
+      <c r="U3" s="83"/>
+      <c r="V3" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="W3" s="64"/>
-      <c r="X3" s="64"/>
-      <c r="Y3" s="64" t="s">
+      <c r="W3" s="58"/>
+      <c r="X3" s="58"/>
+      <c r="Y3" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="Z3" s="64"/>
-      <c r="AA3" s="64"/>
-      <c r="AB3" s="64" t="s">
+      <c r="Z3" s="58"/>
+      <c r="AA3" s="58"/>
+      <c r="AB3" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="AC3" s="64"/>
-      <c r="AD3" s="64"/>
-      <c r="AE3" s="64" t="s">
+      <c r="AC3" s="58"/>
+      <c r="AD3" s="58"/>
+      <c r="AE3" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="AF3" s="64"/>
-      <c r="AG3" s="64"/>
-      <c r="AH3" s="64" t="s">
+      <c r="AF3" s="58"/>
+      <c r="AG3" s="58"/>
+      <c r="AH3" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="AI3" s="64"/>
-      <c r="AJ3" s="64"/>
-      <c r="AK3" s="64" t="s">
-        <v>78</v>
-      </c>
-      <c r="AL3" s="64"/>
-      <c r="AM3" s="64"/>
-      <c r="AN3" s="64" t="s">
-        <v>85</v>
-      </c>
-      <c r="AO3" s="64"/>
-      <c r="AP3" s="64"/>
-      <c r="AQ3" s="64" t="s">
+      <c r="AI3" s="58"/>
+      <c r="AJ3" s="58"/>
+      <c r="AK3" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL3" s="58"/>
+      <c r="AM3" s="58"/>
+      <c r="AN3" s="58" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO3" s="58"/>
+      <c r="AP3" s="58"/>
+      <c r="AQ3" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="AR3" s="64"/>
-      <c r="AS3" s="64"/>
-      <c r="AT3" s="61" t="s">
+      <c r="AR3" s="58"/>
+      <c r="AS3" s="58"/>
+      <c r="AT3" s="84" t="s">
+        <v>86</v>
+      </c>
+      <c r="AU3" s="85"/>
+      <c r="AV3" s="86"/>
+      <c r="AW3" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="AU3" s="62"/>
-      <c r="AV3" s="63"/>
-      <c r="AW3" s="70" t="s">
+      <c r="AX3" s="82"/>
+      <c r="AY3" s="83"/>
+      <c r="AZ3" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="AX3" s="71"/>
-      <c r="AY3" s="72"/>
-      <c r="AZ3" s="70" t="s">
+      <c r="BA3" s="82"/>
+      <c r="BB3" s="83"/>
+      <c r="BC3" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="BA3" s="71"/>
-      <c r="BB3" s="72"/>
-      <c r="BC3" s="70" t="s">
-        <v>23</v>
-      </c>
-      <c r="BD3" s="71"/>
-      <c r="BE3" s="72"/>
+      <c r="BD3" s="82"/>
+      <c r="BE3" s="83"/>
       <c r="BF3" s="61" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="BG3" s="62"/>
       <c r="BH3" s="63"/>
-      <c r="BI3" s="64"/>
-      <c r="BJ3" s="64"/>
-      <c r="BK3" s="64"/>
+      <c r="BI3" s="58"/>
+      <c r="BJ3" s="58"/>
+      <c r="BK3" s="58"/>
     </row>
     <row r="4" spans="1:63" s="15" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A4" s="12"/>
@@ -1555,96 +1582,96 @@
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
       <c r="I4" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="67" t="s">
+      <c r="K4" s="72"/>
+      <c r="L4" s="72"/>
+      <c r="M4" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
-      <c r="M4" s="65" t="s">
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q4" s="59"/>
+      <c r="R4" s="59"/>
+      <c r="S4" s="72" t="s">
+        <v>78</v>
+      </c>
+      <c r="T4" s="74"/>
+      <c r="U4" s="75"/>
+      <c r="V4" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="65"/>
-      <c r="O4" s="65"/>
-      <c r="P4" s="65" t="s">
+      <c r="W4" s="59"/>
+      <c r="X4" s="59"/>
+      <c r="Y4" s="73" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z4" s="73"/>
+      <c r="AA4" s="73"/>
+      <c r="AB4" s="59" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC4" s="59"/>
+      <c r="AD4" s="59"/>
+      <c r="AE4" s="59">
+        <v>2.4</v>
+      </c>
+      <c r="AF4" s="59"/>
+      <c r="AG4" s="59"/>
+      <c r="AH4" s="59" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI4" s="59"/>
+      <c r="AJ4" s="59"/>
+      <c r="AK4" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL4" s="59"/>
+      <c r="AM4" s="59"/>
+      <c r="AN4" s="59" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO4" s="59"/>
+      <c r="AP4" s="59"/>
+      <c r="AQ4" s="59" t="s">
+        <v>29</v>
+      </c>
+      <c r="AR4" s="59"/>
+      <c r="AS4" s="59"/>
+      <c r="AT4" s="87" t="s">
         <v>87</v>
       </c>
-      <c r="Q4" s="65"/>
-      <c r="R4" s="65"/>
-      <c r="S4" s="67" t="s">
+      <c r="AU4" s="88"/>
+      <c r="AV4" s="89"/>
+      <c r="AW4" s="72" t="s">
+        <v>30</v>
+      </c>
+      <c r="AX4" s="74"/>
+      <c r="AY4" s="75"/>
+      <c r="AZ4" s="72" t="s">
+        <v>31</v>
+      </c>
+      <c r="BA4" s="74"/>
+      <c r="BB4" s="75"/>
+      <c r="BC4" s="72" t="s">
+        <v>32</v>
+      </c>
+      <c r="BD4" s="74"/>
+      <c r="BE4" s="75"/>
+      <c r="BF4" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="T4" s="68"/>
-      <c r="U4" s="69"/>
-      <c r="V4" s="65" t="s">
-        <v>27</v>
-      </c>
-      <c r="W4" s="65"/>
-      <c r="X4" s="65"/>
-      <c r="Y4" s="75" t="s">
-        <v>84</v>
-      </c>
-      <c r="Z4" s="75"/>
-      <c r="AA4" s="75"/>
-      <c r="AB4" s="65" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC4" s="65"/>
-      <c r="AD4" s="65"/>
-      <c r="AE4" s="65">
-        <v>2.4</v>
-      </c>
-      <c r="AF4" s="65"/>
-      <c r="AG4" s="65"/>
-      <c r="AH4" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="AI4" s="65"/>
-      <c r="AJ4" s="65"/>
-      <c r="AK4" s="65" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL4" s="65"/>
-      <c r="AM4" s="65"/>
-      <c r="AN4" s="65" t="s">
-        <v>86</v>
-      </c>
-      <c r="AO4" s="65"/>
-      <c r="AP4" s="65"/>
-      <c r="AQ4" s="65" t="s">
-        <v>30</v>
-      </c>
-      <c r="AR4" s="65"/>
-      <c r="AS4" s="65"/>
-      <c r="AT4" s="67" t="s">
-        <v>76</v>
-      </c>
-      <c r="AU4" s="68"/>
-      <c r="AV4" s="69"/>
-      <c r="AW4" s="67" t="s">
-        <v>31</v>
-      </c>
-      <c r="AX4" s="68"/>
-      <c r="AY4" s="69"/>
-      <c r="AZ4" s="67" t="s">
-        <v>32</v>
-      </c>
-      <c r="BA4" s="68"/>
-      <c r="BB4" s="69"/>
-      <c r="BC4" s="67" t="s">
-        <v>33</v>
-      </c>
-      <c r="BD4" s="68"/>
-      <c r="BE4" s="69"/>
-      <c r="BF4" s="82" t="s">
-        <v>82</v>
-      </c>
-      <c r="BG4" s="82"/>
-      <c r="BH4" s="82"/>
-      <c r="BI4" s="65"/>
-      <c r="BJ4" s="65"/>
-      <c r="BK4" s="65"/>
+      <c r="BG4" s="64"/>
+      <c r="BH4" s="64"/>
+      <c r="BI4" s="59"/>
+      <c r="BJ4" s="59"/>
+      <c r="BK4" s="59"/>
     </row>
     <row r="5" spans="1:63" ht="16.5" thickTop="1" thickBot="1">
       <c r="A5" s="16"/>
@@ -1656,692 +1683,692 @@
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
       <c r="I5" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="76">
+        <v>33</v>
+      </c>
+      <c r="J5" s="69">
         <v>41380</v>
       </c>
-      <c r="K5" s="76"/>
-      <c r="L5" s="76"/>
-      <c r="M5" s="77">
+      <c r="K5" s="69"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="70">
         <v>41373</v>
       </c>
-      <c r="N5" s="77"/>
-      <c r="O5" s="77"/>
-      <c r="P5" s="66">
+      <c r="N5" s="70"/>
+      <c r="O5" s="70"/>
+      <c r="P5" s="60">
         <v>41614</v>
       </c>
-      <c r="Q5" s="66"/>
-      <c r="R5" s="78"/>
-      <c r="S5" s="58">
+      <c r="Q5" s="60"/>
+      <c r="R5" s="71"/>
+      <c r="S5" s="79">
         <v>41591</v>
       </c>
-      <c r="T5" s="59"/>
-      <c r="U5" s="60"/>
-      <c r="V5" s="78">
+      <c r="T5" s="80"/>
+      <c r="U5" s="81"/>
+      <c r="V5" s="71">
         <v>41383</v>
       </c>
-      <c r="W5" s="78"/>
-      <c r="X5" s="78"/>
-      <c r="Y5" s="78">
+      <c r="W5" s="71"/>
+      <c r="X5" s="71"/>
+      <c r="Y5" s="71">
         <v>41599</v>
       </c>
-      <c r="Z5" s="78"/>
-      <c r="AA5" s="78"/>
-      <c r="AB5" s="66">
+      <c r="Z5" s="71"/>
+      <c r="AA5" s="71"/>
+      <c r="AB5" s="60">
         <v>41394</v>
       </c>
-      <c r="AC5" s="66"/>
-      <c r="AD5" s="66"/>
-      <c r="AE5" s="66">
+      <c r="AC5" s="60"/>
+      <c r="AD5" s="60"/>
+      <c r="AE5" s="60">
         <v>41388</v>
       </c>
-      <c r="AF5" s="66"/>
-      <c r="AG5" s="66"/>
-      <c r="AH5" s="66">
+      <c r="AF5" s="60"/>
+      <c r="AG5" s="60"/>
+      <c r="AH5" s="60">
         <v>41388</v>
       </c>
-      <c r="AI5" s="66"/>
-      <c r="AJ5" s="66"/>
-      <c r="AK5" s="66">
+      <c r="AI5" s="60"/>
+      <c r="AJ5" s="60"/>
+      <c r="AK5" s="60">
         <v>41571</v>
       </c>
-      <c r="AL5" s="66"/>
-      <c r="AM5" s="66"/>
-      <c r="AN5" s="66">
+      <c r="AL5" s="60"/>
+      <c r="AM5" s="60"/>
+      <c r="AN5" s="60">
         <v>41600</v>
       </c>
-      <c r="AO5" s="66"/>
-      <c r="AP5" s="66"/>
-      <c r="AQ5" s="66">
+      <c r="AO5" s="60"/>
+      <c r="AP5" s="60"/>
+      <c r="AQ5" s="60">
         <v>41431</v>
       </c>
-      <c r="AR5" s="66"/>
-      <c r="AS5" s="66"/>
-      <c r="AT5" s="58">
-        <v>41467</v>
-      </c>
-      <c r="AU5" s="59"/>
-      <c r="AV5" s="60"/>
-      <c r="AW5" s="58">
+      <c r="AR5" s="60"/>
+      <c r="AS5" s="60"/>
+      <c r="AT5" s="90">
+        <v>41618</v>
+      </c>
+      <c r="AU5" s="91"/>
+      <c r="AV5" s="92"/>
+      <c r="AW5" s="79">
         <v>41435</v>
       </c>
-      <c r="AX5" s="59"/>
-      <c r="AY5" s="60"/>
-      <c r="AZ5" s="58">
+      <c r="AX5" s="80"/>
+      <c r="AY5" s="81"/>
+      <c r="AZ5" s="79">
         <v>41449</v>
       </c>
-      <c r="BA5" s="59"/>
-      <c r="BB5" s="60"/>
-      <c r="BC5" s="58">
+      <c r="BA5" s="80"/>
+      <c r="BB5" s="81"/>
+      <c r="BC5" s="79">
         <v>41444</v>
       </c>
-      <c r="BD5" s="59"/>
-      <c r="BE5" s="60"/>
-      <c r="BF5" s="83">
+      <c r="BD5" s="80"/>
+      <c r="BE5" s="81"/>
+      <c r="BF5" s="65">
         <v>41585</v>
       </c>
-      <c r="BG5" s="83"/>
-      <c r="BH5" s="83"/>
-      <c r="BI5" s="66"/>
-      <c r="BJ5" s="66"/>
-      <c r="BK5" s="66"/>
+      <c r="BG5" s="65"/>
+      <c r="BH5" s="65"/>
+      <c r="BI5" s="60"/>
+      <c r="BJ5" s="60"/>
+      <c r="BK5" s="60"/>
     </row>
     <row r="6" spans="1:63" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="79" t="s">
+      <c r="A6" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="19" t="s">
         <v>35</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>36</v>
       </c>
       <c r="C6" s="20">
         <v>1</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" s="22">
         <v>0</v>
       </c>
       <c r="F6" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="H6" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="I6" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="26" t="s">
-        <v>41</v>
-      </c>
       <c r="J6" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M6" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N6" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O6" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P6" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q6" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R6" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S6" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T6" s="24"/>
       <c r="U6" s="24"/>
       <c r="V6" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="W6" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="X6" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y6" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z6" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA6" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB6" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="W6" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="X6" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y6" s="23" t="s">
+      <c r="AC6" s="67"/>
+      <c r="AD6" s="67"/>
+      <c r="AE6" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="Z6" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA6" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB6" s="80" t="s">
+      <c r="AF6" s="67"/>
+      <c r="AG6" s="67"/>
+      <c r="AH6" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="AC6" s="80"/>
-      <c r="AD6" s="80"/>
-      <c r="AE6" s="80" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF6" s="80"/>
-      <c r="AG6" s="80"/>
-      <c r="AH6" s="80" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI6" s="80"/>
-      <c r="AJ6" s="80"/>
+      <c r="AI6" s="67"/>
+      <c r="AJ6" s="67"/>
       <c r="AK6" s="27"/>
       <c r="AL6" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AM6" s="24"/>
       <c r="AN6" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AO6" s="24"/>
       <c r="AP6" s="24"/>
       <c r="AQ6" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AR6" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AS6" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AT6" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AU6" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AV6" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AW6" s="57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AX6" s="57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AY6" s="57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AZ6" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="BA6" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="BB6" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BC6" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BD6" s="24"/>
       <c r="BE6" s="24"/>
       <c r="BF6" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BG6" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BH6" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BI6" s="27"/>
       <c r="BJ6" s="24"/>
       <c r="BK6" s="24"/>
     </row>
     <row r="7" spans="1:63" ht="42.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="79"/>
+      <c r="A7" s="66"/>
       <c r="B7" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" s="20">
         <v>2</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="22">
         <v>0</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="31" t="s">
-        <v>49</v>
-      </c>
       <c r="I7" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J7" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K7" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M7" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N7" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O7" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P7" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q7" s="57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R7" s="57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S7" s="57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T7" s="24"/>
       <c r="U7" s="24"/>
       <c r="V7" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="W7" s="28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X7" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Y7" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Z7" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AA7" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB7" s="80"/>
-      <c r="AC7" s="80"/>
-      <c r="AD7" s="80"/>
-      <c r="AE7" s="80"/>
-      <c r="AF7" s="80"/>
-      <c r="AG7" s="80"/>
-      <c r="AH7" s="80"/>
-      <c r="AI7" s="80"/>
-      <c r="AJ7" s="80"/>
+        <v>42</v>
+      </c>
+      <c r="AB7" s="67"/>
+      <c r="AC7" s="67"/>
+      <c r="AD7" s="67"/>
+      <c r="AE7" s="67"/>
+      <c r="AF7" s="67"/>
+      <c r="AG7" s="67"/>
+      <c r="AH7" s="67"/>
+      <c r="AI7" s="67"/>
+      <c r="AJ7" s="67"/>
       <c r="AK7" s="27"/>
       <c r="AL7" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AM7" s="24"/>
       <c r="AN7" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AO7" s="24"/>
       <c r="AP7" s="24"/>
       <c r="AQ7" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AR7" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AS7" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AT7" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AU7" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AV7" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AW7" s="57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AX7" s="57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AY7" s="57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AZ7" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="BA7" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="BB7" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BC7" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BD7" s="24"/>
       <c r="BE7" s="24"/>
       <c r="BF7" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BG7" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BH7" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BI7" s="27"/>
       <c r="BJ7" s="24"/>
       <c r="BK7" s="24"/>
     </row>
     <row r="8" spans="1:63" ht="43.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A8" s="79"/>
+      <c r="A8" s="66"/>
       <c r="B8" s="30"/>
       <c r="C8" s="20">
         <v>3</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E8" s="22">
         <v>0</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G8" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="31" t="s">
-        <v>52</v>
-      </c>
       <c r="I8" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J8" s="32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L8" s="33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M8" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N8" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O8" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P8" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q8" s="57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R8" s="57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S8" s="57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T8" s="24"/>
       <c r="U8" s="24"/>
       <c r="V8" s="34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W8" s="34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X8" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Y8" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Z8" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AA8" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB8" s="80"/>
-      <c r="AC8" s="80"/>
-      <c r="AD8" s="80"/>
-      <c r="AE8" s="80"/>
-      <c r="AF8" s="80"/>
-      <c r="AG8" s="80"/>
-      <c r="AH8" s="80"/>
-      <c r="AI8" s="80"/>
-      <c r="AJ8" s="80"/>
+        <v>42</v>
+      </c>
+      <c r="AB8" s="67"/>
+      <c r="AC8" s="67"/>
+      <c r="AD8" s="67"/>
+      <c r="AE8" s="67"/>
+      <c r="AF8" s="67"/>
+      <c r="AG8" s="67"/>
+      <c r="AH8" s="67"/>
+      <c r="AI8" s="67"/>
+      <c r="AJ8" s="67"/>
       <c r="AK8" s="27"/>
       <c r="AL8" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AM8" s="24"/>
       <c r="AN8" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AO8" s="24"/>
       <c r="AP8" s="24"/>
       <c r="AQ8" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AR8" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AS8" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AT8" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AU8" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AV8" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AW8" s="57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AX8" s="57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AY8" s="57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AZ8" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BA8" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BB8" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BC8" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BD8" s="24"/>
       <c r="BE8" s="24"/>
       <c r="BF8" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BG8" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BH8" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BI8" s="27"/>
       <c r="BJ8" s="24"/>
       <c r="BK8" s="24"/>
     </row>
     <row r="9" spans="1:63" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A9" s="79"/>
+      <c r="A9" s="66"/>
       <c r="B9" s="30"/>
       <c r="C9" s="20">
         <v>4</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="22">
         <v>0</v>
       </c>
       <c r="F9" s="55" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G9" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="56" t="s">
-        <v>55</v>
-      </c>
       <c r="I9" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J9" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L9" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M9" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N9" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O9" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P9" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q9" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R9" s="57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S9" s="57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T9" s="20"/>
       <c r="U9" s="24"/>
       <c r="V9" s="41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="W9" s="42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X9" s="43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Y9" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Z9" s="21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AA9" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB9" s="80"/>
-      <c r="AC9" s="80"/>
-      <c r="AD9" s="80"/>
-      <c r="AE9" s="80"/>
-      <c r="AF9" s="80"/>
-      <c r="AG9" s="80"/>
-      <c r="AH9" s="80"/>
-      <c r="AI9" s="80"/>
-      <c r="AJ9" s="80"/>
+        <v>42</v>
+      </c>
+      <c r="AB9" s="67"/>
+      <c r="AC9" s="67"/>
+      <c r="AD9" s="67"/>
+      <c r="AE9" s="67"/>
+      <c r="AF9" s="67"/>
+      <c r="AG9" s="67"/>
+      <c r="AH9" s="67"/>
+      <c r="AI9" s="67"/>
+      <c r="AJ9" s="67"/>
       <c r="AK9" s="27"/>
       <c r="AL9" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AM9" s="24"/>
       <c r="AN9" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AO9" s="20"/>
       <c r="AP9" s="24"/>
       <c r="AQ9" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AR9" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AS9" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AT9" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AU9" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AV9" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AW9" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AX9" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AY9" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AZ9" s="44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="BA9" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BB9" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BC9" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BD9" s="20"/>
       <c r="BE9" s="24"/>
       <c r="BF9" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BG9" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BH9" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BI9" s="27"/>
       <c r="BJ9" s="20"/>
@@ -2354,22 +2381,22 @@
         <v>4</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10" s="35">
         <v>1</v>
       </c>
       <c r="F10" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="G10" s="37" t="s">
+      <c r="H10" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="H10" s="38" t="s">
+      <c r="I10" s="26" t="s">
         <v>74</v>
-      </c>
-      <c r="I10" s="26" t="s">
-        <v>75</v>
       </c>
       <c r="J10" s="39"/>
       <c r="K10" s="20"/>
@@ -2378,16 +2405,16 @@
       <c r="N10" s="20"/>
       <c r="O10" s="21"/>
       <c r="P10" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q10" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R10" s="57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S10" s="57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T10" s="20"/>
       <c r="U10" s="24"/>
@@ -2395,28 +2422,28 @@
       <c r="W10" s="42"/>
       <c r="X10" s="43"/>
       <c r="Y10" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Z10" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AA10" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="AB10" s="80"/>
-      <c r="AC10" s="80"/>
-      <c r="AD10" s="80"/>
-      <c r="AE10" s="80"/>
-      <c r="AF10" s="80"/>
-      <c r="AG10" s="80"/>
-      <c r="AH10" s="80"/>
-      <c r="AI10" s="80"/>
-      <c r="AJ10" s="80"/>
+        <v>81</v>
+      </c>
+      <c r="AB10" s="67"/>
+      <c r="AC10" s="67"/>
+      <c r="AD10" s="67"/>
+      <c r="AE10" s="67"/>
+      <c r="AF10" s="67"/>
+      <c r="AG10" s="67"/>
+      <c r="AH10" s="67"/>
+      <c r="AI10" s="67"/>
+      <c r="AJ10" s="67"/>
       <c r="AK10" s="27"/>
       <c r="AL10" s="20"/>
       <c r="AM10" s="24"/>
       <c r="AN10" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AO10" s="20"/>
       <c r="AP10" s="24"/>
@@ -2436,73 +2463,73 @@
       <c r="BD10" s="20"/>
       <c r="BE10" s="24"/>
       <c r="BF10" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BG10" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BH10" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BI10" s="27"/>
       <c r="BJ10" s="20"/>
       <c r="BK10" s="24"/>
     </row>
     <row r="11" spans="1:63" s="46" customFormat="1" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="68" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>56</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>57</v>
       </c>
       <c r="C11" s="24">
         <v>1</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E11" s="24">
         <v>0</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G11" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="H11" s="45" t="s">
-        <v>60</v>
-      </c>
       <c r="I11" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K11" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L11" s="24"/>
       <c r="M11" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N11" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O11" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P11" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q11" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R11" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S11" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T11" s="24"/>
       <c r="U11" s="24"/>
@@ -2510,23 +2537,23 @@
       <c r="W11" s="24"/>
       <c r="X11" s="24"/>
       <c r="Y11" s="23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Z11" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AA11" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB11" s="80"/>
-      <c r="AC11" s="80"/>
-      <c r="AD11" s="80"/>
-      <c r="AE11" s="80"/>
-      <c r="AF11" s="80"/>
-      <c r="AG11" s="80"/>
-      <c r="AH11" s="80"/>
-      <c r="AI11" s="80"/>
-      <c r="AJ11" s="80"/>
+        <v>42</v>
+      </c>
+      <c r="AB11" s="67"/>
+      <c r="AC11" s="67"/>
+      <c r="AD11" s="67"/>
+      <c r="AE11" s="67"/>
+      <c r="AF11" s="67"/>
+      <c r="AG11" s="67"/>
+      <c r="AH11" s="67"/>
+      <c r="AI11" s="67"/>
+      <c r="AJ11" s="67"/>
       <c r="AK11" s="24"/>
       <c r="AL11" s="24"/>
       <c r="AM11" s="24"/>
@@ -2534,104 +2561,104 @@
       <c r="AO11" s="24"/>
       <c r="AP11" s="24"/>
       <c r="AQ11" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AR11" s="24"/>
       <c r="AS11" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AT11" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AU11" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AV11" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AW11" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AX11" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AY11" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AZ11" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BA11" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BB11" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BC11" s="24"/>
       <c r="BD11" s="24"/>
       <c r="BE11" s="24"/>
       <c r="BF11" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BG11" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BH11" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BI11" s="24"/>
       <c r="BJ11" s="24"/>
       <c r="BK11" s="24"/>
     </row>
     <row r="12" spans="1:63" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A12" s="81"/>
+      <c r="A12" s="68"/>
       <c r="B12" s="30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" s="24">
         <v>2</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E12" s="24">
         <v>0</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="H12" s="45" t="s">
-        <v>64</v>
-      </c>
       <c r="I12" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J12" s="24"/>
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N12" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O12" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P12" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q12" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R12" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S12" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T12" s="24"/>
       <c r="U12" s="24"/>
@@ -2639,23 +2666,23 @@
       <c r="W12" s="24"/>
       <c r="X12" s="24"/>
       <c r="Y12" s="23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Z12" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AA12" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB12" s="80"/>
-      <c r="AC12" s="80"/>
-      <c r="AD12" s="80"/>
-      <c r="AE12" s="80"/>
-      <c r="AF12" s="80"/>
-      <c r="AG12" s="80"/>
-      <c r="AH12" s="80"/>
-      <c r="AI12" s="80"/>
-      <c r="AJ12" s="80"/>
+        <v>42</v>
+      </c>
+      <c r="AB12" s="67"/>
+      <c r="AC12" s="67"/>
+      <c r="AD12" s="67"/>
+      <c r="AE12" s="67"/>
+      <c r="AF12" s="67"/>
+      <c r="AG12" s="67"/>
+      <c r="AH12" s="67"/>
+      <c r="AI12" s="67"/>
+      <c r="AJ12" s="67"/>
       <c r="AK12" s="24"/>
       <c r="AL12" s="24"/>
       <c r="AM12" s="24"/>
@@ -2663,78 +2690,78 @@
       <c r="AO12" s="24"/>
       <c r="AP12" s="24"/>
       <c r="AQ12" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AR12" s="24"/>
       <c r="AS12" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AT12" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AU12" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AV12" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AW12" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AX12" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AY12" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AZ12" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BA12" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BB12" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BC12" s="24"/>
       <c r="BD12" s="24"/>
       <c r="BE12" s="24"/>
       <c r="BF12" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BG12" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BH12" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BI12" s="24"/>
       <c r="BJ12" s="24"/>
       <c r="BK12" s="24"/>
     </row>
     <row r="13" spans="1:63" ht="63" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A13" s="81"/>
+      <c r="A13" s="68"/>
       <c r="B13" s="30"/>
       <c r="C13" s="47">
         <v>3</v>
       </c>
       <c r="D13" s="48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E13" s="49">
         <v>0</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G13" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="H13" s="31" t="s">
-        <v>67</v>
-      </c>
       <c r="I13" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J13" s="24"/>
       <c r="K13" s="24"/>
@@ -2754,15 +2781,15 @@
       <c r="Y13" s="24"/>
       <c r="Z13" s="24"/>
       <c r="AA13" s="24"/>
-      <c r="AB13" s="80"/>
-      <c r="AC13" s="80"/>
-      <c r="AD13" s="80"/>
-      <c r="AE13" s="80"/>
-      <c r="AF13" s="80"/>
-      <c r="AG13" s="80"/>
-      <c r="AH13" s="80"/>
-      <c r="AI13" s="80"/>
-      <c r="AJ13" s="80"/>
+      <c r="AB13" s="67"/>
+      <c r="AC13" s="67"/>
+      <c r="AD13" s="67"/>
+      <c r="AE13" s="67"/>
+      <c r="AF13" s="67"/>
+      <c r="AG13" s="67"/>
+      <c r="AH13" s="67"/>
+      <c r="AI13" s="67"/>
+      <c r="AJ13" s="67"/>
       <c r="AK13" s="24"/>
       <c r="AL13" s="24"/>
       <c r="AM13" s="24"/>
@@ -2792,28 +2819,28 @@
       <c r="BK13" s="24"/>
     </row>
     <row r="14" spans="1:63" ht="45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A14" s="81"/>
+      <c r="A14" s="68"/>
       <c r="B14" s="51"/>
       <c r="C14" s="50">
         <v>4</v>
       </c>
       <c r="D14" s="48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E14" s="49">
         <v>0</v>
       </c>
       <c r="F14" s="48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G14" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="H14" s="52" t="s">
-        <v>70</v>
-      </c>
       <c r="I14" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J14" s="53"/>
       <c r="K14" s="53"/>
@@ -2833,15 +2860,15 @@
       <c r="Y14" s="53"/>
       <c r="Z14" s="53"/>
       <c r="AA14" s="53"/>
-      <c r="AB14" s="80"/>
-      <c r="AC14" s="80"/>
-      <c r="AD14" s="80"/>
-      <c r="AE14" s="80"/>
-      <c r="AF14" s="80"/>
-      <c r="AG14" s="80"/>
-      <c r="AH14" s="80"/>
-      <c r="AI14" s="80"/>
-      <c r="AJ14" s="80"/>
+      <c r="AB14" s="67"/>
+      <c r="AC14" s="67"/>
+      <c r="AD14" s="67"/>
+      <c r="AE14" s="67"/>
+      <c r="AF14" s="67"/>
+      <c r="AG14" s="67"/>
+      <c r="AH14" s="67"/>
+      <c r="AI14" s="67"/>
+      <c r="AJ14" s="67"/>
       <c r="AK14" s="53"/>
       <c r="AL14" s="53"/>
       <c r="AM14" s="53"/>
@@ -2873,12 +2900,47 @@
     <row r="15" spans="1:63" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="BI3:BK3"/>
-    <mergeCell ref="BI4:BK4"/>
-    <mergeCell ref="BI5:BK5"/>
-    <mergeCell ref="BF3:BH3"/>
-    <mergeCell ref="BF4:BH4"/>
-    <mergeCell ref="BF5:BH5"/>
+    <mergeCell ref="AW3:AY3"/>
+    <mergeCell ref="AZ3:BB3"/>
+    <mergeCell ref="AB4:AD4"/>
+    <mergeCell ref="AW5:AY5"/>
+    <mergeCell ref="AT5:AV5"/>
+    <mergeCell ref="AT3:AV3"/>
+    <mergeCell ref="AN3:AP3"/>
+    <mergeCell ref="AN4:AP4"/>
+    <mergeCell ref="AN5:AP5"/>
+    <mergeCell ref="AK3:AM3"/>
+    <mergeCell ref="AK4:AM4"/>
+    <mergeCell ref="AK5:AM5"/>
+    <mergeCell ref="AH3:AJ3"/>
+    <mergeCell ref="AQ3:AS3"/>
+    <mergeCell ref="BC4:BE4"/>
+    <mergeCell ref="AZ4:BB4"/>
+    <mergeCell ref="BC3:BE3"/>
+    <mergeCell ref="BC5:BE5"/>
+    <mergeCell ref="AZ5:BB5"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="Y3:AA3"/>
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="AE4:AG4"/>
+    <mergeCell ref="AH4:AJ4"/>
+    <mergeCell ref="AQ4:AS4"/>
+    <mergeCell ref="AT4:AV4"/>
+    <mergeCell ref="AW4:AY4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="S4:U4"/>
     <mergeCell ref="AB5:AD5"/>
     <mergeCell ref="AE5:AG5"/>
     <mergeCell ref="AH5:AJ5"/>
@@ -2893,48 +2955,13 @@
     <mergeCell ref="P5:R5"/>
     <mergeCell ref="V5:X5"/>
     <mergeCell ref="Y5:AA5"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="V4:X4"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="AE4:AG4"/>
-    <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="AQ4:AS4"/>
-    <mergeCell ref="AT4:AV4"/>
-    <mergeCell ref="AW4:AY4"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="Y3:AA3"/>
-    <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:O3"/>
     <mergeCell ref="S5:U5"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="BC4:BE4"/>
-    <mergeCell ref="AZ4:BB4"/>
-    <mergeCell ref="BC3:BE3"/>
-    <mergeCell ref="BC5:BE5"/>
-    <mergeCell ref="AZ5:BB5"/>
-    <mergeCell ref="AK3:AM3"/>
-    <mergeCell ref="AK4:AM4"/>
-    <mergeCell ref="AK5:AM5"/>
-    <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="AQ3:AS3"/>
-    <mergeCell ref="AW3:AY3"/>
-    <mergeCell ref="AZ3:BB3"/>
-    <mergeCell ref="AB4:AD4"/>
-    <mergeCell ref="AW5:AY5"/>
-    <mergeCell ref="AT5:AV5"/>
-    <mergeCell ref="AT3:AV3"/>
-    <mergeCell ref="AN3:AP3"/>
-    <mergeCell ref="AN4:AP4"/>
-    <mergeCell ref="AN5:AP5"/>
+    <mergeCell ref="BI3:BK3"/>
+    <mergeCell ref="BI4:BK4"/>
+    <mergeCell ref="BI5:BK5"/>
+    <mergeCell ref="BF3:BH3"/>
+    <mergeCell ref="BF4:BH4"/>
+    <mergeCell ref="BF5:BH5"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
update Test Case Structure
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -368,13 +368,13 @@
     <t>9.5.0</t>
   </si>
   <si>
-    <t>2.3.0</t>
-  </si>
-  <si>
     <t>Trisotech BPMN 2.0 Web Modeler</t>
   </si>
   <si>
     <t>4.1.8</t>
+  </si>
+  <si>
+    <t>2.4.0</t>
   </si>
 </sst>
 </file>
@@ -778,15 +778,96 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -802,90 +883,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="TableStyleLight1" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -970,9 +970,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1010,7 +1010,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1082,7 +1082,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1261,11 +1261,11 @@
   </sheetPr>
   <dimension ref="A1:AMN15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AB1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AU6" sqref="AU6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="44.85546875" style="1"/>
@@ -1483,94 +1483,94 @@
       <c r="I3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="77" t="s">
+      <c r="J3" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
-      <c r="M3" s="78" t="s">
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="78"/>
-      <c r="O3" s="78"/>
-      <c r="P3" s="58" t="s">
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
+      <c r="P3" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="58"/>
-      <c r="S3" s="77" t="s">
+      <c r="Q3" s="71"/>
+      <c r="R3" s="71"/>
+      <c r="S3" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="T3" s="82"/>
-      <c r="U3" s="83"/>
-      <c r="V3" s="58" t="s">
+      <c r="T3" s="59"/>
+      <c r="U3" s="60"/>
+      <c r="V3" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="W3" s="58"/>
-      <c r="X3" s="58"/>
-      <c r="Y3" s="58" t="s">
+      <c r="W3" s="71"/>
+      <c r="X3" s="71"/>
+      <c r="Y3" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="Z3" s="58"/>
-      <c r="AA3" s="58"/>
-      <c r="AB3" s="58" t="s">
+      <c r="Z3" s="71"/>
+      <c r="AA3" s="71"/>
+      <c r="AB3" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="AC3" s="58"/>
-      <c r="AD3" s="58"/>
-      <c r="AE3" s="58" t="s">
+      <c r="AC3" s="71"/>
+      <c r="AD3" s="71"/>
+      <c r="AE3" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="AF3" s="58"/>
-      <c r="AG3" s="58"/>
-      <c r="AH3" s="58" t="s">
+      <c r="AF3" s="71"/>
+      <c r="AG3" s="71"/>
+      <c r="AH3" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="AI3" s="58"/>
-      <c r="AJ3" s="58"/>
-      <c r="AK3" s="58" t="s">
+      <c r="AI3" s="71"/>
+      <c r="AJ3" s="71"/>
+      <c r="AK3" s="71" t="s">
         <v>76</v>
       </c>
-      <c r="AL3" s="58"/>
-      <c r="AM3" s="58"/>
-      <c r="AN3" s="58" t="s">
+      <c r="AL3" s="71"/>
+      <c r="AM3" s="71"/>
+      <c r="AN3" s="71" t="s">
         <v>83</v>
       </c>
-      <c r="AO3" s="58"/>
-      <c r="AP3" s="58"/>
-      <c r="AQ3" s="58" t="s">
+      <c r="AO3" s="71"/>
+      <c r="AP3" s="71"/>
+      <c r="AQ3" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="AR3" s="58"/>
-      <c r="AS3" s="58"/>
-      <c r="AT3" s="84" t="s">
-        <v>86</v>
-      </c>
-      <c r="AU3" s="85"/>
-      <c r="AV3" s="86"/>
-      <c r="AW3" s="77" t="s">
+      <c r="AR3" s="71"/>
+      <c r="AS3" s="71"/>
+      <c r="AT3" s="68" t="s">
+        <v>85</v>
+      </c>
+      <c r="AU3" s="69"/>
+      <c r="AV3" s="70"/>
+      <c r="AW3" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="AX3" s="82"/>
-      <c r="AY3" s="83"/>
-      <c r="AZ3" s="77" t="s">
+      <c r="AX3" s="59"/>
+      <c r="AY3" s="60"/>
+      <c r="AZ3" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="BA3" s="82"/>
-      <c r="BB3" s="83"/>
-      <c r="BC3" s="77" t="s">
+      <c r="BA3" s="59"/>
+      <c r="BB3" s="60"/>
+      <c r="BC3" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="BD3" s="82"/>
-      <c r="BE3" s="83"/>
-      <c r="BF3" s="61" t="s">
+      <c r="BD3" s="59"/>
+      <c r="BE3" s="60"/>
+      <c r="BF3" s="88" t="s">
         <v>79</v>
       </c>
-      <c r="BG3" s="62"/>
-      <c r="BH3" s="63"/>
-      <c r="BI3" s="58"/>
-      <c r="BJ3" s="58"/>
-      <c r="BK3" s="58"/>
+      <c r="BG3" s="89"/>
+      <c r="BH3" s="90"/>
+      <c r="BI3" s="71"/>
+      <c r="BJ3" s="71"/>
+      <c r="BK3" s="71"/>
     </row>
     <row r="4" spans="1:63" s="15" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A4" s="12"/>
@@ -1584,94 +1584,94 @@
       <c r="I4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="72" t="s">
+      <c r="J4" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="72"/>
-      <c r="L4" s="72"/>
-      <c r="M4" s="59" t="s">
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="N4" s="59"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="59" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q4" s="59"/>
-      <c r="R4" s="59"/>
-      <c r="S4" s="72" t="s">
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
+      <c r="P4" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q4" s="61"/>
+      <c r="R4" s="61"/>
+      <c r="S4" s="73" t="s">
         <v>78</v>
       </c>
       <c r="T4" s="74"/>
       <c r="U4" s="75"/>
-      <c r="V4" s="59" t="s">
+      <c r="V4" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="W4" s="59"/>
-      <c r="X4" s="59"/>
-      <c r="Y4" s="73" t="s">
+      <c r="W4" s="61"/>
+      <c r="X4" s="61"/>
+      <c r="Y4" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="Z4" s="73"/>
-      <c r="AA4" s="73"/>
-      <c r="AB4" s="59" t="s">
+      <c r="Z4" s="81"/>
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="AC4" s="59"/>
-      <c r="AD4" s="59"/>
-      <c r="AE4" s="59">
+      <c r="AC4" s="61"/>
+      <c r="AD4" s="61"/>
+      <c r="AE4" s="61">
         <v>2.4</v>
       </c>
-      <c r="AF4" s="59"/>
-      <c r="AG4" s="59"/>
-      <c r="AH4" s="59" t="s">
+      <c r="AF4" s="61"/>
+      <c r="AG4" s="61"/>
+      <c r="AH4" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="AI4" s="59"/>
-      <c r="AJ4" s="59"/>
-      <c r="AK4" s="59" t="s">
+      <c r="AI4" s="61"/>
+      <c r="AJ4" s="61"/>
+      <c r="AK4" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="AL4" s="59"/>
-      <c r="AM4" s="59"/>
-      <c r="AN4" s="59" t="s">
+      <c r="AL4" s="61"/>
+      <c r="AM4" s="61"/>
+      <c r="AN4" s="61" t="s">
         <v>84</v>
       </c>
-      <c r="AO4" s="59"/>
-      <c r="AP4" s="59"/>
-      <c r="AQ4" s="59" t="s">
+      <c r="AO4" s="61"/>
+      <c r="AP4" s="61"/>
+      <c r="AQ4" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="AR4" s="59"/>
-      <c r="AS4" s="59"/>
-      <c r="AT4" s="87" t="s">
-        <v>87</v>
-      </c>
-      <c r="AU4" s="88"/>
-      <c r="AV4" s="89"/>
-      <c r="AW4" s="72" t="s">
+      <c r="AR4" s="61"/>
+      <c r="AS4" s="61"/>
+      <c r="AT4" s="78" t="s">
+        <v>86</v>
+      </c>
+      <c r="AU4" s="79"/>
+      <c r="AV4" s="80"/>
+      <c r="AW4" s="73" t="s">
         <v>30</v>
       </c>
       <c r="AX4" s="74"/>
       <c r="AY4" s="75"/>
-      <c r="AZ4" s="72" t="s">
+      <c r="AZ4" s="73" t="s">
         <v>31</v>
       </c>
       <c r="BA4" s="74"/>
       <c r="BB4" s="75"/>
-      <c r="BC4" s="72" t="s">
+      <c r="BC4" s="73" t="s">
         <v>32</v>
       </c>
       <c r="BD4" s="74"/>
       <c r="BE4" s="75"/>
-      <c r="BF4" s="64" t="s">
+      <c r="BF4" s="91" t="s">
         <v>80</v>
       </c>
-      <c r="BG4" s="64"/>
-      <c r="BH4" s="64"/>
-      <c r="BI4" s="59"/>
-      <c r="BJ4" s="59"/>
-      <c r="BK4" s="59"/>
+      <c r="BG4" s="91"/>
+      <c r="BH4" s="91"/>
+      <c r="BI4" s="61"/>
+      <c r="BJ4" s="61"/>
+      <c r="BK4" s="61"/>
     </row>
     <row r="5" spans="1:63" ht="16.5" thickTop="1" thickBot="1">
       <c r="A5" s="16"/>
@@ -1685,97 +1685,97 @@
       <c r="I5" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="69">
+      <c r="J5" s="85">
         <v>41380</v>
       </c>
-      <c r="K5" s="69"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="70">
+      <c r="K5" s="85"/>
+      <c r="L5" s="85"/>
+      <c r="M5" s="86">
         <v>41373</v>
       </c>
-      <c r="N5" s="70"/>
-      <c r="O5" s="70"/>
-      <c r="P5" s="60">
-        <v>41614</v>
-      </c>
-      <c r="Q5" s="60"/>
-      <c r="R5" s="71"/>
-      <c r="S5" s="79">
+      <c r="N5" s="86"/>
+      <c r="O5" s="86"/>
+      <c r="P5" s="72">
+        <v>41680</v>
+      </c>
+      <c r="Q5" s="72"/>
+      <c r="R5" s="87"/>
+      <c r="S5" s="62">
         <v>41591</v>
       </c>
-      <c r="T5" s="80"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="71">
+      <c r="T5" s="63"/>
+      <c r="U5" s="64"/>
+      <c r="V5" s="87">
         <v>41383</v>
       </c>
-      <c r="W5" s="71"/>
-      <c r="X5" s="71"/>
-      <c r="Y5" s="71">
+      <c r="W5" s="87"/>
+      <c r="X5" s="87"/>
+      <c r="Y5" s="87">
         <v>41599</v>
       </c>
-      <c r="Z5" s="71"/>
-      <c r="AA5" s="71"/>
-      <c r="AB5" s="60">
+      <c r="Z5" s="87"/>
+      <c r="AA5" s="87"/>
+      <c r="AB5" s="72">
         <v>41394</v>
       </c>
-      <c r="AC5" s="60"/>
-      <c r="AD5" s="60"/>
-      <c r="AE5" s="60">
+      <c r="AC5" s="72"/>
+      <c r="AD5" s="72"/>
+      <c r="AE5" s="72">
         <v>41388</v>
       </c>
-      <c r="AF5" s="60"/>
-      <c r="AG5" s="60"/>
-      <c r="AH5" s="60">
+      <c r="AF5" s="72"/>
+      <c r="AG5" s="72"/>
+      <c r="AH5" s="72">
         <v>41388</v>
       </c>
-      <c r="AI5" s="60"/>
-      <c r="AJ5" s="60"/>
-      <c r="AK5" s="60">
+      <c r="AI5" s="72"/>
+      <c r="AJ5" s="72"/>
+      <c r="AK5" s="72">
         <v>41571</v>
       </c>
-      <c r="AL5" s="60"/>
-      <c r="AM5" s="60"/>
-      <c r="AN5" s="60">
+      <c r="AL5" s="72"/>
+      <c r="AM5" s="72"/>
+      <c r="AN5" s="72">
         <v>41600</v>
       </c>
-      <c r="AO5" s="60"/>
-      <c r="AP5" s="60"/>
-      <c r="AQ5" s="60">
+      <c r="AO5" s="72"/>
+      <c r="AP5" s="72"/>
+      <c r="AQ5" s="72">
         <v>41431</v>
       </c>
-      <c r="AR5" s="60"/>
-      <c r="AS5" s="60"/>
-      <c r="AT5" s="90">
+      <c r="AR5" s="72"/>
+      <c r="AS5" s="72"/>
+      <c r="AT5" s="65">
         <v>41618</v>
       </c>
-      <c r="AU5" s="91"/>
-      <c r="AV5" s="92"/>
-      <c r="AW5" s="79">
+      <c r="AU5" s="66"/>
+      <c r="AV5" s="67"/>
+      <c r="AW5" s="62">
         <v>41435</v>
       </c>
-      <c r="AX5" s="80"/>
-      <c r="AY5" s="81"/>
-      <c r="AZ5" s="79">
+      <c r="AX5" s="63"/>
+      <c r="AY5" s="64"/>
+      <c r="AZ5" s="62">
         <v>41449</v>
       </c>
-      <c r="BA5" s="80"/>
-      <c r="BB5" s="81"/>
-      <c r="BC5" s="79">
+      <c r="BA5" s="63"/>
+      <c r="BB5" s="64"/>
+      <c r="BC5" s="62">
         <v>41444</v>
       </c>
-      <c r="BD5" s="80"/>
-      <c r="BE5" s="81"/>
-      <c r="BF5" s="65">
+      <c r="BD5" s="63"/>
+      <c r="BE5" s="64"/>
+      <c r="BF5" s="92">
         <v>41585</v>
       </c>
-      <c r="BG5" s="65"/>
-      <c r="BH5" s="65"/>
-      <c r="BI5" s="60"/>
-      <c r="BJ5" s="60"/>
-      <c r="BK5" s="60"/>
+      <c r="BG5" s="92"/>
+      <c r="BH5" s="92"/>
+      <c r="BI5" s="72"/>
+      <c r="BJ5" s="72"/>
+      <c r="BK5" s="72"/>
     </row>
     <row r="6" spans="1:63" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="82" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="19" t="s">
@@ -1852,21 +1852,21 @@
       <c r="AA6" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="AB6" s="67" t="s">
+      <c r="AB6" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="AC6" s="67"/>
-      <c r="AD6" s="67"/>
-      <c r="AE6" s="67" t="s">
+      <c r="AC6" s="83"/>
+      <c r="AD6" s="83"/>
+      <c r="AE6" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="AF6" s="67"/>
-      <c r="AG6" s="67"/>
-      <c r="AH6" s="67" t="s">
+      <c r="AF6" s="83"/>
+      <c r="AG6" s="83"/>
+      <c r="AH6" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="AI6" s="67"/>
-      <c r="AJ6" s="67"/>
+      <c r="AI6" s="83"/>
+      <c r="AJ6" s="83"/>
       <c r="AK6" s="27"/>
       <c r="AL6" s="24" t="s">
         <v>42</v>
@@ -1932,7 +1932,7 @@
       <c r="BK6" s="24"/>
     </row>
     <row r="7" spans="1:63" ht="42.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="66"/>
+      <c r="A7" s="82"/>
       <c r="B7" s="30" t="s">
         <v>45</v>
       </c>
@@ -2007,15 +2007,15 @@
       <c r="AA7" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="AB7" s="67"/>
-      <c r="AC7" s="67"/>
-      <c r="AD7" s="67"/>
-      <c r="AE7" s="67"/>
-      <c r="AF7" s="67"/>
-      <c r="AG7" s="67"/>
-      <c r="AH7" s="67"/>
-      <c r="AI7" s="67"/>
-      <c r="AJ7" s="67"/>
+      <c r="AB7" s="83"/>
+      <c r="AC7" s="83"/>
+      <c r="AD7" s="83"/>
+      <c r="AE7" s="83"/>
+      <c r="AF7" s="83"/>
+      <c r="AG7" s="83"/>
+      <c r="AH7" s="83"/>
+      <c r="AI7" s="83"/>
+      <c r="AJ7" s="83"/>
       <c r="AK7" s="27"/>
       <c r="AL7" s="24" t="s">
         <v>42</v>
@@ -2081,7 +2081,7 @@
       <c r="BK7" s="24"/>
     </row>
     <row r="8" spans="1:63" ht="43.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A8" s="66"/>
+      <c r="A8" s="82"/>
       <c r="B8" s="30"/>
       <c r="C8" s="20">
         <v>3</v>
@@ -2154,15 +2154,15 @@
       <c r="AA8" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="AB8" s="67"/>
-      <c r="AC8" s="67"/>
-      <c r="AD8" s="67"/>
-      <c r="AE8" s="67"/>
-      <c r="AF8" s="67"/>
-      <c r="AG8" s="67"/>
-      <c r="AH8" s="67"/>
-      <c r="AI8" s="67"/>
-      <c r="AJ8" s="67"/>
+      <c r="AB8" s="83"/>
+      <c r="AC8" s="83"/>
+      <c r="AD8" s="83"/>
+      <c r="AE8" s="83"/>
+      <c r="AF8" s="83"/>
+      <c r="AG8" s="83"/>
+      <c r="AH8" s="83"/>
+      <c r="AI8" s="83"/>
+      <c r="AJ8" s="83"/>
       <c r="AK8" s="27"/>
       <c r="AL8" s="24" t="s">
         <v>41</v>
@@ -2228,7 +2228,7 @@
       <c r="BK8" s="24"/>
     </row>
     <row r="9" spans="1:63" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A9" s="66"/>
+      <c r="A9" s="82"/>
       <c r="B9" s="30"/>
       <c r="C9" s="20">
         <v>4</v>
@@ -2301,15 +2301,15 @@
       <c r="AA9" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="AB9" s="67"/>
-      <c r="AC9" s="67"/>
-      <c r="AD9" s="67"/>
-      <c r="AE9" s="67"/>
-      <c r="AF9" s="67"/>
-      <c r="AG9" s="67"/>
-      <c r="AH9" s="67"/>
-      <c r="AI9" s="67"/>
-      <c r="AJ9" s="67"/>
+      <c r="AB9" s="83"/>
+      <c r="AC9" s="83"/>
+      <c r="AD9" s="83"/>
+      <c r="AE9" s="83"/>
+      <c r="AF9" s="83"/>
+      <c r="AG9" s="83"/>
+      <c r="AH9" s="83"/>
+      <c r="AI9" s="83"/>
+      <c r="AJ9" s="83"/>
       <c r="AK9" s="27"/>
       <c r="AL9" s="20" t="s">
         <v>41</v>
@@ -2430,15 +2430,15 @@
       <c r="AA10" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="AB10" s="67"/>
-      <c r="AC10" s="67"/>
-      <c r="AD10" s="67"/>
-      <c r="AE10" s="67"/>
-      <c r="AF10" s="67"/>
-      <c r="AG10" s="67"/>
-      <c r="AH10" s="67"/>
-      <c r="AI10" s="67"/>
-      <c r="AJ10" s="67"/>
+      <c r="AB10" s="83"/>
+      <c r="AC10" s="83"/>
+      <c r="AD10" s="83"/>
+      <c r="AE10" s="83"/>
+      <c r="AF10" s="83"/>
+      <c r="AG10" s="83"/>
+      <c r="AH10" s="83"/>
+      <c r="AI10" s="83"/>
+      <c r="AJ10" s="83"/>
       <c r="AK10" s="27"/>
       <c r="AL10" s="20"/>
       <c r="AM10" s="24"/>
@@ -2476,7 +2476,7 @@
       <c r="BK10" s="24"/>
     </row>
     <row r="11" spans="1:63" s="46" customFormat="1" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A11" s="68" t="s">
+      <c r="A11" s="84" t="s">
         <v>55</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -2545,15 +2545,15 @@
       <c r="AA11" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="AB11" s="67"/>
-      <c r="AC11" s="67"/>
-      <c r="AD11" s="67"/>
-      <c r="AE11" s="67"/>
-      <c r="AF11" s="67"/>
-      <c r="AG11" s="67"/>
-      <c r="AH11" s="67"/>
-      <c r="AI11" s="67"/>
-      <c r="AJ11" s="67"/>
+      <c r="AB11" s="83"/>
+      <c r="AC11" s="83"/>
+      <c r="AD11" s="83"/>
+      <c r="AE11" s="83"/>
+      <c r="AF11" s="83"/>
+      <c r="AG11" s="83"/>
+      <c r="AH11" s="83"/>
+      <c r="AI11" s="83"/>
+      <c r="AJ11" s="83"/>
       <c r="AK11" s="24"/>
       <c r="AL11" s="24"/>
       <c r="AM11" s="24"/>
@@ -2611,7 +2611,7 @@
       <c r="BK11" s="24"/>
     </row>
     <row r="12" spans="1:63" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A12" s="68"/>
+      <c r="A12" s="84"/>
       <c r="B12" s="30" t="s">
         <v>60</v>
       </c>
@@ -2674,15 +2674,15 @@
       <c r="AA12" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="AB12" s="67"/>
-      <c r="AC12" s="67"/>
-      <c r="AD12" s="67"/>
-      <c r="AE12" s="67"/>
-      <c r="AF12" s="67"/>
-      <c r="AG12" s="67"/>
-      <c r="AH12" s="67"/>
-      <c r="AI12" s="67"/>
-      <c r="AJ12" s="67"/>
+      <c r="AB12" s="83"/>
+      <c r="AC12" s="83"/>
+      <c r="AD12" s="83"/>
+      <c r="AE12" s="83"/>
+      <c r="AF12" s="83"/>
+      <c r="AG12" s="83"/>
+      <c r="AH12" s="83"/>
+      <c r="AI12" s="83"/>
+      <c r="AJ12" s="83"/>
       <c r="AK12" s="24"/>
       <c r="AL12" s="24"/>
       <c r="AM12" s="24"/>
@@ -2740,7 +2740,7 @@
       <c r="BK12" s="24"/>
     </row>
     <row r="13" spans="1:63" ht="63" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A13" s="68"/>
+      <c r="A13" s="84"/>
       <c r="B13" s="30"/>
       <c r="C13" s="47">
         <v>3</v>
@@ -2781,15 +2781,15 @@
       <c r="Y13" s="24"/>
       <c r="Z13" s="24"/>
       <c r="AA13" s="24"/>
-      <c r="AB13" s="67"/>
-      <c r="AC13" s="67"/>
-      <c r="AD13" s="67"/>
-      <c r="AE13" s="67"/>
-      <c r="AF13" s="67"/>
-      <c r="AG13" s="67"/>
-      <c r="AH13" s="67"/>
-      <c r="AI13" s="67"/>
-      <c r="AJ13" s="67"/>
+      <c r="AB13" s="83"/>
+      <c r="AC13" s="83"/>
+      <c r="AD13" s="83"/>
+      <c r="AE13" s="83"/>
+      <c r="AF13" s="83"/>
+      <c r="AG13" s="83"/>
+      <c r="AH13" s="83"/>
+      <c r="AI13" s="83"/>
+      <c r="AJ13" s="83"/>
       <c r="AK13" s="24"/>
       <c r="AL13" s="24"/>
       <c r="AM13" s="24"/>
@@ -2819,7 +2819,7 @@
       <c r="BK13" s="24"/>
     </row>
     <row r="14" spans="1:63" ht="45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A14" s="68"/>
+      <c r="A14" s="84"/>
       <c r="B14" s="51"/>
       <c r="C14" s="50">
         <v>4</v>
@@ -2860,15 +2860,15 @@
       <c r="Y14" s="53"/>
       <c r="Z14" s="53"/>
       <c r="AA14" s="53"/>
-      <c r="AB14" s="67"/>
-      <c r="AC14" s="67"/>
-      <c r="AD14" s="67"/>
-      <c r="AE14" s="67"/>
-      <c r="AF14" s="67"/>
-      <c r="AG14" s="67"/>
-      <c r="AH14" s="67"/>
-      <c r="AI14" s="67"/>
-      <c r="AJ14" s="67"/>
+      <c r="AB14" s="83"/>
+      <c r="AC14" s="83"/>
+      <c r="AD14" s="83"/>
+      <c r="AE14" s="83"/>
+      <c r="AF14" s="83"/>
+      <c r="AG14" s="83"/>
+      <c r="AH14" s="83"/>
+      <c r="AI14" s="83"/>
+      <c r="AJ14" s="83"/>
       <c r="AK14" s="53"/>
       <c r="AL14" s="53"/>
       <c r="AM14" s="53"/>
@@ -2900,47 +2900,12 @@
     <row r="15" spans="1:63" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="AW3:AY3"/>
-    <mergeCell ref="AZ3:BB3"/>
-    <mergeCell ref="AB4:AD4"/>
-    <mergeCell ref="AW5:AY5"/>
-    <mergeCell ref="AT5:AV5"/>
-    <mergeCell ref="AT3:AV3"/>
-    <mergeCell ref="AN3:AP3"/>
-    <mergeCell ref="AN4:AP4"/>
-    <mergeCell ref="AN5:AP5"/>
-    <mergeCell ref="AK3:AM3"/>
-    <mergeCell ref="AK4:AM4"/>
-    <mergeCell ref="AK5:AM5"/>
-    <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="AQ3:AS3"/>
-    <mergeCell ref="BC4:BE4"/>
-    <mergeCell ref="AZ4:BB4"/>
-    <mergeCell ref="BC3:BE3"/>
-    <mergeCell ref="BC5:BE5"/>
-    <mergeCell ref="AZ5:BB5"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="Y3:AA3"/>
-    <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="AE4:AG4"/>
-    <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="AQ4:AS4"/>
-    <mergeCell ref="AT4:AV4"/>
-    <mergeCell ref="AW4:AY4"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="V4:X4"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="BI3:BK3"/>
+    <mergeCell ref="BI4:BK4"/>
+    <mergeCell ref="BI5:BK5"/>
+    <mergeCell ref="BF3:BH3"/>
+    <mergeCell ref="BF4:BH4"/>
+    <mergeCell ref="BF5:BH5"/>
     <mergeCell ref="AB5:AD5"/>
     <mergeCell ref="AE5:AG5"/>
     <mergeCell ref="AH5:AJ5"/>
@@ -2956,12 +2921,47 @@
     <mergeCell ref="V5:X5"/>
     <mergeCell ref="Y5:AA5"/>
     <mergeCell ref="S5:U5"/>
-    <mergeCell ref="BI3:BK3"/>
-    <mergeCell ref="BI4:BK4"/>
-    <mergeCell ref="BI5:BK5"/>
-    <mergeCell ref="BF3:BH3"/>
-    <mergeCell ref="BF4:BH4"/>
-    <mergeCell ref="BF5:BH5"/>
+    <mergeCell ref="AQ4:AS4"/>
+    <mergeCell ref="AT4:AV4"/>
+    <mergeCell ref="AW4:AY4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="Y3:AA3"/>
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="BC4:BE4"/>
+    <mergeCell ref="AZ4:BB4"/>
+    <mergeCell ref="BC3:BE3"/>
+    <mergeCell ref="BC5:BE5"/>
+    <mergeCell ref="AZ5:BB5"/>
+    <mergeCell ref="AW3:AY3"/>
+    <mergeCell ref="AZ3:BB3"/>
+    <mergeCell ref="AB4:AD4"/>
+    <mergeCell ref="AW5:AY5"/>
+    <mergeCell ref="AT5:AV5"/>
+    <mergeCell ref="AT3:AV3"/>
+    <mergeCell ref="AN3:AP3"/>
+    <mergeCell ref="AN4:AP4"/>
+    <mergeCell ref="AN5:AP5"/>
+    <mergeCell ref="AK3:AM3"/>
+    <mergeCell ref="AK4:AM4"/>
+    <mergeCell ref="AK5:AM5"/>
+    <mergeCell ref="AH3:AJ3"/>
+    <mergeCell ref="AQ3:AS3"/>
+    <mergeCell ref="AE4:AG4"/>
+    <mergeCell ref="AH4:AJ4"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Updated test cases excel for Signavio 7.8.1
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="13830" yWindow="-15" windowWidth="13890" windowHeight="12870" tabRatio="631"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Test Case Structure" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="88">
   <si>
     <t>Note: Tools that are not listed here have either not been tested or may not support both BPMN import and export.</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>11.5.1.30223</t>
-  </si>
-  <si>
-    <t>6.7.5</t>
   </si>
   <si>
     <t>8.0.1</t>
@@ -376,11 +373,14 @@
   <si>
     <t>2.4.0</t>
   </si>
+  <si>
+    <t>7.8.1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -611,7 +611,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -778,6 +778,78 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -787,16 +859,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -817,71 +883,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -970,7 +979,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -1044,7 +1053,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1079,7 +1087,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -1255,14 +1262,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AMN15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1287,18 +1294,18 @@
       </c>
     </row>
     <row r="2" spans="1:63" ht="47.25" thickTop="1" thickBot="1">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76" t="s">
+      <c r="B2" s="85"/>
+      <c r="C2" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76" t="s">
+      <c r="D2" s="85"/>
+      <c r="E2" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="76"/>
+      <c r="F2" s="85"/>
       <c r="G2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1483,94 +1490,94 @@
       <c r="I3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="58" t="s">
+      <c r="J3" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="58"/>
-      <c r="L3" s="58"/>
-      <c r="M3" s="77" t="s">
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="77"/>
-      <c r="O3" s="77"/>
-      <c r="P3" s="71" t="s">
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="71"/>
-      <c r="R3" s="71"/>
-      <c r="S3" s="58" t="s">
-        <v>70</v>
-      </c>
-      <c r="T3" s="59"/>
-      <c r="U3" s="60"/>
-      <c r="V3" s="71" t="s">
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="82" t="s">
+        <v>69</v>
+      </c>
+      <c r="T3" s="83"/>
+      <c r="U3" s="84"/>
+      <c r="V3" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="W3" s="71"/>
-      <c r="X3" s="71"/>
-      <c r="Y3" s="71" t="s">
+      <c r="W3" s="58"/>
+      <c r="X3" s="58"/>
+      <c r="Y3" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="Z3" s="71"/>
-      <c r="AA3" s="71"/>
-      <c r="AB3" s="71" t="s">
+      <c r="Z3" s="58"/>
+      <c r="AA3" s="58"/>
+      <c r="AB3" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="AC3" s="71"/>
-      <c r="AD3" s="71"/>
-      <c r="AE3" s="71" t="s">
+      <c r="AC3" s="58"/>
+      <c r="AD3" s="58"/>
+      <c r="AE3" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="AF3" s="71"/>
-      <c r="AG3" s="71"/>
-      <c r="AH3" s="71" t="s">
+      <c r="AF3" s="58"/>
+      <c r="AG3" s="58"/>
+      <c r="AH3" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="AI3" s="71"/>
-      <c r="AJ3" s="71"/>
-      <c r="AK3" s="71" t="s">
-        <v>76</v>
-      </c>
-      <c r="AL3" s="71"/>
-      <c r="AM3" s="71"/>
-      <c r="AN3" s="71" t="s">
-        <v>83</v>
-      </c>
-      <c r="AO3" s="71"/>
-      <c r="AP3" s="71"/>
-      <c r="AQ3" s="71" t="s">
+      <c r="AI3" s="58"/>
+      <c r="AJ3" s="58"/>
+      <c r="AK3" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL3" s="58"/>
+      <c r="AM3" s="58"/>
+      <c r="AN3" s="58" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO3" s="58"/>
+      <c r="AP3" s="58"/>
+      <c r="AQ3" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="AR3" s="71"/>
-      <c r="AS3" s="71"/>
-      <c r="AT3" s="68" t="s">
-        <v>85</v>
-      </c>
-      <c r="AU3" s="69"/>
-      <c r="AV3" s="70"/>
-      <c r="AW3" s="58" t="s">
+      <c r="AR3" s="58"/>
+      <c r="AS3" s="58"/>
+      <c r="AT3" s="90" t="s">
+        <v>84</v>
+      </c>
+      <c r="AU3" s="91"/>
+      <c r="AV3" s="92"/>
+      <c r="AW3" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="AX3" s="59"/>
-      <c r="AY3" s="60"/>
-      <c r="AZ3" s="58" t="s">
+      <c r="AX3" s="83"/>
+      <c r="AY3" s="84"/>
+      <c r="AZ3" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="BA3" s="59"/>
-      <c r="BB3" s="60"/>
-      <c r="BC3" s="58" t="s">
+      <c r="BA3" s="83"/>
+      <c r="BB3" s="84"/>
+      <c r="BC3" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="BD3" s="59"/>
-      <c r="BE3" s="60"/>
-      <c r="BF3" s="88" t="s">
-        <v>79</v>
-      </c>
-      <c r="BG3" s="89"/>
-      <c r="BH3" s="90"/>
-      <c r="BI3" s="71"/>
-      <c r="BJ3" s="71"/>
-      <c r="BK3" s="71"/>
+      <c r="BD3" s="83"/>
+      <c r="BE3" s="84"/>
+      <c r="BF3" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="BG3" s="62"/>
+      <c r="BH3" s="63"/>
+      <c r="BI3" s="58"/>
+      <c r="BJ3" s="58"/>
+      <c r="BK3" s="58"/>
     </row>
     <row r="4" spans="1:63" s="15" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A4" s="12"/>
@@ -1584,94 +1591,94 @@
       <c r="I4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="73" t="s">
+      <c r="J4" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="61" t="s">
+      <c r="K4" s="78"/>
+      <c r="L4" s="78"/>
+      <c r="M4" s="93" t="s">
+        <v>87</v>
+      </c>
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q4" s="59"/>
+      <c r="R4" s="59"/>
+      <c r="S4" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="T4" s="79"/>
+      <c r="U4" s="80"/>
+      <c r="V4" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="N4" s="61"/>
-      <c r="O4" s="61"/>
-      <c r="P4" s="61" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q4" s="61"/>
-      <c r="R4" s="61"/>
-      <c r="S4" s="73" t="s">
-        <v>78</v>
-      </c>
-      <c r="T4" s="74"/>
-      <c r="U4" s="75"/>
-      <c r="V4" s="61" t="s">
-        <v>26</v>
-      </c>
-      <c r="W4" s="61"/>
-      <c r="X4" s="61"/>
+      <c r="W4" s="59"/>
+      <c r="X4" s="59"/>
       <c r="Y4" s="81" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z4" s="81"/>
       <c r="AA4" s="81"/>
-      <c r="AB4" s="61" t="s">
+      <c r="AB4" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC4" s="59"/>
+      <c r="AD4" s="59"/>
+      <c r="AE4" s="59">
+        <v>2.4</v>
+      </c>
+      <c r="AF4" s="59"/>
+      <c r="AG4" s="59"/>
+      <c r="AH4" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="AC4" s="61"/>
-      <c r="AD4" s="61"/>
-      <c r="AE4" s="61">
-        <v>2.4</v>
-      </c>
-      <c r="AF4" s="61"/>
-      <c r="AG4" s="61"/>
-      <c r="AH4" s="61" t="s">
+      <c r="AI4" s="59"/>
+      <c r="AJ4" s="59"/>
+      <c r="AK4" s="59" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL4" s="59"/>
+      <c r="AM4" s="59"/>
+      <c r="AN4" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO4" s="59"/>
+      <c r="AP4" s="59"/>
+      <c r="AQ4" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="AI4" s="61"/>
-      <c r="AJ4" s="61"/>
-      <c r="AK4" s="61" t="s">
-        <v>77</v>
-      </c>
-      <c r="AL4" s="61"/>
-      <c r="AM4" s="61"/>
-      <c r="AN4" s="61" t="s">
-        <v>84</v>
-      </c>
-      <c r="AO4" s="61"/>
-      <c r="AP4" s="61"/>
-      <c r="AQ4" s="61" t="s">
+      <c r="AR4" s="59"/>
+      <c r="AS4" s="59"/>
+      <c r="AT4" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="AU4" s="76"/>
+      <c r="AV4" s="77"/>
+      <c r="AW4" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="AR4" s="61"/>
-      <c r="AS4" s="61"/>
-      <c r="AT4" s="78" t="s">
-        <v>86</v>
-      </c>
-      <c r="AU4" s="79"/>
-      <c r="AV4" s="80"/>
-      <c r="AW4" s="73" t="s">
+      <c r="AX4" s="79"/>
+      <c r="AY4" s="80"/>
+      <c r="AZ4" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="AX4" s="74"/>
-      <c r="AY4" s="75"/>
-      <c r="AZ4" s="73" t="s">
+      <c r="BA4" s="79"/>
+      <c r="BB4" s="80"/>
+      <c r="BC4" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="BA4" s="74"/>
-      <c r="BB4" s="75"/>
-      <c r="BC4" s="73" t="s">
-        <v>32</v>
-      </c>
-      <c r="BD4" s="74"/>
-      <c r="BE4" s="75"/>
-      <c r="BF4" s="91" t="s">
-        <v>80</v>
-      </c>
-      <c r="BG4" s="91"/>
-      <c r="BH4" s="91"/>
-      <c r="BI4" s="61"/>
-      <c r="BJ4" s="61"/>
-      <c r="BK4" s="61"/>
+      <c r="BD4" s="79"/>
+      <c r="BE4" s="80"/>
+      <c r="BF4" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="BG4" s="64"/>
+      <c r="BH4" s="64"/>
+      <c r="BI4" s="59"/>
+      <c r="BJ4" s="59"/>
+      <c r="BK4" s="59"/>
     </row>
     <row r="5" spans="1:63" ht="16.5" thickTop="1" thickBot="1">
       <c r="A5" s="16"/>
@@ -1683,692 +1690,692 @@
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
       <c r="I5" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="85">
+        <v>32</v>
+      </c>
+      <c r="J5" s="69">
         <v>41380</v>
       </c>
-      <c r="K5" s="85"/>
-      <c r="L5" s="85"/>
-      <c r="M5" s="86">
-        <v>41373</v>
-      </c>
-      <c r="N5" s="86"/>
-      <c r="O5" s="86"/>
-      <c r="P5" s="72">
+      <c r="K5" s="69"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="70">
+        <v>41715</v>
+      </c>
+      <c r="N5" s="70"/>
+      <c r="O5" s="70"/>
+      <c r="P5" s="60">
         <v>41680</v>
       </c>
-      <c r="Q5" s="72"/>
-      <c r="R5" s="87"/>
-      <c r="S5" s="62">
+      <c r="Q5" s="60"/>
+      <c r="R5" s="71"/>
+      <c r="S5" s="72">
         <v>41591</v>
       </c>
-      <c r="T5" s="63"/>
-      <c r="U5" s="64"/>
-      <c r="V5" s="87">
+      <c r="T5" s="73"/>
+      <c r="U5" s="74"/>
+      <c r="V5" s="71">
         <v>41383</v>
       </c>
-      <c r="W5" s="87"/>
-      <c r="X5" s="87"/>
-      <c r="Y5" s="87">
+      <c r="W5" s="71"/>
+      <c r="X5" s="71"/>
+      <c r="Y5" s="71">
         <v>41599</v>
       </c>
-      <c r="Z5" s="87"/>
-      <c r="AA5" s="87"/>
-      <c r="AB5" s="72">
+      <c r="Z5" s="71"/>
+      <c r="AA5" s="71"/>
+      <c r="AB5" s="60">
         <v>41394</v>
       </c>
-      <c r="AC5" s="72"/>
-      <c r="AD5" s="72"/>
-      <c r="AE5" s="72">
+      <c r="AC5" s="60"/>
+      <c r="AD5" s="60"/>
+      <c r="AE5" s="60">
         <v>41388</v>
       </c>
-      <c r="AF5" s="72"/>
-      <c r="AG5" s="72"/>
-      <c r="AH5" s="72">
+      <c r="AF5" s="60"/>
+      <c r="AG5" s="60"/>
+      <c r="AH5" s="60">
         <v>41388</v>
       </c>
-      <c r="AI5" s="72"/>
-      <c r="AJ5" s="72"/>
-      <c r="AK5" s="72">
+      <c r="AI5" s="60"/>
+      <c r="AJ5" s="60"/>
+      <c r="AK5" s="60">
         <v>41571</v>
       </c>
-      <c r="AL5" s="72"/>
-      <c r="AM5" s="72"/>
-      <c r="AN5" s="72">
+      <c r="AL5" s="60"/>
+      <c r="AM5" s="60"/>
+      <c r="AN5" s="60">
         <v>41600</v>
       </c>
-      <c r="AO5" s="72"/>
-      <c r="AP5" s="72"/>
-      <c r="AQ5" s="72">
+      <c r="AO5" s="60"/>
+      <c r="AP5" s="60"/>
+      <c r="AQ5" s="60">
         <v>41431</v>
       </c>
-      <c r="AR5" s="72"/>
-      <c r="AS5" s="72"/>
-      <c r="AT5" s="65">
+      <c r="AR5" s="60"/>
+      <c r="AS5" s="60"/>
+      <c r="AT5" s="87">
         <v>41618</v>
       </c>
-      <c r="AU5" s="66"/>
-      <c r="AV5" s="67"/>
-      <c r="AW5" s="62">
+      <c r="AU5" s="88"/>
+      <c r="AV5" s="89"/>
+      <c r="AW5" s="72">
         <v>41435</v>
       </c>
-      <c r="AX5" s="63"/>
-      <c r="AY5" s="64"/>
-      <c r="AZ5" s="62">
+      <c r="AX5" s="73"/>
+      <c r="AY5" s="74"/>
+      <c r="AZ5" s="72">
         <v>41449</v>
       </c>
-      <c r="BA5" s="63"/>
-      <c r="BB5" s="64"/>
-      <c r="BC5" s="62">
+      <c r="BA5" s="73"/>
+      <c r="BB5" s="74"/>
+      <c r="BC5" s="72">
         <v>41444</v>
       </c>
-      <c r="BD5" s="63"/>
-      <c r="BE5" s="64"/>
-      <c r="BF5" s="92">
+      <c r="BD5" s="73"/>
+      <c r="BE5" s="74"/>
+      <c r="BF5" s="65">
         <v>41585</v>
       </c>
-      <c r="BG5" s="92"/>
-      <c r="BH5" s="92"/>
-      <c r="BI5" s="72"/>
-      <c r="BJ5" s="72"/>
-      <c r="BK5" s="72"/>
+      <c r="BG5" s="65"/>
+      <c r="BH5" s="65"/>
+      <c r="BI5" s="60"/>
+      <c r="BJ5" s="60"/>
+      <c r="BK5" s="60"/>
     </row>
     <row r="6" spans="1:63" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="66" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="19" t="s">
         <v>34</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>35</v>
       </c>
       <c r="C6" s="20">
         <v>1</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" s="22">
         <v>0</v>
       </c>
       <c r="F6" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="H6" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="I6" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="26" t="s">
-        <v>40</v>
-      </c>
       <c r="J6" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M6" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N6" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O6" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P6" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q6" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R6" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S6" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T6" s="24"/>
       <c r="U6" s="24"/>
       <c r="V6" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="W6" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="X6" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y6" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z6" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA6" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB6" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="W6" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="X6" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y6" s="23" t="s">
+      <c r="AC6" s="67"/>
+      <c r="AD6" s="67"/>
+      <c r="AE6" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="Z6" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA6" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB6" s="83" t="s">
+      <c r="AF6" s="67"/>
+      <c r="AG6" s="67"/>
+      <c r="AH6" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="AC6" s="83"/>
-      <c r="AD6" s="83"/>
-      <c r="AE6" s="83" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF6" s="83"/>
-      <c r="AG6" s="83"/>
-      <c r="AH6" s="83" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI6" s="83"/>
-      <c r="AJ6" s="83"/>
+      <c r="AI6" s="67"/>
+      <c r="AJ6" s="67"/>
       <c r="AK6" s="27"/>
       <c r="AL6" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AM6" s="24"/>
       <c r="AN6" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AO6" s="24"/>
       <c r="AP6" s="24"/>
       <c r="AQ6" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AR6" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AS6" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AT6" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AU6" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AV6" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AW6" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AX6" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AY6" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AZ6" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BA6" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BB6" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BC6" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BD6" s="24"/>
       <c r="BE6" s="24"/>
       <c r="BF6" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BG6" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BH6" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BI6" s="27"/>
       <c r="BJ6" s="24"/>
       <c r="BK6" s="24"/>
     </row>
     <row r="7" spans="1:63" ht="42.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="82"/>
+      <c r="A7" s="66"/>
       <c r="B7" s="30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="20">
         <v>2</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="22">
         <v>0</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="31" t="s">
-        <v>48</v>
-      </c>
       <c r="I7" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J7" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K7" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M7" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N7" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O7" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P7" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q7" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R7" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S7" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T7" s="24"/>
       <c r="U7" s="24"/>
       <c r="V7" s="28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W7" s="28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="X7" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Y7" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Z7" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AA7" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB7" s="83"/>
-      <c r="AC7" s="83"/>
-      <c r="AD7" s="83"/>
-      <c r="AE7" s="83"/>
-      <c r="AF7" s="83"/>
-      <c r="AG7" s="83"/>
-      <c r="AH7" s="83"/>
-      <c r="AI7" s="83"/>
-      <c r="AJ7" s="83"/>
+        <v>41</v>
+      </c>
+      <c r="AB7" s="67"/>
+      <c r="AC7" s="67"/>
+      <c r="AD7" s="67"/>
+      <c r="AE7" s="67"/>
+      <c r="AF7" s="67"/>
+      <c r="AG7" s="67"/>
+      <c r="AH7" s="67"/>
+      <c r="AI7" s="67"/>
+      <c r="AJ7" s="67"/>
       <c r="AK7" s="27"/>
       <c r="AL7" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AM7" s="24"/>
       <c r="AN7" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AO7" s="24"/>
       <c r="AP7" s="24"/>
       <c r="AQ7" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AR7" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AS7" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AT7" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AU7" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AV7" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AW7" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AX7" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AY7" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AZ7" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BA7" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BB7" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BC7" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BD7" s="24"/>
       <c r="BE7" s="24"/>
       <c r="BF7" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BG7" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BH7" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BI7" s="27"/>
       <c r="BJ7" s="24"/>
       <c r="BK7" s="24"/>
     </row>
     <row r="8" spans="1:63" ht="43.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A8" s="82"/>
+      <c r="A8" s="66"/>
       <c r="B8" s="30"/>
       <c r="C8" s="20">
         <v>3</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" s="22">
         <v>0</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G8" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="H8" s="31" t="s">
-        <v>51</v>
-      </c>
       <c r="I8" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J8" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L8" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M8" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N8" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O8" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P8" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q8" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R8" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S8" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T8" s="24"/>
       <c r="U8" s="24"/>
       <c r="V8" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W8" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="X8" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Y8" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Z8" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AA8" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB8" s="83"/>
-      <c r="AC8" s="83"/>
-      <c r="AD8" s="83"/>
-      <c r="AE8" s="83"/>
-      <c r="AF8" s="83"/>
-      <c r="AG8" s="83"/>
-      <c r="AH8" s="83"/>
-      <c r="AI8" s="83"/>
-      <c r="AJ8" s="83"/>
+        <v>41</v>
+      </c>
+      <c r="AB8" s="67"/>
+      <c r="AC8" s="67"/>
+      <c r="AD8" s="67"/>
+      <c r="AE8" s="67"/>
+      <c r="AF8" s="67"/>
+      <c r="AG8" s="67"/>
+      <c r="AH8" s="67"/>
+      <c r="AI8" s="67"/>
+      <c r="AJ8" s="67"/>
       <c r="AK8" s="27"/>
       <c r="AL8" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AM8" s="24"/>
       <c r="AN8" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AO8" s="24"/>
       <c r="AP8" s="24"/>
       <c r="AQ8" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AR8" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AS8" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AT8" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AU8" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AV8" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AW8" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AX8" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AY8" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AZ8" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BA8" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BB8" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BC8" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BD8" s="24"/>
       <c r="BE8" s="24"/>
       <c r="BF8" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BG8" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BH8" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BI8" s="27"/>
       <c r="BJ8" s="24"/>
       <c r="BK8" s="24"/>
     </row>
     <row r="9" spans="1:63" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A9" s="82"/>
+      <c r="A9" s="66"/>
       <c r="B9" s="30"/>
       <c r="C9" s="20">
         <v>4</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E9" s="22">
         <v>0</v>
       </c>
       <c r="F9" s="55" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G9" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="H9" s="56" t="s">
-        <v>54</v>
-      </c>
       <c r="I9" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J9" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L9" s="40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M9" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N9" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O9" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P9" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q9" s="57" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R9" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S9" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T9" s="20"/>
       <c r="U9" s="24"/>
       <c r="V9" s="41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W9" s="42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="X9" s="43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Y9" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Z9" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA9" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB9" s="83"/>
-      <c r="AC9" s="83"/>
-      <c r="AD9" s="83"/>
-      <c r="AE9" s="83"/>
-      <c r="AF9" s="83"/>
-      <c r="AG9" s="83"/>
-      <c r="AH9" s="83"/>
-      <c r="AI9" s="83"/>
-      <c r="AJ9" s="83"/>
+        <v>41</v>
+      </c>
+      <c r="AB9" s="67"/>
+      <c r="AC9" s="67"/>
+      <c r="AD9" s="67"/>
+      <c r="AE9" s="67"/>
+      <c r="AF9" s="67"/>
+      <c r="AG9" s="67"/>
+      <c r="AH9" s="67"/>
+      <c r="AI9" s="67"/>
+      <c r="AJ9" s="67"/>
       <c r="AK9" s="27"/>
       <c r="AL9" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AM9" s="24"/>
       <c r="AN9" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AO9" s="20"/>
       <c r="AP9" s="24"/>
       <c r="AQ9" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AR9" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AS9" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AT9" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AU9" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AV9" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AW9" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AX9" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AY9" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AZ9" s="44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BA9" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BB9" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BC9" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BD9" s="20"/>
       <c r="BE9" s="24"/>
       <c r="BF9" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BG9" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BH9" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BI9" s="27"/>
       <c r="BJ9" s="20"/>
@@ -2381,40 +2388,46 @@
         <v>4</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E10" s="35">
         <v>1</v>
       </c>
       <c r="F10" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="G10" s="37" t="s">
+      <c r="H10" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="H10" s="38" t="s">
+      <c r="I10" s="26" t="s">
         <v>73</v>
-      </c>
-      <c r="I10" s="26" t="s">
-        <v>74</v>
       </c>
       <c r="J10" s="39"/>
       <c r="K10" s="20"/>
       <c r="L10" s="40"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="21"/>
+      <c r="M10" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="N10" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="O10" s="95" t="s">
+        <v>41</v>
+      </c>
       <c r="P10" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q10" s="57" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R10" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S10" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T10" s="20"/>
       <c r="U10" s="24"/>
@@ -2422,28 +2435,28 @@
       <c r="W10" s="42"/>
       <c r="X10" s="43"/>
       <c r="Y10" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Z10" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AA10" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="AB10" s="83"/>
-      <c r="AC10" s="83"/>
-      <c r="AD10" s="83"/>
-      <c r="AE10" s="83"/>
-      <c r="AF10" s="83"/>
-      <c r="AG10" s="83"/>
-      <c r="AH10" s="83"/>
-      <c r="AI10" s="83"/>
-      <c r="AJ10" s="83"/>
+        <v>80</v>
+      </c>
+      <c r="AB10" s="67"/>
+      <c r="AC10" s="67"/>
+      <c r="AD10" s="67"/>
+      <c r="AE10" s="67"/>
+      <c r="AF10" s="67"/>
+      <c r="AG10" s="67"/>
+      <c r="AH10" s="67"/>
+      <c r="AI10" s="67"/>
+      <c r="AJ10" s="67"/>
       <c r="AK10" s="27"/>
       <c r="AL10" s="20"/>
       <c r="AM10" s="24"/>
       <c r="AN10" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AO10" s="20"/>
       <c r="AP10" s="24"/>
@@ -2463,73 +2476,73 @@
       <c r="BD10" s="20"/>
       <c r="BE10" s="24"/>
       <c r="BF10" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BG10" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BH10" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BI10" s="27"/>
       <c r="BJ10" s="20"/>
       <c r="BK10" s="24"/>
     </row>
     <row r="11" spans="1:63" s="46" customFormat="1" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A11" s="84" t="s">
+      <c r="A11" s="68" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>55</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>56</v>
       </c>
       <c r="C11" s="24">
         <v>1</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" s="24">
         <v>0</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G11" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="45" t="s">
-        <v>59</v>
-      </c>
       <c r="I11" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K11" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L11" s="24"/>
       <c r="M11" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N11" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O11" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P11" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q11" s="57" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R11" s="57" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="S11" s="57" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T11" s="24"/>
       <c r="U11" s="24"/>
@@ -2537,23 +2550,23 @@
       <c r="W11" s="24"/>
       <c r="X11" s="24"/>
       <c r="Y11" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Z11" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AA11" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB11" s="83"/>
-      <c r="AC11" s="83"/>
-      <c r="AD11" s="83"/>
-      <c r="AE11" s="83"/>
-      <c r="AF11" s="83"/>
-      <c r="AG11" s="83"/>
-      <c r="AH11" s="83"/>
-      <c r="AI11" s="83"/>
-      <c r="AJ11" s="83"/>
+        <v>41</v>
+      </c>
+      <c r="AB11" s="67"/>
+      <c r="AC11" s="67"/>
+      <c r="AD11" s="67"/>
+      <c r="AE11" s="67"/>
+      <c r="AF11" s="67"/>
+      <c r="AG11" s="67"/>
+      <c r="AH11" s="67"/>
+      <c r="AI11" s="67"/>
+      <c r="AJ11" s="67"/>
       <c r="AK11" s="24"/>
       <c r="AL11" s="24"/>
       <c r="AM11" s="24"/>
@@ -2561,104 +2574,104 @@
       <c r="AO11" s="24"/>
       <c r="AP11" s="24"/>
       <c r="AQ11" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AR11" s="24"/>
       <c r="AS11" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AT11" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AU11" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AV11" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AW11" s="57" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AX11" s="57" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AY11" s="57" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AZ11" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BA11" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BB11" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BC11" s="24"/>
       <c r="BD11" s="24"/>
       <c r="BE11" s="24"/>
       <c r="BF11" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BG11" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BH11" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BI11" s="24"/>
       <c r="BJ11" s="24"/>
       <c r="BK11" s="24"/>
     </row>
     <row r="12" spans="1:63" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A12" s="84"/>
+      <c r="A12" s="68"/>
       <c r="B12" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" s="24">
         <v>2</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E12" s="24">
         <v>0</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G12" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="H12" s="45" t="s">
-        <v>63</v>
-      </c>
       <c r="I12" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J12" s="24"/>
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N12" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O12" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P12" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q12" s="57" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R12" s="57" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="S12" s="57" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T12" s="24"/>
       <c r="U12" s="24"/>
@@ -2666,23 +2679,23 @@
       <c r="W12" s="24"/>
       <c r="X12" s="24"/>
       <c r="Y12" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Z12" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AA12" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB12" s="83"/>
-      <c r="AC12" s="83"/>
-      <c r="AD12" s="83"/>
-      <c r="AE12" s="83"/>
-      <c r="AF12" s="83"/>
-      <c r="AG12" s="83"/>
-      <c r="AH12" s="83"/>
-      <c r="AI12" s="83"/>
-      <c r="AJ12" s="83"/>
+        <v>41</v>
+      </c>
+      <c r="AB12" s="67"/>
+      <c r="AC12" s="67"/>
+      <c r="AD12" s="67"/>
+      <c r="AE12" s="67"/>
+      <c r="AF12" s="67"/>
+      <c r="AG12" s="67"/>
+      <c r="AH12" s="67"/>
+      <c r="AI12" s="67"/>
+      <c r="AJ12" s="67"/>
       <c r="AK12" s="24"/>
       <c r="AL12" s="24"/>
       <c r="AM12" s="24"/>
@@ -2690,78 +2703,78 @@
       <c r="AO12" s="24"/>
       <c r="AP12" s="24"/>
       <c r="AQ12" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AR12" s="24"/>
       <c r="AS12" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AT12" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AU12" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AV12" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AW12" s="57" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AX12" s="57" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AY12" s="57" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AZ12" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BA12" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BB12" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BC12" s="24"/>
       <c r="BD12" s="24"/>
       <c r="BE12" s="24"/>
       <c r="BF12" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BG12" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BH12" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BI12" s="24"/>
       <c r="BJ12" s="24"/>
       <c r="BK12" s="24"/>
     </row>
     <row r="13" spans="1:63" ht="63" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A13" s="84"/>
+      <c r="A13" s="68"/>
       <c r="B13" s="30"/>
       <c r="C13" s="47">
         <v>3</v>
       </c>
       <c r="D13" s="48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E13" s="49">
         <v>0</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G13" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="H13" s="31" t="s">
-        <v>66</v>
-      </c>
       <c r="I13" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J13" s="24"/>
       <c r="K13" s="24"/>
@@ -2781,15 +2794,15 @@
       <c r="Y13" s="24"/>
       <c r="Z13" s="24"/>
       <c r="AA13" s="24"/>
-      <c r="AB13" s="83"/>
-      <c r="AC13" s="83"/>
-      <c r="AD13" s="83"/>
-      <c r="AE13" s="83"/>
-      <c r="AF13" s="83"/>
-      <c r="AG13" s="83"/>
-      <c r="AH13" s="83"/>
-      <c r="AI13" s="83"/>
-      <c r="AJ13" s="83"/>
+      <c r="AB13" s="67"/>
+      <c r="AC13" s="67"/>
+      <c r="AD13" s="67"/>
+      <c r="AE13" s="67"/>
+      <c r="AF13" s="67"/>
+      <c r="AG13" s="67"/>
+      <c r="AH13" s="67"/>
+      <c r="AI13" s="67"/>
+      <c r="AJ13" s="67"/>
       <c r="AK13" s="24"/>
       <c r="AL13" s="24"/>
       <c r="AM13" s="24"/>
@@ -2819,28 +2832,28 @@
       <c r="BK13" s="24"/>
     </row>
     <row r="14" spans="1:63" ht="45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A14" s="84"/>
+      <c r="A14" s="68"/>
       <c r="B14" s="51"/>
       <c r="C14" s="50">
         <v>4</v>
       </c>
       <c r="D14" s="48" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E14" s="49">
         <v>0</v>
       </c>
       <c r="F14" s="48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G14" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="H14" s="52" t="s">
-        <v>69</v>
-      </c>
       <c r="I14" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J14" s="53"/>
       <c r="K14" s="53"/>
@@ -2860,15 +2873,15 @@
       <c r="Y14" s="53"/>
       <c r="Z14" s="53"/>
       <c r="AA14" s="53"/>
-      <c r="AB14" s="83"/>
-      <c r="AC14" s="83"/>
-      <c r="AD14" s="83"/>
-      <c r="AE14" s="83"/>
-      <c r="AF14" s="83"/>
-      <c r="AG14" s="83"/>
-      <c r="AH14" s="83"/>
-      <c r="AI14" s="83"/>
-      <c r="AJ14" s="83"/>
+      <c r="AB14" s="67"/>
+      <c r="AC14" s="67"/>
+      <c r="AD14" s="67"/>
+      <c r="AE14" s="67"/>
+      <c r="AF14" s="67"/>
+      <c r="AG14" s="67"/>
+      <c r="AH14" s="67"/>
+      <c r="AI14" s="67"/>
+      <c r="AJ14" s="67"/>
       <c r="AK14" s="53"/>
       <c r="AL14" s="53"/>
       <c r="AM14" s="53"/>
@@ -2900,52 +2913,6 @@
     <row r="15" spans="1:63" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="BI3:BK3"/>
-    <mergeCell ref="BI4:BK4"/>
-    <mergeCell ref="BI5:BK5"/>
-    <mergeCell ref="BF3:BH3"/>
-    <mergeCell ref="BF4:BH4"/>
-    <mergeCell ref="BF5:BH5"/>
-    <mergeCell ref="AB5:AD5"/>
-    <mergeCell ref="AE5:AG5"/>
-    <mergeCell ref="AH5:AJ5"/>
-    <mergeCell ref="AQ5:AS5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="AB6:AD14"/>
-    <mergeCell ref="AE6:AG14"/>
-    <mergeCell ref="AH6:AJ14"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="V5:X5"/>
-    <mergeCell ref="Y5:AA5"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="AQ4:AS4"/>
-    <mergeCell ref="AT4:AV4"/>
-    <mergeCell ref="AW4:AY4"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="V4:X4"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="Y3:AA3"/>
-    <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="BC4:BE4"/>
-    <mergeCell ref="AZ4:BB4"/>
-    <mergeCell ref="BC3:BE3"/>
-    <mergeCell ref="BC5:BE5"/>
-    <mergeCell ref="AZ5:BB5"/>
     <mergeCell ref="AW3:AY3"/>
     <mergeCell ref="AZ3:BB3"/>
     <mergeCell ref="AB4:AD4"/>
@@ -2962,6 +2929,52 @@
     <mergeCell ref="AQ3:AS3"/>
     <mergeCell ref="AE4:AG4"/>
     <mergeCell ref="AH4:AJ4"/>
+    <mergeCell ref="BC4:BE4"/>
+    <mergeCell ref="AZ4:BB4"/>
+    <mergeCell ref="BC3:BE3"/>
+    <mergeCell ref="BC5:BE5"/>
+    <mergeCell ref="AZ5:BB5"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="Y3:AA3"/>
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="AQ4:AS4"/>
+    <mergeCell ref="AT4:AV4"/>
+    <mergeCell ref="AW4:AY4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="AB5:AD5"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AQ5:AS5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="AB6:AD14"/>
+    <mergeCell ref="AE6:AG14"/>
+    <mergeCell ref="AH6:AJ14"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="Y5:AA5"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="BI3:BK3"/>
+    <mergeCell ref="BI4:BK4"/>
+    <mergeCell ref="BI5:BK5"/>
+    <mergeCell ref="BF3:BH3"/>
+    <mergeCell ref="BF4:BH4"/>
+    <mergeCell ref="BF5:BH5"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Proper contribution of the results of the BPMN 2.0 Modeler for Visio (version 4.2.0)
</commit_message>
<xml_diff>
--- a/BPMN MIWG Test Case Structure.xlsx
+++ b/BPMN MIWG Test Case Structure.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="13830" yWindow="-15" windowWidth="13890" windowHeight="12870" tabRatio="631"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="90">
   <si>
     <t>Note: Tools that are not listed here have either not been tested or may not support both BPMN import and export.</t>
   </si>
@@ -376,11 +376,17 @@
   <si>
     <t>7.8.1</t>
   </si>
+  <si>
+    <t>Trisotech BPMN Visio Modeler</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -778,15 +784,105 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -802,99 +898,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="TableStyleLight1" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -979,9 +985,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1019,7 +1025,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1053,6 +1059,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1087,9 +1094,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1262,17 +1270,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AMN15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AQ1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BN9" sqref="BN9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="44.85546875" style="1"/>
@@ -1294,18 +1302,18 @@
       </c>
     </row>
     <row r="2" spans="1:63" ht="47.25" thickTop="1" thickBot="1">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85" t="s">
+      <c r="B2" s="78"/>
+      <c r="C2" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85" t="s">
+      <c r="D2" s="78"/>
+      <c r="E2" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="85"/>
+      <c r="F2" s="78"/>
       <c r="G2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1490,94 +1498,96 @@
       <c r="I3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="82" t="s">
+      <c r="J3" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="86" t="s">
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="86"/>
-      <c r="O3" s="86"/>
-      <c r="P3" s="58" t="s">
+      <c r="N3" s="79"/>
+      <c r="O3" s="79"/>
+      <c r="P3" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="58"/>
-      <c r="S3" s="82" t="s">
+      <c r="Q3" s="73"/>
+      <c r="R3" s="73"/>
+      <c r="S3" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="T3" s="83"/>
-      <c r="U3" s="84"/>
-      <c r="V3" s="58" t="s">
+      <c r="T3" s="61"/>
+      <c r="U3" s="62"/>
+      <c r="V3" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="W3" s="58"/>
-      <c r="X3" s="58"/>
-      <c r="Y3" s="58" t="s">
+      <c r="W3" s="73"/>
+      <c r="X3" s="73"/>
+      <c r="Y3" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="Z3" s="58"/>
-      <c r="AA3" s="58"/>
-      <c r="AB3" s="58" t="s">
+      <c r="Z3" s="73"/>
+      <c r="AA3" s="73"/>
+      <c r="AB3" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="AC3" s="58"/>
-      <c r="AD3" s="58"/>
-      <c r="AE3" s="58" t="s">
+      <c r="AC3" s="73"/>
+      <c r="AD3" s="73"/>
+      <c r="AE3" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="AF3" s="58"/>
-      <c r="AG3" s="58"/>
-      <c r="AH3" s="58" t="s">
+      <c r="AF3" s="73"/>
+      <c r="AG3" s="73"/>
+      <c r="AH3" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="AI3" s="58"/>
-      <c r="AJ3" s="58"/>
-      <c r="AK3" s="58" t="s">
+      <c r="AI3" s="73"/>
+      <c r="AJ3" s="73"/>
+      <c r="AK3" s="73" t="s">
         <v>75</v>
       </c>
-      <c r="AL3" s="58"/>
-      <c r="AM3" s="58"/>
-      <c r="AN3" s="58" t="s">
+      <c r="AL3" s="73"/>
+      <c r="AM3" s="73"/>
+      <c r="AN3" s="73" t="s">
         <v>82</v>
       </c>
-      <c r="AO3" s="58"/>
-      <c r="AP3" s="58"/>
-      <c r="AQ3" s="58" t="s">
+      <c r="AO3" s="73"/>
+      <c r="AP3" s="73"/>
+      <c r="AQ3" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="AR3" s="58"/>
-      <c r="AS3" s="58"/>
-      <c r="AT3" s="90" t="s">
+      <c r="AR3" s="73"/>
+      <c r="AS3" s="73"/>
+      <c r="AT3" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="AU3" s="91"/>
-      <c r="AV3" s="92"/>
-      <c r="AW3" s="82" t="s">
+      <c r="AU3" s="71"/>
+      <c r="AV3" s="72"/>
+      <c r="AW3" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="AX3" s="83"/>
-      <c r="AY3" s="84"/>
-      <c r="AZ3" s="82" t="s">
+      <c r="AX3" s="61"/>
+      <c r="AY3" s="62"/>
+      <c r="AZ3" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="BA3" s="83"/>
-      <c r="BB3" s="84"/>
-      <c r="BC3" s="82" t="s">
+      <c r="BA3" s="61"/>
+      <c r="BB3" s="62"/>
+      <c r="BC3" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="BD3" s="83"/>
-      <c r="BE3" s="84"/>
-      <c r="BF3" s="61" t="s">
+      <c r="BD3" s="61"/>
+      <c r="BE3" s="62"/>
+      <c r="BF3" s="91" t="s">
         <v>78</v>
       </c>
-      <c r="BG3" s="62"/>
-      <c r="BH3" s="63"/>
-      <c r="BI3" s="58"/>
-      <c r="BJ3" s="58"/>
-      <c r="BK3" s="58"/>
+      <c r="BG3" s="92"/>
+      <c r="BH3" s="93"/>
+      <c r="BI3" s="73" t="s">
+        <v>88</v>
+      </c>
+      <c r="BJ3" s="73"/>
+      <c r="BK3" s="73"/>
     </row>
     <row r="4" spans="1:63" s="15" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A4" s="12"/>
@@ -1591,94 +1601,96 @@
       <c r="I4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="78" t="s">
+      <c r="J4" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="78"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="93" t="s">
+      <c r="K4" s="75"/>
+      <c r="L4" s="75"/>
+      <c r="M4" s="83" t="s">
         <v>87</v>
       </c>
-      <c r="N4" s="59"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="59" t="s">
+      <c r="N4" s="63"/>
+      <c r="O4" s="63"/>
+      <c r="P4" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="Q4" s="59"/>
-      <c r="R4" s="59"/>
-      <c r="S4" s="78" t="s">
+      <c r="Q4" s="63"/>
+      <c r="R4" s="63"/>
+      <c r="S4" s="75" t="s">
         <v>77</v>
       </c>
-      <c r="T4" s="79"/>
-      <c r="U4" s="80"/>
-      <c r="V4" s="59" t="s">
+      <c r="T4" s="76"/>
+      <c r="U4" s="77"/>
+      <c r="V4" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="W4" s="59"/>
-      <c r="X4" s="59"/>
-      <c r="Y4" s="81" t="s">
+      <c r="W4" s="63"/>
+      <c r="X4" s="63"/>
+      <c r="Y4" s="84" t="s">
         <v>81</v>
       </c>
-      <c r="Z4" s="81"/>
-      <c r="AA4" s="81"/>
-      <c r="AB4" s="59" t="s">
+      <c r="Z4" s="84"/>
+      <c r="AA4" s="84"/>
+      <c r="AB4" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="AC4" s="59"/>
-      <c r="AD4" s="59"/>
-      <c r="AE4" s="59">
+      <c r="AC4" s="63"/>
+      <c r="AD4" s="63"/>
+      <c r="AE4" s="63">
         <v>2.4</v>
       </c>
-      <c r="AF4" s="59"/>
-      <c r="AG4" s="59"/>
-      <c r="AH4" s="59" t="s">
+      <c r="AF4" s="63"/>
+      <c r="AG4" s="63"/>
+      <c r="AH4" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="AI4" s="59"/>
-      <c r="AJ4" s="59"/>
-      <c r="AK4" s="59" t="s">
+      <c r="AI4" s="63"/>
+      <c r="AJ4" s="63"/>
+      <c r="AK4" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="AL4" s="59"/>
-      <c r="AM4" s="59"/>
-      <c r="AN4" s="59" t="s">
+      <c r="AL4" s="63"/>
+      <c r="AM4" s="63"/>
+      <c r="AN4" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="AO4" s="59"/>
-      <c r="AP4" s="59"/>
-      <c r="AQ4" s="59" t="s">
+      <c r="AO4" s="63"/>
+      <c r="AP4" s="63"/>
+      <c r="AQ4" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="AR4" s="59"/>
-      <c r="AS4" s="59"/>
-      <c r="AT4" s="75" t="s">
+      <c r="AR4" s="63"/>
+      <c r="AS4" s="63"/>
+      <c r="AT4" s="80" t="s">
         <v>85</v>
       </c>
-      <c r="AU4" s="76"/>
-      <c r="AV4" s="77"/>
-      <c r="AW4" s="78" t="s">
+      <c r="AU4" s="81"/>
+      <c r="AV4" s="82"/>
+      <c r="AW4" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="AX4" s="79"/>
-      <c r="AY4" s="80"/>
-      <c r="AZ4" s="78" t="s">
+      <c r="AX4" s="76"/>
+      <c r="AY4" s="77"/>
+      <c r="AZ4" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="BA4" s="79"/>
-      <c r="BB4" s="80"/>
-      <c r="BC4" s="78" t="s">
+      <c r="BA4" s="76"/>
+      <c r="BB4" s="77"/>
+      <c r="BC4" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="BD4" s="79"/>
-      <c r="BE4" s="80"/>
-      <c r="BF4" s="64" t="s">
+      <c r="BD4" s="76"/>
+      <c r="BE4" s="77"/>
+      <c r="BF4" s="94" t="s">
         <v>79</v>
       </c>
-      <c r="BG4" s="64"/>
-      <c r="BH4" s="64"/>
-      <c r="BI4" s="59"/>
-      <c r="BJ4" s="59"/>
-      <c r="BK4" s="59"/>
+      <c r="BG4" s="94"/>
+      <c r="BH4" s="94"/>
+      <c r="BI4" s="63" t="s">
+        <v>89</v>
+      </c>
+      <c r="BJ4" s="63"/>
+      <c r="BK4" s="63"/>
     </row>
     <row r="5" spans="1:63" ht="16.5" thickTop="1" thickBot="1">
       <c r="A5" s="16"/>
@@ -1692,97 +1704,99 @@
       <c r="I5" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="69">
+      <c r="J5" s="88">
         <v>41380</v>
       </c>
-      <c r="K5" s="69"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="70">
+      <c r="K5" s="88"/>
+      <c r="L5" s="88"/>
+      <c r="M5" s="89">
         <v>41715</v>
       </c>
-      <c r="N5" s="70"/>
-      <c r="O5" s="70"/>
-      <c r="P5" s="60">
+      <c r="N5" s="89"/>
+      <c r="O5" s="89"/>
+      <c r="P5" s="74">
         <v>41680</v>
       </c>
-      <c r="Q5" s="60"/>
-      <c r="R5" s="71"/>
-      <c r="S5" s="72">
+      <c r="Q5" s="74"/>
+      <c r="R5" s="90"/>
+      <c r="S5" s="64">
         <v>41591</v>
       </c>
-      <c r="T5" s="73"/>
-      <c r="U5" s="74"/>
-      <c r="V5" s="71">
+      <c r="T5" s="65"/>
+      <c r="U5" s="66"/>
+      <c r="V5" s="90">
         <v>41383</v>
       </c>
-      <c r="W5" s="71"/>
-      <c r="X5" s="71"/>
-      <c r="Y5" s="71">
+      <c r="W5" s="90"/>
+      <c r="X5" s="90"/>
+      <c r="Y5" s="90">
         <v>41599</v>
       </c>
-      <c r="Z5" s="71"/>
-      <c r="AA5" s="71"/>
-      <c r="AB5" s="60">
+      <c r="Z5" s="90"/>
+      <c r="AA5" s="90"/>
+      <c r="AB5" s="74">
         <v>41394</v>
       </c>
-      <c r="AC5" s="60"/>
-      <c r="AD5" s="60"/>
-      <c r="AE5" s="60">
+      <c r="AC5" s="74"/>
+      <c r="AD5" s="74"/>
+      <c r="AE5" s="74">
         <v>41388</v>
       </c>
-      <c r="AF5" s="60"/>
-      <c r="AG5" s="60"/>
-      <c r="AH5" s="60">
+      <c r="AF5" s="74"/>
+      <c r="AG5" s="74"/>
+      <c r="AH5" s="74">
         <v>41388</v>
       </c>
-      <c r="AI5" s="60"/>
-      <c r="AJ5" s="60"/>
-      <c r="AK5" s="60">
+      <c r="AI5" s="74"/>
+      <c r="AJ5" s="74"/>
+      <c r="AK5" s="74">
         <v>41571</v>
       </c>
-      <c r="AL5" s="60"/>
-      <c r="AM5" s="60"/>
-      <c r="AN5" s="60">
+      <c r="AL5" s="74"/>
+      <c r="AM5" s="74"/>
+      <c r="AN5" s="74">
         <v>41600</v>
       </c>
-      <c r="AO5" s="60"/>
-      <c r="AP5" s="60"/>
-      <c r="AQ5" s="60">
+      <c r="AO5" s="74"/>
+      <c r="AP5" s="74"/>
+      <c r="AQ5" s="74">
         <v>41431</v>
       </c>
-      <c r="AR5" s="60"/>
-      <c r="AS5" s="60"/>
-      <c r="AT5" s="87">
+      <c r="AR5" s="74"/>
+      <c r="AS5" s="74"/>
+      <c r="AT5" s="67">
         <v>41618</v>
       </c>
-      <c r="AU5" s="88"/>
-      <c r="AV5" s="89"/>
-      <c r="AW5" s="72">
+      <c r="AU5" s="68"/>
+      <c r="AV5" s="69"/>
+      <c r="AW5" s="64">
         <v>41435</v>
       </c>
-      <c r="AX5" s="73"/>
-      <c r="AY5" s="74"/>
-      <c r="AZ5" s="72">
+      <c r="AX5" s="65"/>
+      <c r="AY5" s="66"/>
+      <c r="AZ5" s="64">
         <v>41449</v>
       </c>
-      <c r="BA5" s="73"/>
-      <c r="BB5" s="74"/>
-      <c r="BC5" s="72">
+      <c r="BA5" s="65"/>
+      <c r="BB5" s="66"/>
+      <c r="BC5" s="64">
         <v>41444</v>
       </c>
-      <c r="BD5" s="73"/>
-      <c r="BE5" s="74"/>
-      <c r="BF5" s="65">
+      <c r="BD5" s="65"/>
+      <c r="BE5" s="66"/>
+      <c r="BF5" s="95">
         <v>41585</v>
       </c>
-      <c r="BG5" s="65"/>
-      <c r="BH5" s="65"/>
-      <c r="BI5" s="60"/>
-      <c r="BJ5" s="60"/>
-      <c r="BK5" s="60"/>
+      <c r="BG5" s="95"/>
+      <c r="BH5" s="95"/>
+      <c r="BI5" s="74">
+        <v>41716</v>
+      </c>
+      <c r="BJ5" s="74"/>
+      <c r="BK5" s="74"/>
     </row>
     <row r="6" spans="1:63" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="85" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="19" t="s">
@@ -1859,21 +1873,21 @@
       <c r="AA6" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="AB6" s="67" t="s">
+      <c r="AB6" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="AC6" s="67"/>
-      <c r="AD6" s="67"/>
-      <c r="AE6" s="67" t="s">
+      <c r="AC6" s="86"/>
+      <c r="AD6" s="86"/>
+      <c r="AE6" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="AF6" s="67"/>
-      <c r="AG6" s="67"/>
-      <c r="AH6" s="67" t="s">
+      <c r="AF6" s="86"/>
+      <c r="AG6" s="86"/>
+      <c r="AH6" s="86" t="s">
         <v>43</v>
       </c>
-      <c r="AI6" s="67"/>
-      <c r="AJ6" s="67"/>
+      <c r="AI6" s="86"/>
+      <c r="AJ6" s="86"/>
       <c r="AK6" s="27"/>
       <c r="AL6" s="24" t="s">
         <v>41</v>
@@ -1934,12 +1948,18 @@
       <c r="BH6" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="BI6" s="27"/>
-      <c r="BJ6" s="24"/>
-      <c r="BK6" s="24"/>
+      <c r="BI6" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="BJ6" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="BK6" s="24" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="7" spans="1:63" ht="42.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="66"/>
+      <c r="A7" s="85"/>
       <c r="B7" s="30" t="s">
         <v>44</v>
       </c>
@@ -2014,15 +2034,15 @@
       <c r="AA7" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="AB7" s="67"/>
-      <c r="AC7" s="67"/>
-      <c r="AD7" s="67"/>
-      <c r="AE7" s="67"/>
-      <c r="AF7" s="67"/>
-      <c r="AG7" s="67"/>
-      <c r="AH7" s="67"/>
-      <c r="AI7" s="67"/>
-      <c r="AJ7" s="67"/>
+      <c r="AB7" s="86"/>
+      <c r="AC7" s="86"/>
+      <c r="AD7" s="86"/>
+      <c r="AE7" s="86"/>
+      <c r="AF7" s="86"/>
+      <c r="AG7" s="86"/>
+      <c r="AH7" s="86"/>
+      <c r="AI7" s="86"/>
+      <c r="AJ7" s="86"/>
       <c r="AK7" s="27"/>
       <c r="AL7" s="24" t="s">
         <v>41</v>
@@ -2083,12 +2103,18 @@
       <c r="BH7" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="BI7" s="27"/>
-      <c r="BJ7" s="24"/>
-      <c r="BK7" s="24"/>
+      <c r="BI7" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="BJ7" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="BK7" s="24" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="8" spans="1:63" ht="43.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A8" s="66"/>
+      <c r="A8" s="85"/>
       <c r="B8" s="30"/>
       <c r="C8" s="20">
         <v>3</v>
@@ -2161,15 +2187,15 @@
       <c r="AA8" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="AB8" s="67"/>
-      <c r="AC8" s="67"/>
-      <c r="AD8" s="67"/>
-      <c r="AE8" s="67"/>
-      <c r="AF8" s="67"/>
-      <c r="AG8" s="67"/>
-      <c r="AH8" s="67"/>
-      <c r="AI8" s="67"/>
-      <c r="AJ8" s="67"/>
+      <c r="AB8" s="86"/>
+      <c r="AC8" s="86"/>
+      <c r="AD8" s="86"/>
+      <c r="AE8" s="86"/>
+      <c r="AF8" s="86"/>
+      <c r="AG8" s="86"/>
+      <c r="AH8" s="86"/>
+      <c r="AI8" s="86"/>
+      <c r="AJ8" s="86"/>
       <c r="AK8" s="27"/>
       <c r="AL8" s="24" t="s">
         <v>40</v>
@@ -2230,12 +2256,18 @@
       <c r="BH8" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="BI8" s="27"/>
-      <c r="BJ8" s="24"/>
-      <c r="BK8" s="24"/>
+      <c r="BI8" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="BJ8" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="BK8" s="24" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="9" spans="1:63" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A9" s="66"/>
+      <c r="A9" s="85"/>
       <c r="B9" s="30"/>
       <c r="C9" s="20">
         <v>4</v>
@@ -2308,15 +2340,15 @@
       <c r="AA9" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="AB9" s="67"/>
-      <c r="AC9" s="67"/>
-      <c r="AD9" s="67"/>
-      <c r="AE9" s="67"/>
-      <c r="AF9" s="67"/>
-      <c r="AG9" s="67"/>
-      <c r="AH9" s="67"/>
-      <c r="AI9" s="67"/>
-      <c r="AJ9" s="67"/>
+      <c r="AB9" s="86"/>
+      <c r="AC9" s="86"/>
+      <c r="AD9" s="86"/>
+      <c r="AE9" s="86"/>
+      <c r="AF9" s="86"/>
+      <c r="AG9" s="86"/>
+      <c r="AH9" s="86"/>
+      <c r="AI9" s="86"/>
+      <c r="AJ9" s="86"/>
       <c r="AK9" s="27"/>
       <c r="AL9" s="20" t="s">
         <v>40</v>
@@ -2377,9 +2409,15 @@
       <c r="BH9" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="BI9" s="27"/>
-      <c r="BJ9" s="20"/>
-      <c r="BK9" s="24"/>
+      <c r="BI9" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="BJ9" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="BK9" s="24" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="10" spans="1:63" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A10" s="54"/>
@@ -2408,13 +2446,13 @@
       <c r="J10" s="39"/>
       <c r="K10" s="20"/>
       <c r="L10" s="40"/>
-      <c r="M10" s="94" t="s">
-        <v>41</v>
-      </c>
-      <c r="N10" s="94" t="s">
-        <v>41</v>
-      </c>
-      <c r="O10" s="95" t="s">
+      <c r="M10" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="N10" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="O10" s="59" t="s">
         <v>41</v>
       </c>
       <c r="P10" s="20" t="s">
@@ -2443,15 +2481,15 @@
       <c r="AA10" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="AB10" s="67"/>
-      <c r="AC10" s="67"/>
-      <c r="AD10" s="67"/>
-      <c r="AE10" s="67"/>
-      <c r="AF10" s="67"/>
-      <c r="AG10" s="67"/>
-      <c r="AH10" s="67"/>
-      <c r="AI10" s="67"/>
-      <c r="AJ10" s="67"/>
+      <c r="AB10" s="86"/>
+      <c r="AC10" s="86"/>
+      <c r="AD10" s="86"/>
+      <c r="AE10" s="86"/>
+      <c r="AF10" s="86"/>
+      <c r="AG10" s="86"/>
+      <c r="AH10" s="86"/>
+      <c r="AI10" s="86"/>
+      <c r="AJ10" s="86"/>
       <c r="AK10" s="27"/>
       <c r="AL10" s="20"/>
       <c r="AM10" s="24"/>
@@ -2463,9 +2501,15 @@
       <c r="AQ10" s="24"/>
       <c r="AR10" s="20"/>
       <c r="AS10" s="24"/>
-      <c r="AT10" s="24"/>
-      <c r="AU10" s="24"/>
-      <c r="AV10" s="24"/>
+      <c r="AT10" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="AU10" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="AV10" s="24" t="s">
+        <v>41</v>
+      </c>
       <c r="AW10" s="21"/>
       <c r="AX10" s="21"/>
       <c r="AY10" s="21"/>
@@ -2484,12 +2528,18 @@
       <c r="BH10" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="BI10" s="27"/>
-      <c r="BJ10" s="20"/>
-      <c r="BK10" s="24"/>
+      <c r="BI10" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="BJ10" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="BK10" s="24" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" spans="1:63" s="46" customFormat="1" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A11" s="68" t="s">
+      <c r="A11" s="87" t="s">
         <v>54</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -2558,15 +2608,15 @@
       <c r="AA11" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="AB11" s="67"/>
-      <c r="AC11" s="67"/>
-      <c r="AD11" s="67"/>
-      <c r="AE11" s="67"/>
-      <c r="AF11" s="67"/>
-      <c r="AG11" s="67"/>
-      <c r="AH11" s="67"/>
-      <c r="AI11" s="67"/>
-      <c r="AJ11" s="67"/>
+      <c r="AB11" s="86"/>
+      <c r="AC11" s="86"/>
+      <c r="AD11" s="86"/>
+      <c r="AE11" s="86"/>
+      <c r="AF11" s="86"/>
+      <c r="AG11" s="86"/>
+      <c r="AH11" s="86"/>
+      <c r="AI11" s="86"/>
+      <c r="AJ11" s="86"/>
       <c r="AK11" s="24"/>
       <c r="AL11" s="24"/>
       <c r="AM11" s="24"/>
@@ -2619,12 +2669,18 @@
       <c r="BH11" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="BI11" s="24"/>
-      <c r="BJ11" s="24"/>
-      <c r="BK11" s="24"/>
+      <c r="BI11" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="BJ11" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="BK11" s="24" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="12" spans="1:63" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A12" s="68"/>
+      <c r="A12" s="87"/>
       <c r="B12" s="30" t="s">
         <v>59</v>
       </c>
@@ -2687,15 +2743,15 @@
       <c r="AA12" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="AB12" s="67"/>
-      <c r="AC12" s="67"/>
-      <c r="AD12" s="67"/>
-      <c r="AE12" s="67"/>
-      <c r="AF12" s="67"/>
-      <c r="AG12" s="67"/>
-      <c r="AH12" s="67"/>
-      <c r="AI12" s="67"/>
-      <c r="AJ12" s="67"/>
+      <c r="AB12" s="86"/>
+      <c r="AC12" s="86"/>
+      <c r="AD12" s="86"/>
+      <c r="AE12" s="86"/>
+      <c r="AF12" s="86"/>
+      <c r="AG12" s="86"/>
+      <c r="AH12" s="86"/>
+      <c r="AI12" s="86"/>
+      <c r="AJ12" s="86"/>
       <c r="AK12" s="24"/>
       <c r="AL12" s="24"/>
       <c r="AM12" s="24"/>
@@ -2748,12 +2804,18 @@
       <c r="BH12" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="BI12" s="24"/>
-      <c r="BJ12" s="24"/>
-      <c r="BK12" s="24"/>
+      <c r="BI12" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="BJ12" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="BK12" s="24" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="13" spans="1:63" ht="63" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A13" s="68"/>
+      <c r="A13" s="87"/>
       <c r="B13" s="30"/>
       <c r="C13" s="47">
         <v>3</v>
@@ -2794,15 +2856,15 @@
       <c r="Y13" s="24"/>
       <c r="Z13" s="24"/>
       <c r="AA13" s="24"/>
-      <c r="AB13" s="67"/>
-      <c r="AC13" s="67"/>
-      <c r="AD13" s="67"/>
-      <c r="AE13" s="67"/>
-      <c r="AF13" s="67"/>
-      <c r="AG13" s="67"/>
-      <c r="AH13" s="67"/>
-      <c r="AI13" s="67"/>
-      <c r="AJ13" s="67"/>
+      <c r="AB13" s="86"/>
+      <c r="AC13" s="86"/>
+      <c r="AD13" s="86"/>
+      <c r="AE13" s="86"/>
+      <c r="AF13" s="86"/>
+      <c r="AG13" s="86"/>
+      <c r="AH13" s="86"/>
+      <c r="AI13" s="86"/>
+      <c r="AJ13" s="86"/>
       <c r="AK13" s="24"/>
       <c r="AL13" s="24"/>
       <c r="AM13" s="24"/>
@@ -2832,7 +2894,7 @@
       <c r="BK13" s="24"/>
     </row>
     <row r="14" spans="1:63" ht="45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A14" s="68"/>
+      <c r="A14" s="87"/>
       <c r="B14" s="51"/>
       <c r="C14" s="50">
         <v>4</v>
@@ -2873,15 +2935,15 @@
       <c r="Y14" s="53"/>
       <c r="Z14" s="53"/>
       <c r="AA14" s="53"/>
-      <c r="AB14" s="67"/>
-      <c r="AC14" s="67"/>
-      <c r="AD14" s="67"/>
-      <c r="AE14" s="67"/>
-      <c r="AF14" s="67"/>
-      <c r="AG14" s="67"/>
-      <c r="AH14" s="67"/>
-      <c r="AI14" s="67"/>
-      <c r="AJ14" s="67"/>
+      <c r="AB14" s="86"/>
+      <c r="AC14" s="86"/>
+      <c r="AD14" s="86"/>
+      <c r="AE14" s="86"/>
+      <c r="AF14" s="86"/>
+      <c r="AG14" s="86"/>
+      <c r="AH14" s="86"/>
+      <c r="AI14" s="86"/>
+      <c r="AJ14" s="86"/>
       <c r="AK14" s="53"/>
       <c r="AL14" s="53"/>
       <c r="AM14" s="53"/>
@@ -2913,6 +2975,52 @@
     <row r="15" spans="1:63" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="62">
+    <mergeCell ref="BI3:BK3"/>
+    <mergeCell ref="BI4:BK4"/>
+    <mergeCell ref="BI5:BK5"/>
+    <mergeCell ref="BF3:BH3"/>
+    <mergeCell ref="BF4:BH4"/>
+    <mergeCell ref="BF5:BH5"/>
+    <mergeCell ref="AB5:AD5"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AQ5:AS5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="AB6:AD14"/>
+    <mergeCell ref="AE6:AG14"/>
+    <mergeCell ref="AH6:AJ14"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="Y5:AA5"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="AQ4:AS4"/>
+    <mergeCell ref="AT4:AV4"/>
+    <mergeCell ref="AW4:AY4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="Y3:AA3"/>
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="BC4:BE4"/>
+    <mergeCell ref="AZ4:BB4"/>
+    <mergeCell ref="BC3:BE3"/>
+    <mergeCell ref="BC5:BE5"/>
+    <mergeCell ref="AZ5:BB5"/>
     <mergeCell ref="AW3:AY3"/>
     <mergeCell ref="AZ3:BB3"/>
     <mergeCell ref="AB4:AD4"/>
@@ -2929,52 +3037,6 @@
     <mergeCell ref="AQ3:AS3"/>
     <mergeCell ref="AE4:AG4"/>
     <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="BC4:BE4"/>
-    <mergeCell ref="AZ4:BB4"/>
-    <mergeCell ref="BC3:BE3"/>
-    <mergeCell ref="BC5:BE5"/>
-    <mergeCell ref="AZ5:BB5"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="Y3:AA3"/>
-    <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="AQ4:AS4"/>
-    <mergeCell ref="AT4:AV4"/>
-    <mergeCell ref="AW4:AY4"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="V4:X4"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="AB5:AD5"/>
-    <mergeCell ref="AE5:AG5"/>
-    <mergeCell ref="AH5:AJ5"/>
-    <mergeCell ref="AQ5:AS5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="AB6:AD14"/>
-    <mergeCell ref="AE6:AG14"/>
-    <mergeCell ref="AH6:AJ14"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="V5:X5"/>
-    <mergeCell ref="Y5:AA5"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="BI3:BK3"/>
-    <mergeCell ref="BI4:BK4"/>
-    <mergeCell ref="BI5:BK5"/>
-    <mergeCell ref="BF3:BH3"/>
-    <mergeCell ref="BF4:BH4"/>
-    <mergeCell ref="BF5:BH5"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>